<commit_message>
update effort log 27/11 - Khang
</commit_message>
<xml_diff>
--- a/1. Project management/9. Timelog/individual time log/AS_PM_TimeLog_DeadlineTeam_KhangHuynh.xlsx
+++ b/1. Project management/9. Timelog/individual time log/AS_PM_TimeLog_DeadlineTeam_KhangHuynh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19440" windowHeight="7695" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="List main task" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="137">
   <si>
     <t>Week</t>
   </si>
@@ -342,9 +342,6 @@
     <t>Review Requirement Plan, Architert Plan, Master Plan, Mapping with Scrum and ACDM</t>
   </si>
   <si>
-    <t>Devide work task about ACDM</t>
-  </si>
-  <si>
     <t>Conduct work assign</t>
   </si>
   <si>
@@ -443,6 +440,22 @@
   </si>
   <si>
     <t>Miss file Measurement Template</t>
+  </si>
+  <si>
+    <t>3:50PM</t>
+  </si>
+  <si>
+    <t>Raise some question for future system</t>
+  </si>
+  <si>
+    <t>4:20PM</t>
+  </si>
+  <si>
+    <t>Collect questions from members
+Establish meeting with customer</t>
+  </si>
+  <si>
+    <t>Question - Tong hop</t>
   </si>
 </sst>
 </file>
@@ -957,6 +970,63 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -966,13 +1036,130 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -982,180 +1169,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1468,7 +1481,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1591,13 +1604,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O179"/>
+  <dimension ref="A1:O180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="6" topLeftCell="G19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="6" topLeftCell="G34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomRight" activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1618,81 +1631,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="121"/>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122"/>
-      <c r="K1" s="122"/>
-      <c r="L1" s="122"/>
-      <c r="M1" s="122"/>
-      <c r="N1" s="123"/>
+      <c r="A1" s="73"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="75"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="104"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="124" t="s">
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="125"/>
-      <c r="I2" s="125"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="125"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="126"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="78"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="106" t="s">
+      <c r="A3" s="97" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="107"/>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="128"/>
-      <c r="M3" s="128"/>
-      <c r="N3" s="129"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="81"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="109"/>
-      <c r="B4" s="110"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="111"/>
-      <c r="G4" s="130"/>
-      <c r="H4" s="131"/>
-      <c r="I4" s="131"/>
-      <c r="J4" s="131"/>
-      <c r="K4" s="131"/>
-      <c r="L4" s="131"/>
-      <c r="M4" s="131"/>
-      <c r="N4" s="132"/>
+      <c r="A4" s="100"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="84"/>
     </row>
     <row r="5" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="116"/>
-      <c r="B5" s="117"/>
-      <c r="C5" s="117"/>
-      <c r="D5" s="117"/>
-      <c r="E5" s="118"/>
+      <c r="A5" s="107"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="109"/>
       <c r="F5" s="15"/>
       <c r="H5" s="41" t="s">
         <v>64</v>
@@ -1737,13 +1750,13 @@
       <c r="J6" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="136"/>
-      <c r="L6" s="136"/>
-      <c r="M6" s="136"/>
-      <c r="N6" s="136"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="88"/>
+      <c r="M6" s="88"/>
+      <c r="N6" s="88"/>
     </row>
     <row r="7" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="133">
+      <c r="A7" s="85">
         <v>1</v>
       </c>
       <c r="B7" s="16">
@@ -1769,21 +1782,21 @@
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="29"/>
-      <c r="K7" s="81" t="s">
+      <c r="K7" s="115" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="81"/>
+      <c r="L7" s="115"/>
       <c r="M7" s="32">
-        <f>SUM(M8:M53)</f>
-        <v>50.489999999999995</v>
+        <f>SUM(M8:M54)</f>
+        <v>53.319999999999993</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="134"/>
-      <c r="B8" s="112">
+      <c r="A8" s="86"/>
+      <c r="B8" s="103">
         <v>41586</v>
       </c>
       <c r="C8" s="17">
@@ -1795,7 +1808,7 @@
       <c r="E8" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="114">
+      <c r="F8" s="105">
         <v>1.67</v>
       </c>
       <c r="G8" s="19" t="s">
@@ -1819,8 +1832,8 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="135"/>
-      <c r="B9" s="113"/>
+      <c r="A9" s="87"/>
+      <c r="B9" s="104"/>
       <c r="C9" s="17">
         <v>0.63194444444444442</v>
       </c>
@@ -1830,7 +1843,7 @@
       <c r="E9" s="18">
         <v>0.5</v>
       </c>
-      <c r="F9" s="115"/>
+      <c r="F9" s="106"/>
       <c r="G9" s="29" t="s">
         <v>23</v>
       </c>
@@ -1841,10 +1854,10 @@
       <c r="J9" s="29"/>
     </row>
     <row r="10" spans="1:15" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="90">
+      <c r="A10" s="124">
         <v>2</v>
       </c>
-      <c r="B10" s="93">
+      <c r="B10" s="127">
         <v>41589</v>
       </c>
       <c r="C10" s="58" t="s">
@@ -1856,7 +1869,7 @@
       <c r="E10" s="59">
         <v>2.5</v>
       </c>
-      <c r="F10" s="95">
+      <c r="F10" s="129">
         <f>SUM(E10:E11)</f>
         <v>5</v>
       </c>
@@ -1870,8 +1883,8 @@
       <c r="J10" s="60"/>
     </row>
     <row r="11" spans="1:15" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="91"/>
-      <c r="B11" s="94"/>
+      <c r="A11" s="125"/>
+      <c r="B11" s="128"/>
       <c r="C11" s="58" t="s">
         <v>76</v>
       </c>
@@ -1881,7 +1894,7 @@
       <c r="E11" s="59">
         <v>2.5</v>
       </c>
-      <c r="F11" s="96"/>
+      <c r="F11" s="130"/>
       <c r="G11" s="60" t="s">
         <v>22</v>
       </c>
@@ -1894,8 +1907,8 @@
       <c r="J11" s="60"/>
     </row>
     <row r="12" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="91"/>
-      <c r="B12" s="82">
+      <c r="A12" s="125"/>
+      <c r="B12" s="116">
         <v>41590</v>
       </c>
       <c r="C12" s="22">
@@ -1907,7 +1920,7 @@
       <c r="E12" s="23">
         <v>2.25</v>
       </c>
-      <c r="F12" s="84">
+      <c r="F12" s="118">
         <v>3.75</v>
       </c>
       <c r="G12" s="30" t="s">
@@ -1934,8 +1947,8 @@
       <c r="O12" s="34"/>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="91"/>
-      <c r="B13" s="83"/>
+      <c r="A13" s="125"/>
+      <c r="B13" s="117"/>
       <c r="C13" s="22">
         <v>0.91666666666666663</v>
       </c>
@@ -1945,7 +1958,7 @@
       <c r="E13" s="23">
         <v>1.5</v>
       </c>
-      <c r="F13" s="85"/>
+      <c r="F13" s="119"/>
       <c r="G13" s="45" t="s">
         <v>28</v>
       </c>
@@ -1961,8 +1974,8 @@
       <c r="O13" s="34"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="91"/>
-      <c r="B14" s="82">
+      <c r="A14" s="125"/>
+      <c r="B14" s="116">
         <v>41591</v>
       </c>
       <c r="C14" s="22">
@@ -1974,7 +1987,7 @@
       <c r="E14" s="23">
         <v>2</v>
       </c>
-      <c r="F14" s="87">
+      <c r="F14" s="121">
         <v>4.5</v>
       </c>
       <c r="G14" s="45" t="s">
@@ -1992,8 +2005,8 @@
       <c r="O14" s="34"/>
     </row>
     <row r="15" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="91"/>
-      <c r="B15" s="86"/>
+      <c r="A15" s="125"/>
+      <c r="B15" s="120"/>
       <c r="C15" s="25">
         <v>0.5625</v>
       </c>
@@ -2003,7 +2016,7 @@
       <c r="E15" s="28">
         <v>2</v>
       </c>
-      <c r="F15" s="88"/>
+      <c r="F15" s="122"/>
       <c r="G15" s="30" t="s">
         <v>19</v>
       </c>
@@ -2020,8 +2033,8 @@
       <c r="N15" s="3"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="91"/>
-      <c r="B16" s="83"/>
+      <c r="A16" s="125"/>
+      <c r="B16" s="117"/>
       <c r="C16" s="25">
         <v>0.83333333333333337</v>
       </c>
@@ -2031,7 +2044,7 @@
       <c r="E16" s="28">
         <v>0.5</v>
       </c>
-      <c r="F16" s="89"/>
+      <c r="F16" s="123"/>
       <c r="G16" s="45" t="s">
         <v>28</v>
       </c>
@@ -2055,7 +2068,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="91"/>
+      <c r="A17" s="125"/>
       <c r="B17" s="47">
         <v>41592</v>
       </c>
@@ -2082,19 +2095,19 @@
       </c>
       <c r="J17" s="37"/>
       <c r="K17" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="9">
-        <f>SUM(F33:F40)</f>
-        <v>8.75</v>
+        <f>SUM(F33:F41)</f>
+        <v>11.58</v>
       </c>
       <c r="N17" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="92"/>
+      <c r="A18" s="126"/>
       <c r="B18" s="42">
         <v>41593</v>
       </c>
@@ -2125,7 +2138,7 @@
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="9">
-        <f>SUM(E41:E45)</f>
+        <f>SUM(E42:E46)</f>
         <v>0</v>
       </c>
       <c r="N18" s="3" t="s">
@@ -2133,10 +2146,10 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="100">
+      <c r="A19" s="133">
         <v>3</v>
       </c>
-      <c r="B19" s="97">
+      <c r="B19" s="131">
         <v>41596</v>
       </c>
       <c r="C19" s="53" t="s">
@@ -2148,7 +2161,7 @@
       <c r="E19" s="50">
         <v>0.5</v>
       </c>
-      <c r="F19" s="99">
+      <c r="F19" s="89">
         <f>SUM(E19:E20)</f>
         <v>3.5</v>
       </c>
@@ -2167,7 +2180,7 @@
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="9">
-        <f>SUM(E56:E60)</f>
+        <f>SUM(E57:E61)</f>
         <v>0</v>
       </c>
       <c r="N19" s="3" t="s">
@@ -2175,8 +2188,8 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="101"/>
-      <c r="B20" s="98"/>
+      <c r="A20" s="134"/>
+      <c r="B20" s="132"/>
       <c r="C20" s="53" t="s">
         <v>81</v>
       </c>
@@ -2186,7 +2199,7 @@
       <c r="E20" s="50">
         <v>3</v>
       </c>
-      <c r="F20" s="77"/>
+      <c r="F20" s="90"/>
       <c r="G20" s="49" t="s">
         <v>22</v>
       </c>
@@ -2203,8 +2216,8 @@
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="101"/>
-      <c r="B21" s="97">
+      <c r="A21" s="134"/>
+      <c r="B21" s="131">
         <v>41597</v>
       </c>
       <c r="C21" s="53" t="s">
@@ -2216,7 +2229,7 @@
       <c r="E21" s="50">
         <v>2</v>
       </c>
-      <c r="F21" s="99">
+      <c r="F21" s="89">
         <f>SUM(E21:E22)</f>
         <v>2.5</v>
       </c>
@@ -2236,8 +2249,8 @@
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="101"/>
-      <c r="B22" s="98"/>
+      <c r="A22" s="134"/>
+      <c r="B22" s="132"/>
       <c r="C22" s="53" t="s">
         <v>84</v>
       </c>
@@ -2247,7 +2260,7 @@
       <c r="E22" s="50">
         <v>0.5</v>
       </c>
-      <c r="F22" s="77"/>
+      <c r="F22" s="90"/>
       <c r="G22" s="49" t="s">
         <v>22</v>
       </c>
@@ -2263,7 +2276,7 @@
       </c>
       <c r="L22" s="5"/>
       <c r="M22" s="9">
-        <f>SUM(E61:E65)</f>
+        <f>SUM(E62:E66)</f>
         <v>0</v>
       </c>
       <c r="N22" s="3" t="s">
@@ -2271,7 +2284,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="101"/>
+      <c r="A23" s="134"/>
       <c r="B23" s="26">
         <v>41598</v>
       </c>
@@ -2285,7 +2298,7 @@
         <v>4</v>
       </c>
       <c r="F23" s="55">
-        <f t="shared" ref="F23:F62" si="0">E23</f>
+        <f t="shared" ref="F23:F63" si="0">E23</f>
         <v>4</v>
       </c>
       <c r="G23" s="57" t="s">
@@ -2303,7 +2316,7 @@
       </c>
       <c r="L23" s="5"/>
       <c r="M23" s="9">
-        <f>SUM(E66:E70)</f>
+        <f>SUM(E67:E71)</f>
         <v>0</v>
       </c>
       <c r="N23" s="3" t="s">
@@ -2311,7 +2324,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="101"/>
+      <c r="A24" s="134"/>
       <c r="B24" s="26">
         <v>41599</v>
       </c>
@@ -2324,7 +2337,7 @@
       <c r="E24" s="50">
         <v>1</v>
       </c>
-      <c r="F24" s="99">
+      <c r="F24" s="89">
         <f>SUM(E24:E28)</f>
         <v>6.9</v>
       </c>
@@ -2342,7 +2355,7 @@
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="101"/>
+      <c r="A25" s="134"/>
       <c r="B25" s="26">
         <v>41599</v>
       </c>
@@ -2355,12 +2368,12 @@
       <c r="E25" s="50">
         <v>1.3</v>
       </c>
-      <c r="F25" s="119"/>
+      <c r="F25" s="112"/>
       <c r="G25" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="51" t="s">
-        <v>101</v>
+      <c r="H25" s="51">
+        <v>1</v>
       </c>
       <c r="I25" s="56"/>
       <c r="J25" s="39"/>
@@ -2370,7 +2383,7 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="101"/>
+      <c r="A26" s="134"/>
       <c r="B26" s="26">
         <v>41599</v>
       </c>
@@ -2383,15 +2396,15 @@
       <c r="E26" s="50">
         <v>1.5</v>
       </c>
-      <c r="F26" s="119"/>
+      <c r="F26" s="112"/>
       <c r="G26" s="57" t="s">
         <v>22</v>
       </c>
       <c r="H26" s="51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I26" s="56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J26" s="39"/>
       <c r="K26" s="7"/>
@@ -2400,7 +2413,7 @@
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="101"/>
+      <c r="A27" s="134"/>
       <c r="B27" s="26">
         <v>41599</v>
       </c>
@@ -2413,12 +2426,12 @@
       <c r="E27" s="50">
         <v>2.1</v>
       </c>
-      <c r="F27" s="119"/>
+      <c r="F27" s="112"/>
       <c r="G27" s="29" t="s">
         <v>19</v>
       </c>
       <c r="H27" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I27" s="29"/>
       <c r="J27" s="39"/>
@@ -2427,7 +2440,7 @@
       </c>
       <c r="L27" s="5"/>
       <c r="M27" s="9">
-        <f>SUM(E71:E75)</f>
+        <f>SUM(E72:E76)</f>
         <v>0</v>
       </c>
       <c r="N27" s="3" t="s">
@@ -2435,7 +2448,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="101"/>
+      <c r="A28" s="134"/>
       <c r="B28" s="26">
         <v>41599</v>
       </c>
@@ -2443,17 +2456,17 @@
         <v>76</v>
       </c>
       <c r="D28" s="64" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E28" s="50">
         <v>1</v>
       </c>
-      <c r="F28" s="120"/>
+      <c r="F28" s="113"/>
       <c r="G28" s="29" t="s">
         <v>22</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I28" s="29"/>
       <c r="J28" s="39"/>
@@ -2463,20 +2476,20 @@
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="101"/>
+      <c r="A29" s="134"/>
       <c r="B29" s="26">
         <v>41600</v>
       </c>
       <c r="C29" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" s="64" t="s">
         <v>107</v>
-      </c>
-      <c r="D29" s="64" t="s">
-        <v>108</v>
       </c>
       <c r="E29" s="50">
         <v>1.2</v>
       </c>
-      <c r="F29" s="99">
+      <c r="F29" s="89">
         <f>SUM(E29:E30)</f>
         <v>3.2</v>
       </c>
@@ -2492,25 +2505,25 @@
       <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:14" ht="51" x14ac:dyDescent="0.25">
-      <c r="A30" s="101"/>
+      <c r="A30" s="134"/>
       <c r="B30" s="26">
         <v>41600</v>
       </c>
       <c r="C30" s="55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D30" s="55" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E30" s="50">
         <v>2</v>
       </c>
-      <c r="F30" s="77"/>
+      <c r="F30" s="90"/>
       <c r="G30" s="57" t="s">
         <v>22</v>
       </c>
       <c r="H30" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I30" s="39"/>
       <c r="J30" s="39"/>
@@ -2519,7 +2532,7 @@
       </c>
       <c r="L30" s="5"/>
       <c r="M30" s="9">
-        <f>SUM(E76:E80)</f>
+        <f>SUM(E77:E81)</f>
         <v>0</v>
       </c>
       <c r="N30" s="3" t="s">
@@ -2527,20 +2540,20 @@
       </c>
     </row>
     <row r="31" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="101"/>
+      <c r="A31" s="134"/>
       <c r="B31" s="26">
         <v>41601</v>
       </c>
       <c r="C31" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="55" t="s">
         <v>111</v>
-      </c>
-      <c r="D31" s="55" t="s">
-        <v>112</v>
       </c>
       <c r="E31" s="50">
         <v>3.5</v>
       </c>
-      <c r="F31" s="99">
+      <c r="F31" s="89">
         <f>SUM(E31:E32)</f>
         <v>4.4000000000000004</v>
       </c>
@@ -2548,7 +2561,7 @@
         <v>22</v>
       </c>
       <c r="H31" s="65" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I31" s="56" t="s">
         <v>91</v>
@@ -2560,25 +2573,25 @@
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="102"/>
+      <c r="A32" s="135"/>
       <c r="B32" s="26">
         <v>41601</v>
       </c>
       <c r="C32" s="55" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" s="55" t="s">
         <v>114</v>
-      </c>
-      <c r="D32" s="55" t="s">
-        <v>115</v>
       </c>
       <c r="E32" s="50">
         <v>0.9</v>
       </c>
-      <c r="F32" s="77"/>
+      <c r="F32" s="90"/>
       <c r="G32" s="57" t="s">
         <v>22</v>
       </c>
       <c r="H32" s="65" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I32" s="56" t="s">
         <v>91</v>
@@ -2590,14 +2603,14 @@
       <c r="N32" s="3"/>
     </row>
     <row r="33" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="72">
+      <c r="A33" s="91">
         <v>4</v>
       </c>
       <c r="B33" s="27">
         <v>41603</v>
       </c>
       <c r="C33" s="69" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D33" s="69" t="s">
         <v>82</v>
@@ -2613,10 +2626,10 @@
         <v>22</v>
       </c>
       <c r="H33" s="71" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I33" s="67" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J33" s="67"/>
       <c r="K33" s="7" t="s">
@@ -2624,7 +2637,7 @@
       </c>
       <c r="L33" s="5"/>
       <c r="M33" s="9">
-        <f>SUM(E81:E85)</f>
+        <f>SUM(E82:E86)</f>
         <v>0</v>
       </c>
       <c r="N33" s="3" t="s">
@@ -2632,20 +2645,20 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="73"/>
+      <c r="A34" s="92"/>
       <c r="B34" s="27">
         <v>41604</v>
       </c>
       <c r="C34" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" s="69" t="s">
         <v>121</v>
-      </c>
-      <c r="D34" s="69" t="s">
-        <v>122</v>
       </c>
       <c r="E34" s="28">
         <v>1</v>
       </c>
-      <c r="F34" s="138">
+      <c r="F34" s="114">
         <f>SUM(E34:E37)</f>
         <v>5.75</v>
       </c>
@@ -2653,7 +2666,7 @@
         <v>22</v>
       </c>
       <c r="H34" s="71" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I34" s="67"/>
       <c r="J34" s="67"/>
@@ -2663,28 +2676,28 @@
       <c r="N34" s="3"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="73"/>
+      <c r="A35" s="92"/>
       <c r="B35" s="27">
         <v>41604</v>
       </c>
       <c r="C35" s="69" t="s">
-        <v>122</v>
-      </c>
-      <c r="D35" s="137" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="72" t="s">
         <v>77</v>
       </c>
       <c r="E35" s="28">
         <v>1.5</v>
       </c>
-      <c r="F35" s="73"/>
+      <c r="F35" s="92"/>
       <c r="G35" s="67" t="s">
         <v>23</v>
       </c>
       <c r="H35" s="71" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I35" s="67" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J35" s="67"/>
       <c r="K35" s="7"/>
@@ -2693,28 +2706,28 @@
       <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="73"/>
+      <c r="A36" s="92"/>
       <c r="B36" s="27">
         <v>41604</v>
       </c>
       <c r="C36" s="69" t="s">
-        <v>107</v>
-      </c>
-      <c r="D36" s="137" t="s">
-        <v>123</v>
+        <v>106</v>
+      </c>
+      <c r="D36" s="72" t="s">
+        <v>122</v>
       </c>
       <c r="E36" s="28">
         <v>1.25</v>
       </c>
-      <c r="F36" s="73"/>
+      <c r="F36" s="92"/>
       <c r="G36" s="67" t="s">
         <v>19</v>
       </c>
       <c r="H36" s="71" t="s">
+        <v>126</v>
+      </c>
+      <c r="I36" s="67" t="s">
         <v>127</v>
-      </c>
-      <c r="I36" s="67" t="s">
-        <v>128</v>
       </c>
       <c r="J36" s="67"/>
       <c r="K36" s="7"/>
@@ -2723,38 +2736,38 @@
       <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14" ht="51" x14ac:dyDescent="0.25">
-      <c r="A37" s="73"/>
+      <c r="A37" s="92"/>
       <c r="B37" s="27">
         <v>41604</v>
       </c>
       <c r="C37" s="69" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" s="69" t="s">
         <v>123</v>
-      </c>
-      <c r="D37" s="69" t="s">
-        <v>124</v>
       </c>
       <c r="E37" s="69">
         <v>2</v>
       </c>
-      <c r="F37" s="74"/>
+      <c r="F37" s="93"/>
       <c r="G37" s="67" t="s">
         <v>22</v>
       </c>
       <c r="H37" s="71" t="s">
+        <v>130</v>
+      </c>
+      <c r="I37" s="71" t="s">
+        <v>129</v>
+      </c>
+      <c r="J37" s="67" t="s">
         <v>131</v>
-      </c>
-      <c r="I37" s="71" t="s">
-        <v>130</v>
-      </c>
-      <c r="J37" s="67" t="s">
-        <v>132</v>
       </c>
       <c r="K37" s="7" t="s">
         <v>37</v>
       </c>
       <c r="L37" s="5"/>
       <c r="M37" s="9">
-        <f>SUM(E86:E90)</f>
+        <f>SUM(E87:E91)</f>
         <v>0</v>
       </c>
       <c r="N37" s="3" t="s">
@@ -2762,19 +2775,29 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="73"/>
+      <c r="A38" s="92"/>
       <c r="B38" s="27">
         <v>41605</v>
       </c>
-      <c r="C38" s="69"/>
-      <c r="D38" s="69"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="69">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G38" s="67"/>
-      <c r="H38" s="67"/>
+      <c r="C38" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" s="69" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" s="69">
+        <v>2.33</v>
+      </c>
+      <c r="F38" s="91">
+        <f>SUM(E38:E39)</f>
+        <v>2.83</v>
+      </c>
+      <c r="G38" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="67" t="s">
+        <v>133</v>
+      </c>
       <c r="I38" s="67"/>
       <c r="J38" s="67"/>
       <c r="K38" s="7" t="s">
@@ -2782,45 +2805,47 @@
       </c>
       <c r="L38" s="5"/>
       <c r="M38" s="9">
-        <f>SUM(E91:E95)</f>
+        <f>SUM(E92:E96)</f>
         <v>0</v>
       </c>
       <c r="N38" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="73"/>
+    <row r="39" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="92"/>
       <c r="B39" s="27">
+        <v>41605</v>
+      </c>
+      <c r="C39" s="69" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="E39" s="69">
+        <v>0.5</v>
+      </c>
+      <c r="F39" s="93"/>
+      <c r="G39" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="I39" s="67" t="s">
+        <v>136</v>
+      </c>
+      <c r="J39" s="67"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="3"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="92"/>
+      <c r="B40" s="27">
         <v>41606</v>
-      </c>
-      <c r="C39" s="69"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="69">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G39" s="67"/>
-      <c r="H39" s="67"/>
-      <c r="I39" s="67"/>
-      <c r="J39" s="67"/>
-      <c r="K39" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L39" s="5"/>
-      <c r="M39" s="9">
-        <f>SUM(E96:E100)</f>
-        <v>0</v>
-      </c>
-      <c r="N39" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="74"/>
-      <c r="B40" s="27">
-        <v>41607</v>
       </c>
       <c r="C40" s="69"/>
       <c r="D40" s="69"/>
@@ -2834,11 +2859,11 @@
       <c r="I40" s="67"/>
       <c r="J40" s="67"/>
       <c r="K40" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L40" s="5"/>
       <c r="M40" s="9">
-        <f>SUM(E101:E105)</f>
+        <f>SUM(E97:E101)</f>
         <v>0</v>
       </c>
       <c r="N40" s="3" t="s">
@@ -2846,29 +2871,27 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="75">
-        <v>5</v>
-      </c>
-      <c r="B41" s="26">
-        <v>41610</v>
-      </c>
-      <c r="C41" s="55"/>
-      <c r="D41" s="55"/>
-      <c r="E41" s="55"/>
-      <c r="F41" s="55">
+      <c r="A41" s="93"/>
+      <c r="B41" s="27">
+        <v>41607</v>
+      </c>
+      <c r="C41" s="69"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="69">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
-      <c r="J41" s="29"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="67"/>
+      <c r="I41" s="67"/>
+      <c r="J41" s="67"/>
       <c r="K41" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L41" s="5"/>
       <c r="M41" s="9">
-        <f>SUM(E106:E110)</f>
+        <f>SUM(E102:E106)</f>
         <v>0</v>
       </c>
       <c r="N41" s="3" t="s">
@@ -2876,9 +2899,11 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="76"/>
+      <c r="A42" s="110">
+        <v>5</v>
+      </c>
       <c r="B42" s="26">
-        <v>41611</v>
+        <v>41610</v>
       </c>
       <c r="C42" s="55"/>
       <c r="D42" s="55"/>
@@ -2892,11 +2917,11 @@
       <c r="I42" s="29"/>
       <c r="J42" s="29"/>
       <c r="K42" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="9">
-        <f>SUM(E111:E115)</f>
+        <f>SUM(E107:E111)</f>
         <v>0</v>
       </c>
       <c r="N42" s="3" t="s">
@@ -2904,9 +2929,9 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="76"/>
+      <c r="A43" s="111"/>
       <c r="B43" s="26">
-        <v>41612</v>
+        <v>41611</v>
       </c>
       <c r="C43" s="55"/>
       <c r="D43" s="55"/>
@@ -2920,11 +2945,11 @@
       <c r="I43" s="29"/>
       <c r="J43" s="29"/>
       <c r="K43" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L43" s="5"/>
       <c r="M43" s="9">
-        <f>SUM(E116:E120)</f>
+        <f>SUM(E112:E116)</f>
         <v>0</v>
       </c>
       <c r="N43" s="3" t="s">
@@ -2932,9 +2957,9 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="76"/>
+      <c r="A44" s="111"/>
       <c r="B44" s="26">
-        <v>41613</v>
+        <v>41612</v>
       </c>
       <c r="C44" s="55"/>
       <c r="D44" s="55"/>
@@ -2948,11 +2973,11 @@
       <c r="I44" s="29"/>
       <c r="J44" s="29"/>
       <c r="K44" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L44" s="5"/>
       <c r="M44" s="9">
-        <f>SUM(E121:E125)</f>
+        <f>SUM(E117:E121)</f>
         <v>0</v>
       </c>
       <c r="N44" s="3" t="s">
@@ -2960,9 +2985,9 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="77"/>
+      <c r="A45" s="111"/>
       <c r="B45" s="26">
-        <v>41614</v>
+        <v>41613</v>
       </c>
       <c r="C45" s="55"/>
       <c r="D45" s="55"/>
@@ -2976,11 +3001,11 @@
       <c r="I45" s="29"/>
       <c r="J45" s="29"/>
       <c r="K45" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L45" s="5"/>
       <c r="M45" s="9">
-        <f>SUM(E126:E130)</f>
+        <f>SUM(E122:E126)</f>
         <v>0</v>
       </c>
       <c r="N45" s="3" t="s">
@@ -2988,29 +3013,27 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="72">
-        <v>6</v>
-      </c>
-      <c r="B46" s="27">
-        <v>41617</v>
-      </c>
-      <c r="C46" s="69"/>
-      <c r="D46" s="69"/>
-      <c r="E46" s="69"/>
-      <c r="F46" s="69">
+      <c r="A46" s="90"/>
+      <c r="B46" s="26">
+        <v>41614</v>
+      </c>
+      <c r="C46" s="55"/>
+      <c r="D46" s="55"/>
+      <c r="E46" s="55"/>
+      <c r="F46" s="55">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G46" s="67"/>
-      <c r="H46" s="67"/>
-      <c r="I46" s="67"/>
-      <c r="J46" s="67"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
       <c r="K46" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L46" s="5"/>
       <c r="M46" s="9">
-        <f>SUM(E131:E135)</f>
+        <f>SUM(E127:E131)</f>
         <v>0</v>
       </c>
       <c r="N46" s="3" t="s">
@@ -3018,9 +3041,11 @@
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="73"/>
+      <c r="A47" s="91">
+        <v>6</v>
+      </c>
       <c r="B47" s="27">
-        <v>41618</v>
+        <v>41617</v>
       </c>
       <c r="C47" s="69"/>
       <c r="D47" s="69"/>
@@ -3034,11 +3059,11 @@
       <c r="I47" s="67"/>
       <c r="J47" s="67"/>
       <c r="K47" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L47" s="5"/>
       <c r="M47" s="9">
-        <f>SUM(E136:E140)</f>
+        <f>SUM(E132:E136)</f>
         <v>0</v>
       </c>
       <c r="N47" s="3" t="s">
@@ -3046,9 +3071,9 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="73"/>
+      <c r="A48" s="92"/>
       <c r="B48" s="27">
-        <v>41619</v>
+        <v>41618</v>
       </c>
       <c r="C48" s="69"/>
       <c r="D48" s="69"/>
@@ -3062,11 +3087,11 @@
       <c r="I48" s="67"/>
       <c r="J48" s="67"/>
       <c r="K48" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L48" s="5"/>
       <c r="M48" s="9">
-        <f>SUM(E141:E145)</f>
+        <f>SUM(E137:E141)</f>
         <v>0</v>
       </c>
       <c r="N48" s="3" t="s">
@@ -3074,9 +3099,9 @@
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="73"/>
+      <c r="A49" s="92"/>
       <c r="B49" s="27">
-        <v>41620</v>
+        <v>41619</v>
       </c>
       <c r="C49" s="69"/>
       <c r="D49" s="69"/>
@@ -3090,11 +3115,11 @@
       <c r="I49" s="67"/>
       <c r="J49" s="67"/>
       <c r="K49" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L49" s="5"/>
       <c r="M49" s="9">
-        <f>SUM(E146:E150)</f>
+        <f>SUM(E142:E146)</f>
         <v>0</v>
       </c>
       <c r="N49" s="3" t="s">
@@ -3102,9 +3127,9 @@
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="74"/>
+      <c r="A50" s="92"/>
       <c r="B50" s="27">
-        <v>41621</v>
+        <v>41620</v>
       </c>
       <c r="C50" s="69"/>
       <c r="D50" s="69"/>
@@ -3118,11 +3143,11 @@
       <c r="I50" s="67"/>
       <c r="J50" s="67"/>
       <c r="K50" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L50" s="5"/>
       <c r="M50" s="9">
-        <f>SUM(E151:E155)</f>
+        <f>SUM(E147:E151)</f>
         <v>0</v>
       </c>
       <c r="N50" s="3" t="s">
@@ -3130,29 +3155,27 @@
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="75">
-        <v>7</v>
-      </c>
-      <c r="B51" s="26">
-        <v>41624</v>
-      </c>
-      <c r="C51" s="55"/>
-      <c r="D51" s="55"/>
-      <c r="E51" s="55"/>
-      <c r="F51" s="55">
+      <c r="A51" s="93"/>
+      <c r="B51" s="27">
+        <v>41621</v>
+      </c>
+      <c r="C51" s="69"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="69">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G51" s="29"/>
-      <c r="H51" s="29"/>
-      <c r="I51" s="29"/>
-      <c r="J51" s="29"/>
+      <c r="G51" s="67"/>
+      <c r="H51" s="67"/>
+      <c r="I51" s="67"/>
+      <c r="J51" s="67"/>
       <c r="K51" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L51" s="5"/>
       <c r="M51" s="9">
-        <f>SUM(E156:E160)</f>
+        <f>SUM(E152:E156)</f>
         <v>0</v>
       </c>
       <c r="N51" s="3" t="s">
@@ -3160,9 +3183,11 @@
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="76"/>
+      <c r="A52" s="110">
+        <v>7</v>
+      </c>
       <c r="B52" s="26">
-        <v>41625</v>
+        <v>41624</v>
       </c>
       <c r="C52" s="55"/>
       <c r="D52" s="55"/>
@@ -3176,11 +3201,11 @@
       <c r="I52" s="29"/>
       <c r="J52" s="29"/>
       <c r="K52" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L52" s="5"/>
       <c r="M52" s="9">
-        <f>SUM(E161:E165)</f>
+        <f>SUM(E157:E161)</f>
         <v>0</v>
       </c>
       <c r="N52" s="3" t="s">
@@ -3188,9 +3213,9 @@
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="76"/>
+      <c r="A53" s="111"/>
       <c r="B53" s="26">
-        <v>41626</v>
+        <v>41625</v>
       </c>
       <c r="C53" s="55"/>
       <c r="D53" s="55"/>
@@ -3204,11 +3229,11 @@
       <c r="I53" s="29"/>
       <c r="J53" s="29"/>
       <c r="K53" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L53" s="5"/>
       <c r="M53" s="9">
-        <f>SUM(E166:E170)</f>
+        <f>SUM(E162:E166)</f>
         <v>0</v>
       </c>
       <c r="N53" s="3" t="s">
@@ -3216,9 +3241,9 @@
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="76"/>
+      <c r="A54" s="111"/>
       <c r="B54" s="26">
-        <v>41627</v>
+        <v>41626</v>
       </c>
       <c r="C54" s="55"/>
       <c r="D54" s="55"/>
@@ -3231,11 +3256,22 @@
       <c r="H54" s="29"/>
       <c r="I54" s="29"/>
       <c r="J54" s="29"/>
+      <c r="K54" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L54" s="5"/>
+      <c r="M54" s="9">
+        <f>SUM(E167:E171)</f>
+        <v>0</v>
+      </c>
+      <c r="N54" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="77"/>
+      <c r="A55" s="111"/>
       <c r="B55" s="26">
-        <v>41628</v>
+        <v>41627</v>
       </c>
       <c r="C55" s="55"/>
       <c r="D55" s="55"/>
@@ -3250,28 +3286,28 @@
       <c r="J55" s="29"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="72">
+      <c r="A56" s="90"/>
+      <c r="B56" s="26">
+        <v>41628</v>
+      </c>
+      <c r="C56" s="55"/>
+      <c r="D56" s="55"/>
+      <c r="E56" s="55"/>
+      <c r="F56" s="55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G56" s="29"/>
+      <c r="H56" s="29"/>
+      <c r="I56" s="29"/>
+      <c r="J56" s="29"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="91">
         <v>8</v>
       </c>
-      <c r="B56" s="27">
+      <c r="B57" s="27">
         <v>41631</v>
-      </c>
-      <c r="C56" s="69"/>
-      <c r="D56" s="69"/>
-      <c r="E56" s="69"/>
-      <c r="F56" s="69">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G56" s="67"/>
-      <c r="H56" s="67"/>
-      <c r="I56" s="67"/>
-      <c r="J56" s="67"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="73"/>
-      <c r="B57" s="27">
-        <v>41632</v>
       </c>
       <c r="C57" s="69"/>
       <c r="D57" s="69"/>
@@ -3286,9 +3322,9 @@
       <c r="J57" s="67"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="73"/>
+      <c r="A58" s="92"/>
       <c r="B58" s="27">
-        <v>41633</v>
+        <v>41632</v>
       </c>
       <c r="C58" s="69"/>
       <c r="D58" s="69"/>
@@ -3303,9 +3339,9 @@
       <c r="J58" s="67"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="73"/>
+      <c r="A59" s="92"/>
       <c r="B59" s="27">
-        <v>41634</v>
+        <v>41633</v>
       </c>
       <c r="C59" s="69"/>
       <c r="D59" s="69"/>
@@ -3320,9 +3356,9 @@
       <c r="J59" s="67"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="74"/>
+      <c r="A60" s="92"/>
       <c r="B60" s="27">
-        <v>41635</v>
+        <v>41634</v>
       </c>
       <c r="C60" s="69"/>
       <c r="D60" s="69"/>
@@ -3337,28 +3373,28 @@
       <c r="J60" s="67"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="75">
+      <c r="A61" s="93"/>
+      <c r="B61" s="27">
+        <v>41635</v>
+      </c>
+      <c r="C61" s="69"/>
+      <c r="D61" s="69"/>
+      <c r="E61" s="69"/>
+      <c r="F61" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G61" s="67"/>
+      <c r="H61" s="67"/>
+      <c r="I61" s="67"/>
+      <c r="J61" s="67"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="110">
         <v>9</v>
       </c>
-      <c r="B61" s="26">
+      <c r="B62" s="26">
         <v>41638</v>
-      </c>
-      <c r="C61" s="55"/>
-      <c r="D61" s="55"/>
-      <c r="E61" s="55"/>
-      <c r="F61" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G61" s="29"/>
-      <c r="H61" s="29"/>
-      <c r="I61" s="29"/>
-      <c r="J61" s="29"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="76"/>
-      <c r="B62" s="26">
-        <v>41639</v>
       </c>
       <c r="C62" s="55"/>
       <c r="D62" s="55"/>
@@ -3373,15 +3409,15 @@
       <c r="J62" s="29"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="76"/>
+      <c r="A63" s="111"/>
       <c r="B63" s="26">
-        <v>41640</v>
+        <v>41639</v>
       </c>
       <c r="C63" s="55"/>
       <c r="D63" s="55"/>
       <c r="E63" s="55"/>
       <c r="F63" s="55">
-        <f t="shared" ref="F63:F94" si="1">E63</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G63" s="29"/>
@@ -3390,15 +3426,15 @@
       <c r="J63" s="29"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="76"/>
+      <c r="A64" s="111"/>
       <c r="B64" s="26">
-        <v>41641</v>
+        <v>41640</v>
       </c>
       <c r="C64" s="55"/>
       <c r="D64" s="55"/>
       <c r="E64" s="55"/>
       <c r="F64" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F64:F95" si="1">E64</f>
         <v>0</v>
       </c>
       <c r="G64" s="29"/>
@@ -3407,9 +3443,9 @@
       <c r="J64" s="29"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="77"/>
+      <c r="A65" s="111"/>
       <c r="B65" s="26">
-        <v>41642</v>
+        <v>41641</v>
       </c>
       <c r="C65" s="55"/>
       <c r="D65" s="55"/>
@@ -3424,28 +3460,28 @@
       <c r="J65" s="29"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="72">
+      <c r="A66" s="90"/>
+      <c r="B66" s="26">
+        <v>41642</v>
+      </c>
+      <c r="C66" s="55"/>
+      <c r="D66" s="55"/>
+      <c r="E66" s="55"/>
+      <c r="F66" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G66" s="29"/>
+      <c r="H66" s="29"/>
+      <c r="I66" s="29"/>
+      <c r="J66" s="29"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="91">
         <v>10</v>
       </c>
-      <c r="B66" s="27">
+      <c r="B67" s="27">
         <v>41645</v>
-      </c>
-      <c r="C66" s="69"/>
-      <c r="D66" s="69"/>
-      <c r="E66" s="69"/>
-      <c r="F66" s="69">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G66" s="67"/>
-      <c r="H66" s="67"/>
-      <c r="I66" s="67"/>
-      <c r="J66" s="67"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="73"/>
-      <c r="B67" s="27">
-        <v>41646</v>
       </c>
       <c r="C67" s="69"/>
       <c r="D67" s="69"/>
@@ -3460,9 +3496,9 @@
       <c r="J67" s="67"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="73"/>
+      <c r="A68" s="92"/>
       <c r="B68" s="27">
-        <v>41647</v>
+        <v>41646</v>
       </c>
       <c r="C68" s="69"/>
       <c r="D68" s="69"/>
@@ -3477,9 +3513,9 @@
       <c r="J68" s="67"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="73"/>
+      <c r="A69" s="92"/>
       <c r="B69" s="27">
-        <v>41648</v>
+        <v>41647</v>
       </c>
       <c r="C69" s="69"/>
       <c r="D69" s="69"/>
@@ -3494,9 +3530,9 @@
       <c r="J69" s="67"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="74"/>
+      <c r="A70" s="92"/>
       <c r="B70" s="27">
-        <v>41649</v>
+        <v>41648</v>
       </c>
       <c r="C70" s="69"/>
       <c r="D70" s="69"/>
@@ -3511,28 +3547,28 @@
       <c r="J70" s="67"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="75">
+      <c r="A71" s="93"/>
+      <c r="B71" s="27">
+        <v>41649</v>
+      </c>
+      <c r="C71" s="69"/>
+      <c r="D71" s="69"/>
+      <c r="E71" s="69"/>
+      <c r="F71" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G71" s="67"/>
+      <c r="H71" s="67"/>
+      <c r="I71" s="67"/>
+      <c r="J71" s="67"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="110">
         <v>11</v>
       </c>
-      <c r="B71" s="26">
+      <c r="B72" s="26">
         <v>41652</v>
-      </c>
-      <c r="C71" s="55"/>
-      <c r="D71" s="55"/>
-      <c r="E71" s="55"/>
-      <c r="F71" s="55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G71" s="29"/>
-      <c r="H71" s="29"/>
-      <c r="I71" s="29"/>
-      <c r="J71" s="29"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="76"/>
-      <c r="B72" s="26">
-        <v>41653</v>
       </c>
       <c r="C72" s="55"/>
       <c r="D72" s="55"/>
@@ -3547,9 +3583,9 @@
       <c r="J72" s="29"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="76"/>
+      <c r="A73" s="111"/>
       <c r="B73" s="26">
-        <v>41654</v>
+        <v>41653</v>
       </c>
       <c r="C73" s="55"/>
       <c r="D73" s="55"/>
@@ -3564,9 +3600,9 @@
       <c r="J73" s="29"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="76"/>
+      <c r="A74" s="111"/>
       <c r="B74" s="26">
-        <v>41655</v>
+        <v>41654</v>
       </c>
       <c r="C74" s="55"/>
       <c r="D74" s="55"/>
@@ -3581,9 +3617,9 @@
       <c r="J74" s="29"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="77"/>
+      <c r="A75" s="111"/>
       <c r="B75" s="26">
-        <v>41656</v>
+        <v>41655</v>
       </c>
       <c r="C75" s="55"/>
       <c r="D75" s="55"/>
@@ -3598,28 +3634,28 @@
       <c r="J75" s="29"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="72">
+      <c r="A76" s="90"/>
+      <c r="B76" s="26">
+        <v>41656</v>
+      </c>
+      <c r="C76" s="55"/>
+      <c r="D76" s="55"/>
+      <c r="E76" s="55"/>
+      <c r="F76" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G76" s="29"/>
+      <c r="H76" s="29"/>
+      <c r="I76" s="29"/>
+      <c r="J76" s="29"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="91">
         <v>12</v>
       </c>
-      <c r="B76" s="27">
+      <c r="B77" s="27">
         <v>41659</v>
-      </c>
-      <c r="C76" s="69"/>
-      <c r="D76" s="69"/>
-      <c r="E76" s="69"/>
-      <c r="F76" s="69">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G76" s="67"/>
-      <c r="H76" s="67"/>
-      <c r="I76" s="67"/>
-      <c r="J76" s="67"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="73"/>
-      <c r="B77" s="27">
-        <v>41660</v>
       </c>
       <c r="C77" s="69"/>
       <c r="D77" s="69"/>
@@ -3634,9 +3670,9 @@
       <c r="J77" s="67"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="73"/>
+      <c r="A78" s="92"/>
       <c r="B78" s="27">
-        <v>41661</v>
+        <v>41660</v>
       </c>
       <c r="C78" s="69"/>
       <c r="D78" s="69"/>
@@ -3651,9 +3687,9 @@
       <c r="J78" s="67"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="73"/>
+      <c r="A79" s="92"/>
       <c r="B79" s="27">
-        <v>41662</v>
+        <v>41661</v>
       </c>
       <c r="C79" s="69"/>
       <c r="D79" s="69"/>
@@ -3668,9 +3704,9 @@
       <c r="J79" s="67"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="74"/>
+      <c r="A80" s="92"/>
       <c r="B80" s="27">
-        <v>41663</v>
+        <v>41662</v>
       </c>
       <c r="C80" s="69"/>
       <c r="D80" s="69"/>
@@ -3685,30 +3721,28 @@
       <c r="J80" s="67"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="75">
+      <c r="A81" s="93"/>
+      <c r="B81" s="27">
+        <v>41663</v>
+      </c>
+      <c r="C81" s="69"/>
+      <c r="D81" s="69"/>
+      <c r="E81" s="69"/>
+      <c r="F81" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G81" s="67"/>
+      <c r="H81" s="67"/>
+      <c r="I81" s="67"/>
+      <c r="J81" s="67"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="110">
         <v>13</v>
       </c>
-      <c r="B81" s="26">
+      <c r="B82" s="26">
         <v>41666</v>
-      </c>
-      <c r="C81" s="55"/>
-      <c r="D81" s="55"/>
-      <c r="E81" s="55"/>
-      <c r="F81" s="55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G81" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="H81" s="29"/>
-      <c r="I81" s="29"/>
-      <c r="J81" s="29"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="76"/>
-      <c r="B82" s="26">
-        <v>41667</v>
       </c>
       <c r="C82" s="55"/>
       <c r="D82" s="55"/>
@@ -3725,9 +3759,9 @@
       <c r="J82" s="29"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="76"/>
+      <c r="A83" s="111"/>
       <c r="B83" s="26">
-        <v>41668</v>
+        <v>41667</v>
       </c>
       <c r="C83" s="55"/>
       <c r="D83" s="55"/>
@@ -3744,9 +3778,9 @@
       <c r="J83" s="29"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="76"/>
+      <c r="A84" s="111"/>
       <c r="B84" s="26">
-        <v>41669</v>
+        <v>41668</v>
       </c>
       <c r="C84" s="55"/>
       <c r="D84" s="55"/>
@@ -3763,9 +3797,9 @@
       <c r="J84" s="29"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="77"/>
+      <c r="A85" s="111"/>
       <c r="B85" s="26">
-        <v>41670</v>
+        <v>41669</v>
       </c>
       <c r="C85" s="55"/>
       <c r="D85" s="55"/>
@@ -3782,30 +3816,30 @@
       <c r="J85" s="29"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="72">
+      <c r="A86" s="90"/>
+      <c r="B86" s="26">
+        <v>41670</v>
+      </c>
+      <c r="C86" s="55"/>
+      <c r="D86" s="55"/>
+      <c r="E86" s="55"/>
+      <c r="F86" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G86" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="H86" s="29"/>
+      <c r="I86" s="29"/>
+      <c r="J86" s="29"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="91">
         <v>14</v>
       </c>
-      <c r="B86" s="27">
+      <c r="B87" s="27">
         <v>41673</v>
-      </c>
-      <c r="C86" s="69"/>
-      <c r="D86" s="69"/>
-      <c r="E86" s="69"/>
-      <c r="F86" s="69">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G86" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="H86" s="67"/>
-      <c r="I86" s="67"/>
-      <c r="J86" s="67"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="73"/>
-      <c r="B87" s="27">
-        <v>41674</v>
       </c>
       <c r="C87" s="69"/>
       <c r="D87" s="69"/>
@@ -3822,9 +3856,9 @@
       <c r="J87" s="67"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="73"/>
+      <c r="A88" s="92"/>
       <c r="B88" s="27">
-        <v>41675</v>
+        <v>41674</v>
       </c>
       <c r="C88" s="69"/>
       <c r="D88" s="69"/>
@@ -3841,9 +3875,9 @@
       <c r="J88" s="67"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="73"/>
+      <c r="A89" s="92"/>
       <c r="B89" s="27">
-        <v>41676</v>
+        <v>41675</v>
       </c>
       <c r="C89" s="69"/>
       <c r="D89" s="69"/>
@@ -3860,9 +3894,9 @@
       <c r="J89" s="67"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="74"/>
+      <c r="A90" s="92"/>
       <c r="B90" s="27">
-        <v>41677</v>
+        <v>41676</v>
       </c>
       <c r="C90" s="69"/>
       <c r="D90" s="69"/>
@@ -3879,28 +3913,30 @@
       <c r="J90" s="67"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="75">
+      <c r="A91" s="93"/>
+      <c r="B91" s="27">
+        <v>41677</v>
+      </c>
+      <c r="C91" s="69"/>
+      <c r="D91" s="69"/>
+      <c r="E91" s="69"/>
+      <c r="F91" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G91" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="H91" s="67"/>
+      <c r="I91" s="67"/>
+      <c r="J91" s="67"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="110">
         <v>15</v>
       </c>
-      <c r="B91" s="26">
+      <c r="B92" s="26">
         <v>41680</v>
-      </c>
-      <c r="C91" s="55"/>
-      <c r="D91" s="55"/>
-      <c r="E91" s="55"/>
-      <c r="F91" s="55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G91" s="29"/>
-      <c r="H91" s="29"/>
-      <c r="I91" s="29"/>
-      <c r="J91" s="29"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="76"/>
-      <c r="B92" s="26">
-        <v>41681</v>
       </c>
       <c r="C92" s="55"/>
       <c r="D92" s="55"/>
@@ -3915,9 +3951,9 @@
       <c r="J92" s="29"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="76"/>
+      <c r="A93" s="111"/>
       <c r="B93" s="26">
-        <v>41682</v>
+        <v>41681</v>
       </c>
       <c r="C93" s="55"/>
       <c r="D93" s="55"/>
@@ -3932,9 +3968,9 @@
       <c r="J93" s="29"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="76"/>
+      <c r="A94" s="111"/>
       <c r="B94" s="26">
-        <v>41683</v>
+        <v>41682</v>
       </c>
       <c r="C94" s="55"/>
       <c r="D94" s="55"/>
@@ -3949,15 +3985,15 @@
       <c r="J94" s="29"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="77"/>
+      <c r="A95" s="111"/>
       <c r="B95" s="26">
-        <v>41684</v>
+        <v>41683</v>
       </c>
       <c r="C95" s="55"/>
       <c r="D95" s="55"/>
       <c r="E95" s="55"/>
       <c r="F95" s="55">
-        <f t="shared" ref="F95:F126" si="2">E95</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G95" s="29"/>
@@ -3966,28 +4002,28 @@
       <c r="J95" s="29"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="72">
+      <c r="A96" s="90"/>
+      <c r="B96" s="26">
+        <v>41684</v>
+      </c>
+      <c r="C96" s="55"/>
+      <c r="D96" s="55"/>
+      <c r="E96" s="55"/>
+      <c r="F96" s="55">
+        <f t="shared" ref="F96:F127" si="2">E96</f>
+        <v>0</v>
+      </c>
+      <c r="G96" s="29"/>
+      <c r="H96" s="29"/>
+      <c r="I96" s="29"/>
+      <c r="J96" s="29"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="91">
         <v>16</v>
       </c>
-      <c r="B96" s="27">
+      <c r="B97" s="27">
         <v>41687</v>
-      </c>
-      <c r="C96" s="69"/>
-      <c r="D96" s="69"/>
-      <c r="E96" s="69"/>
-      <c r="F96" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G96" s="67"/>
-      <c r="H96" s="67"/>
-      <c r="I96" s="67"/>
-      <c r="J96" s="67"/>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" s="73"/>
-      <c r="B97" s="27">
-        <v>41688</v>
       </c>
       <c r="C97" s="69"/>
       <c r="D97" s="69"/>
@@ -4002,9 +4038,9 @@
       <c r="J97" s="67"/>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" s="73"/>
+      <c r="A98" s="92"/>
       <c r="B98" s="27">
-        <v>41689</v>
+        <v>41688</v>
       </c>
       <c r="C98" s="69"/>
       <c r="D98" s="69"/>
@@ -4019,9 +4055,9 @@
       <c r="J98" s="67"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" s="73"/>
+      <c r="A99" s="92"/>
       <c r="B99" s="27">
-        <v>41690</v>
+        <v>41689</v>
       </c>
       <c r="C99" s="69"/>
       <c r="D99" s="69"/>
@@ -4036,9 +4072,9 @@
       <c r="J99" s="67"/>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" s="74"/>
+      <c r="A100" s="92"/>
       <c r="B100" s="27">
-        <v>41691</v>
+        <v>41690</v>
       </c>
       <c r="C100" s="69"/>
       <c r="D100" s="69"/>
@@ -4053,28 +4089,28 @@
       <c r="J100" s="67"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" s="75">
+      <c r="A101" s="93"/>
+      <c r="B101" s="27">
+        <v>41691</v>
+      </c>
+      <c r="C101" s="69"/>
+      <c r="D101" s="69"/>
+      <c r="E101" s="69"/>
+      <c r="F101" s="69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G101" s="67"/>
+      <c r="H101" s="67"/>
+      <c r="I101" s="67"/>
+      <c r="J101" s="67"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="110">
         <v>17</v>
       </c>
-      <c r="B101" s="26">
+      <c r="B102" s="26">
         <v>41694</v>
-      </c>
-      <c r="C101" s="55"/>
-      <c r="D101" s="55"/>
-      <c r="E101" s="55"/>
-      <c r="F101" s="55">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G101" s="29"/>
-      <c r="H101" s="29"/>
-      <c r="I101" s="29"/>
-      <c r="J101" s="29"/>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="76"/>
-      <c r="B102" s="26">
-        <v>41695</v>
       </c>
       <c r="C102" s="55"/>
       <c r="D102" s="55"/>
@@ -4089,9 +4125,9 @@
       <c r="J102" s="29"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" s="76"/>
+      <c r="A103" s="111"/>
       <c r="B103" s="26">
-        <v>41696</v>
+        <v>41695</v>
       </c>
       <c r="C103" s="55"/>
       <c r="D103" s="55"/>
@@ -4106,9 +4142,9 @@
       <c r="J103" s="29"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" s="76"/>
+      <c r="A104" s="111"/>
       <c r="B104" s="26">
-        <v>41697</v>
+        <v>41696</v>
       </c>
       <c r="C104" s="55"/>
       <c r="D104" s="55"/>
@@ -4123,9 +4159,9 @@
       <c r="J104" s="29"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" s="77"/>
+      <c r="A105" s="111"/>
       <c r="B105" s="26">
-        <v>41698</v>
+        <v>41697</v>
       </c>
       <c r="C105" s="55"/>
       <c r="D105" s="55"/>
@@ -4140,28 +4176,28 @@
       <c r="J105" s="29"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="72">
+      <c r="A106" s="90"/>
+      <c r="B106" s="26">
+        <v>41698</v>
+      </c>
+      <c r="C106" s="55"/>
+      <c r="D106" s="55"/>
+      <c r="E106" s="55"/>
+      <c r="F106" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G106" s="29"/>
+      <c r="H106" s="29"/>
+      <c r="I106" s="29"/>
+      <c r="J106" s="29"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="91">
         <v>18</v>
       </c>
-      <c r="B106" s="27">
+      <c r="B107" s="27">
         <v>41701</v>
-      </c>
-      <c r="C106" s="69"/>
-      <c r="D106" s="69"/>
-      <c r="E106" s="69"/>
-      <c r="F106" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G106" s="67"/>
-      <c r="H106" s="67"/>
-      <c r="I106" s="67"/>
-      <c r="J106" s="67"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="73"/>
-      <c r="B107" s="27">
-        <v>41702</v>
       </c>
       <c r="C107" s="69"/>
       <c r="D107" s="69"/>
@@ -4176,9 +4212,9 @@
       <c r="J107" s="67"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108" s="73"/>
+      <c r="A108" s="92"/>
       <c r="B108" s="27">
-        <v>41703</v>
+        <v>41702</v>
       </c>
       <c r="C108" s="69"/>
       <c r="D108" s="69"/>
@@ -4193,9 +4229,9 @@
       <c r="J108" s="67"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" s="73"/>
+      <c r="A109" s="92"/>
       <c r="B109" s="27">
-        <v>41704</v>
+        <v>41703</v>
       </c>
       <c r="C109" s="69"/>
       <c r="D109" s="69"/>
@@ -4210,9 +4246,9 @@
       <c r="J109" s="67"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" s="74"/>
+      <c r="A110" s="92"/>
       <c r="B110" s="27">
-        <v>41705</v>
+        <v>41704</v>
       </c>
       <c r="C110" s="69"/>
       <c r="D110" s="69"/>
@@ -4227,28 +4263,28 @@
       <c r="J110" s="67"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="75">
+      <c r="A111" s="93"/>
+      <c r="B111" s="27">
+        <v>41705</v>
+      </c>
+      <c r="C111" s="69"/>
+      <c r="D111" s="69"/>
+      <c r="E111" s="69"/>
+      <c r="F111" s="69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G111" s="67"/>
+      <c r="H111" s="67"/>
+      <c r="I111" s="67"/>
+      <c r="J111" s="67"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="110">
         <v>19</v>
       </c>
-      <c r="B111" s="26">
+      <c r="B112" s="26">
         <v>41708</v>
-      </c>
-      <c r="C111" s="55"/>
-      <c r="D111" s="55"/>
-      <c r="E111" s="55"/>
-      <c r="F111" s="55">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G111" s="29"/>
-      <c r="H111" s="29"/>
-      <c r="I111" s="29"/>
-      <c r="J111" s="29"/>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="76"/>
-      <c r="B112" s="26">
-        <v>41709</v>
       </c>
       <c r="C112" s="55"/>
       <c r="D112" s="55"/>
@@ -4263,9 +4299,9 @@
       <c r="J112" s="29"/>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" s="76"/>
+      <c r="A113" s="111"/>
       <c r="B113" s="26">
-        <v>41710</v>
+        <v>41709</v>
       </c>
       <c r="C113" s="55"/>
       <c r="D113" s="55"/>
@@ -4280,9 +4316,9 @@
       <c r="J113" s="29"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" s="76"/>
+      <c r="A114" s="111"/>
       <c r="B114" s="26">
-        <v>41711</v>
+        <v>41710</v>
       </c>
       <c r="C114" s="55"/>
       <c r="D114" s="55"/>
@@ -4297,9 +4333,9 @@
       <c r="J114" s="29"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="77"/>
+      <c r="A115" s="111"/>
       <c r="B115" s="26">
-        <v>41712</v>
+        <v>41711</v>
       </c>
       <c r="C115" s="55"/>
       <c r="D115" s="55"/>
@@ -4314,28 +4350,28 @@
       <c r="J115" s="29"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="72">
+      <c r="A116" s="90"/>
+      <c r="B116" s="26">
+        <v>41712</v>
+      </c>
+      <c r="C116" s="55"/>
+      <c r="D116" s="55"/>
+      <c r="E116" s="55"/>
+      <c r="F116" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G116" s="29"/>
+      <c r="H116" s="29"/>
+      <c r="I116" s="29"/>
+      <c r="J116" s="29"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117" s="91">
         <v>20</v>
       </c>
-      <c r="B116" s="27">
+      <c r="B117" s="27">
         <v>41715</v>
-      </c>
-      <c r="C116" s="69"/>
-      <c r="D116" s="69"/>
-      <c r="E116" s="69"/>
-      <c r="F116" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G116" s="67"/>
-      <c r="H116" s="67"/>
-      <c r="I116" s="67"/>
-      <c r="J116" s="67"/>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="73"/>
-      <c r="B117" s="27">
-        <v>41716</v>
       </c>
       <c r="C117" s="69"/>
       <c r="D117" s="69"/>
@@ -4350,9 +4386,9 @@
       <c r="J117" s="67"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" s="73"/>
+      <c r="A118" s="92"/>
       <c r="B118" s="27">
-        <v>41717</v>
+        <v>41716</v>
       </c>
       <c r="C118" s="69"/>
       <c r="D118" s="69"/>
@@ -4367,9 +4403,9 @@
       <c r="J118" s="67"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119" s="73"/>
+      <c r="A119" s="92"/>
       <c r="B119" s="27">
-        <v>41718</v>
+        <v>41717</v>
       </c>
       <c r="C119" s="69"/>
       <c r="D119" s="69"/>
@@ -4384,9 +4420,9 @@
       <c r="J119" s="67"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" s="74"/>
+      <c r="A120" s="92"/>
       <c r="B120" s="27">
-        <v>41719</v>
+        <v>41718</v>
       </c>
       <c r="C120" s="69"/>
       <c r="D120" s="69"/>
@@ -4401,28 +4437,28 @@
       <c r="J120" s="67"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A121" s="75">
+      <c r="A121" s="93"/>
+      <c r="B121" s="27">
+        <v>41719</v>
+      </c>
+      <c r="C121" s="69"/>
+      <c r="D121" s="69"/>
+      <c r="E121" s="69"/>
+      <c r="F121" s="69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G121" s="67"/>
+      <c r="H121" s="67"/>
+      <c r="I121" s="67"/>
+      <c r="J121" s="67"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A122" s="110">
         <v>21</v>
       </c>
-      <c r="B121" s="26">
+      <c r="B122" s="26">
         <v>41722</v>
-      </c>
-      <c r="C121" s="55"/>
-      <c r="D121" s="55"/>
-      <c r="E121" s="55"/>
-      <c r="F121" s="55">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G121" s="29"/>
-      <c r="H121" s="29"/>
-      <c r="I121" s="29"/>
-      <c r="J121" s="29"/>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A122" s="76"/>
-      <c r="B122" s="26">
-        <v>41723</v>
       </c>
       <c r="C122" s="55"/>
       <c r="D122" s="55"/>
@@ -4437,9 +4473,9 @@
       <c r="J122" s="29"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A123" s="76"/>
+      <c r="A123" s="111"/>
       <c r="B123" s="26">
-        <v>41724</v>
+        <v>41723</v>
       </c>
       <c r="C123" s="55"/>
       <c r="D123" s="55"/>
@@ -4454,9 +4490,9 @@
       <c r="J123" s="29"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A124" s="76"/>
+      <c r="A124" s="111"/>
       <c r="B124" s="26">
-        <v>41725</v>
+        <v>41724</v>
       </c>
       <c r="C124" s="55"/>
       <c r="D124" s="55"/>
@@ -4471,9 +4507,9 @@
       <c r="J124" s="29"/>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A125" s="77"/>
+      <c r="A125" s="111"/>
       <c r="B125" s="26">
-        <v>41726</v>
+        <v>41725</v>
       </c>
       <c r="C125" s="55"/>
       <c r="D125" s="55"/>
@@ -4488,34 +4524,34 @@
       <c r="J125" s="29"/>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A126" s="72">
+      <c r="A126" s="90"/>
+      <c r="B126" s="26">
+        <v>41726</v>
+      </c>
+      <c r="C126" s="55"/>
+      <c r="D126" s="55"/>
+      <c r="E126" s="55"/>
+      <c r="F126" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G126" s="29"/>
+      <c r="H126" s="29"/>
+      <c r="I126" s="29"/>
+      <c r="J126" s="29"/>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A127" s="91">
         <v>22</v>
       </c>
-      <c r="B126" s="27">
+      <c r="B127" s="27">
         <v>41729</v>
-      </c>
-      <c r="C126" s="69"/>
-      <c r="D126" s="69"/>
-      <c r="E126" s="69"/>
-      <c r="F126" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G126" s="67"/>
-      <c r="H126" s="67"/>
-      <c r="I126" s="67"/>
-      <c r="J126" s="67"/>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A127" s="73"/>
-      <c r="B127" s="27">
-        <v>41730</v>
       </c>
       <c r="C127" s="69"/>
       <c r="D127" s="69"/>
       <c r="E127" s="69"/>
       <c r="F127" s="69">
-        <f t="shared" ref="F127:F158" si="3">E127</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G127" s="67"/>
@@ -4524,15 +4560,15 @@
       <c r="J127" s="67"/>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A128" s="73"/>
+      <c r="A128" s="92"/>
       <c r="B128" s="27">
-        <v>41731</v>
+        <v>41730</v>
       </c>
       <c r="C128" s="69"/>
       <c r="D128" s="69"/>
       <c r="E128" s="69"/>
       <c r="F128" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F128:F159" si="3">E128</f>
         <v>0</v>
       </c>
       <c r="G128" s="67"/>
@@ -4541,9 +4577,9 @@
       <c r="J128" s="67"/>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A129" s="73"/>
+      <c r="A129" s="92"/>
       <c r="B129" s="27">
-        <v>41732</v>
+        <v>41731</v>
       </c>
       <c r="C129" s="69"/>
       <c r="D129" s="69"/>
@@ -4558,9 +4594,9 @@
       <c r="J129" s="67"/>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A130" s="74"/>
+      <c r="A130" s="92"/>
       <c r="B130" s="27">
-        <v>41733</v>
+        <v>41732</v>
       </c>
       <c r="C130" s="69"/>
       <c r="D130" s="69"/>
@@ -4575,28 +4611,28 @@
       <c r="J130" s="67"/>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A131" s="75">
+      <c r="A131" s="93"/>
+      <c r="B131" s="27">
+        <v>41733</v>
+      </c>
+      <c r="C131" s="69"/>
+      <c r="D131" s="69"/>
+      <c r="E131" s="69"/>
+      <c r="F131" s="69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G131" s="67"/>
+      <c r="H131" s="67"/>
+      <c r="I131" s="67"/>
+      <c r="J131" s="67"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A132" s="110">
         <v>23</v>
       </c>
-      <c r="B131" s="26">
+      <c r="B132" s="26">
         <v>41736</v>
-      </c>
-      <c r="C131" s="55"/>
-      <c r="D131" s="55"/>
-      <c r="E131" s="55"/>
-      <c r="F131" s="55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G131" s="29"/>
-      <c r="H131" s="29"/>
-      <c r="I131" s="29"/>
-      <c r="J131" s="29"/>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A132" s="76"/>
-      <c r="B132" s="26">
-        <v>41737</v>
       </c>
       <c r="C132" s="55"/>
       <c r="D132" s="55"/>
@@ -4611,9 +4647,9 @@
       <c r="J132" s="29"/>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A133" s="76"/>
+      <c r="A133" s="111"/>
       <c r="B133" s="26">
-        <v>41738</v>
+        <v>41737</v>
       </c>
       <c r="C133" s="55"/>
       <c r="D133" s="55"/>
@@ -4628,9 +4664,9 @@
       <c r="J133" s="29"/>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A134" s="76"/>
+      <c r="A134" s="111"/>
       <c r="B134" s="26">
-        <v>41739</v>
+        <v>41738</v>
       </c>
       <c r="C134" s="55"/>
       <c r="D134" s="55"/>
@@ -4645,9 +4681,9 @@
       <c r="J134" s="29"/>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A135" s="77"/>
+      <c r="A135" s="111"/>
       <c r="B135" s="26">
-        <v>41740</v>
+        <v>41739</v>
       </c>
       <c r="C135" s="55"/>
       <c r="D135" s="55"/>
@@ -4662,28 +4698,28 @@
       <c r="J135" s="29"/>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A136" s="72">
+      <c r="A136" s="90"/>
+      <c r="B136" s="26">
+        <v>41740</v>
+      </c>
+      <c r="C136" s="55"/>
+      <c r="D136" s="55"/>
+      <c r="E136" s="55"/>
+      <c r="F136" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G136" s="29"/>
+      <c r="H136" s="29"/>
+      <c r="I136" s="29"/>
+      <c r="J136" s="29"/>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A137" s="91">
         <v>24</v>
       </c>
-      <c r="B136" s="27">
+      <c r="B137" s="27">
         <v>41743</v>
-      </c>
-      <c r="C136" s="69"/>
-      <c r="D136" s="69"/>
-      <c r="E136" s="69"/>
-      <c r="F136" s="69">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G136" s="67"/>
-      <c r="H136" s="67"/>
-      <c r="I136" s="67"/>
-      <c r="J136" s="67"/>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A137" s="73"/>
-      <c r="B137" s="27">
-        <v>41744</v>
       </c>
       <c r="C137" s="69"/>
       <c r="D137" s="69"/>
@@ -4698,9 +4734,9 @@
       <c r="J137" s="67"/>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A138" s="73"/>
+      <c r="A138" s="92"/>
       <c r="B138" s="27">
-        <v>41745</v>
+        <v>41744</v>
       </c>
       <c r="C138" s="69"/>
       <c r="D138" s="69"/>
@@ -4715,9 +4751,9 @@
       <c r="J138" s="67"/>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A139" s="73"/>
+      <c r="A139" s="92"/>
       <c r="B139" s="27">
-        <v>41746</v>
+        <v>41745</v>
       </c>
       <c r="C139" s="69"/>
       <c r="D139" s="69"/>
@@ -4732,9 +4768,9 @@
       <c r="J139" s="67"/>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A140" s="74"/>
+      <c r="A140" s="92"/>
       <c r="B140" s="27">
-        <v>41747</v>
+        <v>41746</v>
       </c>
       <c r="C140" s="69"/>
       <c r="D140" s="69"/>
@@ -4749,28 +4785,28 @@
       <c r="J140" s="67"/>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A141" s="75">
+      <c r="A141" s="93"/>
+      <c r="B141" s="27">
+        <v>41747</v>
+      </c>
+      <c r="C141" s="69"/>
+      <c r="D141" s="69"/>
+      <c r="E141" s="69"/>
+      <c r="F141" s="69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G141" s="67"/>
+      <c r="H141" s="67"/>
+      <c r="I141" s="67"/>
+      <c r="J141" s="67"/>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A142" s="110">
         <v>25</v>
       </c>
-      <c r="B141" s="26">
+      <c r="B142" s="26">
         <v>41750</v>
-      </c>
-      <c r="C141" s="55"/>
-      <c r="D141" s="55"/>
-      <c r="E141" s="55"/>
-      <c r="F141" s="55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G141" s="29"/>
-      <c r="H141" s="29"/>
-      <c r="I141" s="29"/>
-      <c r="J141" s="29"/>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A142" s="76"/>
-      <c r="B142" s="26">
-        <v>41751</v>
       </c>
       <c r="C142" s="55"/>
       <c r="D142" s="55"/>
@@ -4785,9 +4821,9 @@
       <c r="J142" s="29"/>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A143" s="76"/>
+      <c r="A143" s="111"/>
       <c r="B143" s="26">
-        <v>41752</v>
+        <v>41751</v>
       </c>
       <c r="C143" s="55"/>
       <c r="D143" s="55"/>
@@ -4802,9 +4838,9 @@
       <c r="J143" s="29"/>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A144" s="76"/>
+      <c r="A144" s="111"/>
       <c r="B144" s="26">
-        <v>41753</v>
+        <v>41752</v>
       </c>
       <c r="C144" s="55"/>
       <c r="D144" s="55"/>
@@ -4819,9 +4855,9 @@
       <c r="J144" s="29"/>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A145" s="77"/>
+      <c r="A145" s="111"/>
       <c r="B145" s="26">
-        <v>41754</v>
+        <v>41753</v>
       </c>
       <c r="C145" s="55"/>
       <c r="D145" s="55"/>
@@ -4836,28 +4872,28 @@
       <c r="J145" s="29"/>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A146" s="72">
+      <c r="A146" s="90"/>
+      <c r="B146" s="26">
+        <v>41754</v>
+      </c>
+      <c r="C146" s="55"/>
+      <c r="D146" s="55"/>
+      <c r="E146" s="55"/>
+      <c r="F146" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G146" s="29"/>
+      <c r="H146" s="29"/>
+      <c r="I146" s="29"/>
+      <c r="J146" s="29"/>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A147" s="91">
         <v>26</v>
       </c>
-      <c r="B146" s="27">
+      <c r="B147" s="27">
         <v>41757</v>
-      </c>
-      <c r="C146" s="69"/>
-      <c r="D146" s="69"/>
-      <c r="E146" s="69"/>
-      <c r="F146" s="69">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G146" s="67"/>
-      <c r="H146" s="67"/>
-      <c r="I146" s="67"/>
-      <c r="J146" s="67"/>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A147" s="73"/>
-      <c r="B147" s="27">
-        <v>41758</v>
       </c>
       <c r="C147" s="69"/>
       <c r="D147" s="69"/>
@@ -4872,9 +4908,9 @@
       <c r="J147" s="67"/>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A148" s="73"/>
+      <c r="A148" s="92"/>
       <c r="B148" s="27">
-        <v>41759</v>
+        <v>41758</v>
       </c>
       <c r="C148" s="69"/>
       <c r="D148" s="69"/>
@@ -4889,9 +4925,9 @@
       <c r="J148" s="67"/>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A149" s="73"/>
+      <c r="A149" s="92"/>
       <c r="B149" s="27">
-        <v>41760</v>
+        <v>41759</v>
       </c>
       <c r="C149" s="69"/>
       <c r="D149" s="69"/>
@@ -4906,9 +4942,9 @@
       <c r="J149" s="67"/>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A150" s="74"/>
+      <c r="A150" s="92"/>
       <c r="B150" s="27">
-        <v>41761</v>
+        <v>41760</v>
       </c>
       <c r="C150" s="69"/>
       <c r="D150" s="69"/>
@@ -4923,28 +4959,28 @@
       <c r="J150" s="67"/>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A151" s="75">
+      <c r="A151" s="93"/>
+      <c r="B151" s="27">
+        <v>41761</v>
+      </c>
+      <c r="C151" s="69"/>
+      <c r="D151" s="69"/>
+      <c r="E151" s="69"/>
+      <c r="F151" s="69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G151" s="67"/>
+      <c r="H151" s="67"/>
+      <c r="I151" s="67"/>
+      <c r="J151" s="67"/>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A152" s="110">
         <v>27</v>
       </c>
-      <c r="B151" s="26">
+      <c r="B152" s="26">
         <v>41764</v>
-      </c>
-      <c r="C151" s="55"/>
-      <c r="D151" s="55"/>
-      <c r="E151" s="55"/>
-      <c r="F151" s="55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G151" s="29"/>
-      <c r="H151" s="29"/>
-      <c r="I151" s="29"/>
-      <c r="J151" s="29"/>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A152" s="76"/>
-      <c r="B152" s="26">
-        <v>41765</v>
       </c>
       <c r="C152" s="55"/>
       <c r="D152" s="55"/>
@@ -4959,9 +4995,9 @@
       <c r="J152" s="29"/>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A153" s="76"/>
+      <c r="A153" s="111"/>
       <c r="B153" s="26">
-        <v>41766</v>
+        <v>41765</v>
       </c>
       <c r="C153" s="55"/>
       <c r="D153" s="55"/>
@@ -4976,9 +5012,9 @@
       <c r="J153" s="29"/>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A154" s="76"/>
+      <c r="A154" s="111"/>
       <c r="B154" s="26">
-        <v>41767</v>
+        <v>41766</v>
       </c>
       <c r="C154" s="55"/>
       <c r="D154" s="55"/>
@@ -4993,9 +5029,9 @@
       <c r="J154" s="29"/>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A155" s="77"/>
+      <c r="A155" s="111"/>
       <c r="B155" s="26">
-        <v>41768</v>
+        <v>41767</v>
       </c>
       <c r="C155" s="55"/>
       <c r="D155" s="55"/>
@@ -5010,28 +5046,28 @@
       <c r="J155" s="29"/>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A156" s="72">
+      <c r="A156" s="90"/>
+      <c r="B156" s="26">
+        <v>41768</v>
+      </c>
+      <c r="C156" s="55"/>
+      <c r="D156" s="55"/>
+      <c r="E156" s="55"/>
+      <c r="F156" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G156" s="29"/>
+      <c r="H156" s="29"/>
+      <c r="I156" s="29"/>
+      <c r="J156" s="29"/>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A157" s="91">
         <v>28</v>
       </c>
-      <c r="B156" s="27">
+      <c r="B157" s="27">
         <v>41771</v>
-      </c>
-      <c r="C156" s="69"/>
-      <c r="D156" s="69"/>
-      <c r="E156" s="69"/>
-      <c r="F156" s="69">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G156" s="67"/>
-      <c r="H156" s="67"/>
-      <c r="I156" s="67"/>
-      <c r="J156" s="67"/>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A157" s="73"/>
-      <c r="B157" s="27">
-        <v>41772</v>
       </c>
       <c r="C157" s="69"/>
       <c r="D157" s="69"/>
@@ -5046,9 +5082,9 @@
       <c r="J157" s="67"/>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A158" s="73"/>
+      <c r="A158" s="92"/>
       <c r="B158" s="27">
-        <v>41773</v>
+        <v>41772</v>
       </c>
       <c r="C158" s="69"/>
       <c r="D158" s="69"/>
@@ -5063,15 +5099,15 @@
       <c r="J158" s="67"/>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A159" s="73"/>
+      <c r="A159" s="92"/>
       <c r="B159" s="27">
-        <v>41774</v>
+        <v>41773</v>
       </c>
       <c r="C159" s="69"/>
       <c r="D159" s="69"/>
       <c r="E159" s="69"/>
       <c r="F159" s="69">
-        <f t="shared" ref="F159:F170" si="4">E159</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G159" s="67"/>
@@ -5080,15 +5116,15 @@
       <c r="J159" s="67"/>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A160" s="74"/>
+      <c r="A160" s="92"/>
       <c r="B160" s="27">
-        <v>41775</v>
+        <v>41774</v>
       </c>
       <c r="C160" s="69"/>
       <c r="D160" s="69"/>
       <c r="E160" s="69"/>
       <c r="F160" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F160:F171" si="4">E160</f>
         <v>0</v>
       </c>
       <c r="G160" s="67"/>
@@ -5097,28 +5133,28 @@
       <c r="J160" s="67"/>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A161" s="75">
+      <c r="A161" s="93"/>
+      <c r="B161" s="27">
+        <v>41775</v>
+      </c>
+      <c r="C161" s="69"/>
+      <c r="D161" s="69"/>
+      <c r="E161" s="69"/>
+      <c r="F161" s="69">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G161" s="67"/>
+      <c r="H161" s="67"/>
+      <c r="I161" s="67"/>
+      <c r="J161" s="67"/>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A162" s="110">
         <v>29</v>
       </c>
-      <c r="B161" s="26">
+      <c r="B162" s="26">
         <v>41778</v>
-      </c>
-      <c r="C161" s="55"/>
-      <c r="D161" s="55"/>
-      <c r="E161" s="55"/>
-      <c r="F161" s="55">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G161" s="29"/>
-      <c r="H161" s="29"/>
-      <c r="I161" s="29"/>
-      <c r="J161" s="29"/>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A162" s="76"/>
-      <c r="B162" s="26">
-        <v>41779</v>
       </c>
       <c r="C162" s="55"/>
       <c r="D162" s="55"/>
@@ -5133,9 +5169,9 @@
       <c r="J162" s="29"/>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A163" s="76"/>
+      <c r="A163" s="111"/>
       <c r="B163" s="26">
-        <v>41780</v>
+        <v>41779</v>
       </c>
       <c r="C163" s="55"/>
       <c r="D163" s="55"/>
@@ -5150,9 +5186,9 @@
       <c r="J163" s="29"/>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A164" s="76"/>
+      <c r="A164" s="111"/>
       <c r="B164" s="26">
-        <v>41781</v>
+        <v>41780</v>
       </c>
       <c r="C164" s="55"/>
       <c r="D164" s="55"/>
@@ -5167,9 +5203,9 @@
       <c r="J164" s="29"/>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A165" s="77"/>
+      <c r="A165" s="111"/>
       <c r="B165" s="26">
-        <v>41782</v>
+        <v>41781</v>
       </c>
       <c r="C165" s="55"/>
       <c r="D165" s="55"/>
@@ -5184,28 +5220,28 @@
       <c r="J165" s="29"/>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A166" s="78">
+      <c r="A166" s="90"/>
+      <c r="B166" s="26">
+        <v>41782</v>
+      </c>
+      <c r="C166" s="55"/>
+      <c r="D166" s="55"/>
+      <c r="E166" s="55"/>
+      <c r="F166" s="55">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G166" s="29"/>
+      <c r="H166" s="29"/>
+      <c r="I166" s="29"/>
+      <c r="J166" s="29"/>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A167" s="136">
         <v>30</v>
       </c>
-      <c r="B166" s="27">
+      <c r="B167" s="27">
         <v>41785</v>
-      </c>
-      <c r="C166" s="70"/>
-      <c r="D166" s="70"/>
-      <c r="E166" s="70"/>
-      <c r="F166" s="70">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G166" s="37"/>
-      <c r="H166" s="37"/>
-      <c r="I166" s="37"/>
-      <c r="J166" s="37"/>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A167" s="79"/>
-      <c r="B167" s="27">
-        <v>41786</v>
       </c>
       <c r="C167" s="70"/>
       <c r="D167" s="70"/>
@@ -5220,9 +5256,9 @@
       <c r="J167" s="37"/>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A168" s="79"/>
+      <c r="A168" s="137"/>
       <c r="B168" s="27">
-        <v>41787</v>
+        <v>41786</v>
       </c>
       <c r="C168" s="70"/>
       <c r="D168" s="70"/>
@@ -5237,9 +5273,9 @@
       <c r="J168" s="37"/>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A169" s="79"/>
+      <c r="A169" s="137"/>
       <c r="B169" s="27">
-        <v>41788</v>
+        <v>41787</v>
       </c>
       <c r="C169" s="70"/>
       <c r="D169" s="70"/>
@@ -5254,9 +5290,9 @@
       <c r="J169" s="37"/>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A170" s="80"/>
+      <c r="A170" s="137"/>
       <c r="B170" s="27">
-        <v>41789</v>
+        <v>41788</v>
       </c>
       <c r="C170" s="70"/>
       <c r="D170" s="70"/>
@@ -5271,16 +5307,21 @@
       <c r="J170" s="37"/>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A171" s="68"/>
-      <c r="B171" s="68"/>
-      <c r="C171" s="68"/>
-      <c r="D171" s="68"/>
-      <c r="E171" s="68"/>
-      <c r="F171" s="68"/>
-      <c r="G171" s="68"/>
-      <c r="H171" s="68"/>
-      <c r="I171" s="68"/>
-      <c r="J171" s="68"/>
+      <c r="A171" s="138"/>
+      <c r="B171" s="27">
+        <v>41789</v>
+      </c>
+      <c r="C171" s="70"/>
+      <c r="D171" s="70"/>
+      <c r="E171" s="70"/>
+      <c r="F171" s="70">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G171" s="37"/>
+      <c r="H171" s="37"/>
+      <c r="I171" s="37"/>
+      <c r="J171" s="37"/>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="68"/>
@@ -5378,31 +5419,42 @@
       <c r="I179" s="68"/>
       <c r="J179" s="68"/>
     </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A180" s="68"/>
+      <c r="B180" s="68"/>
+      <c r="C180" s="68"/>
+      <c r="D180" s="68"/>
+      <c r="E180" s="68"/>
+      <c r="F180" s="68"/>
+      <c r="G180" s="68"/>
+      <c r="H180" s="68"/>
+      <c r="I180" s="68"/>
+      <c r="J180" s="68"/>
+    </row>
   </sheetData>
-  <mergeCells count="53">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="G2:N4"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="A66:A70"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F4"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="A51:A55"/>
-    <mergeCell ref="A33:A40"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="A56:A60"/>
-    <mergeCell ref="A61:A65"/>
-    <mergeCell ref="A71:A75"/>
+  <mergeCells count="54">
+    <mergeCell ref="A157:A161"/>
+    <mergeCell ref="A162:A166"/>
+    <mergeCell ref="A167:A171"/>
+    <mergeCell ref="A127:A131"/>
+    <mergeCell ref="A132:A136"/>
+    <mergeCell ref="A137:A141"/>
+    <mergeCell ref="A142:A146"/>
+    <mergeCell ref="A147:A151"/>
+    <mergeCell ref="A107:A111"/>
+    <mergeCell ref="A112:A116"/>
+    <mergeCell ref="A117:A121"/>
+    <mergeCell ref="A122:A126"/>
+    <mergeCell ref="A152:A156"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A87:A91"/>
+    <mergeCell ref="A92:A96"/>
+    <mergeCell ref="A97:A101"/>
+    <mergeCell ref="A102:A106"/>
+    <mergeCell ref="A77:A81"/>
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="A72:A76"/>
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="F12:F13"/>
@@ -5415,24 +5467,26 @@
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="A19:A32"/>
-    <mergeCell ref="A81:A85"/>
-    <mergeCell ref="A86:A90"/>
-    <mergeCell ref="A91:A95"/>
-    <mergeCell ref="A96:A100"/>
-    <mergeCell ref="A101:A105"/>
-    <mergeCell ref="A106:A110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A120"/>
-    <mergeCell ref="A121:A125"/>
-    <mergeCell ref="A151:A155"/>
-    <mergeCell ref="A156:A160"/>
-    <mergeCell ref="A161:A165"/>
-    <mergeCell ref="A166:A170"/>
-    <mergeCell ref="A126:A130"/>
-    <mergeCell ref="A131:A135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A145"/>
-    <mergeCell ref="A146:A150"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F4"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="A33:A41"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="G2:N4"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="F31:F32"/>
   </mergeCells>
   <conditionalFormatting sqref="M7">
     <cfRule type="cellIs" dxfId="3" priority="7" operator="greaterThan">
@@ -5664,29 +5718,10 @@
               <x14:cfIcon iconSet="3Symbols" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>M38</xm:sqref>
+          <xm:sqref>M38:M39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="29" id="{87212A6D-7255-4CD9-B0F3-3C906F80977E}">
-            <x14:iconSet custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>25</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num" gte="0">
-                <xm:f>168</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols" iconId="1"/>
-              <x14:cfIcon iconSet="3Symbols" iconId="2"/>
-              <x14:cfIcon iconSet="3Symbols" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>M39</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="28" id="{BEBCA1A1-AA3F-4294-8922-9827332C0668}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5705,7 +5740,7 @@
           <xm:sqref>M40</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="27" id="{3793385C-190C-4A90-AF72-EEE9712F504F}">
+          <x14:cfRule type="iconSet" priority="28" id="{BEBCA1A1-AA3F-4294-8922-9827332C0668}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5724,7 +5759,7 @@
           <xm:sqref>M41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="26" id="{21C6FD3D-522C-4661-AE5D-284F6FC787D0}">
+          <x14:cfRule type="iconSet" priority="27" id="{3793385C-190C-4A90-AF72-EEE9712F504F}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5743,7 +5778,7 @@
           <xm:sqref>M42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="25" id="{09871DA7-81C7-4675-89F3-BE2EDB05B9C9}">
+          <x14:cfRule type="iconSet" priority="26" id="{21C6FD3D-522C-4661-AE5D-284F6FC787D0}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5762,7 +5797,7 @@
           <xm:sqref>M43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="24" id="{50D35A91-6584-4A00-B008-2B93AA187052}">
+          <x14:cfRule type="iconSet" priority="25" id="{09871DA7-81C7-4675-89F3-BE2EDB05B9C9}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5781,7 +5816,7 @@
           <xm:sqref>M44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="23" id="{10AA0BAB-E7C1-450C-B7A5-276ADB69B0B2}">
+          <x14:cfRule type="iconSet" priority="24" id="{50D35A91-6584-4A00-B008-2B93AA187052}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5800,7 +5835,7 @@
           <xm:sqref>M45</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="22" id="{0A1ADE65-D185-454C-92B2-B6FA367CBA04}">
+          <x14:cfRule type="iconSet" priority="23" id="{10AA0BAB-E7C1-450C-B7A5-276ADB69B0B2}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5819,7 +5854,7 @@
           <xm:sqref>M46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="21" id="{E0DFC09D-C053-4D3D-A1C1-C5AF640FB5CD}">
+          <x14:cfRule type="iconSet" priority="22" id="{0A1ADE65-D185-454C-92B2-B6FA367CBA04}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5838,7 +5873,7 @@
           <xm:sqref>M47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="20" id="{F1B6F2BC-B2AE-42D9-8427-52A717AE39CD}">
+          <x14:cfRule type="iconSet" priority="21" id="{E0DFC09D-C053-4D3D-A1C1-C5AF640FB5CD}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5857,7 +5892,7 @@
           <xm:sqref>M48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="19" id="{EEF8AB81-584A-4839-AEE8-98BCAAB29DD2}">
+          <x14:cfRule type="iconSet" priority="20" id="{F1B6F2BC-B2AE-42D9-8427-52A717AE39CD}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5876,7 +5911,7 @@
           <xm:sqref>M49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="18" id="{A1F90B4F-0784-43A3-A2A1-2A7C9438EE1A}">
+          <x14:cfRule type="iconSet" priority="19" id="{EEF8AB81-584A-4839-AEE8-98BCAAB29DD2}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5895,7 +5930,7 @@
           <xm:sqref>M50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="17" id="{CDF48798-0C78-453D-9E98-93D1BB3C878A}">
+          <x14:cfRule type="iconSet" priority="18" id="{A1F90B4F-0784-43A3-A2A1-2A7C9438EE1A}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5914,7 +5949,7 @@
           <xm:sqref>M51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="16" id="{524804E6-2BBA-4071-AB71-18BD193B4497}">
+          <x14:cfRule type="iconSet" priority="17" id="{CDF48798-0C78-453D-9E98-93D1BB3C878A}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5933,7 +5968,7 @@
           <xm:sqref>M52</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="15" id="{F466D4E3-91DB-49AA-8E5A-7BD04BE8813F}">
+          <x14:cfRule type="iconSet" priority="16" id="{524804E6-2BBA-4071-AB71-18BD193B4497}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5950,6 +5985,25 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>M53</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="15" id="{F466D4E3-91DB-49AA-8E5A-7BD04BE8813F}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>25</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>168</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols" iconId="1"/>
+              <x14:cfIcon iconSet="3Symbols" iconId="2"/>
+              <x14:cfIcon iconSet="3Symbols" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>M54</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="14" id="{C4227F9F-08CD-4A7C-B706-2C35F19616E7}">
@@ -6025,7 +6079,7 @@
               <x14:cfIcon iconSet="3Symbols" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>F14 F7:F8 F12 F18:F19 F21 F23:F24 F29 F33:F34 F38:F170</xm:sqref>
+          <xm:sqref>F14 F7:F8 F12 F18:F19 F21 F23:F24 F29 F33:F34 F38 F40:F171</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="2" id="{35213755-788E-43C8-B75E-72DA17285D4A}">

</xml_diff>

<commit_message>
update effort log 28/11 - Khang
</commit_message>
<xml_diff>
--- a/1. Project management/9. Timelog/individual time log/AS_PM_TimeLog_DeadlineTeam_KhangHuynh.xlsx
+++ b/1. Project management/9. Timelog/individual time log/AS_PM_TimeLog_DeadlineTeam_KhangHuynh.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="144">
   <si>
     <t>Week</t>
   </si>
@@ -456,6 +456,28 @@
   </si>
   <si>
     <t>Question - Tong hop</t>
+  </si>
+  <si>
+    <t>9:15AM</t>
+  </si>
+  <si>
+    <t>11:00AM</t>
+  </si>
+  <si>
+    <t>4:15PM</t>
+  </si>
+  <si>
+    <t>Review question have prepared for system</t>
+  </si>
+  <si>
+    <t>Collect architect drivers raw and develop user stories</t>
+  </si>
+  <si>
+    <t>Đã thực hiện file phân công ngày 28/11</t>
+  </si>
+  <si>
+    <t>Analyse architect drivers raw "Bảng tin" and "Danh mục"
+Draw activity diagrams business process</t>
   </si>
 </sst>
 </file>
@@ -973,6 +995,156 @@
     <xf numFmtId="20" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1020,156 +1192,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1481,7 +1503,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1492,7 +1514,7 @@
   <dimension ref="A3:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,13 +1626,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O180"/>
+  <dimension ref="A1:O182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="6" topLeftCell="G34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="6" topLeftCell="G39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I39" sqref="I39"/>
+      <selection pane="bottomRight" activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1623,7 +1645,7 @@
     <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="46.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="47.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="1"/>
     <col min="13" max="14" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -1631,81 +1653,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="73"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="75"/>
+      <c r="A1" s="123"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124"/>
+      <c r="K1" s="124"/>
+      <c r="L1" s="124"/>
+      <c r="M1" s="124"/>
+      <c r="N1" s="125"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="76" t="s">
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="78"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="127"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="127"/>
+      <c r="M2" s="127"/>
+      <c r="N2" s="128"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="107" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="81"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="130"/>
+      <c r="L3" s="130"/>
+      <c r="M3" s="130"/>
+      <c r="N3" s="131"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="100"/>
-      <c r="B4" s="101"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="84"/>
+      <c r="A4" s="110"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="111"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="132"/>
+      <c r="H4" s="133"/>
+      <c r="I4" s="133"/>
+      <c r="J4" s="133"/>
+      <c r="K4" s="133"/>
+      <c r="L4" s="133"/>
+      <c r="M4" s="133"/>
+      <c r="N4" s="134"/>
     </row>
     <row r="5" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="107"/>
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="109"/>
+      <c r="A5" s="117"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="119"/>
       <c r="F5" s="15"/>
       <c r="H5" s="41" t="s">
         <v>64</v>
@@ -1750,13 +1772,13 @@
       <c r="J6" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="88"/>
-      <c r="L6" s="88"/>
-      <c r="M6" s="88"/>
-      <c r="N6" s="88"/>
+      <c r="K6" s="138"/>
+      <c r="L6" s="138"/>
+      <c r="M6" s="138"/>
+      <c r="N6" s="138"/>
     </row>
     <row r="7" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="85">
+      <c r="A7" s="135">
         <v>1</v>
       </c>
       <c r="B7" s="16">
@@ -1782,21 +1804,21 @@
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="29"/>
-      <c r="K7" s="115" t="s">
+      <c r="K7" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="115"/>
+      <c r="L7" s="82"/>
       <c r="M7" s="32">
-        <f>SUM(M8:M54)</f>
-        <v>53.319999999999993</v>
+        <f>SUM(M8:M56)</f>
+        <v>59.149999999999991</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="86"/>
-      <c r="B8" s="103">
+      <c r="A8" s="136"/>
+      <c r="B8" s="113">
         <v>41586</v>
       </c>
       <c r="C8" s="17">
@@ -1808,7 +1830,7 @@
       <c r="E8" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="105">
+      <c r="F8" s="115">
         <v>1.67</v>
       </c>
       <c r="G8" s="19" t="s">
@@ -1832,8 +1854,8 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="87"/>
-      <c r="B9" s="104"/>
+      <c r="A9" s="137"/>
+      <c r="B9" s="114"/>
       <c r="C9" s="17">
         <v>0.63194444444444442</v>
       </c>
@@ -1843,7 +1865,7 @@
       <c r="E9" s="18">
         <v>0.5</v>
       </c>
-      <c r="F9" s="106"/>
+      <c r="F9" s="116"/>
       <c r="G9" s="29" t="s">
         <v>23</v>
       </c>
@@ -1854,10 +1876,10 @@
       <c r="J9" s="29"/>
     </row>
     <row r="10" spans="1:15" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="124">
+      <c r="A10" s="91">
         <v>2</v>
       </c>
-      <c r="B10" s="127">
+      <c r="B10" s="94">
         <v>41589</v>
       </c>
       <c r="C10" s="58" t="s">
@@ -1869,7 +1891,7 @@
       <c r="E10" s="59">
         <v>2.5</v>
       </c>
-      <c r="F10" s="129">
+      <c r="F10" s="96">
         <f>SUM(E10:E11)</f>
         <v>5</v>
       </c>
@@ -1883,8 +1905,8 @@
       <c r="J10" s="60"/>
     </row>
     <row r="11" spans="1:15" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="125"/>
-      <c r="B11" s="128"/>
+      <c r="A11" s="92"/>
+      <c r="B11" s="95"/>
       <c r="C11" s="58" t="s">
         <v>76</v>
       </c>
@@ -1894,7 +1916,7 @@
       <c r="E11" s="59">
         <v>2.5</v>
       </c>
-      <c r="F11" s="130"/>
+      <c r="F11" s="97"/>
       <c r="G11" s="60" t="s">
         <v>22</v>
       </c>
@@ -1907,8 +1929,8 @@
       <c r="J11" s="60"/>
     </row>
     <row r="12" spans="1:15" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="125"/>
-      <c r="B12" s="116">
+      <c r="A12" s="92"/>
+      <c r="B12" s="83">
         <v>41590</v>
       </c>
       <c r="C12" s="22">
@@ -1920,7 +1942,7 @@
       <c r="E12" s="23">
         <v>2.25</v>
       </c>
-      <c r="F12" s="118">
+      <c r="F12" s="85">
         <v>3.75</v>
       </c>
       <c r="G12" s="30" t="s">
@@ -1947,8 +1969,8 @@
       <c r="O12" s="34"/>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="125"/>
-      <c r="B13" s="117"/>
+      <c r="A13" s="92"/>
+      <c r="B13" s="84"/>
       <c r="C13" s="22">
         <v>0.91666666666666663</v>
       </c>
@@ -1958,7 +1980,7 @@
       <c r="E13" s="23">
         <v>1.5</v>
       </c>
-      <c r="F13" s="119"/>
+      <c r="F13" s="86"/>
       <c r="G13" s="45" t="s">
         <v>28</v>
       </c>
@@ -1974,8 +1996,8 @@
       <c r="O13" s="34"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="125"/>
-      <c r="B14" s="116">
+      <c r="A14" s="92"/>
+      <c r="B14" s="83">
         <v>41591</v>
       </c>
       <c r="C14" s="22">
@@ -1987,7 +2009,7 @@
       <c r="E14" s="23">
         <v>2</v>
       </c>
-      <c r="F14" s="121">
+      <c r="F14" s="88">
         <v>4.5</v>
       </c>
       <c r="G14" s="45" t="s">
@@ -2005,8 +2027,8 @@
       <c r="O14" s="34"/>
     </row>
     <row r="15" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="125"/>
-      <c r="B15" s="120"/>
+      <c r="A15" s="92"/>
+      <c r="B15" s="87"/>
       <c r="C15" s="25">
         <v>0.5625</v>
       </c>
@@ -2016,7 +2038,7 @@
       <c r="E15" s="28">
         <v>2</v>
       </c>
-      <c r="F15" s="122"/>
+      <c r="F15" s="89"/>
       <c r="G15" s="30" t="s">
         <v>19</v>
       </c>
@@ -2033,8 +2055,8 @@
       <c r="N15" s="3"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="125"/>
-      <c r="B16" s="117"/>
+      <c r="A16" s="92"/>
+      <c r="B16" s="84"/>
       <c r="C16" s="25">
         <v>0.83333333333333337</v>
       </c>
@@ -2044,7 +2066,7 @@
       <c r="E16" s="28">
         <v>0.5</v>
       </c>
-      <c r="F16" s="123"/>
+      <c r="F16" s="90"/>
       <c r="G16" s="45" t="s">
         <v>28</v>
       </c>
@@ -2068,7 +2090,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="125"/>
+      <c r="A17" s="92"/>
       <c r="B17" s="47">
         <v>41592</v>
       </c>
@@ -2099,15 +2121,15 @@
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="9">
-        <f>SUM(F33:F41)</f>
-        <v>11.58</v>
+        <f>SUM(F33:F43)</f>
+        <v>17.41</v>
       </c>
       <c r="N17" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="126"/>
+      <c r="A18" s="93"/>
       <c r="B18" s="42">
         <v>41593</v>
       </c>
@@ -2138,7 +2160,7 @@
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="9">
-        <f>SUM(E42:E46)</f>
+        <f>SUM(E44:E48)</f>
         <v>0</v>
       </c>
       <c r="N18" s="3" t="s">
@@ -2146,10 +2168,10 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="133">
+      <c r="A19" s="101">
         <v>3</v>
       </c>
-      <c r="B19" s="131">
+      <c r="B19" s="98">
         <v>41596</v>
       </c>
       <c r="C19" s="53" t="s">
@@ -2161,7 +2183,7 @@
       <c r="E19" s="50">
         <v>0.5</v>
       </c>
-      <c r="F19" s="89">
+      <c r="F19" s="100">
         <f>SUM(E19:E20)</f>
         <v>3.5</v>
       </c>
@@ -2180,7 +2202,7 @@
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="9">
-        <f>SUM(E57:E61)</f>
+        <f>SUM(E59:E63)</f>
         <v>0</v>
       </c>
       <c r="N19" s="3" t="s">
@@ -2188,8 +2210,8 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="134"/>
-      <c r="B20" s="132"/>
+      <c r="A20" s="102"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="53" t="s">
         <v>81</v>
       </c>
@@ -2199,7 +2221,7 @@
       <c r="E20" s="50">
         <v>3</v>
       </c>
-      <c r="F20" s="90"/>
+      <c r="F20" s="78"/>
       <c r="G20" s="49" t="s">
         <v>22</v>
       </c>
@@ -2216,8 +2238,8 @@
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="134"/>
-      <c r="B21" s="131">
+      <c r="A21" s="102"/>
+      <c r="B21" s="98">
         <v>41597</v>
       </c>
       <c r="C21" s="53" t="s">
@@ -2229,7 +2251,7 @@
       <c r="E21" s="50">
         <v>2</v>
       </c>
-      <c r="F21" s="89">
+      <c r="F21" s="100">
         <f>SUM(E21:E22)</f>
         <v>2.5</v>
       </c>
@@ -2249,8 +2271,8 @@
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="134"/>
-      <c r="B22" s="132"/>
+      <c r="A22" s="102"/>
+      <c r="B22" s="99"/>
       <c r="C22" s="53" t="s">
         <v>84</v>
       </c>
@@ -2260,7 +2282,7 @@
       <c r="E22" s="50">
         <v>0.5</v>
       </c>
-      <c r="F22" s="90"/>
+      <c r="F22" s="78"/>
       <c r="G22" s="49" t="s">
         <v>22</v>
       </c>
@@ -2276,7 +2298,7 @@
       </c>
       <c r="L22" s="5"/>
       <c r="M22" s="9">
-        <f>SUM(E62:E66)</f>
+        <f>SUM(E64:E68)</f>
         <v>0</v>
       </c>
       <c r="N22" s="3" t="s">
@@ -2284,7 +2306,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="134"/>
+      <c r="A23" s="102"/>
       <c r="B23" s="26">
         <v>41598</v>
       </c>
@@ -2298,7 +2320,7 @@
         <v>4</v>
       </c>
       <c r="F23" s="55">
-        <f t="shared" ref="F23:F63" si="0">E23</f>
+        <f t="shared" ref="F23:F65" si="0">E23</f>
         <v>4</v>
       </c>
       <c r="G23" s="57" t="s">
@@ -2316,7 +2338,7 @@
       </c>
       <c r="L23" s="5"/>
       <c r="M23" s="9">
-        <f>SUM(E67:E71)</f>
+        <f>SUM(E69:E73)</f>
         <v>0</v>
       </c>
       <c r="N23" s="3" t="s">
@@ -2324,7 +2346,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="134"/>
+      <c r="A24" s="102"/>
       <c r="B24" s="26">
         <v>41599</v>
       </c>
@@ -2337,7 +2359,7 @@
       <c r="E24" s="50">
         <v>1</v>
       </c>
-      <c r="F24" s="89">
+      <c r="F24" s="100">
         <f>SUM(E24:E28)</f>
         <v>6.9</v>
       </c>
@@ -2355,7 +2377,7 @@
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="134"/>
+      <c r="A25" s="102"/>
       <c r="B25" s="26">
         <v>41599</v>
       </c>
@@ -2368,7 +2390,7 @@
       <c r="E25" s="50">
         <v>1.3</v>
       </c>
-      <c r="F25" s="112"/>
+      <c r="F25" s="120"/>
       <c r="G25" s="57" t="s">
         <v>19</v>
       </c>
@@ -2383,7 +2405,7 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="134"/>
+      <c r="A26" s="102"/>
       <c r="B26" s="26">
         <v>41599</v>
       </c>
@@ -2396,7 +2418,7 @@
       <c r="E26" s="50">
         <v>1.5</v>
       </c>
-      <c r="F26" s="112"/>
+      <c r="F26" s="120"/>
       <c r="G26" s="57" t="s">
         <v>22</v>
       </c>
@@ -2413,7 +2435,7 @@
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="134"/>
+      <c r="A27" s="102"/>
       <c r="B27" s="26">
         <v>41599</v>
       </c>
@@ -2426,7 +2448,7 @@
       <c r="E27" s="50">
         <v>2.1</v>
       </c>
-      <c r="F27" s="112"/>
+      <c r="F27" s="120"/>
       <c r="G27" s="29" t="s">
         <v>19</v>
       </c>
@@ -2440,7 +2462,7 @@
       </c>
       <c r="L27" s="5"/>
       <c r="M27" s="9">
-        <f>SUM(E72:E76)</f>
+        <f>SUM(E74:E78)</f>
         <v>0</v>
       </c>
       <c r="N27" s="3" t="s">
@@ -2448,7 +2470,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="134"/>
+      <c r="A28" s="102"/>
       <c r="B28" s="26">
         <v>41599</v>
       </c>
@@ -2461,7 +2483,7 @@
       <c r="E28" s="50">
         <v>1</v>
       </c>
-      <c r="F28" s="113"/>
+      <c r="F28" s="121"/>
       <c r="G28" s="29" t="s">
         <v>22</v>
       </c>
@@ -2476,7 +2498,7 @@
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="134"/>
+      <c r="A29" s="102"/>
       <c r="B29" s="26">
         <v>41600</v>
       </c>
@@ -2489,7 +2511,7 @@
       <c r="E29" s="50">
         <v>1.2</v>
       </c>
-      <c r="F29" s="89">
+      <c r="F29" s="100">
         <f>SUM(E29:E30)</f>
         <v>3.2</v>
       </c>
@@ -2505,7 +2527,7 @@
       <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:14" ht="51" x14ac:dyDescent="0.25">
-      <c r="A30" s="134"/>
+      <c r="A30" s="102"/>
       <c r="B30" s="26">
         <v>41600</v>
       </c>
@@ -2518,7 +2540,7 @@
       <c r="E30" s="50">
         <v>2</v>
       </c>
-      <c r="F30" s="90"/>
+      <c r="F30" s="78"/>
       <c r="G30" s="57" t="s">
         <v>22</v>
       </c>
@@ -2532,7 +2554,7 @@
       </c>
       <c r="L30" s="5"/>
       <c r="M30" s="9">
-        <f>SUM(E77:E81)</f>
+        <f>SUM(E79:E83)</f>
         <v>0</v>
       </c>
       <c r="N30" s="3" t="s">
@@ -2540,7 +2562,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="134"/>
+      <c r="A31" s="102"/>
       <c r="B31" s="26">
         <v>41601</v>
       </c>
@@ -2553,7 +2575,7 @@
       <c r="E31" s="50">
         <v>3.5</v>
       </c>
-      <c r="F31" s="89">
+      <c r="F31" s="100">
         <f>SUM(E31:E32)</f>
         <v>4.4000000000000004</v>
       </c>
@@ -2573,7 +2595,7 @@
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="135"/>
+      <c r="A32" s="103"/>
       <c r="B32" s="26">
         <v>41601</v>
       </c>
@@ -2586,7 +2608,7 @@
       <c r="E32" s="50">
         <v>0.9</v>
       </c>
-      <c r="F32" s="90"/>
+      <c r="F32" s="78"/>
       <c r="G32" s="57" t="s">
         <v>22</v>
       </c>
@@ -2603,7 +2625,7 @@
       <c r="N32" s="3"/>
     </row>
     <row r="33" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="91">
+      <c r="A33" s="73">
         <v>4</v>
       </c>
       <c r="B33" s="27">
@@ -2637,7 +2659,7 @@
       </c>
       <c r="L33" s="5"/>
       <c r="M33" s="9">
-        <f>SUM(E82:E86)</f>
+        <f>SUM(E84:E88)</f>
         <v>0</v>
       </c>
       <c r="N33" s="3" t="s">
@@ -2645,7 +2667,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="92"/>
+      <c r="A34" s="74"/>
       <c r="B34" s="27">
         <v>41604</v>
       </c>
@@ -2658,7 +2680,7 @@
       <c r="E34" s="28">
         <v>1</v>
       </c>
-      <c r="F34" s="114">
+      <c r="F34" s="122">
         <f>SUM(E34:E37)</f>
         <v>5.75</v>
       </c>
@@ -2676,7 +2698,7 @@
       <c r="N34" s="3"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="92"/>
+      <c r="A35" s="74"/>
       <c r="B35" s="27">
         <v>41604</v>
       </c>
@@ -2689,7 +2711,7 @@
       <c r="E35" s="28">
         <v>1.5</v>
       </c>
-      <c r="F35" s="92"/>
+      <c r="F35" s="74"/>
       <c r="G35" s="67" t="s">
         <v>23</v>
       </c>
@@ -2706,7 +2728,7 @@
       <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="92"/>
+      <c r="A36" s="74"/>
       <c r="B36" s="27">
         <v>41604</v>
       </c>
@@ -2719,7 +2741,7 @@
       <c r="E36" s="28">
         <v>1.25</v>
       </c>
-      <c r="F36" s="92"/>
+      <c r="F36" s="74"/>
       <c r="G36" s="67" t="s">
         <v>19</v>
       </c>
@@ -2736,7 +2758,7 @@
       <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14" ht="51" x14ac:dyDescent="0.25">
-      <c r="A37" s="92"/>
+      <c r="A37" s="74"/>
       <c r="B37" s="27">
         <v>41604</v>
       </c>
@@ -2749,7 +2771,7 @@
       <c r="E37" s="69">
         <v>2</v>
       </c>
-      <c r="F37" s="93"/>
+      <c r="F37" s="75"/>
       <c r="G37" s="67" t="s">
         <v>22</v>
       </c>
@@ -2767,7 +2789,7 @@
       </c>
       <c r="L37" s="5"/>
       <c r="M37" s="9">
-        <f>SUM(E87:E91)</f>
+        <f>SUM(E89:E93)</f>
         <v>0</v>
       </c>
       <c r="N37" s="3" t="s">
@@ -2775,7 +2797,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="92"/>
+      <c r="A38" s="74"/>
       <c r="B38" s="27">
         <v>41605</v>
       </c>
@@ -2788,7 +2810,7 @@
       <c r="E38" s="69">
         <v>2.33</v>
       </c>
-      <c r="F38" s="91">
+      <c r="F38" s="73">
         <f>SUM(E38:E39)</f>
         <v>2.83</v>
       </c>
@@ -2805,7 +2827,7 @@
       </c>
       <c r="L38" s="5"/>
       <c r="M38" s="9">
-        <f>SUM(E92:E96)</f>
+        <f>SUM(E94:E98)</f>
         <v>0</v>
       </c>
       <c r="N38" s="3" t="s">
@@ -2813,7 +2835,7 @@
       </c>
     </row>
     <row r="39" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="92"/>
+      <c r="A39" s="74"/>
       <c r="B39" s="27">
         <v>41605</v>
       </c>
@@ -2826,7 +2848,7 @@
       <c r="E39" s="69">
         <v>0.5</v>
       </c>
-      <c r="F39" s="93"/>
+      <c r="F39" s="75"/>
       <c r="G39" s="67" t="s">
         <v>22</v>
       </c>
@@ -2843,85 +2865,95 @@
       <c r="N39" s="3"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="92"/>
+      <c r="A40" s="74"/>
       <c r="B40" s="27">
         <v>41606</v>
       </c>
-      <c r="C40" s="69"/>
-      <c r="D40" s="69"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="69">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G40" s="67"/>
-      <c r="H40" s="67"/>
+      <c r="C40" s="69" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="72" t="s">
+        <v>137</v>
+      </c>
+      <c r="E40" s="69">
+        <v>1.33</v>
+      </c>
+      <c r="F40" s="73">
+        <f>SUM(E40:E42)</f>
+        <v>5.83</v>
+      </c>
+      <c r="G40" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" s="71" t="s">
+        <v>140</v>
+      </c>
       <c r="I40" s="67"/>
       <c r="J40" s="67"/>
-      <c r="K40" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="K40" s="7"/>
       <c r="L40" s="5"/>
-      <c r="M40" s="9">
-        <f>SUM(E97:E101)</f>
-        <v>0</v>
-      </c>
-      <c r="N40" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="M40" s="9"/>
+      <c r="N40" s="3"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="93"/>
+      <c r="A41" s="74"/>
       <c r="B41" s="27">
-        <v>41607</v>
-      </c>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
-      <c r="E41" s="69"/>
-      <c r="F41" s="69">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G41" s="67"/>
-      <c r="H41" s="67"/>
+        <v>41606</v>
+      </c>
+      <c r="C41" s="69" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" s="72" t="s">
+        <v>138</v>
+      </c>
+      <c r="E41" s="69">
+        <v>1.75</v>
+      </c>
+      <c r="F41" s="74"/>
+      <c r="G41" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" s="71" t="s">
+        <v>141</v>
+      </c>
       <c r="I41" s="67"/>
       <c r="J41" s="67"/>
-      <c r="K41" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="K41" s="7"/>
       <c r="L41" s="5"/>
-      <c r="M41" s="9">
-        <f>SUM(E102:E106)</f>
-        <v>0</v>
-      </c>
-      <c r="N41" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="110">
-        <v>5</v>
-      </c>
-      <c r="B42" s="26">
-        <v>41610</v>
-      </c>
-      <c r="C42" s="55"/>
-      <c r="D42" s="55"/>
-      <c r="E42" s="55"/>
-      <c r="F42" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="3"/>
+    </row>
+    <row r="42" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="74"/>
+      <c r="B42" s="27">
+        <v>41606</v>
+      </c>
+      <c r="C42" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" s="69" t="s">
+        <v>139</v>
+      </c>
+      <c r="E42" s="69">
+        <v>2.75</v>
+      </c>
+      <c r="F42" s="75"/>
+      <c r="G42" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="I42" s="67"/>
+      <c r="J42" s="67" t="s">
+        <v>142</v>
+      </c>
       <c r="K42" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="9">
-        <f>SUM(E107:E111)</f>
+        <f>SUM(E99:E103)</f>
         <v>0</v>
       </c>
       <c r="N42" s="3" t="s">
@@ -2929,27 +2961,27 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="111"/>
-      <c r="B43" s="26">
-        <v>41611</v>
-      </c>
-      <c r="C43" s="55"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="55"/>
-      <c r="F43" s="55">
+      <c r="A43" s="75"/>
+      <c r="B43" s="27">
+        <v>41607</v>
+      </c>
+      <c r="C43" s="69"/>
+      <c r="D43" s="69"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="69">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="67"/>
+      <c r="I43" s="67"/>
+      <c r="J43" s="67"/>
       <c r="K43" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L43" s="5"/>
       <c r="M43" s="9">
-        <f>SUM(E112:E116)</f>
+        <f>SUM(E104:E108)</f>
         <v>0</v>
       </c>
       <c r="N43" s="3" t="s">
@@ -2957,9 +2989,11 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="111"/>
+      <c r="A44" s="76">
+        <v>5</v>
+      </c>
       <c r="B44" s="26">
-        <v>41612</v>
+        <v>41610</v>
       </c>
       <c r="C44" s="55"/>
       <c r="D44" s="55"/>
@@ -2973,11 +3007,11 @@
       <c r="I44" s="29"/>
       <c r="J44" s="29"/>
       <c r="K44" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L44" s="5"/>
       <c r="M44" s="9">
-        <f>SUM(E117:E121)</f>
+        <f>SUM(E109:E113)</f>
         <v>0</v>
       </c>
       <c r="N44" s="3" t="s">
@@ -2985,9 +3019,9 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="111"/>
+      <c r="A45" s="77"/>
       <c r="B45" s="26">
-        <v>41613</v>
+        <v>41611</v>
       </c>
       <c r="C45" s="55"/>
       <c r="D45" s="55"/>
@@ -3001,11 +3035,11 @@
       <c r="I45" s="29"/>
       <c r="J45" s="29"/>
       <c r="K45" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L45" s="5"/>
       <c r="M45" s="9">
-        <f>SUM(E122:E126)</f>
+        <f>SUM(E114:E118)</f>
         <v>0</v>
       </c>
       <c r="N45" s="3" t="s">
@@ -3013,9 +3047,9 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="90"/>
+      <c r="A46" s="77"/>
       <c r="B46" s="26">
-        <v>41614</v>
+        <v>41612</v>
       </c>
       <c r="C46" s="55"/>
       <c r="D46" s="55"/>
@@ -3029,11 +3063,11 @@
       <c r="I46" s="29"/>
       <c r="J46" s="29"/>
       <c r="K46" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L46" s="5"/>
       <c r="M46" s="9">
-        <f>SUM(E127:E131)</f>
+        <f>SUM(E119:E123)</f>
         <v>0</v>
       </c>
       <c r="N46" s="3" t="s">
@@ -3041,29 +3075,27 @@
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="91">
-        <v>6</v>
-      </c>
-      <c r="B47" s="27">
-        <v>41617</v>
-      </c>
-      <c r="C47" s="69"/>
-      <c r="D47" s="69"/>
-      <c r="E47" s="69"/>
-      <c r="F47" s="69">
+      <c r="A47" s="77"/>
+      <c r="B47" s="26">
+        <v>41613</v>
+      </c>
+      <c r="C47" s="55"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="55"/>
+      <c r="F47" s="55">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G47" s="67"/>
-      <c r="H47" s="67"/>
-      <c r="I47" s="67"/>
-      <c r="J47" s="67"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
       <c r="K47" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L47" s="5"/>
       <c r="M47" s="9">
-        <f>SUM(E132:E136)</f>
+        <f>SUM(E124:E128)</f>
         <v>0</v>
       </c>
       <c r="N47" s="3" t="s">
@@ -3071,27 +3103,27 @@
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="92"/>
-      <c r="B48" s="27">
-        <v>41618</v>
-      </c>
-      <c r="C48" s="69"/>
-      <c r="D48" s="69"/>
-      <c r="E48" s="69"/>
-      <c r="F48" s="69">
+      <c r="A48" s="78"/>
+      <c r="B48" s="26">
+        <v>41614</v>
+      </c>
+      <c r="C48" s="55"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="55">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G48" s="67"/>
-      <c r="H48" s="67"/>
-      <c r="I48" s="67"/>
-      <c r="J48" s="67"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="29"/>
       <c r="K48" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L48" s="5"/>
       <c r="M48" s="9">
-        <f>SUM(E137:E141)</f>
+        <f>SUM(E129:E133)</f>
         <v>0</v>
       </c>
       <c r="N48" s="3" t="s">
@@ -3099,9 +3131,11 @@
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="92"/>
+      <c r="A49" s="73">
+        <v>6</v>
+      </c>
       <c r="B49" s="27">
-        <v>41619</v>
+        <v>41617</v>
       </c>
       <c r="C49" s="69"/>
       <c r="D49" s="69"/>
@@ -3115,11 +3149,11 @@
       <c r="I49" s="67"/>
       <c r="J49" s="67"/>
       <c r="K49" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L49" s="5"/>
       <c r="M49" s="9">
-        <f>SUM(E142:E146)</f>
+        <f>SUM(E134:E138)</f>
         <v>0</v>
       </c>
       <c r="N49" s="3" t="s">
@@ -3127,9 +3161,9 @@
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="92"/>
+      <c r="A50" s="74"/>
       <c r="B50" s="27">
-        <v>41620</v>
+        <v>41618</v>
       </c>
       <c r="C50" s="69"/>
       <c r="D50" s="69"/>
@@ -3143,11 +3177,11 @@
       <c r="I50" s="67"/>
       <c r="J50" s="67"/>
       <c r="K50" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L50" s="5"/>
       <c r="M50" s="9">
-        <f>SUM(E147:E151)</f>
+        <f>SUM(E139:E143)</f>
         <v>0</v>
       </c>
       <c r="N50" s="3" t="s">
@@ -3155,9 +3189,9 @@
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="93"/>
+      <c r="A51" s="74"/>
       <c r="B51" s="27">
-        <v>41621</v>
+        <v>41619</v>
       </c>
       <c r="C51" s="69"/>
       <c r="D51" s="69"/>
@@ -3171,11 +3205,11 @@
       <c r="I51" s="67"/>
       <c r="J51" s="67"/>
       <c r="K51" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L51" s="5"/>
       <c r="M51" s="9">
-        <f>SUM(E152:E156)</f>
+        <f>SUM(E144:E148)</f>
         <v>0</v>
       </c>
       <c r="N51" s="3" t="s">
@@ -3183,29 +3217,27 @@
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="110">
-        <v>7</v>
-      </c>
-      <c r="B52" s="26">
-        <v>41624</v>
-      </c>
-      <c r="C52" s="55"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55">
+      <c r="A52" s="74"/>
+      <c r="B52" s="27">
+        <v>41620</v>
+      </c>
+      <c r="C52" s="69"/>
+      <c r="D52" s="69"/>
+      <c r="E52" s="69"/>
+      <c r="F52" s="69">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G52" s="29"/>
-      <c r="H52" s="29"/>
-      <c r="I52" s="29"/>
-      <c r="J52" s="29"/>
+      <c r="G52" s="67"/>
+      <c r="H52" s="67"/>
+      <c r="I52" s="67"/>
+      <c r="J52" s="67"/>
       <c r="K52" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L52" s="5"/>
       <c r="M52" s="9">
-        <f>SUM(E157:E161)</f>
+        <f>SUM(E149:E153)</f>
         <v>0</v>
       </c>
       <c r="N52" s="3" t="s">
@@ -3213,27 +3245,27 @@
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="111"/>
-      <c r="B53" s="26">
-        <v>41625</v>
-      </c>
-      <c r="C53" s="55"/>
-      <c r="D53" s="55"/>
-      <c r="E53" s="55"/>
-      <c r="F53" s="55">
+      <c r="A53" s="75"/>
+      <c r="B53" s="27">
+        <v>41621</v>
+      </c>
+      <c r="C53" s="69"/>
+      <c r="D53" s="69"/>
+      <c r="E53" s="69"/>
+      <c r="F53" s="69">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G53" s="29"/>
-      <c r="H53" s="29"/>
-      <c r="I53" s="29"/>
-      <c r="J53" s="29"/>
+      <c r="G53" s="67"/>
+      <c r="H53" s="67"/>
+      <c r="I53" s="67"/>
+      <c r="J53" s="67"/>
       <c r="K53" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L53" s="5"/>
       <c r="M53" s="9">
-        <f>SUM(E162:E166)</f>
+        <f>SUM(E154:E158)</f>
         <v>0</v>
       </c>
       <c r="N53" s="3" t="s">
@@ -3241,9 +3273,11 @@
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="111"/>
+      <c r="A54" s="76">
+        <v>7</v>
+      </c>
       <c r="B54" s="26">
-        <v>41626</v>
+        <v>41624</v>
       </c>
       <c r="C54" s="55"/>
       <c r="D54" s="55"/>
@@ -3257,11 +3291,11 @@
       <c r="I54" s="29"/>
       <c r="J54" s="29"/>
       <c r="K54" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L54" s="5"/>
       <c r="M54" s="9">
-        <f>SUM(E167:E171)</f>
+        <f>SUM(E159:E163)</f>
         <v>0</v>
       </c>
       <c r="N54" s="3" t="s">
@@ -3269,9 +3303,9 @@
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="111"/>
+      <c r="A55" s="77"/>
       <c r="B55" s="26">
-        <v>41627</v>
+        <v>41625</v>
       </c>
       <c r="C55" s="55"/>
       <c r="D55" s="55"/>
@@ -3284,11 +3318,22 @@
       <c r="H55" s="29"/>
       <c r="I55" s="29"/>
       <c r="J55" s="29"/>
+      <c r="K55" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="L55" s="5"/>
+      <c r="M55" s="9">
+        <f>SUM(E164:E168)</f>
+        <v>0</v>
+      </c>
+      <c r="N55" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="90"/>
+      <c r="A56" s="77"/>
       <c r="B56" s="26">
-        <v>41628</v>
+        <v>41626</v>
       </c>
       <c r="C56" s="55"/>
       <c r="D56" s="55"/>
@@ -3301,47 +3346,58 @@
       <c r="H56" s="29"/>
       <c r="I56" s="29"/>
       <c r="J56" s="29"/>
+      <c r="K56" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L56" s="5"/>
+      <c r="M56" s="9">
+        <f>SUM(E169:E173)</f>
+        <v>0</v>
+      </c>
+      <c r="N56" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="91">
+      <c r="A57" s="77"/>
+      <c r="B57" s="26">
+        <v>41627</v>
+      </c>
+      <c r="C57" s="55"/>
+      <c r="D57" s="55"/>
+      <c r="E57" s="55"/>
+      <c r="F57" s="55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G57" s="29"/>
+      <c r="H57" s="29"/>
+      <c r="I57" s="29"/>
+      <c r="J57" s="29"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="78"/>
+      <c r="B58" s="26">
+        <v>41628</v>
+      </c>
+      <c r="C58" s="55"/>
+      <c r="D58" s="55"/>
+      <c r="E58" s="55"/>
+      <c r="F58" s="55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G58" s="29"/>
+      <c r="H58" s="29"/>
+      <c r="I58" s="29"/>
+      <c r="J58" s="29"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="73">
         <v>8</v>
       </c>
-      <c r="B57" s="27">
+      <c r="B59" s="27">
         <v>41631</v>
-      </c>
-      <c r="C57" s="69"/>
-      <c r="D57" s="69"/>
-      <c r="E57" s="69"/>
-      <c r="F57" s="69">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G57" s="67"/>
-      <c r="H57" s="67"/>
-      <c r="I57" s="67"/>
-      <c r="J57" s="67"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="92"/>
-      <c r="B58" s="27">
-        <v>41632</v>
-      </c>
-      <c r="C58" s="69"/>
-      <c r="D58" s="69"/>
-      <c r="E58" s="69"/>
-      <c r="F58" s="69">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G58" s="67"/>
-      <c r="H58" s="67"/>
-      <c r="I58" s="67"/>
-      <c r="J58" s="67"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="92"/>
-      <c r="B59" s="27">
-        <v>41633</v>
       </c>
       <c r="C59" s="69"/>
       <c r="D59" s="69"/>
@@ -3356,9 +3412,9 @@
       <c r="J59" s="67"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="92"/>
+      <c r="A60" s="74"/>
       <c r="B60" s="27">
-        <v>41634</v>
+        <v>41632</v>
       </c>
       <c r="C60" s="69"/>
       <c r="D60" s="69"/>
@@ -3373,9 +3429,9 @@
       <c r="J60" s="67"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="93"/>
+      <c r="A61" s="74"/>
       <c r="B61" s="27">
-        <v>41635</v>
+        <v>41633</v>
       </c>
       <c r="C61" s="69"/>
       <c r="D61" s="69"/>
@@ -3390,51 +3446,51 @@
       <c r="J61" s="67"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="110">
+      <c r="A62" s="74"/>
+      <c r="B62" s="27">
+        <v>41634</v>
+      </c>
+      <c r="C62" s="69"/>
+      <c r="D62" s="69"/>
+      <c r="E62" s="69"/>
+      <c r="F62" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G62" s="67"/>
+      <c r="H62" s="67"/>
+      <c r="I62" s="67"/>
+      <c r="J62" s="67"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" s="75"/>
+      <c r="B63" s="27">
+        <v>41635</v>
+      </c>
+      <c r="C63" s="69"/>
+      <c r="D63" s="69"/>
+      <c r="E63" s="69"/>
+      <c r="F63" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G63" s="67"/>
+      <c r="H63" s="67"/>
+      <c r="I63" s="67"/>
+      <c r="J63" s="67"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" s="76">
         <v>9</v>
       </c>
-      <c r="B62" s="26">
+      <c r="B64" s="26">
         <v>41638</v>
-      </c>
-      <c r="C62" s="55"/>
-      <c r="D62" s="55"/>
-      <c r="E62" s="55"/>
-      <c r="F62" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G62" s="29"/>
-      <c r="H62" s="29"/>
-      <c r="I62" s="29"/>
-      <c r="J62" s="29"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="111"/>
-      <c r="B63" s="26">
-        <v>41639</v>
-      </c>
-      <c r="C63" s="55"/>
-      <c r="D63" s="55"/>
-      <c r="E63" s="55"/>
-      <c r="F63" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G63" s="29"/>
-      <c r="H63" s="29"/>
-      <c r="I63" s="29"/>
-      <c r="J63" s="29"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="111"/>
-      <c r="B64" s="26">
-        <v>41640</v>
       </c>
       <c r="C64" s="55"/>
       <c r="D64" s="55"/>
       <c r="E64" s="55"/>
       <c r="F64" s="55">
-        <f t="shared" ref="F64:F95" si="1">E64</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G64" s="29"/>
@@ -3443,15 +3499,15 @@
       <c r="J64" s="29"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="111"/>
+      <c r="A65" s="77"/>
       <c r="B65" s="26">
-        <v>41641</v>
+        <v>41639</v>
       </c>
       <c r="C65" s="55"/>
       <c r="D65" s="55"/>
       <c r="E65" s="55"/>
       <c r="F65" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G65" s="29"/>
@@ -3460,15 +3516,15 @@
       <c r="J65" s="29"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="90"/>
+      <c r="A66" s="77"/>
       <c r="B66" s="26">
-        <v>41642</v>
+        <v>41640</v>
       </c>
       <c r="C66" s="55"/>
       <c r="D66" s="55"/>
       <c r="E66" s="55"/>
       <c r="F66" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F66:F97" si="1">E66</f>
         <v>0</v>
       </c>
       <c r="G66" s="29"/>
@@ -3477,45 +3533,45 @@
       <c r="J66" s="29"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="91">
+      <c r="A67" s="77"/>
+      <c r="B67" s="26">
+        <v>41641</v>
+      </c>
+      <c r="C67" s="55"/>
+      <c r="D67" s="55"/>
+      <c r="E67" s="55"/>
+      <c r="F67" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G67" s="29"/>
+      <c r="H67" s="29"/>
+      <c r="I67" s="29"/>
+      <c r="J67" s="29"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="78"/>
+      <c r="B68" s="26">
+        <v>41642</v>
+      </c>
+      <c r="C68" s="55"/>
+      <c r="D68" s="55"/>
+      <c r="E68" s="55"/>
+      <c r="F68" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G68" s="29"/>
+      <c r="H68" s="29"/>
+      <c r="I68" s="29"/>
+      <c r="J68" s="29"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="73">
         <v>10</v>
       </c>
-      <c r="B67" s="27">
+      <c r="B69" s="27">
         <v>41645</v>
-      </c>
-      <c r="C67" s="69"/>
-      <c r="D67" s="69"/>
-      <c r="E67" s="69"/>
-      <c r="F67" s="69">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G67" s="67"/>
-      <c r="H67" s="67"/>
-      <c r="I67" s="67"/>
-      <c r="J67" s="67"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="92"/>
-      <c r="B68" s="27">
-        <v>41646</v>
-      </c>
-      <c r="C68" s="69"/>
-      <c r="D68" s="69"/>
-      <c r="E68" s="69"/>
-      <c r="F68" s="69">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G68" s="67"/>
-      <c r="H68" s="67"/>
-      <c r="I68" s="67"/>
-      <c r="J68" s="67"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="92"/>
-      <c r="B69" s="27">
-        <v>41647</v>
       </c>
       <c r="C69" s="69"/>
       <c r="D69" s="69"/>
@@ -3530,9 +3586,9 @@
       <c r="J69" s="67"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="92"/>
+      <c r="A70" s="74"/>
       <c r="B70" s="27">
-        <v>41648</v>
+        <v>41646</v>
       </c>
       <c r="C70" s="69"/>
       <c r="D70" s="69"/>
@@ -3547,9 +3603,9 @@
       <c r="J70" s="67"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="93"/>
+      <c r="A71" s="74"/>
       <c r="B71" s="27">
-        <v>41649</v>
+        <v>41647</v>
       </c>
       <c r="C71" s="69"/>
       <c r="D71" s="69"/>
@@ -3564,45 +3620,45 @@
       <c r="J71" s="67"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="110">
+      <c r="A72" s="74"/>
+      <c r="B72" s="27">
+        <v>41648</v>
+      </c>
+      <c r="C72" s="69"/>
+      <c r="D72" s="69"/>
+      <c r="E72" s="69"/>
+      <c r="F72" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G72" s="67"/>
+      <c r="H72" s="67"/>
+      <c r="I72" s="67"/>
+      <c r="J72" s="67"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="75"/>
+      <c r="B73" s="27">
+        <v>41649</v>
+      </c>
+      <c r="C73" s="69"/>
+      <c r="D73" s="69"/>
+      <c r="E73" s="69"/>
+      <c r="F73" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G73" s="67"/>
+      <c r="H73" s="67"/>
+      <c r="I73" s="67"/>
+      <c r="J73" s="67"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="76">
         <v>11</v>
       </c>
-      <c r="B72" s="26">
+      <c r="B74" s="26">
         <v>41652</v>
-      </c>
-      <c r="C72" s="55"/>
-      <c r="D72" s="55"/>
-      <c r="E72" s="55"/>
-      <c r="F72" s="55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G72" s="29"/>
-      <c r="H72" s="29"/>
-      <c r="I72" s="29"/>
-      <c r="J72" s="29"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="111"/>
-      <c r="B73" s="26">
-        <v>41653</v>
-      </c>
-      <c r="C73" s="55"/>
-      <c r="D73" s="55"/>
-      <c r="E73" s="55"/>
-      <c r="F73" s="55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G73" s="29"/>
-      <c r="H73" s="29"/>
-      <c r="I73" s="29"/>
-      <c r="J73" s="29"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="111"/>
-      <c r="B74" s="26">
-        <v>41654</v>
       </c>
       <c r="C74" s="55"/>
       <c r="D74" s="55"/>
@@ -3617,9 +3673,9 @@
       <c r="J74" s="29"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="111"/>
+      <c r="A75" s="77"/>
       <c r="B75" s="26">
-        <v>41655</v>
+        <v>41653</v>
       </c>
       <c r="C75" s="55"/>
       <c r="D75" s="55"/>
@@ -3634,9 +3690,9 @@
       <c r="J75" s="29"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="90"/>
+      <c r="A76" s="77"/>
       <c r="B76" s="26">
-        <v>41656</v>
+        <v>41654</v>
       </c>
       <c r="C76" s="55"/>
       <c r="D76" s="55"/>
@@ -3651,45 +3707,45 @@
       <c r="J76" s="29"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="91">
+      <c r="A77" s="77"/>
+      <c r="B77" s="26">
+        <v>41655</v>
+      </c>
+      <c r="C77" s="55"/>
+      <c r="D77" s="55"/>
+      <c r="E77" s="55"/>
+      <c r="F77" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G77" s="29"/>
+      <c r="H77" s="29"/>
+      <c r="I77" s="29"/>
+      <c r="J77" s="29"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="78"/>
+      <c r="B78" s="26">
+        <v>41656</v>
+      </c>
+      <c r="C78" s="55"/>
+      <c r="D78" s="55"/>
+      <c r="E78" s="55"/>
+      <c r="F78" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G78" s="29"/>
+      <c r="H78" s="29"/>
+      <c r="I78" s="29"/>
+      <c r="J78" s="29"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="73">
         <v>12</v>
       </c>
-      <c r="B77" s="27">
+      <c r="B79" s="27">
         <v>41659</v>
-      </c>
-      <c r="C77" s="69"/>
-      <c r="D77" s="69"/>
-      <c r="E77" s="69"/>
-      <c r="F77" s="69">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G77" s="67"/>
-      <c r="H77" s="67"/>
-      <c r="I77" s="67"/>
-      <c r="J77" s="67"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="92"/>
-      <c r="B78" s="27">
-        <v>41660</v>
-      </c>
-      <c r="C78" s="69"/>
-      <c r="D78" s="69"/>
-      <c r="E78" s="69"/>
-      <c r="F78" s="69">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G78" s="67"/>
-      <c r="H78" s="67"/>
-      <c r="I78" s="67"/>
-      <c r="J78" s="67"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="92"/>
-      <c r="B79" s="27">
-        <v>41661</v>
       </c>
       <c r="C79" s="69"/>
       <c r="D79" s="69"/>
@@ -3704,9 +3760,9 @@
       <c r="J79" s="67"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="92"/>
+      <c r="A80" s="74"/>
       <c r="B80" s="27">
-        <v>41662</v>
+        <v>41660</v>
       </c>
       <c r="C80" s="69"/>
       <c r="D80" s="69"/>
@@ -3721,9 +3777,9 @@
       <c r="J80" s="67"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="93"/>
+      <c r="A81" s="74"/>
       <c r="B81" s="27">
-        <v>41663</v>
+        <v>41661</v>
       </c>
       <c r="C81" s="69"/>
       <c r="D81" s="69"/>
@@ -3738,49 +3794,45 @@
       <c r="J81" s="67"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="110">
+      <c r="A82" s="74"/>
+      <c r="B82" s="27">
+        <v>41662</v>
+      </c>
+      <c r="C82" s="69"/>
+      <c r="D82" s="69"/>
+      <c r="E82" s="69"/>
+      <c r="F82" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G82" s="67"/>
+      <c r="H82" s="67"/>
+      <c r="I82" s="67"/>
+      <c r="J82" s="67"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="75"/>
+      <c r="B83" s="27">
+        <v>41663</v>
+      </c>
+      <c r="C83" s="69"/>
+      <c r="D83" s="69"/>
+      <c r="E83" s="69"/>
+      <c r="F83" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G83" s="67"/>
+      <c r="H83" s="67"/>
+      <c r="I83" s="67"/>
+      <c r="J83" s="67"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="76">
         <v>13</v>
       </c>
-      <c r="B82" s="26">
+      <c r="B84" s="26">
         <v>41666</v>
-      </c>
-      <c r="C82" s="55"/>
-      <c r="D82" s="55"/>
-      <c r="E82" s="55"/>
-      <c r="F82" s="55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G82" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="H82" s="29"/>
-      <c r="I82" s="29"/>
-      <c r="J82" s="29"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="111"/>
-      <c r="B83" s="26">
-        <v>41667</v>
-      </c>
-      <c r="C83" s="55"/>
-      <c r="D83" s="55"/>
-      <c r="E83" s="55"/>
-      <c r="F83" s="55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G83" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="H83" s="29"/>
-      <c r="I83" s="29"/>
-      <c r="J83" s="29"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="111"/>
-      <c r="B84" s="26">
-        <v>41668</v>
       </c>
       <c r="C84" s="55"/>
       <c r="D84" s="55"/>
@@ -3797,9 +3849,9 @@
       <c r="J84" s="29"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="111"/>
+      <c r="A85" s="77"/>
       <c r="B85" s="26">
-        <v>41669</v>
+        <v>41667</v>
       </c>
       <c r="C85" s="55"/>
       <c r="D85" s="55"/>
@@ -3816,9 +3868,9 @@
       <c r="J85" s="29"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="90"/>
+      <c r="A86" s="77"/>
       <c r="B86" s="26">
-        <v>41670</v>
+        <v>41668</v>
       </c>
       <c r="C86" s="55"/>
       <c r="D86" s="55"/>
@@ -3835,49 +3887,49 @@
       <c r="J86" s="29"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="91">
+      <c r="A87" s="77"/>
+      <c r="B87" s="26">
+        <v>41669</v>
+      </c>
+      <c r="C87" s="55"/>
+      <c r="D87" s="55"/>
+      <c r="E87" s="55"/>
+      <c r="F87" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G87" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="H87" s="29"/>
+      <c r="I87" s="29"/>
+      <c r="J87" s="29"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="78"/>
+      <c r="B88" s="26">
+        <v>41670</v>
+      </c>
+      <c r="C88" s="55"/>
+      <c r="D88" s="55"/>
+      <c r="E88" s="55"/>
+      <c r="F88" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G88" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="H88" s="29"/>
+      <c r="I88" s="29"/>
+      <c r="J88" s="29"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="73">
         <v>14</v>
       </c>
-      <c r="B87" s="27">
+      <c r="B89" s="27">
         <v>41673</v>
-      </c>
-      <c r="C87" s="69"/>
-      <c r="D87" s="69"/>
-      <c r="E87" s="69"/>
-      <c r="F87" s="69">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G87" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="H87" s="67"/>
-      <c r="I87" s="67"/>
-      <c r="J87" s="67"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="92"/>
-      <c r="B88" s="27">
-        <v>41674</v>
-      </c>
-      <c r="C88" s="69"/>
-      <c r="D88" s="69"/>
-      <c r="E88" s="69"/>
-      <c r="F88" s="69">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G88" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="H88" s="67"/>
-      <c r="I88" s="67"/>
-      <c r="J88" s="67"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="92"/>
-      <c r="B89" s="27">
-        <v>41675</v>
       </c>
       <c r="C89" s="69"/>
       <c r="D89" s="69"/>
@@ -3894,9 +3946,9 @@
       <c r="J89" s="67"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="92"/>
+      <c r="A90" s="74"/>
       <c r="B90" s="27">
-        <v>41676</v>
+        <v>41674</v>
       </c>
       <c r="C90" s="69"/>
       <c r="D90" s="69"/>
@@ -3913,9 +3965,9 @@
       <c r="J90" s="67"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="93"/>
+      <c r="A91" s="74"/>
       <c r="B91" s="27">
-        <v>41677</v>
+        <v>41675</v>
       </c>
       <c r="C91" s="69"/>
       <c r="D91" s="69"/>
@@ -3932,45 +3984,49 @@
       <c r="J91" s="67"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="110">
+      <c r="A92" s="74"/>
+      <c r="B92" s="27">
+        <v>41676</v>
+      </c>
+      <c r="C92" s="69"/>
+      <c r="D92" s="69"/>
+      <c r="E92" s="69"/>
+      <c r="F92" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G92" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="H92" s="67"/>
+      <c r="I92" s="67"/>
+      <c r="J92" s="67"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="75"/>
+      <c r="B93" s="27">
+        <v>41677</v>
+      </c>
+      <c r="C93" s="69"/>
+      <c r="D93" s="69"/>
+      <c r="E93" s="69"/>
+      <c r="F93" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G93" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="H93" s="67"/>
+      <c r="I93" s="67"/>
+      <c r="J93" s="67"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="76">
         <v>15</v>
       </c>
-      <c r="B92" s="26">
+      <c r="B94" s="26">
         <v>41680</v>
-      </c>
-      <c r="C92" s="55"/>
-      <c r="D92" s="55"/>
-      <c r="E92" s="55"/>
-      <c r="F92" s="55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G92" s="29"/>
-      <c r="H92" s="29"/>
-      <c r="I92" s="29"/>
-      <c r="J92" s="29"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="111"/>
-      <c r="B93" s="26">
-        <v>41681</v>
-      </c>
-      <c r="C93" s="55"/>
-      <c r="D93" s="55"/>
-      <c r="E93" s="55"/>
-      <c r="F93" s="55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G93" s="29"/>
-      <c r="H93" s="29"/>
-      <c r="I93" s="29"/>
-      <c r="J93" s="29"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="111"/>
-      <c r="B94" s="26">
-        <v>41682</v>
       </c>
       <c r="C94" s="55"/>
       <c r="D94" s="55"/>
@@ -3985,9 +4041,9 @@
       <c r="J94" s="29"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="111"/>
+      <c r="A95" s="77"/>
       <c r="B95" s="26">
-        <v>41683</v>
+        <v>41681</v>
       </c>
       <c r="C95" s="55"/>
       <c r="D95" s="55"/>
@@ -4002,15 +4058,15 @@
       <c r="J95" s="29"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="90"/>
+      <c r="A96" s="77"/>
       <c r="B96" s="26">
-        <v>41684</v>
+        <v>41682</v>
       </c>
       <c r="C96" s="55"/>
       <c r="D96" s="55"/>
       <c r="E96" s="55"/>
       <c r="F96" s="55">
-        <f t="shared" ref="F96:F127" si="2">E96</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G96" s="29"/>
@@ -4019,45 +4075,45 @@
       <c r="J96" s="29"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" s="91">
+      <c r="A97" s="77"/>
+      <c r="B97" s="26">
+        <v>41683</v>
+      </c>
+      <c r="C97" s="55"/>
+      <c r="D97" s="55"/>
+      <c r="E97" s="55"/>
+      <c r="F97" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G97" s="29"/>
+      <c r="H97" s="29"/>
+      <c r="I97" s="29"/>
+      <c r="J97" s="29"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="78"/>
+      <c r="B98" s="26">
+        <v>41684</v>
+      </c>
+      <c r="C98" s="55"/>
+      <c r="D98" s="55"/>
+      <c r="E98" s="55"/>
+      <c r="F98" s="55">
+        <f t="shared" ref="F98:F129" si="2">E98</f>
+        <v>0</v>
+      </c>
+      <c r="G98" s="29"/>
+      <c r="H98" s="29"/>
+      <c r="I98" s="29"/>
+      <c r="J98" s="29"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="73">
         <v>16</v>
       </c>
-      <c r="B97" s="27">
+      <c r="B99" s="27">
         <v>41687</v>
-      </c>
-      <c r="C97" s="69"/>
-      <c r="D97" s="69"/>
-      <c r="E97" s="69"/>
-      <c r="F97" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G97" s="67"/>
-      <c r="H97" s="67"/>
-      <c r="I97" s="67"/>
-      <c r="J97" s="67"/>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" s="92"/>
-      <c r="B98" s="27">
-        <v>41688</v>
-      </c>
-      <c r="C98" s="69"/>
-      <c r="D98" s="69"/>
-      <c r="E98" s="69"/>
-      <c r="F98" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G98" s="67"/>
-      <c r="H98" s="67"/>
-      <c r="I98" s="67"/>
-      <c r="J98" s="67"/>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" s="92"/>
-      <c r="B99" s="27">
-        <v>41689</v>
       </c>
       <c r="C99" s="69"/>
       <c r="D99" s="69"/>
@@ -4072,9 +4128,9 @@
       <c r="J99" s="67"/>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" s="92"/>
+      <c r="A100" s="74"/>
       <c r="B100" s="27">
-        <v>41690</v>
+        <v>41688</v>
       </c>
       <c r="C100" s="69"/>
       <c r="D100" s="69"/>
@@ -4089,9 +4145,9 @@
       <c r="J100" s="67"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" s="93"/>
+      <c r="A101" s="74"/>
       <c r="B101" s="27">
-        <v>41691</v>
+        <v>41689</v>
       </c>
       <c r="C101" s="69"/>
       <c r="D101" s="69"/>
@@ -4106,45 +4162,45 @@
       <c r="J101" s="67"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="110">
+      <c r="A102" s="74"/>
+      <c r="B102" s="27">
+        <v>41690</v>
+      </c>
+      <c r="C102" s="69"/>
+      <c r="D102" s="69"/>
+      <c r="E102" s="69"/>
+      <c r="F102" s="69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G102" s="67"/>
+      <c r="H102" s="67"/>
+      <c r="I102" s="67"/>
+      <c r="J102" s="67"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="75"/>
+      <c r="B103" s="27">
+        <v>41691</v>
+      </c>
+      <c r="C103" s="69"/>
+      <c r="D103" s="69"/>
+      <c r="E103" s="69"/>
+      <c r="F103" s="69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G103" s="67"/>
+      <c r="H103" s="67"/>
+      <c r="I103" s="67"/>
+      <c r="J103" s="67"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="76">
         <v>17</v>
       </c>
-      <c r="B102" s="26">
+      <c r="B104" s="26">
         <v>41694</v>
-      </c>
-      <c r="C102" s="55"/>
-      <c r="D102" s="55"/>
-      <c r="E102" s="55"/>
-      <c r="F102" s="55">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G102" s="29"/>
-      <c r="H102" s="29"/>
-      <c r="I102" s="29"/>
-      <c r="J102" s="29"/>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" s="111"/>
-      <c r="B103" s="26">
-        <v>41695</v>
-      </c>
-      <c r="C103" s="55"/>
-      <c r="D103" s="55"/>
-      <c r="E103" s="55"/>
-      <c r="F103" s="55">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G103" s="29"/>
-      <c r="H103" s="29"/>
-      <c r="I103" s="29"/>
-      <c r="J103" s="29"/>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" s="111"/>
-      <c r="B104" s="26">
-        <v>41696</v>
       </c>
       <c r="C104" s="55"/>
       <c r="D104" s="55"/>
@@ -4159,9 +4215,9 @@
       <c r="J104" s="29"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" s="111"/>
+      <c r="A105" s="77"/>
       <c r="B105" s="26">
-        <v>41697</v>
+        <v>41695</v>
       </c>
       <c r="C105" s="55"/>
       <c r="D105" s="55"/>
@@ -4176,9 +4232,9 @@
       <c r="J105" s="29"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="90"/>
+      <c r="A106" s="77"/>
       <c r="B106" s="26">
-        <v>41698</v>
+        <v>41696</v>
       </c>
       <c r="C106" s="55"/>
       <c r="D106" s="55"/>
@@ -4193,45 +4249,45 @@
       <c r="J106" s="29"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="91">
+      <c r="A107" s="77"/>
+      <c r="B107" s="26">
+        <v>41697</v>
+      </c>
+      <c r="C107" s="55"/>
+      <c r="D107" s="55"/>
+      <c r="E107" s="55"/>
+      <c r="F107" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G107" s="29"/>
+      <c r="H107" s="29"/>
+      <c r="I107" s="29"/>
+      <c r="J107" s="29"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="78"/>
+      <c r="B108" s="26">
+        <v>41698</v>
+      </c>
+      <c r="C108" s="55"/>
+      <c r="D108" s="55"/>
+      <c r="E108" s="55"/>
+      <c r="F108" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G108" s="29"/>
+      <c r="H108" s="29"/>
+      <c r="I108" s="29"/>
+      <c r="J108" s="29"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="73">
         <v>18</v>
       </c>
-      <c r="B107" s="27">
+      <c r="B109" s="27">
         <v>41701</v>
-      </c>
-      <c r="C107" s="69"/>
-      <c r="D107" s="69"/>
-      <c r="E107" s="69"/>
-      <c r="F107" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G107" s="67"/>
-      <c r="H107" s="67"/>
-      <c r="I107" s="67"/>
-      <c r="J107" s="67"/>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108" s="92"/>
-      <c r="B108" s="27">
-        <v>41702</v>
-      </c>
-      <c r="C108" s="69"/>
-      <c r="D108" s="69"/>
-      <c r="E108" s="69"/>
-      <c r="F108" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G108" s="67"/>
-      <c r="H108" s="67"/>
-      <c r="I108" s="67"/>
-      <c r="J108" s="67"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" s="92"/>
-      <c r="B109" s="27">
-        <v>41703</v>
       </c>
       <c r="C109" s="69"/>
       <c r="D109" s="69"/>
@@ -4246,9 +4302,9 @@
       <c r="J109" s="67"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" s="92"/>
+      <c r="A110" s="74"/>
       <c r="B110" s="27">
-        <v>41704</v>
+        <v>41702</v>
       </c>
       <c r="C110" s="69"/>
       <c r="D110" s="69"/>
@@ -4263,9 +4319,9 @@
       <c r="J110" s="67"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" s="93"/>
+      <c r="A111" s="74"/>
       <c r="B111" s="27">
-        <v>41705</v>
+        <v>41703</v>
       </c>
       <c r="C111" s="69"/>
       <c r="D111" s="69"/>
@@ -4280,45 +4336,45 @@
       <c r="J111" s="67"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" s="110">
+      <c r="A112" s="74"/>
+      <c r="B112" s="27">
+        <v>41704</v>
+      </c>
+      <c r="C112" s="69"/>
+      <c r="D112" s="69"/>
+      <c r="E112" s="69"/>
+      <c r="F112" s="69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G112" s="67"/>
+      <c r="H112" s="67"/>
+      <c r="I112" s="67"/>
+      <c r="J112" s="67"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="75"/>
+      <c r="B113" s="27">
+        <v>41705</v>
+      </c>
+      <c r="C113" s="69"/>
+      <c r="D113" s="69"/>
+      <c r="E113" s="69"/>
+      <c r="F113" s="69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G113" s="67"/>
+      <c r="H113" s="67"/>
+      <c r="I113" s="67"/>
+      <c r="J113" s="67"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="76">
         <v>19</v>
       </c>
-      <c r="B112" s="26">
+      <c r="B114" s="26">
         <v>41708</v>
-      </c>
-      <c r="C112" s="55"/>
-      <c r="D112" s="55"/>
-      <c r="E112" s="55"/>
-      <c r="F112" s="55">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G112" s="29"/>
-      <c r="H112" s="29"/>
-      <c r="I112" s="29"/>
-      <c r="J112" s="29"/>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" s="111"/>
-      <c r="B113" s="26">
-        <v>41709</v>
-      </c>
-      <c r="C113" s="55"/>
-      <c r="D113" s="55"/>
-      <c r="E113" s="55"/>
-      <c r="F113" s="55">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G113" s="29"/>
-      <c r="H113" s="29"/>
-      <c r="I113" s="29"/>
-      <c r="J113" s="29"/>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" s="111"/>
-      <c r="B114" s="26">
-        <v>41710</v>
       </c>
       <c r="C114" s="55"/>
       <c r="D114" s="55"/>
@@ -4333,9 +4389,9 @@
       <c r="J114" s="29"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" s="111"/>
+      <c r="A115" s="77"/>
       <c r="B115" s="26">
-        <v>41711</v>
+        <v>41709</v>
       </c>
       <c r="C115" s="55"/>
       <c r="D115" s="55"/>
@@ -4350,9 +4406,9 @@
       <c r="J115" s="29"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" s="90"/>
+      <c r="A116" s="77"/>
       <c r="B116" s="26">
-        <v>41712</v>
+        <v>41710</v>
       </c>
       <c r="C116" s="55"/>
       <c r="D116" s="55"/>
@@ -4367,45 +4423,45 @@
       <c r="J116" s="29"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" s="91">
+      <c r="A117" s="77"/>
+      <c r="B117" s="26">
+        <v>41711</v>
+      </c>
+      <c r="C117" s="55"/>
+      <c r="D117" s="55"/>
+      <c r="E117" s="55"/>
+      <c r="F117" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G117" s="29"/>
+      <c r="H117" s="29"/>
+      <c r="I117" s="29"/>
+      <c r="J117" s="29"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A118" s="78"/>
+      <c r="B118" s="26">
+        <v>41712</v>
+      </c>
+      <c r="C118" s="55"/>
+      <c r="D118" s="55"/>
+      <c r="E118" s="55"/>
+      <c r="F118" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G118" s="29"/>
+      <c r="H118" s="29"/>
+      <c r="I118" s="29"/>
+      <c r="J118" s="29"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119" s="73">
         <v>20</v>
       </c>
-      <c r="B117" s="27">
+      <c r="B119" s="27">
         <v>41715</v>
-      </c>
-      <c r="C117" s="69"/>
-      <c r="D117" s="69"/>
-      <c r="E117" s="69"/>
-      <c r="F117" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G117" s="67"/>
-      <c r="H117" s="67"/>
-      <c r="I117" s="67"/>
-      <c r="J117" s="67"/>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" s="92"/>
-      <c r="B118" s="27">
-        <v>41716</v>
-      </c>
-      <c r="C118" s="69"/>
-      <c r="D118" s="69"/>
-      <c r="E118" s="69"/>
-      <c r="F118" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G118" s="67"/>
-      <c r="H118" s="67"/>
-      <c r="I118" s="67"/>
-      <c r="J118" s="67"/>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119" s="92"/>
-      <c r="B119" s="27">
-        <v>41717</v>
       </c>
       <c r="C119" s="69"/>
       <c r="D119" s="69"/>
@@ -4420,9 +4476,9 @@
       <c r="J119" s="67"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" s="92"/>
+      <c r="A120" s="74"/>
       <c r="B120" s="27">
-        <v>41718</v>
+        <v>41716</v>
       </c>
       <c r="C120" s="69"/>
       <c r="D120" s="69"/>
@@ -4437,9 +4493,9 @@
       <c r="J120" s="67"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A121" s="93"/>
+      <c r="A121" s="74"/>
       <c r="B121" s="27">
-        <v>41719</v>
+        <v>41717</v>
       </c>
       <c r="C121" s="69"/>
       <c r="D121" s="69"/>
@@ -4454,45 +4510,45 @@
       <c r="J121" s="67"/>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A122" s="110">
+      <c r="A122" s="74"/>
+      <c r="B122" s="27">
+        <v>41718</v>
+      </c>
+      <c r="C122" s="69"/>
+      <c r="D122" s="69"/>
+      <c r="E122" s="69"/>
+      <c r="F122" s="69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G122" s="67"/>
+      <c r="H122" s="67"/>
+      <c r="I122" s="67"/>
+      <c r="J122" s="67"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A123" s="75"/>
+      <c r="B123" s="27">
+        <v>41719</v>
+      </c>
+      <c r="C123" s="69"/>
+      <c r="D123" s="69"/>
+      <c r="E123" s="69"/>
+      <c r="F123" s="69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G123" s="67"/>
+      <c r="H123" s="67"/>
+      <c r="I123" s="67"/>
+      <c r="J123" s="67"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A124" s="76">
         <v>21</v>
       </c>
-      <c r="B122" s="26">
+      <c r="B124" s="26">
         <v>41722</v>
-      </c>
-      <c r="C122" s="55"/>
-      <c r="D122" s="55"/>
-      <c r="E122" s="55"/>
-      <c r="F122" s="55">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G122" s="29"/>
-      <c r="H122" s="29"/>
-      <c r="I122" s="29"/>
-      <c r="J122" s="29"/>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A123" s="111"/>
-      <c r="B123" s="26">
-        <v>41723</v>
-      </c>
-      <c r="C123" s="55"/>
-      <c r="D123" s="55"/>
-      <c r="E123" s="55"/>
-      <c r="F123" s="55">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G123" s="29"/>
-      <c r="H123" s="29"/>
-      <c r="I123" s="29"/>
-      <c r="J123" s="29"/>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A124" s="111"/>
-      <c r="B124" s="26">
-        <v>41724</v>
       </c>
       <c r="C124" s="55"/>
       <c r="D124" s="55"/>
@@ -4507,9 +4563,9 @@
       <c r="J124" s="29"/>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A125" s="111"/>
+      <c r="A125" s="77"/>
       <c r="B125" s="26">
-        <v>41725</v>
+        <v>41723</v>
       </c>
       <c r="C125" s="55"/>
       <c r="D125" s="55"/>
@@ -4524,9 +4580,9 @@
       <c r="J125" s="29"/>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A126" s="90"/>
+      <c r="A126" s="77"/>
       <c r="B126" s="26">
-        <v>41726</v>
+        <v>41724</v>
       </c>
       <c r="C126" s="55"/>
       <c r="D126" s="55"/>
@@ -4541,51 +4597,51 @@
       <c r="J126" s="29"/>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A127" s="91">
+      <c r="A127" s="77"/>
+      <c r="B127" s="26">
+        <v>41725</v>
+      </c>
+      <c r="C127" s="55"/>
+      <c r="D127" s="55"/>
+      <c r="E127" s="55"/>
+      <c r="F127" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G127" s="29"/>
+      <c r="H127" s="29"/>
+      <c r="I127" s="29"/>
+      <c r="J127" s="29"/>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A128" s="78"/>
+      <c r="B128" s="26">
+        <v>41726</v>
+      </c>
+      <c r="C128" s="55"/>
+      <c r="D128" s="55"/>
+      <c r="E128" s="55"/>
+      <c r="F128" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G128" s="29"/>
+      <c r="H128" s="29"/>
+      <c r="I128" s="29"/>
+      <c r="J128" s="29"/>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A129" s="73">
         <v>22</v>
       </c>
-      <c r="B127" s="27">
+      <c r="B129" s="27">
         <v>41729</v>
-      </c>
-      <c r="C127" s="69"/>
-      <c r="D127" s="69"/>
-      <c r="E127" s="69"/>
-      <c r="F127" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G127" s="67"/>
-      <c r="H127" s="67"/>
-      <c r="I127" s="67"/>
-      <c r="J127" s="67"/>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A128" s="92"/>
-      <c r="B128" s="27">
-        <v>41730</v>
-      </c>
-      <c r="C128" s="69"/>
-      <c r="D128" s="69"/>
-      <c r="E128" s="69"/>
-      <c r="F128" s="69">
-        <f t="shared" ref="F128:F159" si="3">E128</f>
-        <v>0</v>
-      </c>
-      <c r="G128" s="67"/>
-      <c r="H128" s="67"/>
-      <c r="I128" s="67"/>
-      <c r="J128" s="67"/>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A129" s="92"/>
-      <c r="B129" s="27">
-        <v>41731</v>
       </c>
       <c r="C129" s="69"/>
       <c r="D129" s="69"/>
       <c r="E129" s="69"/>
       <c r="F129" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G129" s="67"/>
@@ -4594,15 +4650,15 @@
       <c r="J129" s="67"/>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A130" s="92"/>
+      <c r="A130" s="74"/>
       <c r="B130" s="27">
-        <v>41732</v>
+        <v>41730</v>
       </c>
       <c r="C130" s="69"/>
       <c r="D130" s="69"/>
       <c r="E130" s="69"/>
       <c r="F130" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F130:F161" si="3">E130</f>
         <v>0</v>
       </c>
       <c r="G130" s="67"/>
@@ -4611,9 +4667,9 @@
       <c r="J130" s="67"/>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A131" s="93"/>
+      <c r="A131" s="74"/>
       <c r="B131" s="27">
-        <v>41733</v>
+        <v>41731</v>
       </c>
       <c r="C131" s="69"/>
       <c r="D131" s="69"/>
@@ -4628,45 +4684,45 @@
       <c r="J131" s="67"/>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A132" s="110">
+      <c r="A132" s="74"/>
+      <c r="B132" s="27">
+        <v>41732</v>
+      </c>
+      <c r="C132" s="69"/>
+      <c r="D132" s="69"/>
+      <c r="E132" s="69"/>
+      <c r="F132" s="69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G132" s="67"/>
+      <c r="H132" s="67"/>
+      <c r="I132" s="67"/>
+      <c r="J132" s="67"/>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A133" s="75"/>
+      <c r="B133" s="27">
+        <v>41733</v>
+      </c>
+      <c r="C133" s="69"/>
+      <c r="D133" s="69"/>
+      <c r="E133" s="69"/>
+      <c r="F133" s="69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G133" s="67"/>
+      <c r="H133" s="67"/>
+      <c r="I133" s="67"/>
+      <c r="J133" s="67"/>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A134" s="76">
         <v>23</v>
       </c>
-      <c r="B132" s="26">
+      <c r="B134" s="26">
         <v>41736</v>
-      </c>
-      <c r="C132" s="55"/>
-      <c r="D132" s="55"/>
-      <c r="E132" s="55"/>
-      <c r="F132" s="55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G132" s="29"/>
-      <c r="H132" s="29"/>
-      <c r="I132" s="29"/>
-      <c r="J132" s="29"/>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A133" s="111"/>
-      <c r="B133" s="26">
-        <v>41737</v>
-      </c>
-      <c r="C133" s="55"/>
-      <c r="D133" s="55"/>
-      <c r="E133" s="55"/>
-      <c r="F133" s="55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G133" s="29"/>
-      <c r="H133" s="29"/>
-      <c r="I133" s="29"/>
-      <c r="J133" s="29"/>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A134" s="111"/>
-      <c r="B134" s="26">
-        <v>41738</v>
       </c>
       <c r="C134" s="55"/>
       <c r="D134" s="55"/>
@@ -4681,9 +4737,9 @@
       <c r="J134" s="29"/>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A135" s="111"/>
+      <c r="A135" s="77"/>
       <c r="B135" s="26">
-        <v>41739</v>
+        <v>41737</v>
       </c>
       <c r="C135" s="55"/>
       <c r="D135" s="55"/>
@@ -4698,9 +4754,9 @@
       <c r="J135" s="29"/>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A136" s="90"/>
+      <c r="A136" s="77"/>
       <c r="B136" s="26">
-        <v>41740</v>
+        <v>41738</v>
       </c>
       <c r="C136" s="55"/>
       <c r="D136" s="55"/>
@@ -4715,45 +4771,45 @@
       <c r="J136" s="29"/>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A137" s="91">
+      <c r="A137" s="77"/>
+      <c r="B137" s="26">
+        <v>41739</v>
+      </c>
+      <c r="C137" s="55"/>
+      <c r="D137" s="55"/>
+      <c r="E137" s="55"/>
+      <c r="F137" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G137" s="29"/>
+      <c r="H137" s="29"/>
+      <c r="I137" s="29"/>
+      <c r="J137" s="29"/>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A138" s="78"/>
+      <c r="B138" s="26">
+        <v>41740</v>
+      </c>
+      <c r="C138" s="55"/>
+      <c r="D138" s="55"/>
+      <c r="E138" s="55"/>
+      <c r="F138" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G138" s="29"/>
+      <c r="H138" s="29"/>
+      <c r="I138" s="29"/>
+      <c r="J138" s="29"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139" s="73">
         <v>24</v>
       </c>
-      <c r="B137" s="27">
+      <c r="B139" s="27">
         <v>41743</v>
-      </c>
-      <c r="C137" s="69"/>
-      <c r="D137" s="69"/>
-      <c r="E137" s="69"/>
-      <c r="F137" s="69">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G137" s="67"/>
-      <c r="H137" s="67"/>
-      <c r="I137" s="67"/>
-      <c r="J137" s="67"/>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A138" s="92"/>
-      <c r="B138" s="27">
-        <v>41744</v>
-      </c>
-      <c r="C138" s="69"/>
-      <c r="D138" s="69"/>
-      <c r="E138" s="69"/>
-      <c r="F138" s="69">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G138" s="67"/>
-      <c r="H138" s="67"/>
-      <c r="I138" s="67"/>
-      <c r="J138" s="67"/>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A139" s="92"/>
-      <c r="B139" s="27">
-        <v>41745</v>
       </c>
       <c r="C139" s="69"/>
       <c r="D139" s="69"/>
@@ -4768,9 +4824,9 @@
       <c r="J139" s="67"/>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A140" s="92"/>
+      <c r="A140" s="74"/>
       <c r="B140" s="27">
-        <v>41746</v>
+        <v>41744</v>
       </c>
       <c r="C140" s="69"/>
       <c r="D140" s="69"/>
@@ -4785,9 +4841,9 @@
       <c r="J140" s="67"/>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A141" s="93"/>
+      <c r="A141" s="74"/>
       <c r="B141" s="27">
-        <v>41747</v>
+        <v>41745</v>
       </c>
       <c r="C141" s="69"/>
       <c r="D141" s="69"/>
@@ -4802,45 +4858,45 @@
       <c r="J141" s="67"/>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A142" s="110">
+      <c r="A142" s="74"/>
+      <c r="B142" s="27">
+        <v>41746</v>
+      </c>
+      <c r="C142" s="69"/>
+      <c r="D142" s="69"/>
+      <c r="E142" s="69"/>
+      <c r="F142" s="69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G142" s="67"/>
+      <c r="H142" s="67"/>
+      <c r="I142" s="67"/>
+      <c r="J142" s="67"/>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143" s="75"/>
+      <c r="B143" s="27">
+        <v>41747</v>
+      </c>
+      <c r="C143" s="69"/>
+      <c r="D143" s="69"/>
+      <c r="E143" s="69"/>
+      <c r="F143" s="69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G143" s="67"/>
+      <c r="H143" s="67"/>
+      <c r="I143" s="67"/>
+      <c r="J143" s="67"/>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A144" s="76">
         <v>25</v>
       </c>
-      <c r="B142" s="26">
+      <c r="B144" s="26">
         <v>41750</v>
-      </c>
-      <c r="C142" s="55"/>
-      <c r="D142" s="55"/>
-      <c r="E142" s="55"/>
-      <c r="F142" s="55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G142" s="29"/>
-      <c r="H142" s="29"/>
-      <c r="I142" s="29"/>
-      <c r="J142" s="29"/>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A143" s="111"/>
-      <c r="B143" s="26">
-        <v>41751</v>
-      </c>
-      <c r="C143" s="55"/>
-      <c r="D143" s="55"/>
-      <c r="E143" s="55"/>
-      <c r="F143" s="55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G143" s="29"/>
-      <c r="H143" s="29"/>
-      <c r="I143" s="29"/>
-      <c r="J143" s="29"/>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A144" s="111"/>
-      <c r="B144" s="26">
-        <v>41752</v>
       </c>
       <c r="C144" s="55"/>
       <c r="D144" s="55"/>
@@ -4855,9 +4911,9 @@
       <c r="J144" s="29"/>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A145" s="111"/>
+      <c r="A145" s="77"/>
       <c r="B145" s="26">
-        <v>41753</v>
+        <v>41751</v>
       </c>
       <c r="C145" s="55"/>
       <c r="D145" s="55"/>
@@ -4872,9 +4928,9 @@
       <c r="J145" s="29"/>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A146" s="90"/>
+      <c r="A146" s="77"/>
       <c r="B146" s="26">
-        <v>41754</v>
+        <v>41752</v>
       </c>
       <c r="C146" s="55"/>
       <c r="D146" s="55"/>
@@ -4889,45 +4945,45 @@
       <c r="J146" s="29"/>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A147" s="91">
+      <c r="A147" s="77"/>
+      <c r="B147" s="26">
+        <v>41753</v>
+      </c>
+      <c r="C147" s="55"/>
+      <c r="D147" s="55"/>
+      <c r="E147" s="55"/>
+      <c r="F147" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G147" s="29"/>
+      <c r="H147" s="29"/>
+      <c r="I147" s="29"/>
+      <c r="J147" s="29"/>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A148" s="78"/>
+      <c r="B148" s="26">
+        <v>41754</v>
+      </c>
+      <c r="C148" s="55"/>
+      <c r="D148" s="55"/>
+      <c r="E148" s="55"/>
+      <c r="F148" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G148" s="29"/>
+      <c r="H148" s="29"/>
+      <c r="I148" s="29"/>
+      <c r="J148" s="29"/>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A149" s="73">
         <v>26</v>
       </c>
-      <c r="B147" s="27">
+      <c r="B149" s="27">
         <v>41757</v>
-      </c>
-      <c r="C147" s="69"/>
-      <c r="D147" s="69"/>
-      <c r="E147" s="69"/>
-      <c r="F147" s="69">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G147" s="67"/>
-      <c r="H147" s="67"/>
-      <c r="I147" s="67"/>
-      <c r="J147" s="67"/>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A148" s="92"/>
-      <c r="B148" s="27">
-        <v>41758</v>
-      </c>
-      <c r="C148" s="69"/>
-      <c r="D148" s="69"/>
-      <c r="E148" s="69"/>
-      <c r="F148" s="69">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G148" s="67"/>
-      <c r="H148" s="67"/>
-      <c r="I148" s="67"/>
-      <c r="J148" s="67"/>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A149" s="92"/>
-      <c r="B149" s="27">
-        <v>41759</v>
       </c>
       <c r="C149" s="69"/>
       <c r="D149" s="69"/>
@@ -4942,9 +4998,9 @@
       <c r="J149" s="67"/>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A150" s="92"/>
+      <c r="A150" s="74"/>
       <c r="B150" s="27">
-        <v>41760</v>
+        <v>41758</v>
       </c>
       <c r="C150" s="69"/>
       <c r="D150" s="69"/>
@@ -4959,9 +5015,9 @@
       <c r="J150" s="67"/>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A151" s="93"/>
+      <c r="A151" s="74"/>
       <c r="B151" s="27">
-        <v>41761</v>
+        <v>41759</v>
       </c>
       <c r="C151" s="69"/>
       <c r="D151" s="69"/>
@@ -4976,45 +5032,45 @@
       <c r="J151" s="67"/>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A152" s="110">
+      <c r="A152" s="74"/>
+      <c r="B152" s="27">
+        <v>41760</v>
+      </c>
+      <c r="C152" s="69"/>
+      <c r="D152" s="69"/>
+      <c r="E152" s="69"/>
+      <c r="F152" s="69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G152" s="67"/>
+      <c r="H152" s="67"/>
+      <c r="I152" s="67"/>
+      <c r="J152" s="67"/>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A153" s="75"/>
+      <c r="B153" s="27">
+        <v>41761</v>
+      </c>
+      <c r="C153" s="69"/>
+      <c r="D153" s="69"/>
+      <c r="E153" s="69"/>
+      <c r="F153" s="69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G153" s="67"/>
+      <c r="H153" s="67"/>
+      <c r="I153" s="67"/>
+      <c r="J153" s="67"/>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A154" s="76">
         <v>27</v>
       </c>
-      <c r="B152" s="26">
+      <c r="B154" s="26">
         <v>41764</v>
-      </c>
-      <c r="C152" s="55"/>
-      <c r="D152" s="55"/>
-      <c r="E152" s="55"/>
-      <c r="F152" s="55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G152" s="29"/>
-      <c r="H152" s="29"/>
-      <c r="I152" s="29"/>
-      <c r="J152" s="29"/>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A153" s="111"/>
-      <c r="B153" s="26">
-        <v>41765</v>
-      </c>
-      <c r="C153" s="55"/>
-      <c r="D153" s="55"/>
-      <c r="E153" s="55"/>
-      <c r="F153" s="55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G153" s="29"/>
-      <c r="H153" s="29"/>
-      <c r="I153" s="29"/>
-      <c r="J153" s="29"/>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A154" s="111"/>
-      <c r="B154" s="26">
-        <v>41766</v>
       </c>
       <c r="C154" s="55"/>
       <c r="D154" s="55"/>
@@ -5029,9 +5085,9 @@
       <c r="J154" s="29"/>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A155" s="111"/>
+      <c r="A155" s="77"/>
       <c r="B155" s="26">
-        <v>41767</v>
+        <v>41765</v>
       </c>
       <c r="C155" s="55"/>
       <c r="D155" s="55"/>
@@ -5046,9 +5102,9 @@
       <c r="J155" s="29"/>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A156" s="90"/>
+      <c r="A156" s="77"/>
       <c r="B156" s="26">
-        <v>41768</v>
+        <v>41766</v>
       </c>
       <c r="C156" s="55"/>
       <c r="D156" s="55"/>
@@ -5063,45 +5119,45 @@
       <c r="J156" s="29"/>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A157" s="91">
+      <c r="A157" s="77"/>
+      <c r="B157" s="26">
+        <v>41767</v>
+      </c>
+      <c r="C157" s="55"/>
+      <c r="D157" s="55"/>
+      <c r="E157" s="55"/>
+      <c r="F157" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G157" s="29"/>
+      <c r="H157" s="29"/>
+      <c r="I157" s="29"/>
+      <c r="J157" s="29"/>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A158" s="78"/>
+      <c r="B158" s="26">
+        <v>41768</v>
+      </c>
+      <c r="C158" s="55"/>
+      <c r="D158" s="55"/>
+      <c r="E158" s="55"/>
+      <c r="F158" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G158" s="29"/>
+      <c r="H158" s="29"/>
+      <c r="I158" s="29"/>
+      <c r="J158" s="29"/>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A159" s="73">
         <v>28</v>
       </c>
-      <c r="B157" s="27">
+      <c r="B159" s="27">
         <v>41771</v>
-      </c>
-      <c r="C157" s="69"/>
-      <c r="D157" s="69"/>
-      <c r="E157" s="69"/>
-      <c r="F157" s="69">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G157" s="67"/>
-      <c r="H157" s="67"/>
-      <c r="I157" s="67"/>
-      <c r="J157" s="67"/>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A158" s="92"/>
-      <c r="B158" s="27">
-        <v>41772</v>
-      </c>
-      <c r="C158" s="69"/>
-      <c r="D158" s="69"/>
-      <c r="E158" s="69"/>
-      <c r="F158" s="69">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G158" s="67"/>
-      <c r="H158" s="67"/>
-      <c r="I158" s="67"/>
-      <c r="J158" s="67"/>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A159" s="92"/>
-      <c r="B159" s="27">
-        <v>41773</v>
       </c>
       <c r="C159" s="69"/>
       <c r="D159" s="69"/>
@@ -5116,15 +5172,15 @@
       <c r="J159" s="67"/>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A160" s="92"/>
+      <c r="A160" s="74"/>
       <c r="B160" s="27">
-        <v>41774</v>
+        <v>41772</v>
       </c>
       <c r="C160" s="69"/>
       <c r="D160" s="69"/>
       <c r="E160" s="69"/>
       <c r="F160" s="69">
-        <f t="shared" ref="F160:F171" si="4">E160</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G160" s="67"/>
@@ -5133,15 +5189,15 @@
       <c r="J160" s="67"/>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A161" s="93"/>
+      <c r="A161" s="74"/>
       <c r="B161" s="27">
-        <v>41775</v>
+        <v>41773</v>
       </c>
       <c r="C161" s="69"/>
       <c r="D161" s="69"/>
       <c r="E161" s="69"/>
       <c r="F161" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G161" s="67"/>
@@ -5150,45 +5206,45 @@
       <c r="J161" s="67"/>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A162" s="110">
+      <c r="A162" s="74"/>
+      <c r="B162" s="27">
+        <v>41774</v>
+      </c>
+      <c r="C162" s="69"/>
+      <c r="D162" s="69"/>
+      <c r="E162" s="69"/>
+      <c r="F162" s="69">
+        <f t="shared" ref="F162:F173" si="4">E162</f>
+        <v>0</v>
+      </c>
+      <c r="G162" s="67"/>
+      <c r="H162" s="67"/>
+      <c r="I162" s="67"/>
+      <c r="J162" s="67"/>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A163" s="75"/>
+      <c r="B163" s="27">
+        <v>41775</v>
+      </c>
+      <c r="C163" s="69"/>
+      <c r="D163" s="69"/>
+      <c r="E163" s="69"/>
+      <c r="F163" s="69">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G163" s="67"/>
+      <c r="H163" s="67"/>
+      <c r="I163" s="67"/>
+      <c r="J163" s="67"/>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A164" s="76">
         <v>29</v>
       </c>
-      <c r="B162" s="26">
+      <c r="B164" s="26">
         <v>41778</v>
-      </c>
-      <c r="C162" s="55"/>
-      <c r="D162" s="55"/>
-      <c r="E162" s="55"/>
-      <c r="F162" s="55">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G162" s="29"/>
-      <c r="H162" s="29"/>
-      <c r="I162" s="29"/>
-      <c r="J162" s="29"/>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A163" s="111"/>
-      <c r="B163" s="26">
-        <v>41779</v>
-      </c>
-      <c r="C163" s="55"/>
-      <c r="D163" s="55"/>
-      <c r="E163" s="55"/>
-      <c r="F163" s="55">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G163" s="29"/>
-      <c r="H163" s="29"/>
-      <c r="I163" s="29"/>
-      <c r="J163" s="29"/>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A164" s="111"/>
-      <c r="B164" s="26">
-        <v>41780</v>
       </c>
       <c r="C164" s="55"/>
       <c r="D164" s="55"/>
@@ -5203,9 +5259,9 @@
       <c r="J164" s="29"/>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A165" s="111"/>
+      <c r="A165" s="77"/>
       <c r="B165" s="26">
-        <v>41781</v>
+        <v>41779</v>
       </c>
       <c r="C165" s="55"/>
       <c r="D165" s="55"/>
@@ -5220,9 +5276,9 @@
       <c r="J165" s="29"/>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A166" s="90"/>
+      <c r="A166" s="77"/>
       <c r="B166" s="26">
-        <v>41782</v>
+        <v>41780</v>
       </c>
       <c r="C166" s="55"/>
       <c r="D166" s="55"/>
@@ -5237,45 +5293,45 @@
       <c r="J166" s="29"/>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A167" s="136">
+      <c r="A167" s="77"/>
+      <c r="B167" s="26">
+        <v>41781</v>
+      </c>
+      <c r="C167" s="55"/>
+      <c r="D167" s="55"/>
+      <c r="E167" s="55"/>
+      <c r="F167" s="55">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G167" s="29"/>
+      <c r="H167" s="29"/>
+      <c r="I167" s="29"/>
+      <c r="J167" s="29"/>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A168" s="78"/>
+      <c r="B168" s="26">
+        <v>41782</v>
+      </c>
+      <c r="C168" s="55"/>
+      <c r="D168" s="55"/>
+      <c r="E168" s="55"/>
+      <c r="F168" s="55">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G168" s="29"/>
+      <c r="H168" s="29"/>
+      <c r="I168" s="29"/>
+      <c r="J168" s="29"/>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A169" s="79">
         <v>30</v>
       </c>
-      <c r="B167" s="27">
+      <c r="B169" s="27">
         <v>41785</v>
-      </c>
-      <c r="C167" s="70"/>
-      <c r="D167" s="70"/>
-      <c r="E167" s="70"/>
-      <c r="F167" s="70">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G167" s="37"/>
-      <c r="H167" s="37"/>
-      <c r="I167" s="37"/>
-      <c r="J167" s="37"/>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A168" s="137"/>
-      <c r="B168" s="27">
-        <v>41786</v>
-      </c>
-      <c r="C168" s="70"/>
-      <c r="D168" s="70"/>
-      <c r="E168" s="70"/>
-      <c r="F168" s="70">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G168" s="37"/>
-      <c r="H168" s="37"/>
-      <c r="I168" s="37"/>
-      <c r="J168" s="37"/>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A169" s="137"/>
-      <c r="B169" s="27">
-        <v>41787</v>
       </c>
       <c r="C169" s="70"/>
       <c r="D169" s="70"/>
@@ -5290,9 +5346,9 @@
       <c r="J169" s="37"/>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A170" s="137"/>
+      <c r="A170" s="80"/>
       <c r="B170" s="27">
-        <v>41788</v>
+        <v>41786</v>
       </c>
       <c r="C170" s="70"/>
       <c r="D170" s="70"/>
@@ -5307,9 +5363,9 @@
       <c r="J170" s="37"/>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A171" s="138"/>
+      <c r="A171" s="80"/>
       <c r="B171" s="27">
-        <v>41789</v>
+        <v>41787</v>
       </c>
       <c r="C171" s="70"/>
       <c r="D171" s="70"/>
@@ -5324,28 +5380,38 @@
       <c r="J171" s="37"/>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A172" s="68"/>
-      <c r="B172" s="68"/>
-      <c r="C172" s="68"/>
-      <c r="D172" s="68"/>
-      <c r="E172" s="68"/>
-      <c r="F172" s="68"/>
-      <c r="G172" s="68"/>
-      <c r="H172" s="68"/>
-      <c r="I172" s="68"/>
-      <c r="J172" s="68"/>
+      <c r="A172" s="80"/>
+      <c r="B172" s="27">
+        <v>41788</v>
+      </c>
+      <c r="C172" s="70"/>
+      <c r="D172" s="70"/>
+      <c r="E172" s="70"/>
+      <c r="F172" s="70">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G172" s="37"/>
+      <c r="H172" s="37"/>
+      <c r="I172" s="37"/>
+      <c r="J172" s="37"/>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A173" s="68"/>
-      <c r="B173" s="68"/>
-      <c r="C173" s="68"/>
-      <c r="D173" s="68"/>
-      <c r="E173" s="68"/>
-      <c r="F173" s="68"/>
-      <c r="G173" s="68"/>
-      <c r="H173" s="68"/>
-      <c r="I173" s="68"/>
-      <c r="J173" s="68"/>
+      <c r="A173" s="81"/>
+      <c r="B173" s="27">
+        <v>41789</v>
+      </c>
+      <c r="C173" s="70"/>
+      <c r="D173" s="70"/>
+      <c r="E173" s="70"/>
+      <c r="F173" s="70">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G173" s="37"/>
+      <c r="H173" s="37"/>
+      <c r="I173" s="37"/>
+      <c r="J173" s="37"/>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="68"/>
@@ -5431,30 +5497,57 @@
       <c r="I180" s="68"/>
       <c r="J180" s="68"/>
     </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A181" s="68"/>
+      <c r="B181" s="68"/>
+      <c r="C181" s="68"/>
+      <c r="D181" s="68"/>
+      <c r="E181" s="68"/>
+      <c r="F181" s="68"/>
+      <c r="G181" s="68"/>
+      <c r="H181" s="68"/>
+      <c r="I181" s="68"/>
+      <c r="J181" s="68"/>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A182" s="68"/>
+      <c r="B182" s="68"/>
+      <c r="C182" s="68"/>
+      <c r="D182" s="68"/>
+      <c r="E182" s="68"/>
+      <c r="F182" s="68"/>
+      <c r="G182" s="68"/>
+      <c r="H182" s="68"/>
+      <c r="I182" s="68"/>
+      <c r="J182" s="68"/>
+    </row>
   </sheetData>
-  <mergeCells count="54">
-    <mergeCell ref="A157:A161"/>
-    <mergeCell ref="A162:A166"/>
-    <mergeCell ref="A167:A171"/>
-    <mergeCell ref="A127:A131"/>
-    <mergeCell ref="A132:A136"/>
-    <mergeCell ref="A137:A141"/>
-    <mergeCell ref="A142:A146"/>
-    <mergeCell ref="A147:A151"/>
-    <mergeCell ref="A107:A111"/>
-    <mergeCell ref="A112:A116"/>
-    <mergeCell ref="A117:A121"/>
-    <mergeCell ref="A122:A126"/>
-    <mergeCell ref="A152:A156"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="A87:A91"/>
-    <mergeCell ref="A92:A96"/>
-    <mergeCell ref="A97:A101"/>
-    <mergeCell ref="A102:A106"/>
-    <mergeCell ref="A77:A81"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="A72:A76"/>
+  <mergeCells count="55">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="G2:N4"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F4"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="A33:A43"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="A79:A83"/>
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A74:A78"/>
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="F12:F13"/>
@@ -5467,38 +5560,36 @@
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="A19:A32"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F4"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="A52:A56"/>
-    <mergeCell ref="A33:A41"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="G2:N4"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="A84:A88"/>
+    <mergeCell ref="A89:A93"/>
+    <mergeCell ref="A94:A98"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A104:A108"/>
+    <mergeCell ref="A109:A113"/>
+    <mergeCell ref="A114:A118"/>
+    <mergeCell ref="A119:A123"/>
+    <mergeCell ref="A124:A128"/>
+    <mergeCell ref="A154:A158"/>
+    <mergeCell ref="A159:A163"/>
+    <mergeCell ref="A164:A168"/>
+    <mergeCell ref="A169:A173"/>
+    <mergeCell ref="A129:A133"/>
+    <mergeCell ref="A134:A138"/>
+    <mergeCell ref="A139:A143"/>
+    <mergeCell ref="A144:A148"/>
+    <mergeCell ref="A149:A153"/>
   </mergeCells>
   <conditionalFormatting sqref="M7">
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="greaterThan">
       <formula>5000</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="lessThan">
       <formula>700</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="greaterThan">
       <formula>4704</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="between">
       <formula>700</formula>
       <formula>4704</formula>
     </cfRule>
@@ -5512,7 +5603,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="43" id="{0DBDD361-8DEA-4440-A822-84D52DAF7126}">
+          <x14:cfRule type="iconSet" priority="45" id="{0DBDD361-8DEA-4440-A822-84D52DAF7126}">
             <x14:iconSet iconSet="3Symbols" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5531,7 +5622,7 @@
           <xm:sqref>M12:M14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="42" id="{B559C907-CDCA-4CF9-AE11-AB3B902CAD1C}">
+          <x14:cfRule type="iconSet" priority="44" id="{B559C907-CDCA-4CF9-AE11-AB3B902CAD1C}">
             <x14:iconSet iconSet="3Symbols" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5550,7 +5641,7 @@
           <xm:sqref>M16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="40" id="{71646626-2950-4450-989F-AF3A1BD8FAC2}">
+          <x14:cfRule type="iconSet" priority="42" id="{71646626-2950-4450-989F-AF3A1BD8FAC2}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5569,7 +5660,7 @@
           <xm:sqref>M18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="37" id="{F3D4927F-C508-4AEC-AE77-5B47D8246C97}">
+          <x14:cfRule type="iconSet" priority="39" id="{F3D4927F-C508-4AEC-AE77-5B47D8246C97}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5588,7 +5679,7 @@
           <xm:sqref>M19:M21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="36" id="{6C6B1EFA-99FD-4C7D-9FDE-A1C62DFDC4A6}">
+          <x14:cfRule type="iconSet" priority="38" id="{6C6B1EFA-99FD-4C7D-9FDE-A1C62DFDC4A6}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5607,7 +5698,7 @@
           <xm:sqref>M22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="35" id="{728DDD0C-59C2-4EAA-A943-37D530A87696}">
+          <x14:cfRule type="iconSet" priority="37" id="{728DDD0C-59C2-4EAA-A943-37D530A87696}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5626,7 +5717,7 @@
           <xm:sqref>M23:M26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="34" id="{9AF6B611-56EC-46E2-A851-4E09E28F0C39}">
+          <x14:cfRule type="iconSet" priority="36" id="{9AF6B611-56EC-46E2-A851-4E09E28F0C39}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5645,7 +5736,7 @@
           <xm:sqref>M27:M29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="33" id="{7A1C8DB1-F7B5-44DF-B6AD-BD94518E2F59}">
+          <x14:cfRule type="iconSet" priority="35" id="{7A1C8DB1-F7B5-44DF-B6AD-BD94518E2F59}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5664,7 +5755,7 @@
           <xm:sqref>M30:M32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="32" id="{798FB9D7-6FEF-4CEA-8CC2-45EE73486721}">
+          <x14:cfRule type="iconSet" priority="34" id="{798FB9D7-6FEF-4CEA-8CC2-45EE73486721}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5683,7 +5774,7 @@
           <xm:sqref>M33:M36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="31" id="{9D5A3639-C9C5-40BD-82EE-496926295966}">
+          <x14:cfRule type="iconSet" priority="33" id="{9D5A3639-C9C5-40BD-82EE-496926295966}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5702,7 +5793,7 @@
           <xm:sqref>M37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="30" id="{042E6B91-B838-419B-9746-9D04172CBCE2}">
+          <x14:cfRule type="iconSet" priority="32" id="{042E6B91-B838-419B-9746-9D04172CBCE2}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5718,48 +5809,10 @@
               <x14:cfIcon iconSet="3Symbols" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>M38:M39</xm:sqref>
+          <xm:sqref>M38:M41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="29" id="{87212A6D-7255-4CD9-B0F3-3C906F80977E}">
-            <x14:iconSet custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>25</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num" gte="0">
-                <xm:f>168</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols" iconId="1"/>
-              <x14:cfIcon iconSet="3Symbols" iconId="2"/>
-              <x14:cfIcon iconSet="3Symbols" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>M40</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="28" id="{BEBCA1A1-AA3F-4294-8922-9827332C0668}">
-            <x14:iconSet custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>25</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num" gte="0">
-                <xm:f>168</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols" iconId="1"/>
-              <x14:cfIcon iconSet="3Symbols" iconId="2"/>
-              <x14:cfIcon iconSet="3Symbols" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>M41</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="27" id="{3793385C-190C-4A90-AF72-EEE9712F504F}">
+          <x14:cfRule type="iconSet" priority="31" id="{87212A6D-7255-4CD9-B0F3-3C906F80977E}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5778,7 +5831,7 @@
           <xm:sqref>M42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="26" id="{21C6FD3D-522C-4661-AE5D-284F6FC787D0}">
+          <x14:cfRule type="iconSet" priority="30" id="{BEBCA1A1-AA3F-4294-8922-9827332C0668}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5797,7 +5850,7 @@
           <xm:sqref>M43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="25" id="{09871DA7-81C7-4675-89F3-BE2EDB05B9C9}">
+          <x14:cfRule type="iconSet" priority="29" id="{3793385C-190C-4A90-AF72-EEE9712F504F}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5816,7 +5869,7 @@
           <xm:sqref>M44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="24" id="{50D35A91-6584-4A00-B008-2B93AA187052}">
+          <x14:cfRule type="iconSet" priority="28" id="{21C6FD3D-522C-4661-AE5D-284F6FC787D0}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5835,7 +5888,7 @@
           <xm:sqref>M45</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="23" id="{10AA0BAB-E7C1-450C-B7A5-276ADB69B0B2}">
+          <x14:cfRule type="iconSet" priority="27" id="{09871DA7-81C7-4675-89F3-BE2EDB05B9C9}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5854,7 +5907,7 @@
           <xm:sqref>M46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="22" id="{0A1ADE65-D185-454C-92B2-B6FA367CBA04}">
+          <x14:cfRule type="iconSet" priority="26" id="{50D35A91-6584-4A00-B008-2B93AA187052}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5873,7 +5926,7 @@
           <xm:sqref>M47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="21" id="{E0DFC09D-C053-4D3D-A1C1-C5AF640FB5CD}">
+          <x14:cfRule type="iconSet" priority="25" id="{10AA0BAB-E7C1-450C-B7A5-276ADB69B0B2}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5892,7 +5945,7 @@
           <xm:sqref>M48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="20" id="{F1B6F2BC-B2AE-42D9-8427-52A717AE39CD}">
+          <x14:cfRule type="iconSet" priority="24" id="{0A1ADE65-D185-454C-92B2-B6FA367CBA04}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5911,7 +5964,7 @@
           <xm:sqref>M49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="19" id="{EEF8AB81-584A-4839-AEE8-98BCAAB29DD2}">
+          <x14:cfRule type="iconSet" priority="23" id="{E0DFC09D-C053-4D3D-A1C1-C5AF640FB5CD}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5930,7 +5983,7 @@
           <xm:sqref>M50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="18" id="{A1F90B4F-0784-43A3-A2A1-2A7C9438EE1A}">
+          <x14:cfRule type="iconSet" priority="22" id="{F1B6F2BC-B2AE-42D9-8427-52A717AE39CD}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5949,7 +6002,7 @@
           <xm:sqref>M51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="17" id="{CDF48798-0C78-453D-9E98-93D1BB3C878A}">
+          <x14:cfRule type="iconSet" priority="21" id="{EEF8AB81-584A-4839-AEE8-98BCAAB29DD2}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5968,7 +6021,7 @@
           <xm:sqref>M52</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="16" id="{524804E6-2BBA-4071-AB71-18BD193B4497}">
+          <x14:cfRule type="iconSet" priority="20" id="{A1F90B4F-0784-43A3-A2A1-2A7C9438EE1A}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -5987,7 +6040,7 @@
           <xm:sqref>M53</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="15" id="{F466D4E3-91DB-49AA-8E5A-7BD04BE8813F}">
+          <x14:cfRule type="iconSet" priority="19" id="{CDF48798-0C78-453D-9E98-93D1BB3C878A}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6006,7 +6059,45 @@
           <xm:sqref>M54</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="14" id="{C4227F9F-08CD-4A7C-B706-2C35F19616E7}">
+          <x14:cfRule type="iconSet" priority="18" id="{524804E6-2BBA-4071-AB71-18BD193B4497}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>25</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>168</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols" iconId="1"/>
+              <x14:cfIcon iconSet="3Symbols" iconId="2"/>
+              <x14:cfIcon iconSet="3Symbols" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>M55</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="17" id="{F466D4E3-91DB-49AA-8E5A-7BD04BE8813F}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>25</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>168</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols" iconId="1"/>
+              <x14:cfIcon iconSet="3Symbols" iconId="2"/>
+              <x14:cfIcon iconSet="3Symbols" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>M56</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="16" id="{C4227F9F-08CD-4A7C-B706-2C35F19616E7}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6025,7 +6116,7 @@
           <xm:sqref>M8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="6" id="{6C49D5EC-FFC3-40B5-BEF3-C08FEAABBFA7}">
+          <x14:cfRule type="iconSet" priority="8" id="{6C49D5EC-FFC3-40B5-BEF3-C08FEAABBFA7}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6044,7 +6135,7 @@
           <xm:sqref>F17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="4" id="{13950B4A-31F8-40DD-922D-DC2CA60F3002}">
+          <x14:cfRule type="iconSet" priority="6" id="{13950B4A-31F8-40DD-922D-DC2CA60F3002}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6063,7 +6154,7 @@
           <xm:sqref>F10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="45" id="{F4E0A23A-4149-4A2A-B8B1-3E1EE910632F}">
+          <x14:cfRule type="iconSet" priority="47" id="{F4E0A23A-4149-4A2A-B8B1-3E1EE910632F}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6079,10 +6170,10 @@
               <x14:cfIcon iconSet="3Symbols" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>F14 F7:F8 F12 F18:F19 F21 F23:F24 F29 F33:F34 F38 F40:F171</xm:sqref>
+          <xm:sqref>F14 F7:F8 F12 F18:F19 F21 F23:F24 F29 F33:F34 F38 F43:F173</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{35213755-788E-43C8-B75E-72DA17285D4A}">
+          <x14:cfRule type="iconSet" priority="4" id="{35213755-788E-43C8-B75E-72DA17285D4A}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6101,7 +6192,7 @@
           <xm:sqref>F31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{D436B0D1-9C41-4290-A1C3-9BA213613E2C}">
+          <x14:cfRule type="iconSet" priority="3" id="{D436B0D1-9C41-4290-A1C3-9BA213613E2C}">
             <x14:iconSet iconSet="3Symbols" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6119,6 +6210,25 @@
           </x14:cfRule>
           <xm:sqref>M17</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{814260D3-C9B5-4AD4-A23C-2BEE7D803396}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>5</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>24</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols" iconId="1"/>
+              <x14:cfIcon iconSet="3Symbols" iconId="2"/>
+              <x14:cfIcon iconSet="3Symbols" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>F40</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
effort log 08/12/2013 - Khang
</commit_message>
<xml_diff>
--- a/1. Project management/9. Timelog/individual time log/AS_PM_TimeLog_DeadlineTeam_KhangHuynh.xlsx
+++ b/1. Project management/9. Timelog/individual time log/AS_PM_TimeLog_DeadlineTeam_KhangHuynh.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="183">
   <si>
     <t>Week</t>
   </si>
@@ -624,6 +624,25 @@
   <si>
     <t xml:space="preserve"> - Update timelog for team
  - Update timelog</t>
+  </si>
+  <si>
+    <t>6:30PM</t>
+  </si>
+  <si>
+    <t>- Update architectural drivers specification
+    + Entties
+    + List functional
+    + Use model
+    + Requirement Traceability Matrix
+- Create architectural driver specification - Viet version</t>
+  </si>
+  <si>
+    <t>AS_RE_ArchitectureDriverSpecification-EN-version.docx
+AS_RE_ArchitectureDriverSpecification-VN-version.docx
+usecase-diagram.vsd</t>
+  </si>
+  <si>
+    <t>Không gửi tài liệu cho khách hàng review được do thành viên vẽ use case còn nhiều sai sót</t>
   </si>
 </sst>
 </file>
@@ -955,7 +974,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1153,6 +1172,162 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1162,15 +1337,33 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1180,179 +1373,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1664,7 +1686,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1790,10 +1812,10 @@
   <dimension ref="A1:O193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="6" topLeftCell="G52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="6" topLeftCell="G51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H54" sqref="H54"/>
+      <selection pane="bottomRight" activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1807,7 +1829,7 @@
     <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="59.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="47.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="49.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="73.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="1"/>
     <col min="13" max="14" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -1815,81 +1837,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="111"/>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="113"/>
+      <c r="A1" s="81"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="83"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="97" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="114" t="s">
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
-      <c r="J2" s="115"/>
-      <c r="K2" s="115"/>
-      <c r="L2" s="115"/>
-      <c r="M2" s="115"/>
-      <c r="N2" s="116"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="86"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="100" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
-      <c r="D3" s="131"/>
-      <c r="E3" s="131"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="117"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="118"/>
-      <c r="J3" s="118"/>
-      <c r="K3" s="118"/>
-      <c r="L3" s="118"/>
-      <c r="M3" s="118"/>
-      <c r="N3" s="119"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="88"/>
+      <c r="M3" s="88"/>
+      <c r="N3" s="89"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="133"/>
-      <c r="B4" s="134"/>
-      <c r="C4" s="134"/>
-      <c r="D4" s="134"/>
-      <c r="E4" s="134"/>
-      <c r="F4" s="135"/>
-      <c r="G4" s="120"/>
-      <c r="H4" s="121"/>
-      <c r="I4" s="121"/>
-      <c r="J4" s="121"/>
-      <c r="K4" s="121"/>
-      <c r="L4" s="121"/>
-      <c r="M4" s="121"/>
-      <c r="N4" s="122"/>
+      <c r="A4" s="103"/>
+      <c r="B4" s="104"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="92"/>
     </row>
     <row r="5" spans="1:15" ht="39" customHeight="1">
-      <c r="A5" s="140"/>
-      <c r="B5" s="141"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="141"/>
-      <c r="E5" s="142"/>
+      <c r="A5" s="110"/>
+      <c r="B5" s="111"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="112"/>
       <c r="F5" s="15"/>
       <c r="H5" s="41" t="s">
         <v>64</v>
@@ -1934,13 +1956,13 @@
       <c r="J6" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="126"/>
-      <c r="L6" s="126"/>
-      <c r="M6" s="126"/>
-      <c r="N6" s="126"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="96"/>
+      <c r="M6" s="96"/>
+      <c r="N6" s="96"/>
     </row>
     <row r="7" spans="1:15" ht="38.25">
-      <c r="A7" s="123">
+      <c r="A7" s="93">
         <v>1</v>
       </c>
       <c r="B7" s="16">
@@ -1966,21 +1988,21 @@
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="29"/>
-      <c r="K7" s="102" t="s">
+      <c r="K7" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="102"/>
+      <c r="L7" s="120"/>
       <c r="M7" s="32">
         <f>SUM(M8:M67)</f>
-        <v>94.18</v>
+        <v>97.68</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="25.5">
-      <c r="A8" s="124"/>
-      <c r="B8" s="136">
+      <c r="A8" s="94"/>
+      <c r="B8" s="106">
         <v>41586</v>
       </c>
       <c r="C8" s="17">
@@ -1992,7 +2014,7 @@
       <c r="E8" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="138">
+      <c r="F8" s="108">
         <v>1.67</v>
       </c>
       <c r="G8" s="19" t="s">
@@ -2016,8 +2038,8 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="125"/>
-      <c r="B9" s="137"/>
+      <c r="A9" s="95"/>
+      <c r="B9" s="107"/>
       <c r="C9" s="17">
         <v>0.63194444444444442</v>
       </c>
@@ -2027,7 +2049,7 @@
       <c r="E9" s="18">
         <v>0.5</v>
       </c>
-      <c r="F9" s="139"/>
+      <c r="F9" s="109"/>
       <c r="G9" s="29" t="s">
         <v>23</v>
       </c>
@@ -2038,10 +2060,10 @@
       <c r="J9" s="29"/>
     </row>
     <row r="10" spans="1:15" s="63" customFormat="1">
-      <c r="A10" s="95">
+      <c r="A10" s="113">
         <v>2</v>
       </c>
-      <c r="B10" s="98">
+      <c r="B10" s="116">
         <v>41589</v>
       </c>
       <c r="C10" s="58" t="s">
@@ -2053,7 +2075,7 @@
       <c r="E10" s="59">
         <v>2.5</v>
       </c>
-      <c r="F10" s="100">
+      <c r="F10" s="118">
         <f>SUM(E10:E11)</f>
         <v>5</v>
       </c>
@@ -2067,8 +2089,8 @@
       <c r="J10" s="60"/>
     </row>
     <row r="11" spans="1:15" s="63" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A11" s="96"/>
-      <c r="B11" s="99"/>
+      <c r="A11" s="114"/>
+      <c r="B11" s="117"/>
       <c r="C11" s="58" t="s">
         <v>76</v>
       </c>
@@ -2078,7 +2100,7 @@
       <c r="E11" s="59">
         <v>2.5</v>
       </c>
-      <c r="F11" s="101"/>
+      <c r="F11" s="119"/>
       <c r="G11" s="60" t="s">
         <v>22</v>
       </c>
@@ -2091,8 +2113,8 @@
       <c r="J11" s="60"/>
     </row>
     <row r="12" spans="1:15" ht="51">
-      <c r="A12" s="96"/>
-      <c r="B12" s="103">
+      <c r="A12" s="114"/>
+      <c r="B12" s="121">
         <v>41590</v>
       </c>
       <c r="C12" s="22">
@@ -2104,7 +2126,7 @@
       <c r="E12" s="23">
         <v>2.25</v>
       </c>
-      <c r="F12" s="105">
+      <c r="F12" s="123">
         <v>3.75</v>
       </c>
       <c r="G12" s="30" t="s">
@@ -2131,8 +2153,8 @@
       <c r="O12" s="34"/>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A13" s="96"/>
-      <c r="B13" s="104"/>
+      <c r="A13" s="114"/>
+      <c r="B13" s="122"/>
       <c r="C13" s="22">
         <v>0.91666666666666663</v>
       </c>
@@ -2142,7 +2164,7 @@
       <c r="E13" s="23">
         <v>1.5</v>
       </c>
-      <c r="F13" s="106"/>
+      <c r="F13" s="124"/>
       <c r="G13" s="45" t="s">
         <v>28</v>
       </c>
@@ -2158,8 +2180,8 @@
       <c r="O13" s="34"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A14" s="96"/>
-      <c r="B14" s="103">
+      <c r="A14" s="114"/>
+      <c r="B14" s="121">
         <v>41591</v>
       </c>
       <c r="C14" s="22">
@@ -2171,7 +2193,7 @@
       <c r="E14" s="23">
         <v>2</v>
       </c>
-      <c r="F14" s="108">
+      <c r="F14" s="126">
         <v>4.5</v>
       </c>
       <c r="G14" s="45" t="s">
@@ -2189,8 +2211,8 @@
       <c r="O14" s="34"/>
     </row>
     <row r="15" spans="1:15" ht="25.5">
-      <c r="A15" s="96"/>
-      <c r="B15" s="107"/>
+      <c r="A15" s="114"/>
+      <c r="B15" s="125"/>
       <c r="C15" s="25">
         <v>0.5625</v>
       </c>
@@ -2200,7 +2222,7 @@
       <c r="E15" s="28">
         <v>2</v>
       </c>
-      <c r="F15" s="109"/>
+      <c r="F15" s="127"/>
       <c r="G15" s="30" t="s">
         <v>19</v>
       </c>
@@ -2217,8 +2239,8 @@
       <c r="N15" s="3"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A16" s="96"/>
-      <c r="B16" s="104"/>
+      <c r="A16" s="114"/>
+      <c r="B16" s="122"/>
       <c r="C16" s="25">
         <v>0.83333333333333337</v>
       </c>
@@ -2228,7 +2250,7 @@
       <c r="E16" s="28">
         <v>0.5</v>
       </c>
-      <c r="F16" s="110"/>
+      <c r="F16" s="128"/>
       <c r="G16" s="45" t="s">
         <v>28</v>
       </c>
@@ -2252,7 +2274,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A17" s="96"/>
+      <c r="A17" s="114"/>
       <c r="B17" s="47">
         <v>41592</v>
       </c>
@@ -2291,7 +2313,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="25.5">
-      <c r="A18" s="97"/>
+      <c r="A18" s="115"/>
       <c r="B18" s="42">
         <v>41593</v>
       </c>
@@ -2323,17 +2345,17 @@
       <c r="L18" s="5"/>
       <c r="M18" s="9">
         <f>SUM(E47:E59)</f>
-        <v>26.07</v>
+        <v>29.57</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="89">
+      <c r="A19" s="135">
         <v>3</v>
       </c>
-      <c r="B19" s="87">
+      <c r="B19" s="132">
         <v>41596</v>
       </c>
       <c r="C19" s="53" t="s">
@@ -2345,7 +2367,7 @@
       <c r="E19" s="50">
         <v>0.5</v>
       </c>
-      <c r="F19" s="86">
+      <c r="F19" s="78">
         <f>SUM(E19:E20)</f>
         <v>3.5</v>
       </c>
@@ -2372,8 +2394,8 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="90"/>
-      <c r="B20" s="88"/>
+      <c r="A20" s="136"/>
+      <c r="B20" s="133"/>
       <c r="C20" s="53" t="s">
         <v>81</v>
       </c>
@@ -2383,7 +2405,7 @@
       <c r="E20" s="50">
         <v>3</v>
       </c>
-      <c r="F20" s="82"/>
+      <c r="F20" s="134"/>
       <c r="G20" s="49" t="s">
         <v>22</v>
       </c>
@@ -2400,8 +2422,8 @@
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="90"/>
-      <c r="B21" s="87">
+      <c r="A21" s="136"/>
+      <c r="B21" s="132">
         <v>41597</v>
       </c>
       <c r="C21" s="53" t="s">
@@ -2413,7 +2435,7 @@
       <c r="E21" s="50">
         <v>2</v>
       </c>
-      <c r="F21" s="86">
+      <c r="F21" s="78">
         <f>SUM(E21:E22)</f>
         <v>2.5</v>
       </c>
@@ -2433,8 +2455,8 @@
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="90"/>
-      <c r="B22" s="88"/>
+      <c r="A22" s="136"/>
+      <c r="B22" s="133"/>
       <c r="C22" s="53" t="s">
         <v>84</v>
       </c>
@@ -2444,7 +2466,7 @@
       <c r="E22" s="50">
         <v>0.5</v>
       </c>
-      <c r="F22" s="82"/>
+      <c r="F22" s="134"/>
       <c r="G22" s="49" t="s">
         <v>22</v>
       </c>
@@ -2468,7 +2490,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="26.25">
-      <c r="A23" s="90"/>
+      <c r="A23" s="136"/>
       <c r="B23" s="26">
         <v>41598</v>
       </c>
@@ -2508,7 +2530,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="26.25">
-      <c r="A24" s="90"/>
+      <c r="A24" s="136"/>
       <c r="B24" s="26">
         <v>41599</v>
       </c>
@@ -2521,7 +2543,7 @@
       <c r="E24" s="50">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F24" s="86">
+      <c r="F24" s="78">
         <f>SUM(E24:E28)</f>
         <v>7.0600000000000005</v>
       </c>
@@ -2539,7 +2561,7 @@
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="90"/>
+      <c r="A25" s="136"/>
       <c r="B25" s="26">
         <v>41599</v>
       </c>
@@ -2552,7 +2574,7 @@
       <c r="E25" s="50">
         <v>1.3</v>
       </c>
-      <c r="F25" s="92"/>
+      <c r="F25" s="79"/>
       <c r="G25" s="57" t="s">
         <v>19</v>
       </c>
@@ -2567,7 +2589,7 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="90"/>
+      <c r="A26" s="136"/>
       <c r="B26" s="26">
         <v>41599</v>
       </c>
@@ -2580,7 +2602,7 @@
       <c r="E26" s="50">
         <v>1.5</v>
       </c>
-      <c r="F26" s="92"/>
+      <c r="F26" s="79"/>
       <c r="G26" s="57" t="s">
         <v>24</v>
       </c>
@@ -2597,7 +2619,7 @@
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="90"/>
+      <c r="A27" s="136"/>
       <c r="B27" s="26">
         <v>41599</v>
       </c>
@@ -2610,7 +2632,7 @@
       <c r="E27" s="50">
         <v>2.1</v>
       </c>
-      <c r="F27" s="92"/>
+      <c r="F27" s="79"/>
       <c r="G27" s="29" t="s">
         <v>19</v>
       </c>
@@ -2632,7 +2654,7 @@
       </c>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="90"/>
+      <c r="A28" s="136"/>
       <c r="B28" s="26">
         <v>41599</v>
       </c>
@@ -2645,7 +2667,7 @@
       <c r="E28" s="50">
         <v>1</v>
       </c>
-      <c r="F28" s="93"/>
+      <c r="F28" s="80"/>
       <c r="G28" s="29" t="s">
         <v>22</v>
       </c>
@@ -2660,7 +2682,7 @@
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="90"/>
+      <c r="A29" s="136"/>
       <c r="B29" s="26">
         <v>41600</v>
       </c>
@@ -2673,7 +2695,7 @@
       <c r="E29" s="50">
         <v>1.25</v>
       </c>
-      <c r="F29" s="86">
+      <c r="F29" s="78">
         <f>SUM(E29:E30)</f>
         <v>3.25</v>
       </c>
@@ -2689,7 +2711,7 @@
       <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:14" ht="51">
-      <c r="A30" s="90"/>
+      <c r="A30" s="136"/>
       <c r="B30" s="26">
         <v>41600</v>
       </c>
@@ -2702,7 +2724,7 @@
       <c r="E30" s="50">
         <v>2</v>
       </c>
-      <c r="F30" s="82"/>
+      <c r="F30" s="134"/>
       <c r="G30" s="57" t="s">
         <v>22</v>
       </c>
@@ -2724,7 +2746,7 @@
       </c>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="90"/>
+      <c r="A31" s="136"/>
       <c r="B31" s="26">
         <v>41601</v>
       </c>
@@ -2737,7 +2759,7 @@
       <c r="E31" s="74">
         <v>0.25</v>
       </c>
-      <c r="F31" s="86">
+      <c r="F31" s="78">
         <f>SUM(E31:E33)</f>
         <v>4.6500000000000004</v>
       </c>
@@ -2751,7 +2773,7 @@
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="90"/>
+      <c r="A32" s="136"/>
       <c r="B32" s="26">
         <v>41601</v>
       </c>
@@ -2764,7 +2786,7 @@
       <c r="E32" s="50">
         <v>3.5</v>
       </c>
-      <c r="F32" s="92"/>
+      <c r="F32" s="79"/>
       <c r="G32" s="57" t="s">
         <v>22</v>
       </c>
@@ -2781,7 +2803,7 @@
       <c r="N32" s="3"/>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="91"/>
+      <c r="A33" s="137"/>
       <c r="B33" s="26">
         <v>41601</v>
       </c>
@@ -2794,7 +2816,7 @@
       <c r="E33" s="50">
         <v>0.9</v>
       </c>
-      <c r="F33" s="93"/>
+      <c r="F33" s="80"/>
       <c r="G33" s="57" t="s">
         <v>22</v>
       </c>
@@ -2811,7 +2833,7 @@
       <c r="N33" s="3"/>
     </row>
     <row r="34" spans="1:14" ht="38.25">
-      <c r="A34" s="77">
+      <c r="A34" s="129">
         <v>4</v>
       </c>
       <c r="B34" s="27">
@@ -2853,7 +2875,7 @@
       </c>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="78"/>
+      <c r="A35" s="130"/>
       <c r="B35" s="27">
         <v>41604</v>
       </c>
@@ -2866,7 +2888,7 @@
       <c r="E35" s="28">
         <v>1</v>
       </c>
-      <c r="F35" s="94">
+      <c r="F35" s="138">
         <f>SUM(E35:E38)</f>
         <v>6.75</v>
       </c>
@@ -2884,7 +2906,7 @@
       <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="78"/>
+      <c r="A36" s="130"/>
       <c r="B36" s="27">
         <v>41604</v>
       </c>
@@ -2897,7 +2919,7 @@
       <c r="E36" s="76">
         <v>2.5</v>
       </c>
-      <c r="F36" s="78"/>
+      <c r="F36" s="130"/>
       <c r="G36" s="67" t="s">
         <v>23</v>
       </c>
@@ -2914,7 +2936,7 @@
       <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="78"/>
+      <c r="A37" s="130"/>
       <c r="B37" s="27">
         <v>41604</v>
       </c>
@@ -2927,7 +2949,7 @@
       <c r="E37" s="76">
         <v>1.25</v>
       </c>
-      <c r="F37" s="78"/>
+      <c r="F37" s="130"/>
       <c r="G37" s="67" t="s">
         <v>24</v>
       </c>
@@ -2944,7 +2966,7 @@
       <c r="N37" s="3"/>
     </row>
     <row r="38" spans="1:14" ht="51">
-      <c r="A38" s="78"/>
+      <c r="A38" s="130"/>
       <c r="B38" s="27">
         <v>41604</v>
       </c>
@@ -2957,7 +2979,7 @@
       <c r="E38" s="69">
         <v>2</v>
       </c>
-      <c r="F38" s="79"/>
+      <c r="F38" s="131"/>
       <c r="G38" s="67" t="s">
         <v>22</v>
       </c>
@@ -2983,7 +3005,7 @@
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="78"/>
+      <c r="A39" s="130"/>
       <c r="B39" s="27">
         <v>41605</v>
       </c>
@@ -2996,7 +3018,7 @@
       <c r="E39" s="69">
         <v>2.33</v>
       </c>
-      <c r="F39" s="77">
+      <c r="F39" s="129">
         <f>SUM(E39:E40)</f>
         <v>2.83</v>
       </c>
@@ -3021,7 +3043,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" ht="25.5">
-      <c r="A40" s="78"/>
+      <c r="A40" s="130"/>
       <c r="B40" s="27">
         <v>41605</v>
       </c>
@@ -3034,7 +3056,7 @@
       <c r="E40" s="69">
         <v>0.5</v>
       </c>
-      <c r="F40" s="79"/>
+      <c r="F40" s="131"/>
       <c r="G40" s="67" t="s">
         <v>24</v>
       </c>
@@ -3051,7 +3073,7 @@
       <c r="N40" s="3"/>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="78"/>
+      <c r="A41" s="130"/>
       <c r="B41" s="27">
         <v>41606</v>
       </c>
@@ -3064,7 +3086,7 @@
       <c r="E41" s="69">
         <v>1.33</v>
       </c>
-      <c r="F41" s="77">
+      <c r="F41" s="129">
         <f>SUM(E41:E43)</f>
         <v>5.83</v>
       </c>
@@ -3082,7 +3104,7 @@
       <c r="N41" s="3"/>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="78"/>
+      <c r="A42" s="130"/>
       <c r="B42" s="27">
         <v>41606</v>
       </c>
@@ -3095,7 +3117,7 @@
       <c r="E42" s="69">
         <v>1.75</v>
       </c>
-      <c r="F42" s="78"/>
+      <c r="F42" s="130"/>
       <c r="G42" s="67" t="s">
         <v>25</v>
       </c>
@@ -3110,7 +3132,7 @@
       <c r="N42" s="3"/>
     </row>
     <row r="43" spans="1:14" ht="25.5">
-      <c r="A43" s="78"/>
+      <c r="A43" s="130"/>
       <c r="B43" s="27">
         <v>41606</v>
       </c>
@@ -3123,7 +3145,7 @@
       <c r="E43" s="69">
         <v>2.75</v>
       </c>
-      <c r="F43" s="79"/>
+      <c r="F43" s="131"/>
       <c r="G43" s="67" t="s">
         <v>19</v>
       </c>
@@ -3147,7 +3169,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" ht="51">
-      <c r="A44" s="78"/>
+      <c r="A44" s="130"/>
       <c r="B44" s="27">
         <v>41607</v>
       </c>
@@ -3187,7 +3209,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" ht="38.25">
-      <c r="A45" s="78"/>
+      <c r="A45" s="130"/>
       <c r="B45" s="27">
         <v>41609</v>
       </c>
@@ -3200,7 +3222,7 @@
       <c r="E45" s="69">
         <v>2</v>
       </c>
-      <c r="F45" s="77">
+      <c r="F45" s="129">
         <f>SUM(E45:E46)</f>
         <v>4</v>
       </c>
@@ -3220,7 +3242,7 @@
       <c r="N45" s="3"/>
     </row>
     <row r="46" spans="1:14" ht="25.5">
-      <c r="A46" s="79"/>
+      <c r="A46" s="131"/>
       <c r="B46" s="27">
         <v>41609</v>
       </c>
@@ -3233,7 +3255,7 @@
       <c r="E46" s="69">
         <v>2</v>
       </c>
-      <c r="F46" s="79"/>
+      <c r="F46" s="131"/>
       <c r="G46" s="67" t="s">
         <v>22</v>
       </c>
@@ -3252,7 +3274,7 @@
       <c r="N46" s="3"/>
     </row>
     <row r="47" spans="1:14" ht="63.75">
-      <c r="A47" s="80">
+      <c r="A47" s="139">
         <v>5</v>
       </c>
       <c r="B47" s="26">
@@ -3292,7 +3314,7 @@
       </c>
     </row>
     <row r="48" spans="1:14" ht="38.25">
-      <c r="A48" s="81"/>
+      <c r="A48" s="140"/>
       <c r="B48" s="26">
         <v>41611</v>
       </c>
@@ -3305,7 +3327,7 @@
       <c r="E48" s="55">
         <v>1.5</v>
       </c>
-      <c r="F48" s="80">
+      <c r="F48" s="139">
         <f>SUM(E48:E50)</f>
         <v>7</v>
       </c>
@@ -3323,7 +3345,7 @@
       <c r="N48" s="3"/>
     </row>
     <row r="49" spans="1:14" ht="51.75" customHeight="1">
-      <c r="A49" s="81"/>
+      <c r="A49" s="140"/>
       <c r="B49" s="26">
         <v>41611</v>
       </c>
@@ -3336,7 +3358,7 @@
       <c r="E49" s="55">
         <v>3.5</v>
       </c>
-      <c r="F49" s="81"/>
+      <c r="F49" s="140"/>
       <c r="G49" s="29" t="s">
         <v>19</v>
       </c>
@@ -3358,7 +3380,7 @@
       </c>
     </row>
     <row r="50" spans="1:14" ht="38.25">
-      <c r="A50" s="81"/>
+      <c r="A50" s="140"/>
       <c r="B50" s="26">
         <v>41611</v>
       </c>
@@ -3371,7 +3393,7 @@
       <c r="E50" s="55">
         <v>2</v>
       </c>
-      <c r="F50" s="82"/>
+      <c r="F50" s="134"/>
       <c r="G50" s="29" t="s">
         <v>22</v>
       </c>
@@ -3390,7 +3412,7 @@
       <c r="N50" s="3"/>
     </row>
     <row r="51" spans="1:14" ht="38.25">
-      <c r="A51" s="81"/>
+      <c r="A51" s="140"/>
       <c r="B51" s="26">
         <v>41612</v>
       </c>
@@ -3403,7 +3425,7 @@
       <c r="E51" s="55">
         <v>0.75</v>
       </c>
-      <c r="F51" s="80">
+      <c r="F51" s="139">
         <f>SUM(E52:E53)</f>
         <v>6.5</v>
       </c>
@@ -3432,7 +3454,7 @@
       </c>
     </row>
     <row r="52" spans="1:14" ht="76.5">
-      <c r="A52" s="81"/>
+      <c r="A52" s="140"/>
       <c r="B52" s="26">
         <v>41612</v>
       </c>
@@ -3445,7 +3467,7 @@
       <c r="E52" s="55">
         <v>4.5</v>
       </c>
-      <c r="F52" s="81"/>
+      <c r="F52" s="140"/>
       <c r="G52" s="29" t="s">
         <v>19</v>
       </c>
@@ -3460,7 +3482,7 @@
       <c r="N52" s="3"/>
     </row>
     <row r="53" spans="1:14" ht="38.25">
-      <c r="A53" s="81"/>
+      <c r="A53" s="140"/>
       <c r="B53" s="26">
         <v>41612</v>
       </c>
@@ -3473,7 +3495,7 @@
       <c r="E53" s="55">
         <v>2</v>
       </c>
-      <c r="F53" s="82"/>
+      <c r="F53" s="134"/>
       <c r="G53" s="29" t="s">
         <v>22</v>
       </c>
@@ -3490,7 +3512,7 @@
       <c r="N53" s="3"/>
     </row>
     <row r="54" spans="1:14" ht="38.25">
-      <c r="A54" s="81"/>
+      <c r="A54" s="140"/>
       <c r="B54" s="26">
         <v>41613</v>
       </c>
@@ -3503,14 +3525,14 @@
       <c r="E54" s="74">
         <v>3</v>
       </c>
-      <c r="F54" s="86">
+      <c r="F54" s="78">
         <f>SUM(E54:E58)</f>
         <v>7.82</v>
       </c>
       <c r="G54" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="H54" s="143" t="s">
+      <c r="H54" s="77" t="s">
         <v>174</v>
       </c>
       <c r="I54" s="65"/>
@@ -3521,7 +3543,7 @@
       <c r="N54" s="3"/>
     </row>
     <row r="55" spans="1:14">
-      <c r="A55" s="81"/>
+      <c r="A55" s="140"/>
       <c r="B55" s="26">
         <v>41613</v>
       </c>
@@ -3534,11 +3556,11 @@
       <c r="E55" s="74">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F55" s="92"/>
+      <c r="F55" s="79"/>
       <c r="G55" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="H55" s="143" t="s">
+      <c r="H55" s="77" t="s">
         <v>175</v>
       </c>
       <c r="I55" s="65"/>
@@ -3549,7 +3571,7 @@
       <c r="N55" s="3"/>
     </row>
     <row r="56" spans="1:14" ht="51">
-      <c r="A56" s="81"/>
+      <c r="A56" s="140"/>
       <c r="B56" s="26">
         <v>41613</v>
       </c>
@@ -3562,11 +3584,11 @@
       <c r="E56" s="74">
         <v>1.5</v>
       </c>
-      <c r="F56" s="92"/>
+      <c r="F56" s="79"/>
       <c r="G56" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="H56" s="143" t="s">
+      <c r="H56" s="77" t="s">
         <v>176</v>
       </c>
       <c r="I56" s="65"/>
@@ -3577,7 +3599,7 @@
       <c r="N56" s="3"/>
     </row>
     <row r="57" spans="1:14" ht="25.5">
-      <c r="A57" s="81"/>
+      <c r="A57" s="140"/>
       <c r="B57" s="26">
         <v>41613</v>
       </c>
@@ -3590,11 +3612,11 @@
       <c r="E57" s="74">
         <v>0.66</v>
       </c>
-      <c r="F57" s="92"/>
+      <c r="F57" s="79"/>
       <c r="G57" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="H57" s="143" t="s">
+      <c r="H57" s="77" t="s">
         <v>177</v>
       </c>
       <c r="I57" s="65"/>
@@ -3605,7 +3627,7 @@
       <c r="N57" s="3"/>
     </row>
     <row r="58" spans="1:14" ht="25.5">
-      <c r="A58" s="81"/>
+      <c r="A58" s="140"/>
       <c r="B58" s="26">
         <v>41613</v>
       </c>
@@ -3618,11 +3640,11 @@
       <c r="E58" s="74">
         <v>1.5</v>
       </c>
-      <c r="F58" s="93"/>
+      <c r="F58" s="80"/>
       <c r="G58" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="H58" s="143" t="s">
+      <c r="H58" s="77" t="s">
         <v>178</v>
       </c>
       <c r="I58" s="29"/>
@@ -3639,22 +3661,36 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
-      <c r="A59" s="82"/>
+    <row r="59" spans="1:14" ht="76.5">
+      <c r="A59" s="134"/>
       <c r="B59" s="26">
-        <v>41614</v>
-      </c>
-      <c r="C59" s="55"/>
-      <c r="D59" s="55"/>
-      <c r="E59" s="55"/>
+        <v>41616</v>
+      </c>
+      <c r="C59" s="55" t="s">
+        <v>179</v>
+      </c>
+      <c r="D59" s="144" t="s">
+        <v>160</v>
+      </c>
+      <c r="E59" s="55">
+        <v>3.5</v>
+      </c>
       <c r="F59" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G59" s="29"/>
-      <c r="H59" s="29"/>
-      <c r="I59" s="29"/>
-      <c r="J59" s="29"/>
+        <v>3.5</v>
+      </c>
+      <c r="G59" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H59" s="77" t="s">
+        <v>180</v>
+      </c>
+      <c r="I59" s="65" t="s">
+        <v>181</v>
+      </c>
+      <c r="J59" s="29" t="s">
+        <v>182</v>
+      </c>
       <c r="K59" s="7" t="s">
         <v>45</v>
       </c>
@@ -3668,7 +3704,7 @@
       </c>
     </row>
     <row r="60" spans="1:14">
-      <c r="A60" s="77">
+      <c r="A60" s="129">
         <v>6</v>
       </c>
       <c r="B60" s="27">
@@ -3698,7 +3734,7 @@
       </c>
     </row>
     <row r="61" spans="1:14">
-      <c r="A61" s="78"/>
+      <c r="A61" s="130"/>
       <c r="B61" s="27">
         <v>41618</v>
       </c>
@@ -3726,7 +3762,7 @@
       </c>
     </row>
     <row r="62" spans="1:14">
-      <c r="A62" s="78"/>
+      <c r="A62" s="130"/>
       <c r="B62" s="27">
         <v>41619</v>
       </c>
@@ -3754,7 +3790,7 @@
       </c>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="78"/>
+      <c r="A63" s="130"/>
       <c r="B63" s="27">
         <v>41620</v>
       </c>
@@ -3782,7 +3818,7 @@
       </c>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="79"/>
+      <c r="A64" s="131"/>
       <c r="B64" s="27">
         <v>41621</v>
       </c>
@@ -3810,7 +3846,7 @@
       </c>
     </row>
     <row r="65" spans="1:14">
-      <c r="A65" s="80">
+      <c r="A65" s="139">
         <v>7</v>
       </c>
       <c r="B65" s="26">
@@ -3840,7 +3876,7 @@
       </c>
     </row>
     <row r="66" spans="1:14">
-      <c r="A66" s="81"/>
+      <c r="A66" s="140"/>
       <c r="B66" s="26">
         <v>41625</v>
       </c>
@@ -3868,7 +3904,7 @@
       </c>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="81"/>
+      <c r="A67" s="140"/>
       <c r="B67" s="26">
         <v>41626</v>
       </c>
@@ -3896,7 +3932,7 @@
       </c>
     </row>
     <row r="68" spans="1:14">
-      <c r="A68" s="81"/>
+      <c r="A68" s="140"/>
       <c r="B68" s="26">
         <v>41627</v>
       </c>
@@ -3913,7 +3949,7 @@
       <c r="J68" s="29"/>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="82"/>
+      <c r="A69" s="134"/>
       <c r="B69" s="26">
         <v>41628</v>
       </c>
@@ -3930,7 +3966,7 @@
       <c r="J69" s="29"/>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="77">
+      <c r="A70" s="129">
         <v>8</v>
       </c>
       <c r="B70" s="27">
@@ -3949,7 +3985,7 @@
       <c r="J70" s="67"/>
     </row>
     <row r="71" spans="1:14">
-      <c r="A71" s="78"/>
+      <c r="A71" s="130"/>
       <c r="B71" s="27">
         <v>41632</v>
       </c>
@@ -3966,7 +4002,7 @@
       <c r="J71" s="67"/>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="78"/>
+      <c r="A72" s="130"/>
       <c r="B72" s="27">
         <v>41633</v>
       </c>
@@ -3983,7 +4019,7 @@
       <c r="J72" s="67"/>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="78"/>
+      <c r="A73" s="130"/>
       <c r="B73" s="27">
         <v>41634</v>
       </c>
@@ -4000,7 +4036,7 @@
       <c r="J73" s="67"/>
     </row>
     <row r="74" spans="1:14">
-      <c r="A74" s="79"/>
+      <c r="A74" s="131"/>
       <c r="B74" s="27">
         <v>41635</v>
       </c>
@@ -4017,7 +4053,7 @@
       <c r="J74" s="67"/>
     </row>
     <row r="75" spans="1:14">
-      <c r="A75" s="80">
+      <c r="A75" s="139">
         <v>9</v>
       </c>
       <c r="B75" s="26">
@@ -4036,7 +4072,7 @@
       <c r="J75" s="29"/>
     </row>
     <row r="76" spans="1:14">
-      <c r="A76" s="81"/>
+      <c r="A76" s="140"/>
       <c r="B76" s="26">
         <v>41639</v>
       </c>
@@ -4053,7 +4089,7 @@
       <c r="J76" s="29"/>
     </row>
     <row r="77" spans="1:14">
-      <c r="A77" s="81"/>
+      <c r="A77" s="140"/>
       <c r="B77" s="26">
         <v>41640</v>
       </c>
@@ -4070,7 +4106,7 @@
       <c r="J77" s="29"/>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="81"/>
+      <c r="A78" s="140"/>
       <c r="B78" s="26">
         <v>41641</v>
       </c>
@@ -4087,7 +4123,7 @@
       <c r="J78" s="29"/>
     </row>
     <row r="79" spans="1:14">
-      <c r="A79" s="82"/>
+      <c r="A79" s="134"/>
       <c r="B79" s="26">
         <v>41642</v>
       </c>
@@ -4104,7 +4140,7 @@
       <c r="J79" s="29"/>
     </row>
     <row r="80" spans="1:14">
-      <c r="A80" s="77">
+      <c r="A80" s="129">
         <v>10</v>
       </c>
       <c r="B80" s="27">
@@ -4123,7 +4159,7 @@
       <c r="J80" s="67"/>
     </row>
     <row r="81" spans="1:10">
-      <c r="A81" s="78"/>
+      <c r="A81" s="130"/>
       <c r="B81" s="27">
         <v>41646</v>
       </c>
@@ -4140,7 +4176,7 @@
       <c r="J81" s="67"/>
     </row>
     <row r="82" spans="1:10">
-      <c r="A82" s="78"/>
+      <c r="A82" s="130"/>
       <c r="B82" s="27">
         <v>41647</v>
       </c>
@@ -4157,7 +4193,7 @@
       <c r="J82" s="67"/>
     </row>
     <row r="83" spans="1:10">
-      <c r="A83" s="78"/>
+      <c r="A83" s="130"/>
       <c r="B83" s="27">
         <v>41648</v>
       </c>
@@ -4174,7 +4210,7 @@
       <c r="J83" s="67"/>
     </row>
     <row r="84" spans="1:10">
-      <c r="A84" s="79"/>
+      <c r="A84" s="131"/>
       <c r="B84" s="27">
         <v>41649</v>
       </c>
@@ -4191,7 +4227,7 @@
       <c r="J84" s="67"/>
     </row>
     <row r="85" spans="1:10">
-      <c r="A85" s="80">
+      <c r="A85" s="139">
         <v>11</v>
       </c>
       <c r="B85" s="26">
@@ -4210,7 +4246,7 @@
       <c r="J85" s="29"/>
     </row>
     <row r="86" spans="1:10">
-      <c r="A86" s="81"/>
+      <c r="A86" s="140"/>
       <c r="B86" s="26">
         <v>41653</v>
       </c>
@@ -4227,7 +4263,7 @@
       <c r="J86" s="29"/>
     </row>
     <row r="87" spans="1:10">
-      <c r="A87" s="81"/>
+      <c r="A87" s="140"/>
       <c r="B87" s="26">
         <v>41654</v>
       </c>
@@ -4244,7 +4280,7 @@
       <c r="J87" s="29"/>
     </row>
     <row r="88" spans="1:10">
-      <c r="A88" s="81"/>
+      <c r="A88" s="140"/>
       <c r="B88" s="26">
         <v>41655</v>
       </c>
@@ -4261,7 +4297,7 @@
       <c r="J88" s="29"/>
     </row>
     <row r="89" spans="1:10">
-      <c r="A89" s="82"/>
+      <c r="A89" s="134"/>
       <c r="B89" s="26">
         <v>41656</v>
       </c>
@@ -4278,7 +4314,7 @@
       <c r="J89" s="29"/>
     </row>
     <row r="90" spans="1:10">
-      <c r="A90" s="77">
+      <c r="A90" s="129">
         <v>12</v>
       </c>
       <c r="B90" s="27">
@@ -4297,7 +4333,7 @@
       <c r="J90" s="67"/>
     </row>
     <row r="91" spans="1:10">
-      <c r="A91" s="78"/>
+      <c r="A91" s="130"/>
       <c r="B91" s="27">
         <v>41660</v>
       </c>
@@ -4314,7 +4350,7 @@
       <c r="J91" s="67"/>
     </row>
     <row r="92" spans="1:10">
-      <c r="A92" s="78"/>
+      <c r="A92" s="130"/>
       <c r="B92" s="27">
         <v>41661</v>
       </c>
@@ -4331,7 +4367,7 @@
       <c r="J92" s="67"/>
     </row>
     <row r="93" spans="1:10">
-      <c r="A93" s="78"/>
+      <c r="A93" s="130"/>
       <c r="B93" s="27">
         <v>41662</v>
       </c>
@@ -4348,7 +4384,7 @@
       <c r="J93" s="67"/>
     </row>
     <row r="94" spans="1:10">
-      <c r="A94" s="79"/>
+      <c r="A94" s="131"/>
       <c r="B94" s="27">
         <v>41663</v>
       </c>
@@ -4365,7 +4401,7 @@
       <c r="J94" s="67"/>
     </row>
     <row r="95" spans="1:10">
-      <c r="A95" s="80">
+      <c r="A95" s="139">
         <v>13</v>
       </c>
       <c r="B95" s="26">
@@ -4386,7 +4422,7 @@
       <c r="J95" s="29"/>
     </row>
     <row r="96" spans="1:10">
-      <c r="A96" s="81"/>
+      <c r="A96" s="140"/>
       <c r="B96" s="26">
         <v>41667</v>
       </c>
@@ -4405,7 +4441,7 @@
       <c r="J96" s="29"/>
     </row>
     <row r="97" spans="1:10">
-      <c r="A97" s="81"/>
+      <c r="A97" s="140"/>
       <c r="B97" s="26">
         <v>41668</v>
       </c>
@@ -4424,7 +4460,7 @@
       <c r="J97" s="29"/>
     </row>
     <row r="98" spans="1:10">
-      <c r="A98" s="81"/>
+      <c r="A98" s="140"/>
       <c r="B98" s="26">
         <v>41669</v>
       </c>
@@ -4443,7 +4479,7 @@
       <c r="J98" s="29"/>
     </row>
     <row r="99" spans="1:10">
-      <c r="A99" s="82"/>
+      <c r="A99" s="134"/>
       <c r="B99" s="26">
         <v>41670</v>
       </c>
@@ -4462,7 +4498,7 @@
       <c r="J99" s="29"/>
     </row>
     <row r="100" spans="1:10">
-      <c r="A100" s="77">
+      <c r="A100" s="129">
         <v>14</v>
       </c>
       <c r="B100" s="27">
@@ -4483,7 +4519,7 @@
       <c r="J100" s="67"/>
     </row>
     <row r="101" spans="1:10">
-      <c r="A101" s="78"/>
+      <c r="A101" s="130"/>
       <c r="B101" s="27">
         <v>41674</v>
       </c>
@@ -4502,7 +4538,7 @@
       <c r="J101" s="67"/>
     </row>
     <row r="102" spans="1:10">
-      <c r="A102" s="78"/>
+      <c r="A102" s="130"/>
       <c r="B102" s="27">
         <v>41675</v>
       </c>
@@ -4521,7 +4557,7 @@
       <c r="J102" s="67"/>
     </row>
     <row r="103" spans="1:10">
-      <c r="A103" s="78"/>
+      <c r="A103" s="130"/>
       <c r="B103" s="27">
         <v>41676</v>
       </c>
@@ -4540,7 +4576,7 @@
       <c r="J103" s="67"/>
     </row>
     <row r="104" spans="1:10">
-      <c r="A104" s="79"/>
+      <c r="A104" s="131"/>
       <c r="B104" s="27">
         <v>41677</v>
       </c>
@@ -4559,7 +4595,7 @@
       <c r="J104" s="67"/>
     </row>
     <row r="105" spans="1:10">
-      <c r="A105" s="80">
+      <c r="A105" s="139">
         <v>15</v>
       </c>
       <c r="B105" s="26">
@@ -4578,7 +4614,7 @@
       <c r="J105" s="29"/>
     </row>
     <row r="106" spans="1:10">
-      <c r="A106" s="81"/>
+      <c r="A106" s="140"/>
       <c r="B106" s="26">
         <v>41681</v>
       </c>
@@ -4595,7 +4631,7 @@
       <c r="J106" s="29"/>
     </row>
     <row r="107" spans="1:10">
-      <c r="A107" s="81"/>
+      <c r="A107" s="140"/>
       <c r="B107" s="26">
         <v>41682</v>
       </c>
@@ -4612,7 +4648,7 @@
       <c r="J107" s="29"/>
     </row>
     <row r="108" spans="1:10">
-      <c r="A108" s="81"/>
+      <c r="A108" s="140"/>
       <c r="B108" s="26">
         <v>41683</v>
       </c>
@@ -4629,7 +4665,7 @@
       <c r="J108" s="29"/>
     </row>
     <row r="109" spans="1:10">
-      <c r="A109" s="82"/>
+      <c r="A109" s="134"/>
       <c r="B109" s="26">
         <v>41684</v>
       </c>
@@ -4646,7 +4682,7 @@
       <c r="J109" s="29"/>
     </row>
     <row r="110" spans="1:10">
-      <c r="A110" s="77">
+      <c r="A110" s="129">
         <v>16</v>
       </c>
       <c r="B110" s="27">
@@ -4665,7 +4701,7 @@
       <c r="J110" s="67"/>
     </row>
     <row r="111" spans="1:10">
-      <c r="A111" s="78"/>
+      <c r="A111" s="130"/>
       <c r="B111" s="27">
         <v>41688</v>
       </c>
@@ -4682,7 +4718,7 @@
       <c r="J111" s="67"/>
     </row>
     <row r="112" spans="1:10">
-      <c r="A112" s="78"/>
+      <c r="A112" s="130"/>
       <c r="B112" s="27">
         <v>41689</v>
       </c>
@@ -4699,7 +4735,7 @@
       <c r="J112" s="67"/>
     </row>
     <row r="113" spans="1:10">
-      <c r="A113" s="78"/>
+      <c r="A113" s="130"/>
       <c r="B113" s="27">
         <v>41690</v>
       </c>
@@ -4716,7 +4752,7 @@
       <c r="J113" s="67"/>
     </row>
     <row r="114" spans="1:10">
-      <c r="A114" s="79"/>
+      <c r="A114" s="131"/>
       <c r="B114" s="27">
         <v>41691</v>
       </c>
@@ -4733,7 +4769,7 @@
       <c r="J114" s="67"/>
     </row>
     <row r="115" spans="1:10">
-      <c r="A115" s="80">
+      <c r="A115" s="139">
         <v>17</v>
       </c>
       <c r="B115" s="26">
@@ -4752,7 +4788,7 @@
       <c r="J115" s="29"/>
     </row>
     <row r="116" spans="1:10">
-      <c r="A116" s="81"/>
+      <c r="A116" s="140"/>
       <c r="B116" s="26">
         <v>41695</v>
       </c>
@@ -4769,7 +4805,7 @@
       <c r="J116" s="29"/>
     </row>
     <row r="117" spans="1:10">
-      <c r="A117" s="81"/>
+      <c r="A117" s="140"/>
       <c r="B117" s="26">
         <v>41696</v>
       </c>
@@ -4786,7 +4822,7 @@
       <c r="J117" s="29"/>
     </row>
     <row r="118" spans="1:10">
-      <c r="A118" s="81"/>
+      <c r="A118" s="140"/>
       <c r="B118" s="26">
         <v>41697</v>
       </c>
@@ -4803,7 +4839,7 @@
       <c r="J118" s="29"/>
     </row>
     <row r="119" spans="1:10">
-      <c r="A119" s="82"/>
+      <c r="A119" s="134"/>
       <c r="B119" s="26">
         <v>41698</v>
       </c>
@@ -4820,7 +4856,7 @@
       <c r="J119" s="29"/>
     </row>
     <row r="120" spans="1:10">
-      <c r="A120" s="77">
+      <c r="A120" s="129">
         <v>18</v>
       </c>
       <c r="B120" s="27">
@@ -4839,7 +4875,7 @@
       <c r="J120" s="67"/>
     </row>
     <row r="121" spans="1:10">
-      <c r="A121" s="78"/>
+      <c r="A121" s="130"/>
       <c r="B121" s="27">
         <v>41702</v>
       </c>
@@ -4856,7 +4892,7 @@
       <c r="J121" s="67"/>
     </row>
     <row r="122" spans="1:10">
-      <c r="A122" s="78"/>
+      <c r="A122" s="130"/>
       <c r="B122" s="27">
         <v>41703</v>
       </c>
@@ -4873,7 +4909,7 @@
       <c r="J122" s="67"/>
     </row>
     <row r="123" spans="1:10">
-      <c r="A123" s="78"/>
+      <c r="A123" s="130"/>
       <c r="B123" s="27">
         <v>41704</v>
       </c>
@@ -4890,7 +4926,7 @@
       <c r="J123" s="67"/>
     </row>
     <row r="124" spans="1:10">
-      <c r="A124" s="79"/>
+      <c r="A124" s="131"/>
       <c r="B124" s="27">
         <v>41705</v>
       </c>
@@ -4907,7 +4943,7 @@
       <c r="J124" s="67"/>
     </row>
     <row r="125" spans="1:10">
-      <c r="A125" s="80">
+      <c r="A125" s="139">
         <v>19</v>
       </c>
       <c r="B125" s="26">
@@ -4926,7 +4962,7 @@
       <c r="J125" s="29"/>
     </row>
     <row r="126" spans="1:10">
-      <c r="A126" s="81"/>
+      <c r="A126" s="140"/>
       <c r="B126" s="26">
         <v>41709</v>
       </c>
@@ -4943,7 +4979,7 @@
       <c r="J126" s="29"/>
     </row>
     <row r="127" spans="1:10">
-      <c r="A127" s="81"/>
+      <c r="A127" s="140"/>
       <c r="B127" s="26">
         <v>41710</v>
       </c>
@@ -4960,7 +4996,7 @@
       <c r="J127" s="29"/>
     </row>
     <row r="128" spans="1:10">
-      <c r="A128" s="81"/>
+      <c r="A128" s="140"/>
       <c r="B128" s="26">
         <v>41711</v>
       </c>
@@ -4977,7 +5013,7 @@
       <c r="J128" s="29"/>
     </row>
     <row r="129" spans="1:10">
-      <c r="A129" s="82"/>
+      <c r="A129" s="134"/>
       <c r="B129" s="26">
         <v>41712</v>
       </c>
@@ -4994,7 +5030,7 @@
       <c r="J129" s="29"/>
     </row>
     <row r="130" spans="1:10">
-      <c r="A130" s="77">
+      <c r="A130" s="129">
         <v>20</v>
       </c>
       <c r="B130" s="27">
@@ -5013,7 +5049,7 @@
       <c r="J130" s="67"/>
     </row>
     <row r="131" spans="1:10">
-      <c r="A131" s="78"/>
+      <c r="A131" s="130"/>
       <c r="B131" s="27">
         <v>41716</v>
       </c>
@@ -5030,7 +5066,7 @@
       <c r="J131" s="67"/>
     </row>
     <row r="132" spans="1:10">
-      <c r="A132" s="78"/>
+      <c r="A132" s="130"/>
       <c r="B132" s="27">
         <v>41717</v>
       </c>
@@ -5047,7 +5083,7 @@
       <c r="J132" s="67"/>
     </row>
     <row r="133" spans="1:10">
-      <c r="A133" s="78"/>
+      <c r="A133" s="130"/>
       <c r="B133" s="27">
         <v>41718</v>
       </c>
@@ -5064,7 +5100,7 @@
       <c r="J133" s="67"/>
     </row>
     <row r="134" spans="1:10">
-      <c r="A134" s="79"/>
+      <c r="A134" s="131"/>
       <c r="B134" s="27">
         <v>41719</v>
       </c>
@@ -5081,7 +5117,7 @@
       <c r="J134" s="67"/>
     </row>
     <row r="135" spans="1:10">
-      <c r="A135" s="80">
+      <c r="A135" s="139">
         <v>21</v>
       </c>
       <c r="B135" s="26">
@@ -5100,7 +5136,7 @@
       <c r="J135" s="29"/>
     </row>
     <row r="136" spans="1:10">
-      <c r="A136" s="81"/>
+      <c r="A136" s="140"/>
       <c r="B136" s="26">
         <v>41723</v>
       </c>
@@ -5117,7 +5153,7 @@
       <c r="J136" s="29"/>
     </row>
     <row r="137" spans="1:10">
-      <c r="A137" s="81"/>
+      <c r="A137" s="140"/>
       <c r="B137" s="26">
         <v>41724</v>
       </c>
@@ -5134,7 +5170,7 @@
       <c r="J137" s="29"/>
     </row>
     <row r="138" spans="1:10">
-      <c r="A138" s="81"/>
+      <c r="A138" s="140"/>
       <c r="B138" s="26">
         <v>41725</v>
       </c>
@@ -5151,7 +5187,7 @@
       <c r="J138" s="29"/>
     </row>
     <row r="139" spans="1:10">
-      <c r="A139" s="82"/>
+      <c r="A139" s="134"/>
       <c r="B139" s="26">
         <v>41726</v>
       </c>
@@ -5168,7 +5204,7 @@
       <c r="J139" s="29"/>
     </row>
     <row r="140" spans="1:10">
-      <c r="A140" s="77">
+      <c r="A140" s="129">
         <v>22</v>
       </c>
       <c r="B140" s="27">
@@ -5187,7 +5223,7 @@
       <c r="J140" s="67"/>
     </row>
     <row r="141" spans="1:10">
-      <c r="A141" s="78"/>
+      <c r="A141" s="130"/>
       <c r="B141" s="27">
         <v>41730</v>
       </c>
@@ -5204,7 +5240,7 @@
       <c r="J141" s="67"/>
     </row>
     <row r="142" spans="1:10">
-      <c r="A142" s="78"/>
+      <c r="A142" s="130"/>
       <c r="B142" s="27">
         <v>41731</v>
       </c>
@@ -5221,7 +5257,7 @@
       <c r="J142" s="67"/>
     </row>
     <row r="143" spans="1:10">
-      <c r="A143" s="78"/>
+      <c r="A143" s="130"/>
       <c r="B143" s="27">
         <v>41732</v>
       </c>
@@ -5238,7 +5274,7 @@
       <c r="J143" s="67"/>
     </row>
     <row r="144" spans="1:10">
-      <c r="A144" s="79"/>
+      <c r="A144" s="131"/>
       <c r="B144" s="27">
         <v>41733</v>
       </c>
@@ -5255,7 +5291,7 @@
       <c r="J144" s="67"/>
     </row>
     <row r="145" spans="1:10">
-      <c r="A145" s="80">
+      <c r="A145" s="139">
         <v>23</v>
       </c>
       <c r="B145" s="26">
@@ -5274,7 +5310,7 @@
       <c r="J145" s="29"/>
     </row>
     <row r="146" spans="1:10">
-      <c r="A146" s="81"/>
+      <c r="A146" s="140"/>
       <c r="B146" s="26">
         <v>41737</v>
       </c>
@@ -5291,7 +5327,7 @@
       <c r="J146" s="29"/>
     </row>
     <row r="147" spans="1:10">
-      <c r="A147" s="81"/>
+      <c r="A147" s="140"/>
       <c r="B147" s="26">
         <v>41738</v>
       </c>
@@ -5308,7 +5344,7 @@
       <c r="J147" s="29"/>
     </row>
     <row r="148" spans="1:10">
-      <c r="A148" s="81"/>
+      <c r="A148" s="140"/>
       <c r="B148" s="26">
         <v>41739</v>
       </c>
@@ -5325,7 +5361,7 @@
       <c r="J148" s="29"/>
     </row>
     <row r="149" spans="1:10">
-      <c r="A149" s="82"/>
+      <c r="A149" s="134"/>
       <c r="B149" s="26">
         <v>41740</v>
       </c>
@@ -5342,7 +5378,7 @@
       <c r="J149" s="29"/>
     </row>
     <row r="150" spans="1:10">
-      <c r="A150" s="77">
+      <c r="A150" s="129">
         <v>24</v>
       </c>
       <c r="B150" s="27">
@@ -5361,7 +5397,7 @@
       <c r="J150" s="67"/>
     </row>
     <row r="151" spans="1:10">
-      <c r="A151" s="78"/>
+      <c r="A151" s="130"/>
       <c r="B151" s="27">
         <v>41744</v>
       </c>
@@ -5378,7 +5414,7 @@
       <c r="J151" s="67"/>
     </row>
     <row r="152" spans="1:10">
-      <c r="A152" s="78"/>
+      <c r="A152" s="130"/>
       <c r="B152" s="27">
         <v>41745</v>
       </c>
@@ -5395,7 +5431,7 @@
       <c r="J152" s="67"/>
     </row>
     <row r="153" spans="1:10">
-      <c r="A153" s="78"/>
+      <c r="A153" s="130"/>
       <c r="B153" s="27">
         <v>41746</v>
       </c>
@@ -5412,7 +5448,7 @@
       <c r="J153" s="67"/>
     </row>
     <row r="154" spans="1:10">
-      <c r="A154" s="79"/>
+      <c r="A154" s="131"/>
       <c r="B154" s="27">
         <v>41747</v>
       </c>
@@ -5429,7 +5465,7 @@
       <c r="J154" s="67"/>
     </row>
     <row r="155" spans="1:10">
-      <c r="A155" s="80">
+      <c r="A155" s="139">
         <v>25</v>
       </c>
       <c r="B155" s="26">
@@ -5448,7 +5484,7 @@
       <c r="J155" s="29"/>
     </row>
     <row r="156" spans="1:10">
-      <c r="A156" s="81"/>
+      <c r="A156" s="140"/>
       <c r="B156" s="26">
         <v>41751</v>
       </c>
@@ -5465,7 +5501,7 @@
       <c r="J156" s="29"/>
     </row>
     <row r="157" spans="1:10">
-      <c r="A157" s="81"/>
+      <c r="A157" s="140"/>
       <c r="B157" s="26">
         <v>41752</v>
       </c>
@@ -5482,7 +5518,7 @@
       <c r="J157" s="29"/>
     </row>
     <row r="158" spans="1:10">
-      <c r="A158" s="81"/>
+      <c r="A158" s="140"/>
       <c r="B158" s="26">
         <v>41753</v>
       </c>
@@ -5499,7 +5535,7 @@
       <c r="J158" s="29"/>
     </row>
     <row r="159" spans="1:10">
-      <c r="A159" s="82"/>
+      <c r="A159" s="134"/>
       <c r="B159" s="26">
         <v>41754</v>
       </c>
@@ -5516,7 +5552,7 @@
       <c r="J159" s="29"/>
     </row>
     <row r="160" spans="1:10">
-      <c r="A160" s="77">
+      <c r="A160" s="129">
         <v>26</v>
       </c>
       <c r="B160" s="27">
@@ -5535,7 +5571,7 @@
       <c r="J160" s="67"/>
     </row>
     <row r="161" spans="1:10">
-      <c r="A161" s="78"/>
+      <c r="A161" s="130"/>
       <c r="B161" s="27">
         <v>41758</v>
       </c>
@@ -5552,7 +5588,7 @@
       <c r="J161" s="67"/>
     </row>
     <row r="162" spans="1:10">
-      <c r="A162" s="78"/>
+      <c r="A162" s="130"/>
       <c r="B162" s="27">
         <v>41759</v>
       </c>
@@ -5569,7 +5605,7 @@
       <c r="J162" s="67"/>
     </row>
     <row r="163" spans="1:10">
-      <c r="A163" s="78"/>
+      <c r="A163" s="130"/>
       <c r="B163" s="27">
         <v>41760</v>
       </c>
@@ -5586,7 +5622,7 @@
       <c r="J163" s="67"/>
     </row>
     <row r="164" spans="1:10">
-      <c r="A164" s="79"/>
+      <c r="A164" s="131"/>
       <c r="B164" s="27">
         <v>41761</v>
       </c>
@@ -5603,7 +5639,7 @@
       <c r="J164" s="67"/>
     </row>
     <row r="165" spans="1:10">
-      <c r="A165" s="80">
+      <c r="A165" s="139">
         <v>27</v>
       </c>
       <c r="B165" s="26">
@@ -5622,7 +5658,7 @@
       <c r="J165" s="29"/>
     </row>
     <row r="166" spans="1:10">
-      <c r="A166" s="81"/>
+      <c r="A166" s="140"/>
       <c r="B166" s="26">
         <v>41765</v>
       </c>
@@ -5639,7 +5675,7 @@
       <c r="J166" s="29"/>
     </row>
     <row r="167" spans="1:10">
-      <c r="A167" s="81"/>
+      <c r="A167" s="140"/>
       <c r="B167" s="26">
         <v>41766</v>
       </c>
@@ -5656,7 +5692,7 @@
       <c r="J167" s="29"/>
     </row>
     <row r="168" spans="1:10">
-      <c r="A168" s="81"/>
+      <c r="A168" s="140"/>
       <c r="B168" s="26">
         <v>41767</v>
       </c>
@@ -5673,7 +5709,7 @@
       <c r="J168" s="29"/>
     </row>
     <row r="169" spans="1:10">
-      <c r="A169" s="82"/>
+      <c r="A169" s="134"/>
       <c r="B169" s="26">
         <v>41768</v>
       </c>
@@ -5690,7 +5726,7 @@
       <c r="J169" s="29"/>
     </row>
     <row r="170" spans="1:10">
-      <c r="A170" s="77">
+      <c r="A170" s="129">
         <v>28</v>
       </c>
       <c r="B170" s="27">
@@ -5709,7 +5745,7 @@
       <c r="J170" s="67"/>
     </row>
     <row r="171" spans="1:10">
-      <c r="A171" s="78"/>
+      <c r="A171" s="130"/>
       <c r="B171" s="27">
         <v>41772</v>
       </c>
@@ -5726,7 +5762,7 @@
       <c r="J171" s="67"/>
     </row>
     <row r="172" spans="1:10">
-      <c r="A172" s="78"/>
+      <c r="A172" s="130"/>
       <c r="B172" s="27">
         <v>41773</v>
       </c>
@@ -5743,7 +5779,7 @@
       <c r="J172" s="67"/>
     </row>
     <row r="173" spans="1:10">
-      <c r="A173" s="78"/>
+      <c r="A173" s="130"/>
       <c r="B173" s="27">
         <v>41774</v>
       </c>
@@ -5760,7 +5796,7 @@
       <c r="J173" s="67"/>
     </row>
     <row r="174" spans="1:10">
-      <c r="A174" s="79"/>
+      <c r="A174" s="131"/>
       <c r="B174" s="27">
         <v>41775</v>
       </c>
@@ -5777,7 +5813,7 @@
       <c r="J174" s="67"/>
     </row>
     <row r="175" spans="1:10">
-      <c r="A175" s="80">
+      <c r="A175" s="139">
         <v>29</v>
       </c>
       <c r="B175" s="26">
@@ -5796,7 +5832,7 @@
       <c r="J175" s="29"/>
     </row>
     <row r="176" spans="1:10">
-      <c r="A176" s="81"/>
+      <c r="A176" s="140"/>
       <c r="B176" s="26">
         <v>41779</v>
       </c>
@@ -5813,7 +5849,7 @@
       <c r="J176" s="29"/>
     </row>
     <row r="177" spans="1:10">
-      <c r="A177" s="81"/>
+      <c r="A177" s="140"/>
       <c r="B177" s="26">
         <v>41780</v>
       </c>
@@ -5830,7 +5866,7 @@
       <c r="J177" s="29"/>
     </row>
     <row r="178" spans="1:10">
-      <c r="A178" s="81"/>
+      <c r="A178" s="140"/>
       <c r="B178" s="26">
         <v>41781</v>
       </c>
@@ -5847,7 +5883,7 @@
       <c r="J178" s="29"/>
     </row>
     <row r="179" spans="1:10">
-      <c r="A179" s="82"/>
+      <c r="A179" s="134"/>
       <c r="B179" s="26">
         <v>41782</v>
       </c>
@@ -5864,7 +5900,7 @@
       <c r="J179" s="29"/>
     </row>
     <row r="180" spans="1:10">
-      <c r="A180" s="83">
+      <c r="A180" s="141">
         <v>30</v>
       </c>
       <c r="B180" s="27">
@@ -5883,7 +5919,7 @@
       <c r="J180" s="37"/>
     </row>
     <row r="181" spans="1:10">
-      <c r="A181" s="84"/>
+      <c r="A181" s="142"/>
       <c r="B181" s="27">
         <v>41786</v>
       </c>
@@ -5900,7 +5936,7 @@
       <c r="J181" s="37"/>
     </row>
     <row r="182" spans="1:10">
-      <c r="A182" s="84"/>
+      <c r="A182" s="142"/>
       <c r="B182" s="27">
         <v>41787</v>
       </c>
@@ -5917,7 +5953,7 @@
       <c r="J182" s="37"/>
     </row>
     <row r="183" spans="1:10">
-      <c r="A183" s="84"/>
+      <c r="A183" s="142"/>
       <c r="B183" s="27">
         <v>41788</v>
       </c>
@@ -5934,7 +5970,7 @@
       <c r="J183" s="37"/>
     </row>
     <row r="184" spans="1:10">
-      <c r="A184" s="85"/>
+      <c r="A184" s="143"/>
       <c r="B184" s="27">
         <v>41789</v>
       </c>
@@ -6060,6 +6096,49 @@
     </row>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="A170:A174"/>
+    <mergeCell ref="A175:A179"/>
+    <mergeCell ref="A180:A184"/>
+    <mergeCell ref="A140:A144"/>
+    <mergeCell ref="A145:A149"/>
+    <mergeCell ref="A150:A154"/>
+    <mergeCell ref="A155:A159"/>
+    <mergeCell ref="A160:A164"/>
+    <mergeCell ref="A60:A64"/>
+    <mergeCell ref="A65:A69"/>
+    <mergeCell ref="A47:A59"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A165:A169"/>
+    <mergeCell ref="A120:A124"/>
+    <mergeCell ref="A125:A129"/>
+    <mergeCell ref="A130:A134"/>
+    <mergeCell ref="A135:A139"/>
+    <mergeCell ref="F48:F50"/>
+    <mergeCell ref="F51:F53"/>
+    <mergeCell ref="A105:A109"/>
+    <mergeCell ref="A110:A114"/>
+    <mergeCell ref="A115:A119"/>
+    <mergeCell ref="A90:A94"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="A75:A79"/>
+    <mergeCell ref="A85:A89"/>
+    <mergeCell ref="A80:A84"/>
+    <mergeCell ref="A95:A99"/>
+    <mergeCell ref="A100:A104"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="A34:A46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="F31:F33"/>
     <mergeCell ref="F54:F58"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="G2:N4"/>
@@ -6076,49 +6155,6 @@
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="A34:A46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="A19:A33"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="A75:A79"/>
-    <mergeCell ref="A85:A89"/>
-    <mergeCell ref="A80:A84"/>
-    <mergeCell ref="A95:A99"/>
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="A60:A64"/>
-    <mergeCell ref="A65:A69"/>
-    <mergeCell ref="A47:A59"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="A165:A169"/>
-    <mergeCell ref="A120:A124"/>
-    <mergeCell ref="A125:A129"/>
-    <mergeCell ref="A130:A134"/>
-    <mergeCell ref="A135:A139"/>
-    <mergeCell ref="F48:F50"/>
-    <mergeCell ref="F51:F53"/>
-    <mergeCell ref="A105:A109"/>
-    <mergeCell ref="A110:A114"/>
-    <mergeCell ref="A115:A119"/>
-    <mergeCell ref="A90:A94"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="A170:A174"/>
-    <mergeCell ref="A175:A179"/>
-    <mergeCell ref="A180:A184"/>
-    <mergeCell ref="A140:A144"/>
-    <mergeCell ref="A145:A149"/>
-    <mergeCell ref="A150:A154"/>
-    <mergeCell ref="A155:A159"/>
-    <mergeCell ref="A160:A164"/>
   </mergeCells>
   <conditionalFormatting sqref="M7">
     <cfRule type="cellIs" dxfId="3" priority="11" operator="greaterThan">

</xml_diff>

<commit_message>
effort log cuối ngày 09/12 - khang
</commit_message>
<xml_diff>
--- a/1. Project management/9. Timelog/individual time log/AS_PM_TimeLog_DeadlineTeam_KhangHuynh.xlsx
+++ b/1. Project management/9. Timelog/individual time log/AS_PM_TimeLog_DeadlineTeam_KhangHuynh.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="188">
   <si>
     <t>Week</t>
   </si>
@@ -661,6 +661,12 @@
   </si>
   <si>
     <t>6:-00PM</t>
+  </si>
+  <si>
+    <t>Update drivers specification document -viet version
+ + Use case "Hoi dap"
+ + Quality Attribute
+ + Business and Technical constraint</t>
   </si>
 </sst>
 </file>
@@ -1199,15 +1205,78 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="8" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="8" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1328,74 +1397,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1707,7 +1713,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1830,13 +1836,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O193"/>
+  <dimension ref="A1:O194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="6" topLeftCell="H57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="6" topLeftCell="G60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E61" sqref="E61"/>
+      <selection pane="bottomRight" activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1858,81 +1864,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="83"/>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="85"/>
+      <c r="A1" s="104"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="106"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="120" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="86" t="s">
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
-      <c r="N2" s="88"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="108"/>
+      <c r="M2" s="108"/>
+      <c r="N2" s="109"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="123" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="103"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="91"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="111"/>
+      <c r="M3" s="111"/>
+      <c r="N3" s="112"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="105"/>
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93"/>
-      <c r="J4" s="93"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
-      <c r="M4" s="93"/>
-      <c r="N4" s="94"/>
+      <c r="A4" s="126"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="113"/>
+      <c r="H4" s="114"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="114"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
+      <c r="N4" s="115"/>
     </row>
     <row r="5" spans="1:15" ht="39" customHeight="1">
-      <c r="A5" s="112"/>
-      <c r="B5" s="113"/>
-      <c r="C5" s="113"/>
-      <c r="D5" s="113"/>
-      <c r="E5" s="114"/>
+      <c r="A5" s="133"/>
+      <c r="B5" s="134"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="135"/>
       <c r="F5" s="15"/>
       <c r="H5" s="41" t="s">
         <v>64</v>
@@ -1977,13 +1983,13 @@
       <c r="J6" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="98"/>
-      <c r="L6" s="98"/>
-      <c r="M6" s="98"/>
-      <c r="N6" s="98"/>
+      <c r="K6" s="119"/>
+      <c r="L6" s="119"/>
+      <c r="M6" s="119"/>
+      <c r="N6" s="119"/>
     </row>
     <row r="7" spans="1:15" ht="38.25">
-      <c r="A7" s="95">
+      <c r="A7" s="116">
         <v>1</v>
       </c>
       <c r="B7" s="16">
@@ -2009,12 +2015,12 @@
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="29"/>
-      <c r="K7" s="122" t="s">
+      <c r="K7" s="143" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="122"/>
+      <c r="L7" s="143"/>
       <c r="M7" s="32">
-        <f>SUM(M8:M67)</f>
+        <f>SUM(M8:M68)</f>
         <v>97.68</v>
       </c>
       <c r="N7" s="3" t="s">
@@ -2022,8 +2028,8 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="25.5">
-      <c r="A8" s="96"/>
-      <c r="B8" s="108">
+      <c r="A8" s="117"/>
+      <c r="B8" s="129">
         <v>41586</v>
       </c>
       <c r="C8" s="17">
@@ -2035,7 +2041,7 @@
       <c r="E8" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="110">
+      <c r="F8" s="131">
         <v>1.67</v>
       </c>
       <c r="G8" s="19" t="s">
@@ -2059,8 +2065,8 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="97"/>
-      <c r="B9" s="109"/>
+      <c r="A9" s="118"/>
+      <c r="B9" s="130"/>
       <c r="C9" s="17">
         <v>0.63194444444444442</v>
       </c>
@@ -2070,7 +2076,7 @@
       <c r="E9" s="18">
         <v>0.5</v>
       </c>
-      <c r="F9" s="111"/>
+      <c r="F9" s="132"/>
       <c r="G9" s="29" t="s">
         <v>23</v>
       </c>
@@ -2081,10 +2087,10 @@
       <c r="J9" s="29"/>
     </row>
     <row r="10" spans="1:15" s="63" customFormat="1">
-      <c r="A10" s="115">
+      <c r="A10" s="136">
         <v>2</v>
       </c>
-      <c r="B10" s="118">
+      <c r="B10" s="139">
         <v>41589</v>
       </c>
       <c r="C10" s="58" t="s">
@@ -2096,7 +2102,7 @@
       <c r="E10" s="59">
         <v>2.5</v>
       </c>
-      <c r="F10" s="120">
+      <c r="F10" s="141">
         <f>SUM(E10:E11)</f>
         <v>5</v>
       </c>
@@ -2110,8 +2116,8 @@
       <c r="J10" s="60"/>
     </row>
     <row r="11" spans="1:15" s="63" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A11" s="116"/>
-      <c r="B11" s="119"/>
+      <c r="A11" s="137"/>
+      <c r="B11" s="140"/>
       <c r="C11" s="58" t="s">
         <v>76</v>
       </c>
@@ -2121,7 +2127,7 @@
       <c r="E11" s="59">
         <v>2.5</v>
       </c>
-      <c r="F11" s="121"/>
+      <c r="F11" s="142"/>
       <c r="G11" s="60" t="s">
         <v>22</v>
       </c>
@@ -2134,8 +2140,8 @@
       <c r="J11" s="60"/>
     </row>
     <row r="12" spans="1:15" ht="51">
-      <c r="A12" s="116"/>
-      <c r="B12" s="123">
+      <c r="A12" s="137"/>
+      <c r="B12" s="90">
         <v>41590</v>
       </c>
       <c r="C12" s="22">
@@ -2147,7 +2153,7 @@
       <c r="E12" s="23">
         <v>2.25</v>
       </c>
-      <c r="F12" s="125">
+      <c r="F12" s="144">
         <v>3.75</v>
       </c>
       <c r="G12" s="30" t="s">
@@ -2174,8 +2180,8 @@
       <c r="O12" s="34"/>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A13" s="116"/>
-      <c r="B13" s="124"/>
+      <c r="A13" s="137"/>
+      <c r="B13" s="92"/>
       <c r="C13" s="22">
         <v>0.91666666666666663</v>
       </c>
@@ -2185,7 +2191,7 @@
       <c r="E13" s="23">
         <v>1.5</v>
       </c>
-      <c r="F13" s="126"/>
+      <c r="F13" s="145"/>
       <c r="G13" s="45" t="s">
         <v>28</v>
       </c>
@@ -2201,8 +2207,8 @@
       <c r="O13" s="34"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A14" s="116"/>
-      <c r="B14" s="123">
+      <c r="A14" s="137"/>
+      <c r="B14" s="90">
         <v>41591</v>
       </c>
       <c r="C14" s="22">
@@ -2214,7 +2220,7 @@
       <c r="E14" s="23">
         <v>2</v>
       </c>
-      <c r="F14" s="128">
+      <c r="F14" s="93">
         <v>4.5</v>
       </c>
       <c r="G14" s="45" t="s">
@@ -2232,8 +2238,8 @@
       <c r="O14" s="34"/>
     </row>
     <row r="15" spans="1:15" ht="25.5">
-      <c r="A15" s="116"/>
-      <c r="B15" s="127"/>
+      <c r="A15" s="137"/>
+      <c r="B15" s="91"/>
       <c r="C15" s="25">
         <v>0.5625</v>
       </c>
@@ -2243,7 +2249,7 @@
       <c r="E15" s="28">
         <v>2</v>
       </c>
-      <c r="F15" s="129"/>
+      <c r="F15" s="94"/>
       <c r="G15" s="30" t="s">
         <v>19</v>
       </c>
@@ -2260,8 +2266,8 @@
       <c r="N15" s="3"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A16" s="116"/>
-      <c r="B16" s="124"/>
+      <c r="A16" s="137"/>
+      <c r="B16" s="92"/>
       <c r="C16" s="25">
         <v>0.83333333333333337</v>
       </c>
@@ -2271,7 +2277,7 @@
       <c r="E16" s="28">
         <v>0.5</v>
       </c>
-      <c r="F16" s="130"/>
+      <c r="F16" s="95"/>
       <c r="G16" s="45" t="s">
         <v>28</v>
       </c>
@@ -2295,7 +2301,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A17" s="116"/>
+      <c r="A17" s="137"/>
       <c r="B17" s="47">
         <v>41592</v>
       </c>
@@ -2334,7 +2340,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="25.5">
-      <c r="A18" s="117"/>
+      <c r="A18" s="138"/>
       <c r="B18" s="42">
         <v>41593</v>
       </c>
@@ -2373,10 +2379,10 @@
       </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="137">
+      <c r="A19" s="98">
         <v>3</v>
       </c>
-      <c r="B19" s="134">
+      <c r="B19" s="96">
         <v>41596</v>
       </c>
       <c r="C19" s="53" t="s">
@@ -2388,7 +2394,7 @@
       <c r="E19" s="50">
         <v>0.5</v>
       </c>
-      <c r="F19" s="80">
+      <c r="F19" s="89">
         <f>SUM(E19:E20)</f>
         <v>3.5</v>
       </c>
@@ -2407,7 +2413,7 @@
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="9">
-        <f>SUM(E70:E74)</f>
+        <f>SUM(E71:E75)</f>
         <v>0</v>
       </c>
       <c r="N19" s="3" t="s">
@@ -2415,8 +2421,8 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="138"/>
-      <c r="B20" s="135"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="97"/>
       <c r="C20" s="53" t="s">
         <v>81</v>
       </c>
@@ -2426,7 +2432,7 @@
       <c r="E20" s="50">
         <v>3</v>
       </c>
-      <c r="F20" s="136"/>
+      <c r="F20" s="85"/>
       <c r="G20" s="49" t="s">
         <v>22</v>
       </c>
@@ -2443,8 +2449,8 @@
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="138"/>
-      <c r="B21" s="134">
+      <c r="A21" s="99"/>
+      <c r="B21" s="96">
         <v>41597</v>
       </c>
       <c r="C21" s="53" t="s">
@@ -2456,7 +2462,7 @@
       <c r="E21" s="50">
         <v>2</v>
       </c>
-      <c r="F21" s="80">
+      <c r="F21" s="89">
         <f>SUM(E21:E22)</f>
         <v>2.5</v>
       </c>
@@ -2476,8 +2482,8 @@
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="138"/>
-      <c r="B22" s="135"/>
+      <c r="A22" s="99"/>
+      <c r="B22" s="97"/>
       <c r="C22" s="53" t="s">
         <v>84</v>
       </c>
@@ -2487,7 +2493,7 @@
       <c r="E22" s="50">
         <v>0.5</v>
       </c>
-      <c r="F22" s="136"/>
+      <c r="F22" s="85"/>
       <c r="G22" s="49" t="s">
         <v>22</v>
       </c>
@@ -2503,7 +2509,7 @@
       </c>
       <c r="L22" s="5"/>
       <c r="M22" s="9">
-        <f>SUM(E75:E79)</f>
+        <f>SUM(E76:E80)</f>
         <v>0</v>
       </c>
       <c r="N22" s="3" t="s">
@@ -2511,7 +2517,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="26.25">
-      <c r="A23" s="138"/>
+      <c r="A23" s="99"/>
       <c r="B23" s="26">
         <v>41598</v>
       </c>
@@ -2525,7 +2531,7 @@
         <v>4</v>
       </c>
       <c r="F23" s="55">
-        <f t="shared" ref="F23:F76" si="0">E23</f>
+        <f t="shared" ref="F23:F77" si="0">E23</f>
         <v>4</v>
       </c>
       <c r="G23" s="57" t="s">
@@ -2543,7 +2549,7 @@
       </c>
       <c r="L23" s="5"/>
       <c r="M23" s="9">
-        <f>SUM(E80:E84)</f>
+        <f>SUM(E81:E85)</f>
         <v>0</v>
       </c>
       <c r="N23" s="3" t="s">
@@ -2551,7 +2557,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="26.25">
-      <c r="A24" s="138"/>
+      <c r="A24" s="99"/>
       <c r="B24" s="26">
         <v>41599</v>
       </c>
@@ -2564,7 +2570,7 @@
       <c r="E24" s="50">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F24" s="80">
+      <c r="F24" s="89">
         <f>SUM(E24:E28)</f>
         <v>7.0600000000000005</v>
       </c>
@@ -2582,7 +2588,7 @@
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="138"/>
+      <c r="A25" s="99"/>
       <c r="B25" s="26">
         <v>41599</v>
       </c>
@@ -2595,7 +2601,7 @@
       <c r="E25" s="50">
         <v>1.3</v>
       </c>
-      <c r="F25" s="81"/>
+      <c r="F25" s="101"/>
       <c r="G25" s="57" t="s">
         <v>19</v>
       </c>
@@ -2610,7 +2616,7 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="138"/>
+      <c r="A26" s="99"/>
       <c r="B26" s="26">
         <v>41599</v>
       </c>
@@ -2623,7 +2629,7 @@
       <c r="E26" s="50">
         <v>1.5</v>
       </c>
-      <c r="F26" s="81"/>
+      <c r="F26" s="101"/>
       <c r="G26" s="57" t="s">
         <v>24</v>
       </c>
@@ -2640,7 +2646,7 @@
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="138"/>
+      <c r="A27" s="99"/>
       <c r="B27" s="26">
         <v>41599</v>
       </c>
@@ -2653,7 +2659,7 @@
       <c r="E27" s="50">
         <v>2.1</v>
       </c>
-      <c r="F27" s="81"/>
+      <c r="F27" s="101"/>
       <c r="G27" s="29" t="s">
         <v>19</v>
       </c>
@@ -2667,7 +2673,7 @@
       </c>
       <c r="L27" s="5"/>
       <c r="M27" s="9">
-        <f>SUM(E85:E89)</f>
+        <f>SUM(E86:E90)</f>
         <v>0</v>
       </c>
       <c r="N27" s="3" t="s">
@@ -2675,7 +2681,7 @@
       </c>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="138"/>
+      <c r="A28" s="99"/>
       <c r="B28" s="26">
         <v>41599</v>
       </c>
@@ -2688,7 +2694,7 @@
       <c r="E28" s="50">
         <v>1</v>
       </c>
-      <c r="F28" s="82"/>
+      <c r="F28" s="102"/>
       <c r="G28" s="29" t="s">
         <v>22</v>
       </c>
@@ -2703,7 +2709,7 @@
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="138"/>
+      <c r="A29" s="99"/>
       <c r="B29" s="26">
         <v>41600</v>
       </c>
@@ -2716,7 +2722,7 @@
       <c r="E29" s="50">
         <v>1.25</v>
       </c>
-      <c r="F29" s="80">
+      <c r="F29" s="89">
         <f>SUM(E29:E30)</f>
         <v>3.25</v>
       </c>
@@ -2732,7 +2738,7 @@
       <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:14" ht="51">
-      <c r="A30" s="138"/>
+      <c r="A30" s="99"/>
       <c r="B30" s="26">
         <v>41600</v>
       </c>
@@ -2745,7 +2751,7 @@
       <c r="E30" s="50">
         <v>2</v>
       </c>
-      <c r="F30" s="136"/>
+      <c r="F30" s="85"/>
       <c r="G30" s="57" t="s">
         <v>22</v>
       </c>
@@ -2759,7 +2765,7 @@
       </c>
       <c r="L30" s="5"/>
       <c r="M30" s="9">
-        <f>SUM(E90:E94)</f>
+        <f>SUM(E91:E95)</f>
         <v>0</v>
       </c>
       <c r="N30" s="3" t="s">
@@ -2767,7 +2773,7 @@
       </c>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="138"/>
+      <c r="A31" s="99"/>
       <c r="B31" s="26">
         <v>41601</v>
       </c>
@@ -2780,7 +2786,7 @@
       <c r="E31" s="74">
         <v>0.25</v>
       </c>
-      <c r="F31" s="80">
+      <c r="F31" s="89">
         <f>SUM(E31:E33)</f>
         <v>4.6500000000000004</v>
       </c>
@@ -2794,7 +2800,7 @@
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="138"/>
+      <c r="A32" s="99"/>
       <c r="B32" s="26">
         <v>41601</v>
       </c>
@@ -2807,7 +2813,7 @@
       <c r="E32" s="50">
         <v>3.5</v>
       </c>
-      <c r="F32" s="81"/>
+      <c r="F32" s="101"/>
       <c r="G32" s="57" t="s">
         <v>22</v>
       </c>
@@ -2824,7 +2830,7 @@
       <c r="N32" s="3"/>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="139"/>
+      <c r="A33" s="100"/>
       <c r="B33" s="26">
         <v>41601</v>
       </c>
@@ -2837,7 +2843,7 @@
       <c r="E33" s="50">
         <v>0.9</v>
       </c>
-      <c r="F33" s="82"/>
+      <c r="F33" s="102"/>
       <c r="G33" s="57" t="s">
         <v>22</v>
       </c>
@@ -2854,7 +2860,7 @@
       <c r="N33" s="3"/>
     </row>
     <row r="34" spans="1:14" ht="38.25">
-      <c r="A34" s="131">
+      <c r="A34" s="80">
         <v>4</v>
       </c>
       <c r="B34" s="27">
@@ -2888,7 +2894,7 @@
       </c>
       <c r="L34" s="5"/>
       <c r="M34" s="9">
-        <f>SUM(E95:E99)</f>
+        <f>SUM(E96:E100)</f>
         <v>0</v>
       </c>
       <c r="N34" s="3" t="s">
@@ -2896,7 +2902,7 @@
       </c>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="132"/>
+      <c r="A35" s="81"/>
       <c r="B35" s="27">
         <v>41604</v>
       </c>
@@ -2909,7 +2915,7 @@
       <c r="E35" s="28">
         <v>1</v>
       </c>
-      <c r="F35" s="140">
+      <c r="F35" s="103">
         <f>SUM(E35:E38)</f>
         <v>6.75</v>
       </c>
@@ -2927,7 +2933,7 @@
       <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="132"/>
+      <c r="A36" s="81"/>
       <c r="B36" s="27">
         <v>41604</v>
       </c>
@@ -2940,7 +2946,7 @@
       <c r="E36" s="76">
         <v>2.5</v>
       </c>
-      <c r="F36" s="132"/>
+      <c r="F36" s="81"/>
       <c r="G36" s="67" t="s">
         <v>23</v>
       </c>
@@ -2957,7 +2963,7 @@
       <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="132"/>
+      <c r="A37" s="81"/>
       <c r="B37" s="27">
         <v>41604</v>
       </c>
@@ -2970,7 +2976,7 @@
       <c r="E37" s="76">
         <v>1.25</v>
       </c>
-      <c r="F37" s="132"/>
+      <c r="F37" s="81"/>
       <c r="G37" s="67" t="s">
         <v>24</v>
       </c>
@@ -2987,7 +2993,7 @@
       <c r="N37" s="3"/>
     </row>
     <row r="38" spans="1:14" ht="51">
-      <c r="A38" s="132"/>
+      <c r="A38" s="81"/>
       <c r="B38" s="27">
         <v>41604</v>
       </c>
@@ -3000,7 +3006,7 @@
       <c r="E38" s="69">
         <v>2</v>
       </c>
-      <c r="F38" s="133"/>
+      <c r="F38" s="82"/>
       <c r="G38" s="67" t="s">
         <v>22</v>
       </c>
@@ -3018,7 +3024,7 @@
       </c>
       <c r="L38" s="5"/>
       <c r="M38" s="9">
-        <f>SUM(E100:E104)</f>
+        <f>SUM(E101:E105)</f>
         <v>0</v>
       </c>
       <c r="N38" s="3" t="s">
@@ -3026,7 +3032,7 @@
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="132"/>
+      <c r="A39" s="81"/>
       <c r="B39" s="27">
         <v>41605</v>
       </c>
@@ -3039,7 +3045,7 @@
       <c r="E39" s="69">
         <v>2.33</v>
       </c>
-      <c r="F39" s="131">
+      <c r="F39" s="80">
         <f>SUM(E39:E40)</f>
         <v>2.83</v>
       </c>
@@ -3056,7 +3062,7 @@
       </c>
       <c r="L39" s="5"/>
       <c r="M39" s="9">
-        <f>SUM(E105:E109)</f>
+        <f>SUM(E106:E110)</f>
         <v>0</v>
       </c>
       <c r="N39" s="3" t="s">
@@ -3064,7 +3070,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" ht="25.5">
-      <c r="A40" s="132"/>
+      <c r="A40" s="81"/>
       <c r="B40" s="27">
         <v>41605</v>
       </c>
@@ -3077,7 +3083,7 @@
       <c r="E40" s="69">
         <v>0.5</v>
       </c>
-      <c r="F40" s="133"/>
+      <c r="F40" s="82"/>
       <c r="G40" s="67" t="s">
         <v>24</v>
       </c>
@@ -3094,7 +3100,7 @@
       <c r="N40" s="3"/>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="132"/>
+      <c r="A41" s="81"/>
       <c r="B41" s="27">
         <v>41606</v>
       </c>
@@ -3107,7 +3113,7 @@
       <c r="E41" s="69">
         <v>1.33</v>
       </c>
-      <c r="F41" s="131">
+      <c r="F41" s="80">
         <f>SUM(E41:E43)</f>
         <v>5.83</v>
       </c>
@@ -3125,7 +3131,7 @@
       <c r="N41" s="3"/>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="132"/>
+      <c r="A42" s="81"/>
       <c r="B42" s="27">
         <v>41606</v>
       </c>
@@ -3138,7 +3144,7 @@
       <c r="E42" s="69">
         <v>1.75</v>
       </c>
-      <c r="F42" s="132"/>
+      <c r="F42" s="81"/>
       <c r="G42" s="67" t="s">
         <v>25</v>
       </c>
@@ -3153,7 +3159,7 @@
       <c r="N42" s="3"/>
     </row>
     <row r="43" spans="1:14" ht="25.5">
-      <c r="A43" s="132"/>
+      <c r="A43" s="81"/>
       <c r="B43" s="27">
         <v>41606</v>
       </c>
@@ -3166,7 +3172,7 @@
       <c r="E43" s="69">
         <v>2.75</v>
       </c>
-      <c r="F43" s="133"/>
+      <c r="F43" s="82"/>
       <c r="G43" s="67" t="s">
         <v>19</v>
       </c>
@@ -3182,7 +3188,7 @@
       </c>
       <c r="L43" s="5"/>
       <c r="M43" s="9">
-        <f>SUM(E110:E114)</f>
+        <f>SUM(E111:E115)</f>
         <v>0</v>
       </c>
       <c r="N43" s="3" t="s">
@@ -3190,7 +3196,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" ht="51">
-      <c r="A44" s="132"/>
+      <c r="A44" s="81"/>
       <c r="B44" s="27">
         <v>41607</v>
       </c>
@@ -3222,7 +3228,7 @@
       </c>
       <c r="L44" s="5"/>
       <c r="M44" s="9">
-        <f>SUM(E115:E119)</f>
+        <f>SUM(E116:E120)</f>
         <v>0</v>
       </c>
       <c r="N44" s="3" t="s">
@@ -3230,7 +3236,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" ht="38.25">
-      <c r="A45" s="132"/>
+      <c r="A45" s="81"/>
       <c r="B45" s="27">
         <v>41609</v>
       </c>
@@ -3243,7 +3249,7 @@
       <c r="E45" s="69">
         <v>2</v>
       </c>
-      <c r="F45" s="131">
+      <c r="F45" s="80">
         <f>SUM(E45:E46)</f>
         <v>4</v>
       </c>
@@ -3263,7 +3269,7 @@
       <c r="N45" s="3"/>
     </row>
     <row r="46" spans="1:14" ht="25.5">
-      <c r="A46" s="133"/>
+      <c r="A46" s="82"/>
       <c r="B46" s="27">
         <v>41609</v>
       </c>
@@ -3276,7 +3282,7 @@
       <c r="E46" s="69">
         <v>2</v>
       </c>
-      <c r="F46" s="133"/>
+      <c r="F46" s="82"/>
       <c r="G46" s="67" t="s">
         <v>22</v>
       </c>
@@ -3295,7 +3301,7 @@
       <c r="N46" s="3"/>
     </row>
     <row r="47" spans="1:14" ht="63.75">
-      <c r="A47" s="141">
+      <c r="A47" s="83">
         <v>5</v>
       </c>
       <c r="B47" s="26">
@@ -3327,7 +3333,7 @@
       </c>
       <c r="L47" s="5"/>
       <c r="M47" s="9">
-        <f>SUM(E120:E124)</f>
+        <f>SUM(E121:E125)</f>
         <v>0</v>
       </c>
       <c r="N47" s="3" t="s">
@@ -3335,7 +3341,7 @@
       </c>
     </row>
     <row r="48" spans="1:14" ht="38.25">
-      <c r="A48" s="142"/>
+      <c r="A48" s="84"/>
       <c r="B48" s="26">
         <v>41611</v>
       </c>
@@ -3348,7 +3354,7 @@
       <c r="E48" s="55">
         <v>1.5</v>
       </c>
-      <c r="F48" s="141">
+      <c r="F48" s="83">
         <f>SUM(E48:E50)</f>
         <v>7</v>
       </c>
@@ -3366,7 +3372,7 @@
       <c r="N48" s="3"/>
     </row>
     <row r="49" spans="1:14" ht="51.75" customHeight="1">
-      <c r="A49" s="142"/>
+      <c r="A49" s="84"/>
       <c r="B49" s="26">
         <v>41611</v>
       </c>
@@ -3379,7 +3385,7 @@
       <c r="E49" s="55">
         <v>3.5</v>
       </c>
-      <c r="F49" s="142"/>
+      <c r="F49" s="84"/>
       <c r="G49" s="29" t="s">
         <v>19</v>
       </c>
@@ -3393,7 +3399,7 @@
       </c>
       <c r="L49" s="5"/>
       <c r="M49" s="9">
-        <f>SUM(E125:E129)</f>
+        <f>SUM(E126:E130)</f>
         <v>0</v>
       </c>
       <c r="N49" s="3" t="s">
@@ -3401,7 +3407,7 @@
       </c>
     </row>
     <row r="50" spans="1:14" ht="38.25">
-      <c r="A50" s="142"/>
+      <c r="A50" s="84"/>
       <c r="B50" s="26">
         <v>41611</v>
       </c>
@@ -3414,7 +3420,7 @@
       <c r="E50" s="55">
         <v>2</v>
       </c>
-      <c r="F50" s="136"/>
+      <c r="F50" s="85"/>
       <c r="G50" s="29" t="s">
         <v>22</v>
       </c>
@@ -3433,7 +3439,7 @@
       <c r="N50" s="3"/>
     </row>
     <row r="51" spans="1:14" ht="38.25">
-      <c r="A51" s="142"/>
+      <c r="A51" s="84"/>
       <c r="B51" s="26">
         <v>41612</v>
       </c>
@@ -3446,7 +3452,7 @@
       <c r="E51" s="55">
         <v>0.75</v>
       </c>
-      <c r="F51" s="141">
+      <c r="F51" s="83">
         <f>SUM(E52:E53)</f>
         <v>6.5</v>
       </c>
@@ -3467,7 +3473,7 @@
       </c>
       <c r="L51" s="5"/>
       <c r="M51" s="9">
-        <f>SUM(E130:E134)</f>
+        <f>SUM(E131:E135)</f>
         <v>0</v>
       </c>
       <c r="N51" s="3" t="s">
@@ -3475,7 +3481,7 @@
       </c>
     </row>
     <row r="52" spans="1:14" ht="76.5">
-      <c r="A52" s="142"/>
+      <c r="A52" s="84"/>
       <c r="B52" s="26">
         <v>41612</v>
       </c>
@@ -3488,7 +3494,7 @@
       <c r="E52" s="55">
         <v>4.5</v>
       </c>
-      <c r="F52" s="142"/>
+      <c r="F52" s="84"/>
       <c r="G52" s="29" t="s">
         <v>19</v>
       </c>
@@ -3503,7 +3509,7 @@
       <c r="N52" s="3"/>
     </row>
     <row r="53" spans="1:14" ht="38.25">
-      <c r="A53" s="142"/>
+      <c r="A53" s="84"/>
       <c r="B53" s="26">
         <v>41612</v>
       </c>
@@ -3516,7 +3522,7 @@
       <c r="E53" s="55">
         <v>2</v>
       </c>
-      <c r="F53" s="136"/>
+      <c r="F53" s="85"/>
       <c r="G53" s="29" t="s">
         <v>22</v>
       </c>
@@ -3533,7 +3539,7 @@
       <c r="N53" s="3"/>
     </row>
     <row r="54" spans="1:14" ht="38.25">
-      <c r="A54" s="142"/>
+      <c r="A54" s="84"/>
       <c r="B54" s="26">
         <v>41613</v>
       </c>
@@ -3546,7 +3552,7 @@
       <c r="E54" s="74">
         <v>3</v>
       </c>
-      <c r="F54" s="80">
+      <c r="F54" s="89">
         <f>SUM(E54:E58)</f>
         <v>7.82</v>
       </c>
@@ -3564,7 +3570,7 @@
       <c r="N54" s="3"/>
     </row>
     <row r="55" spans="1:14">
-      <c r="A55" s="142"/>
+      <c r="A55" s="84"/>
       <c r="B55" s="26">
         <v>41613</v>
       </c>
@@ -3577,7 +3583,7 @@
       <c r="E55" s="74">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F55" s="81"/>
+      <c r="F55" s="101"/>
       <c r="G55" s="29" t="s">
         <v>24</v>
       </c>
@@ -3592,7 +3598,7 @@
       <c r="N55" s="3"/>
     </row>
     <row r="56" spans="1:14" ht="51">
-      <c r="A56" s="142"/>
+      <c r="A56" s="84"/>
       <c r="B56" s="26">
         <v>41613</v>
       </c>
@@ -3605,7 +3611,7 @@
       <c r="E56" s="74">
         <v>1.5</v>
       </c>
-      <c r="F56" s="81"/>
+      <c r="F56" s="101"/>
       <c r="G56" s="29" t="s">
         <v>23</v>
       </c>
@@ -3620,7 +3626,7 @@
       <c r="N56" s="3"/>
     </row>
     <row r="57" spans="1:14" ht="25.5">
-      <c r="A57" s="142"/>
+      <c r="A57" s="84"/>
       <c r="B57" s="26">
         <v>41613</v>
       </c>
@@ -3633,7 +3639,7 @@
       <c r="E57" s="74">
         <v>0.66</v>
       </c>
-      <c r="F57" s="81"/>
+      <c r="F57" s="101"/>
       <c r="G57" s="29" t="s">
         <v>19</v>
       </c>
@@ -3648,7 +3654,7 @@
       <c r="N57" s="3"/>
     </row>
     <row r="58" spans="1:14" ht="25.5">
-      <c r="A58" s="142"/>
+      <c r="A58" s="84"/>
       <c r="B58" s="26">
         <v>41613</v>
       </c>
@@ -3661,7 +3667,7 @@
       <c r="E58" s="74">
         <v>1.5</v>
       </c>
-      <c r="F58" s="82"/>
+      <c r="F58" s="102"/>
       <c r="G58" s="29" t="s">
         <v>24</v>
       </c>
@@ -3675,7 +3681,7 @@
       </c>
       <c r="L58" s="5"/>
       <c r="M58" s="9">
-        <f>SUM(E135:E139)</f>
+        <f>SUM(E136:E140)</f>
         <v>0</v>
       </c>
       <c r="N58" s="3" t="s">
@@ -3683,7 +3689,7 @@
       </c>
     </row>
     <row r="59" spans="1:14" ht="76.5">
-      <c r="A59" s="136"/>
+      <c r="A59" s="85"/>
       <c r="B59" s="26">
         <v>41616</v>
       </c>
@@ -3717,7 +3723,7 @@
       </c>
       <c r="L59" s="5"/>
       <c r="M59" s="9">
-        <f>SUM(E140:E144)</f>
+        <f>SUM(E141:E145)</f>
         <v>0</v>
       </c>
       <c r="N59" s="3" t="s">
@@ -3725,7 +3731,7 @@
       </c>
     </row>
     <row r="60" spans="1:14" ht="63.75">
-      <c r="A60" s="131">
+      <c r="A60" s="80">
         <v>6</v>
       </c>
       <c r="B60" s="27">
@@ -3740,9 +3746,9 @@
       <c r="E60" s="69">
         <v>4.5</v>
       </c>
-      <c r="F60" s="69">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
+      <c r="F60" s="80">
+        <f>SUM(E60:E61)</f>
+        <v>6.5</v>
       </c>
       <c r="G60" s="67" t="s">
         <v>19</v>
@@ -3761,45 +3767,47 @@
       </c>
       <c r="L60" s="5"/>
       <c r="M60" s="9">
-        <f>SUM(E145:E149)</f>
+        <f>SUM(E146:E150)</f>
         <v>0</v>
       </c>
       <c r="N60" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
-      <c r="A61" s="132"/>
+    <row r="61" spans="1:14" ht="51">
+      <c r="A61" s="81"/>
       <c r="B61" s="27">
+        <v>41617</v>
+      </c>
+      <c r="C61" s="69" t="s">
+        <v>103</v>
+      </c>
+      <c r="D61" s="69" t="s">
+        <v>169</v>
+      </c>
+      <c r="E61" s="69">
+        <v>2</v>
+      </c>
+      <c r="F61" s="82"/>
+      <c r="G61" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" s="79" t="s">
+        <v>187</v>
+      </c>
+      <c r="I61" s="67" t="s">
+        <v>183</v>
+      </c>
+      <c r="J61" s="71"/>
+      <c r="K61" s="7"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="9"/>
+      <c r="N61" s="3"/>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" s="81"/>
+      <c r="B62" s="27">
         <v>41618</v>
-      </c>
-      <c r="C61" s="69"/>
-      <c r="D61" s="69"/>
-      <c r="E61" s="69"/>
-      <c r="F61" s="69">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G61" s="67"/>
-      <c r="H61" s="67"/>
-      <c r="I61" s="67"/>
-      <c r="J61" s="67"/>
-      <c r="K61" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="L61" s="5"/>
-      <c r="M61" s="9">
-        <f>SUM(E150:E154)</f>
-        <v>0</v>
-      </c>
-      <c r="N61" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14">
-      <c r="A62" s="132"/>
-      <c r="B62" s="27">
-        <v>41619</v>
       </c>
       <c r="C62" s="69"/>
       <c r="D62" s="69"/>
@@ -3813,11 +3821,11 @@
       <c r="I62" s="67"/>
       <c r="J62" s="67"/>
       <c r="K62" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L62" s="5"/>
       <c r="M62" s="9">
-        <f>SUM(E155:E159)</f>
+        <f>SUM(E151:E155)</f>
         <v>0</v>
       </c>
       <c r="N62" s="3" t="s">
@@ -3825,9 +3833,9 @@
       </c>
     </row>
     <row r="63" spans="1:14">
-      <c r="A63" s="132"/>
+      <c r="A63" s="81"/>
       <c r="B63" s="27">
-        <v>41620</v>
+        <v>41619</v>
       </c>
       <c r="C63" s="69"/>
       <c r="D63" s="69"/>
@@ -3841,11 +3849,11 @@
       <c r="I63" s="67"/>
       <c r="J63" s="67"/>
       <c r="K63" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L63" s="5"/>
       <c r="M63" s="9">
-        <f>SUM(E160:E164)</f>
+        <f>SUM(E156:E160)</f>
         <v>0</v>
       </c>
       <c r="N63" s="3" t="s">
@@ -3853,9 +3861,9 @@
       </c>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="133"/>
+      <c r="A64" s="81"/>
       <c r="B64" s="27">
-        <v>41621</v>
+        <v>41620</v>
       </c>
       <c r="C64" s="69"/>
       <c r="D64" s="69"/>
@@ -3869,11 +3877,11 @@
       <c r="I64" s="67"/>
       <c r="J64" s="67"/>
       <c r="K64" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L64" s="5"/>
       <c r="M64" s="9">
-        <f>SUM(E165:E169)</f>
+        <f>SUM(E161:E165)</f>
         <v>0</v>
       </c>
       <c r="N64" s="3" t="s">
@@ -3881,29 +3889,27 @@
       </c>
     </row>
     <row r="65" spans="1:14">
-      <c r="A65" s="141">
-        <v>7</v>
-      </c>
-      <c r="B65" s="26">
-        <v>41624</v>
-      </c>
-      <c r="C65" s="55"/>
-      <c r="D65" s="55"/>
-      <c r="E65" s="55"/>
-      <c r="F65" s="55">
+      <c r="A65" s="82"/>
+      <c r="B65" s="27">
+        <v>41621</v>
+      </c>
+      <c r="C65" s="69"/>
+      <c r="D65" s="69"/>
+      <c r="E65" s="69"/>
+      <c r="F65" s="69">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G65" s="29"/>
-      <c r="H65" s="29"/>
-      <c r="I65" s="29"/>
-      <c r="J65" s="29"/>
+      <c r="G65" s="67"/>
+      <c r="H65" s="67"/>
+      <c r="I65" s="67"/>
+      <c r="J65" s="67"/>
       <c r="K65" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L65" s="5"/>
       <c r="M65" s="9">
-        <f>SUM(E170:E174)</f>
+        <f>SUM(E166:E170)</f>
         <v>0</v>
       </c>
       <c r="N65" s="3" t="s">
@@ -3911,9 +3917,11 @@
       </c>
     </row>
     <row r="66" spans="1:14">
-      <c r="A66" s="142"/>
+      <c r="A66" s="83">
+        <v>7</v>
+      </c>
       <c r="B66" s="26">
-        <v>41625</v>
+        <v>41624</v>
       </c>
       <c r="C66" s="55"/>
       <c r="D66" s="55"/>
@@ -3927,11 +3935,11 @@
       <c r="I66" s="29"/>
       <c r="J66" s="29"/>
       <c r="K66" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L66" s="5"/>
       <c r="M66" s="9">
-        <f>SUM(E175:E179)</f>
+        <f>SUM(E171:E175)</f>
         <v>0</v>
       </c>
       <c r="N66" s="3" t="s">
@@ -3939,9 +3947,9 @@
       </c>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="142"/>
+      <c r="A67" s="84"/>
       <c r="B67" s="26">
-        <v>41626</v>
+        <v>41625</v>
       </c>
       <c r="C67" s="55"/>
       <c r="D67" s="55"/>
@@ -3955,11 +3963,11 @@
       <c r="I67" s="29"/>
       <c r="J67" s="29"/>
       <c r="K67" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L67" s="5"/>
       <c r="M67" s="9">
-        <f>SUM(E180:E184)</f>
+        <f>SUM(E176:E180)</f>
         <v>0</v>
       </c>
       <c r="N67" s="3" t="s">
@@ -3967,9 +3975,9 @@
       </c>
     </row>
     <row r="68" spans="1:14">
-      <c r="A68" s="142"/>
+      <c r="A68" s="84"/>
       <c r="B68" s="26">
-        <v>41627</v>
+        <v>41626</v>
       </c>
       <c r="C68" s="55"/>
       <c r="D68" s="55"/>
@@ -3982,11 +3990,22 @@
       <c r="H68" s="29"/>
       <c r="I68" s="29"/>
       <c r="J68" s="29"/>
+      <c r="K68" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L68" s="5"/>
+      <c r="M68" s="9">
+        <f>SUM(E181:E185)</f>
+        <v>0</v>
+      </c>
+      <c r="N68" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="136"/>
+      <c r="A69" s="84"/>
       <c r="B69" s="26">
-        <v>41628</v>
+        <v>41627</v>
       </c>
       <c r="C69" s="55"/>
       <c r="D69" s="55"/>
@@ -4001,28 +4020,28 @@
       <c r="J69" s="29"/>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="131">
+      <c r="A70" s="85"/>
+      <c r="B70" s="26">
+        <v>41628</v>
+      </c>
+      <c r="C70" s="55"/>
+      <c r="D70" s="55"/>
+      <c r="E70" s="55"/>
+      <c r="F70" s="55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G70" s="29"/>
+      <c r="H70" s="29"/>
+      <c r="I70" s="29"/>
+      <c r="J70" s="29"/>
+    </row>
+    <row r="71" spans="1:14">
+      <c r="A71" s="80">
         <v>8</v>
       </c>
-      <c r="B70" s="27">
+      <c r="B71" s="27">
         <v>41631</v>
-      </c>
-      <c r="C70" s="69"/>
-      <c r="D70" s="69"/>
-      <c r="E70" s="69"/>
-      <c r="F70" s="69">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G70" s="67"/>
-      <c r="H70" s="67"/>
-      <c r="I70" s="67"/>
-      <c r="J70" s="67"/>
-    </row>
-    <row r="71" spans="1:14">
-      <c r="A71" s="132"/>
-      <c r="B71" s="27">
-        <v>41632</v>
       </c>
       <c r="C71" s="69"/>
       <c r="D71" s="69"/>
@@ -4037,9 +4056,9 @@
       <c r="J71" s="67"/>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="132"/>
+      <c r="A72" s="81"/>
       <c r="B72" s="27">
-        <v>41633</v>
+        <v>41632</v>
       </c>
       <c r="C72" s="69"/>
       <c r="D72" s="69"/>
@@ -4054,9 +4073,9 @@
       <c r="J72" s="67"/>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="132"/>
+      <c r="A73" s="81"/>
       <c r="B73" s="27">
-        <v>41634</v>
+        <v>41633</v>
       </c>
       <c r="C73" s="69"/>
       <c r="D73" s="69"/>
@@ -4071,9 +4090,9 @@
       <c r="J73" s="67"/>
     </row>
     <row r="74" spans="1:14">
-      <c r="A74" s="133"/>
+      <c r="A74" s="81"/>
       <c r="B74" s="27">
-        <v>41635</v>
+        <v>41634</v>
       </c>
       <c r="C74" s="69"/>
       <c r="D74" s="69"/>
@@ -4088,28 +4107,28 @@
       <c r="J74" s="67"/>
     </row>
     <row r="75" spans="1:14">
-      <c r="A75" s="141">
+      <c r="A75" s="82"/>
+      <c r="B75" s="27">
+        <v>41635</v>
+      </c>
+      <c r="C75" s="69"/>
+      <c r="D75" s="69"/>
+      <c r="E75" s="69"/>
+      <c r="F75" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G75" s="67"/>
+      <c r="H75" s="67"/>
+      <c r="I75" s="67"/>
+      <c r="J75" s="67"/>
+    </row>
+    <row r="76" spans="1:14">
+      <c r="A76" s="83">
         <v>9</v>
       </c>
-      <c r="B75" s="26">
+      <c r="B76" s="26">
         <v>41638</v>
-      </c>
-      <c r="C75" s="55"/>
-      <c r="D75" s="55"/>
-      <c r="E75" s="55"/>
-      <c r="F75" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G75" s="29"/>
-      <c r="H75" s="29"/>
-      <c r="I75" s="29"/>
-      <c r="J75" s="29"/>
-    </row>
-    <row r="76" spans="1:14">
-      <c r="A76" s="142"/>
-      <c r="B76" s="26">
-        <v>41639</v>
       </c>
       <c r="C76" s="55"/>
       <c r="D76" s="55"/>
@@ -4124,15 +4143,15 @@
       <c r="J76" s="29"/>
     </row>
     <row r="77" spans="1:14">
-      <c r="A77" s="142"/>
+      <c r="A77" s="84"/>
       <c r="B77" s="26">
-        <v>41640</v>
+        <v>41639</v>
       </c>
       <c r="C77" s="55"/>
       <c r="D77" s="55"/>
       <c r="E77" s="55"/>
       <c r="F77" s="55">
-        <f t="shared" ref="F77:F108" si="1">E77</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G77" s="29"/>
@@ -4141,15 +4160,15 @@
       <c r="J77" s="29"/>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="142"/>
+      <c r="A78" s="84"/>
       <c r="B78" s="26">
-        <v>41641</v>
+        <v>41640</v>
       </c>
       <c r="C78" s="55"/>
       <c r="D78" s="55"/>
       <c r="E78" s="55"/>
       <c r="F78" s="55">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F78:F109" si="1">E78</f>
         <v>0</v>
       </c>
       <c r="G78" s="29"/>
@@ -4158,9 +4177,9 @@
       <c r="J78" s="29"/>
     </row>
     <row r="79" spans="1:14">
-      <c r="A79" s="136"/>
+      <c r="A79" s="84"/>
       <c r="B79" s="26">
-        <v>41642</v>
+        <v>41641</v>
       </c>
       <c r="C79" s="55"/>
       <c r="D79" s="55"/>
@@ -4175,28 +4194,28 @@
       <c r="J79" s="29"/>
     </row>
     <row r="80" spans="1:14">
-      <c r="A80" s="131">
+      <c r="A80" s="85"/>
+      <c r="B80" s="26">
+        <v>41642</v>
+      </c>
+      <c r="C80" s="55"/>
+      <c r="D80" s="55"/>
+      <c r="E80" s="55"/>
+      <c r="F80" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G80" s="29"/>
+      <c r="H80" s="29"/>
+      <c r="I80" s="29"/>
+      <c r="J80" s="29"/>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="80">
         <v>10</v>
       </c>
-      <c r="B80" s="27">
+      <c r="B81" s="27">
         <v>41645</v>
-      </c>
-      <c r="C80" s="69"/>
-      <c r="D80" s="69"/>
-      <c r="E80" s="69"/>
-      <c r="F80" s="69">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G80" s="67"/>
-      <c r="H80" s="67"/>
-      <c r="I80" s="67"/>
-      <c r="J80" s="67"/>
-    </row>
-    <row r="81" spans="1:10">
-      <c r="A81" s="132"/>
-      <c r="B81" s="27">
-        <v>41646</v>
       </c>
       <c r="C81" s="69"/>
       <c r="D81" s="69"/>
@@ -4211,9 +4230,9 @@
       <c r="J81" s="67"/>
     </row>
     <row r="82" spans="1:10">
-      <c r="A82" s="132"/>
+      <c r="A82" s="81"/>
       <c r="B82" s="27">
-        <v>41647</v>
+        <v>41646</v>
       </c>
       <c r="C82" s="69"/>
       <c r="D82" s="69"/>
@@ -4228,9 +4247,9 @@
       <c r="J82" s="67"/>
     </row>
     <row r="83" spans="1:10">
-      <c r="A83" s="132"/>
+      <c r="A83" s="81"/>
       <c r="B83" s="27">
-        <v>41648</v>
+        <v>41647</v>
       </c>
       <c r="C83" s="69"/>
       <c r="D83" s="69"/>
@@ -4245,9 +4264,9 @@
       <c r="J83" s="67"/>
     </row>
     <row r="84" spans="1:10">
-      <c r="A84" s="133"/>
+      <c r="A84" s="81"/>
       <c r="B84" s="27">
-        <v>41649</v>
+        <v>41648</v>
       </c>
       <c r="C84" s="69"/>
       <c r="D84" s="69"/>
@@ -4262,28 +4281,28 @@
       <c r="J84" s="67"/>
     </row>
     <row r="85" spans="1:10">
-      <c r="A85" s="141">
+      <c r="A85" s="82"/>
+      <c r="B85" s="27">
+        <v>41649</v>
+      </c>
+      <c r="C85" s="69"/>
+      <c r="D85" s="69"/>
+      <c r="E85" s="69"/>
+      <c r="F85" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G85" s="67"/>
+      <c r="H85" s="67"/>
+      <c r="I85" s="67"/>
+      <c r="J85" s="67"/>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" s="83">
         <v>11</v>
       </c>
-      <c r="B85" s="26">
+      <c r="B86" s="26">
         <v>41652</v>
-      </c>
-      <c r="C85" s="55"/>
-      <c r="D85" s="55"/>
-      <c r="E85" s="55"/>
-      <c r="F85" s="55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G85" s="29"/>
-      <c r="H85" s="29"/>
-      <c r="I85" s="29"/>
-      <c r="J85" s="29"/>
-    </row>
-    <row r="86" spans="1:10">
-      <c r="A86" s="142"/>
-      <c r="B86" s="26">
-        <v>41653</v>
       </c>
       <c r="C86" s="55"/>
       <c r="D86" s="55"/>
@@ -4298,9 +4317,9 @@
       <c r="J86" s="29"/>
     </row>
     <row r="87" spans="1:10">
-      <c r="A87" s="142"/>
+      <c r="A87" s="84"/>
       <c r="B87" s="26">
-        <v>41654</v>
+        <v>41653</v>
       </c>
       <c r="C87" s="55"/>
       <c r="D87" s="55"/>
@@ -4314,10 +4333,10 @@
       <c r="I87" s="29"/>
       <c r="J87" s="29"/>
     </row>
-    <row r="88" spans="1:10">
-      <c r="A88" s="142"/>
+    <row r="88" spans="1:10" ht="409.6">
+      <c r="A88" s="84"/>
       <c r="B88" s="26">
-        <v>41655</v>
+        <v>41654</v>
       </c>
       <c r="C88" s="55"/>
       <c r="D88" s="55"/>
@@ -4332,9 +4351,9 @@
       <c r="J88" s="29"/>
     </row>
     <row r="89" spans="1:10">
-      <c r="A89" s="136"/>
+      <c r="A89" s="84"/>
       <c r="B89" s="26">
-        <v>41656</v>
+        <v>41655</v>
       </c>
       <c r="C89" s="55"/>
       <c r="D89" s="55"/>
@@ -4349,28 +4368,28 @@
       <c r="J89" s="29"/>
     </row>
     <row r="90" spans="1:10">
-      <c r="A90" s="131">
+      <c r="A90" s="85"/>
+      <c r="B90" s="26">
+        <v>41656</v>
+      </c>
+      <c r="C90" s="55"/>
+      <c r="D90" s="55"/>
+      <c r="E90" s="55"/>
+      <c r="F90" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G90" s="29"/>
+      <c r="H90" s="29"/>
+      <c r="I90" s="29"/>
+      <c r="J90" s="29"/>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="80">
         <v>12</v>
       </c>
-      <c r="B90" s="27">
+      <c r="B91" s="27">
         <v>41659</v>
-      </c>
-      <c r="C90" s="69"/>
-      <c r="D90" s="69"/>
-      <c r="E90" s="69"/>
-      <c r="F90" s="69">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G90" s="67"/>
-      <c r="H90" s="67"/>
-      <c r="I90" s="67"/>
-      <c r="J90" s="67"/>
-    </row>
-    <row r="91" spans="1:10">
-      <c r="A91" s="132"/>
-      <c r="B91" s="27">
-        <v>41660</v>
       </c>
       <c r="C91" s="69"/>
       <c r="D91" s="69"/>
@@ -4385,9 +4404,9 @@
       <c r="J91" s="67"/>
     </row>
     <row r="92" spans="1:10">
-      <c r="A92" s="132"/>
+      <c r="A92" s="81"/>
       <c r="B92" s="27">
-        <v>41661</v>
+        <v>41660</v>
       </c>
       <c r="C92" s="69"/>
       <c r="D92" s="69"/>
@@ -4402,9 +4421,9 @@
       <c r="J92" s="67"/>
     </row>
     <row r="93" spans="1:10">
-      <c r="A93" s="132"/>
+      <c r="A93" s="81"/>
       <c r="B93" s="27">
-        <v>41662</v>
+        <v>41661</v>
       </c>
       <c r="C93" s="69"/>
       <c r="D93" s="69"/>
@@ -4419,9 +4438,9 @@
       <c r="J93" s="67"/>
     </row>
     <row r="94" spans="1:10">
-      <c r="A94" s="133"/>
+      <c r="A94" s="81"/>
       <c r="B94" s="27">
-        <v>41663</v>
+        <v>41662</v>
       </c>
       <c r="C94" s="69"/>
       <c r="D94" s="69"/>
@@ -4436,30 +4455,28 @@
       <c r="J94" s="67"/>
     </row>
     <row r="95" spans="1:10">
-      <c r="A95" s="141">
+      <c r="A95" s="82"/>
+      <c r="B95" s="27">
+        <v>41663</v>
+      </c>
+      <c r="C95" s="69"/>
+      <c r="D95" s="69"/>
+      <c r="E95" s="69"/>
+      <c r="F95" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G95" s="67"/>
+      <c r="H95" s="67"/>
+      <c r="I95" s="67"/>
+      <c r="J95" s="67"/>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" s="83">
         <v>13</v>
       </c>
-      <c r="B95" s="26">
+      <c r="B96" s="26">
         <v>41666</v>
-      </c>
-      <c r="C95" s="55"/>
-      <c r="D95" s="55"/>
-      <c r="E95" s="55"/>
-      <c r="F95" s="55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G95" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="H95" s="29"/>
-      <c r="I95" s="29"/>
-      <c r="J95" s="29"/>
-    </row>
-    <row r="96" spans="1:10">
-      <c r="A96" s="142"/>
-      <c r="B96" s="26">
-        <v>41667</v>
       </c>
       <c r="C96" s="55"/>
       <c r="D96" s="55"/>
@@ -4476,9 +4493,9 @@
       <c r="J96" s="29"/>
     </row>
     <row r="97" spans="1:10">
-      <c r="A97" s="142"/>
+      <c r="A97" s="84"/>
       <c r="B97" s="26">
-        <v>41668</v>
+        <v>41667</v>
       </c>
       <c r="C97" s="55"/>
       <c r="D97" s="55"/>
@@ -4495,9 +4512,9 @@
       <c r="J97" s="29"/>
     </row>
     <row r="98" spans="1:10">
-      <c r="A98" s="142"/>
+      <c r="A98" s="84"/>
       <c r="B98" s="26">
-        <v>41669</v>
+        <v>41668</v>
       </c>
       <c r="C98" s="55"/>
       <c r="D98" s="55"/>
@@ -4514,9 +4531,9 @@
       <c r="J98" s="29"/>
     </row>
     <row r="99" spans="1:10">
-      <c r="A99" s="136"/>
+      <c r="A99" s="84"/>
       <c r="B99" s="26">
-        <v>41670</v>
+        <v>41669</v>
       </c>
       <c r="C99" s="55"/>
       <c r="D99" s="55"/>
@@ -4533,30 +4550,30 @@
       <c r="J99" s="29"/>
     </row>
     <row r="100" spans="1:10">
-      <c r="A100" s="131">
+      <c r="A100" s="85"/>
+      <c r="B100" s="26">
+        <v>41670</v>
+      </c>
+      <c r="C100" s="55"/>
+      <c r="D100" s="55"/>
+      <c r="E100" s="55"/>
+      <c r="F100" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G100" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="H100" s="29"/>
+      <c r="I100" s="29"/>
+      <c r="J100" s="29"/>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="80">
         <v>14</v>
       </c>
-      <c r="B100" s="27">
+      <c r="B101" s="27">
         <v>41673</v>
-      </c>
-      <c r="C100" s="69"/>
-      <c r="D100" s="69"/>
-      <c r="E100" s="69"/>
-      <c r="F100" s="69">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G100" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="H100" s="67"/>
-      <c r="I100" s="67"/>
-      <c r="J100" s="67"/>
-    </row>
-    <row r="101" spans="1:10">
-      <c r="A101" s="132"/>
-      <c r="B101" s="27">
-        <v>41674</v>
       </c>
       <c r="C101" s="69"/>
       <c r="D101" s="69"/>
@@ -4573,9 +4590,9 @@
       <c r="J101" s="67"/>
     </row>
     <row r="102" spans="1:10">
-      <c r="A102" s="132"/>
+      <c r="A102" s="81"/>
       <c r="B102" s="27">
-        <v>41675</v>
+        <v>41674</v>
       </c>
       <c r="C102" s="69"/>
       <c r="D102" s="69"/>
@@ -4592,9 +4609,9 @@
       <c r="J102" s="67"/>
     </row>
     <row r="103" spans="1:10">
-      <c r="A103" s="132"/>
+      <c r="A103" s="81"/>
       <c r="B103" s="27">
-        <v>41676</v>
+        <v>41675</v>
       </c>
       <c r="C103" s="69"/>
       <c r="D103" s="69"/>
@@ -4611,9 +4628,9 @@
       <c r="J103" s="67"/>
     </row>
     <row r="104" spans="1:10">
-      <c r="A104" s="133"/>
+      <c r="A104" s="81"/>
       <c r="B104" s="27">
-        <v>41677</v>
+        <v>41676</v>
       </c>
       <c r="C104" s="69"/>
       <c r="D104" s="69"/>
@@ -4630,28 +4647,30 @@
       <c r="J104" s="67"/>
     </row>
     <row r="105" spans="1:10">
-      <c r="A105" s="141">
+      <c r="A105" s="82"/>
+      <c r="B105" s="27">
+        <v>41677</v>
+      </c>
+      <c r="C105" s="69"/>
+      <c r="D105" s="69"/>
+      <c r="E105" s="69"/>
+      <c r="F105" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G105" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="H105" s="67"/>
+      <c r="I105" s="67"/>
+      <c r="J105" s="67"/>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106" s="83">
         <v>15</v>
       </c>
-      <c r="B105" s="26">
+      <c r="B106" s="26">
         <v>41680</v>
-      </c>
-      <c r="C105" s="55"/>
-      <c r="D105" s="55"/>
-      <c r="E105" s="55"/>
-      <c r="F105" s="55">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G105" s="29"/>
-      <c r="H105" s="29"/>
-      <c r="I105" s="29"/>
-      <c r="J105" s="29"/>
-    </row>
-    <row r="106" spans="1:10">
-      <c r="A106" s="142"/>
-      <c r="B106" s="26">
-        <v>41681</v>
       </c>
       <c r="C106" s="55"/>
       <c r="D106" s="55"/>
@@ -4666,9 +4685,9 @@
       <c r="J106" s="29"/>
     </row>
     <row r="107" spans="1:10">
-      <c r="A107" s="142"/>
+      <c r="A107" s="84"/>
       <c r="B107" s="26">
-        <v>41682</v>
+        <v>41681</v>
       </c>
       <c r="C107" s="55"/>
       <c r="D107" s="55"/>
@@ -4683,9 +4702,9 @@
       <c r="J107" s="29"/>
     </row>
     <row r="108" spans="1:10">
-      <c r="A108" s="142"/>
+      <c r="A108" s="84"/>
       <c r="B108" s="26">
-        <v>41683</v>
+        <v>41682</v>
       </c>
       <c r="C108" s="55"/>
       <c r="D108" s="55"/>
@@ -4700,15 +4719,15 @@
       <c r="J108" s="29"/>
     </row>
     <row r="109" spans="1:10">
-      <c r="A109" s="136"/>
+      <c r="A109" s="84"/>
       <c r="B109" s="26">
-        <v>41684</v>
+        <v>41683</v>
       </c>
       <c r="C109" s="55"/>
       <c r="D109" s="55"/>
       <c r="E109" s="55"/>
       <c r="F109" s="55">
-        <f t="shared" ref="F109:F140" si="2">E109</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G109" s="29"/>
@@ -4717,28 +4736,28 @@
       <c r="J109" s="29"/>
     </row>
     <row r="110" spans="1:10">
-      <c r="A110" s="131">
+      <c r="A110" s="85"/>
+      <c r="B110" s="26">
+        <v>41684</v>
+      </c>
+      <c r="C110" s="55"/>
+      <c r="D110" s="55"/>
+      <c r="E110" s="55"/>
+      <c r="F110" s="55">
+        <f t="shared" ref="F110:F141" si="2">E110</f>
+        <v>0</v>
+      </c>
+      <c r="G110" s="29"/>
+      <c r="H110" s="29"/>
+      <c r="I110" s="29"/>
+      <c r="J110" s="29"/>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="A111" s="80">
         <v>16</v>
       </c>
-      <c r="B110" s="27">
+      <c r="B111" s="27">
         <v>41687</v>
-      </c>
-      <c r="C110" s="69"/>
-      <c r="D110" s="69"/>
-      <c r="E110" s="69"/>
-      <c r="F110" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G110" s="67"/>
-      <c r="H110" s="67"/>
-      <c r="I110" s="67"/>
-      <c r="J110" s="67"/>
-    </row>
-    <row r="111" spans="1:10">
-      <c r="A111" s="132"/>
-      <c r="B111" s="27">
-        <v>41688</v>
       </c>
       <c r="C111" s="69"/>
       <c r="D111" s="69"/>
@@ -4753,9 +4772,9 @@
       <c r="J111" s="67"/>
     </row>
     <row r="112" spans="1:10">
-      <c r="A112" s="132"/>
+      <c r="A112" s="81"/>
       <c r="B112" s="27">
-        <v>41689</v>
+        <v>41688</v>
       </c>
       <c r="C112" s="69"/>
       <c r="D112" s="69"/>
@@ -4770,9 +4789,9 @@
       <c r="J112" s="67"/>
     </row>
     <row r="113" spans="1:10">
-      <c r="A113" s="132"/>
+      <c r="A113" s="81"/>
       <c r="B113" s="27">
-        <v>41690</v>
+        <v>41689</v>
       </c>
       <c r="C113" s="69"/>
       <c r="D113" s="69"/>
@@ -4787,9 +4806,9 @@
       <c r="J113" s="67"/>
     </row>
     <row r="114" spans="1:10">
-      <c r="A114" s="133"/>
+      <c r="A114" s="81"/>
       <c r="B114" s="27">
-        <v>41691</v>
+        <v>41690</v>
       </c>
       <c r="C114" s="69"/>
       <c r="D114" s="69"/>
@@ -4804,28 +4823,28 @@
       <c r="J114" s="67"/>
     </row>
     <row r="115" spans="1:10">
-      <c r="A115" s="141">
+      <c r="A115" s="82"/>
+      <c r="B115" s="27">
+        <v>41691</v>
+      </c>
+      <c r="C115" s="69"/>
+      <c r="D115" s="69"/>
+      <c r="E115" s="69"/>
+      <c r="F115" s="69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G115" s="67"/>
+      <c r="H115" s="67"/>
+      <c r="I115" s="67"/>
+      <c r="J115" s="67"/>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" s="83">
         <v>17</v>
       </c>
-      <c r="B115" s="26">
+      <c r="B116" s="26">
         <v>41694</v>
-      </c>
-      <c r="C115" s="55"/>
-      <c r="D115" s="55"/>
-      <c r="E115" s="55"/>
-      <c r="F115" s="55">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G115" s="29"/>
-      <c r="H115" s="29"/>
-      <c r="I115" s="29"/>
-      <c r="J115" s="29"/>
-    </row>
-    <row r="116" spans="1:10">
-      <c r="A116" s="142"/>
-      <c r="B116" s="26">
-        <v>41695</v>
       </c>
       <c r="C116" s="55"/>
       <c r="D116" s="55"/>
@@ -4840,9 +4859,9 @@
       <c r="J116" s="29"/>
     </row>
     <row r="117" spans="1:10">
-      <c r="A117" s="142"/>
+      <c r="A117" s="84"/>
       <c r="B117" s="26">
-        <v>41696</v>
+        <v>41695</v>
       </c>
       <c r="C117" s="55"/>
       <c r="D117" s="55"/>
@@ -4857,9 +4876,9 @@
       <c r="J117" s="29"/>
     </row>
     <row r="118" spans="1:10">
-      <c r="A118" s="142"/>
+      <c r="A118" s="84"/>
       <c r="B118" s="26">
-        <v>41697</v>
+        <v>41696</v>
       </c>
       <c r="C118" s="55"/>
       <c r="D118" s="55"/>
@@ -4874,9 +4893,9 @@
       <c r="J118" s="29"/>
     </row>
     <row r="119" spans="1:10">
-      <c r="A119" s="136"/>
+      <c r="A119" s="84"/>
       <c r="B119" s="26">
-        <v>41698</v>
+        <v>41697</v>
       </c>
       <c r="C119" s="55"/>
       <c r="D119" s="55"/>
@@ -4891,28 +4910,28 @@
       <c r="J119" s="29"/>
     </row>
     <row r="120" spans="1:10">
-      <c r="A120" s="131">
+      <c r="A120" s="85"/>
+      <c r="B120" s="26">
+        <v>41698</v>
+      </c>
+      <c r="C120" s="55"/>
+      <c r="D120" s="55"/>
+      <c r="E120" s="55"/>
+      <c r="F120" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G120" s="29"/>
+      <c r="H120" s="29"/>
+      <c r="I120" s="29"/>
+      <c r="J120" s="29"/>
+    </row>
+    <row r="121" spans="1:10">
+      <c r="A121" s="80">
         <v>18</v>
       </c>
-      <c r="B120" s="27">
+      <c r="B121" s="27">
         <v>41701</v>
-      </c>
-      <c r="C120" s="69"/>
-      <c r="D120" s="69"/>
-      <c r="E120" s="69"/>
-      <c r="F120" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G120" s="67"/>
-      <c r="H120" s="67"/>
-      <c r="I120" s="67"/>
-      <c r="J120" s="67"/>
-    </row>
-    <row r="121" spans="1:10">
-      <c r="A121" s="132"/>
-      <c r="B121" s="27">
-        <v>41702</v>
       </c>
       <c r="C121" s="69"/>
       <c r="D121" s="69"/>
@@ -4927,9 +4946,9 @@
       <c r="J121" s="67"/>
     </row>
     <row r="122" spans="1:10">
-      <c r="A122" s="132"/>
+      <c r="A122" s="81"/>
       <c r="B122" s="27">
-        <v>41703</v>
+        <v>41702</v>
       </c>
       <c r="C122" s="69"/>
       <c r="D122" s="69"/>
@@ -4944,9 +4963,9 @@
       <c r="J122" s="67"/>
     </row>
     <row r="123" spans="1:10">
-      <c r="A123" s="132"/>
+      <c r="A123" s="81"/>
       <c r="B123" s="27">
-        <v>41704</v>
+        <v>41703</v>
       </c>
       <c r="C123" s="69"/>
       <c r="D123" s="69"/>
@@ -4961,9 +4980,9 @@
       <c r="J123" s="67"/>
     </row>
     <row r="124" spans="1:10">
-      <c r="A124" s="133"/>
+      <c r="A124" s="81"/>
       <c r="B124" s="27">
-        <v>41705</v>
+        <v>41704</v>
       </c>
       <c r="C124" s="69"/>
       <c r="D124" s="69"/>
@@ -4978,28 +4997,28 @@
       <c r="J124" s="67"/>
     </row>
     <row r="125" spans="1:10">
-      <c r="A125" s="141">
+      <c r="A125" s="82"/>
+      <c r="B125" s="27">
+        <v>41705</v>
+      </c>
+      <c r="C125" s="69"/>
+      <c r="D125" s="69"/>
+      <c r="E125" s="69"/>
+      <c r="F125" s="69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G125" s="67"/>
+      <c r="H125" s="67"/>
+      <c r="I125" s="67"/>
+      <c r="J125" s="67"/>
+    </row>
+    <row r="126" spans="1:10">
+      <c r="A126" s="83">
         <v>19</v>
       </c>
-      <c r="B125" s="26">
+      <c r="B126" s="26">
         <v>41708</v>
-      </c>
-      <c r="C125" s="55"/>
-      <c r="D125" s="55"/>
-      <c r="E125" s="55"/>
-      <c r="F125" s="55">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G125" s="29"/>
-      <c r="H125" s="29"/>
-      <c r="I125" s="29"/>
-      <c r="J125" s="29"/>
-    </row>
-    <row r="126" spans="1:10">
-      <c r="A126" s="142"/>
-      <c r="B126" s="26">
-        <v>41709</v>
       </c>
       <c r="C126" s="55"/>
       <c r="D126" s="55"/>
@@ -5014,9 +5033,9 @@
       <c r="J126" s="29"/>
     </row>
     <row r="127" spans="1:10">
-      <c r="A127" s="142"/>
+      <c r="A127" s="84"/>
       <c r="B127" s="26">
-        <v>41710</v>
+        <v>41709</v>
       </c>
       <c r="C127" s="55"/>
       <c r="D127" s="55"/>
@@ -5031,9 +5050,9 @@
       <c r="J127" s="29"/>
     </row>
     <row r="128" spans="1:10">
-      <c r="A128" s="142"/>
+      <c r="A128" s="84"/>
       <c r="B128" s="26">
-        <v>41711</v>
+        <v>41710</v>
       </c>
       <c r="C128" s="55"/>
       <c r="D128" s="55"/>
@@ -5048,9 +5067,9 @@
       <c r="J128" s="29"/>
     </row>
     <row r="129" spans="1:10">
-      <c r="A129" s="136"/>
+      <c r="A129" s="84"/>
       <c r="B129" s="26">
-        <v>41712</v>
+        <v>41711</v>
       </c>
       <c r="C129" s="55"/>
       <c r="D129" s="55"/>
@@ -5065,28 +5084,28 @@
       <c r="J129" s="29"/>
     </row>
     <row r="130" spans="1:10">
-      <c r="A130" s="131">
+      <c r="A130" s="85"/>
+      <c r="B130" s="26">
+        <v>41712</v>
+      </c>
+      <c r="C130" s="55"/>
+      <c r="D130" s="55"/>
+      <c r="E130" s="55"/>
+      <c r="F130" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G130" s="29"/>
+      <c r="H130" s="29"/>
+      <c r="I130" s="29"/>
+      <c r="J130" s="29"/>
+    </row>
+    <row r="131" spans="1:10">
+      <c r="A131" s="80">
         <v>20</v>
       </c>
-      <c r="B130" s="27">
+      <c r="B131" s="27">
         <v>41715</v>
-      </c>
-      <c r="C130" s="69"/>
-      <c r="D130" s="69"/>
-      <c r="E130" s="69"/>
-      <c r="F130" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G130" s="67"/>
-      <c r="H130" s="67"/>
-      <c r="I130" s="67"/>
-      <c r="J130" s="67"/>
-    </row>
-    <row r="131" spans="1:10">
-      <c r="A131" s="132"/>
-      <c r="B131" s="27">
-        <v>41716</v>
       </c>
       <c r="C131" s="69"/>
       <c r="D131" s="69"/>
@@ -5101,9 +5120,9 @@
       <c r="J131" s="67"/>
     </row>
     <row r="132" spans="1:10">
-      <c r="A132" s="132"/>
+      <c r="A132" s="81"/>
       <c r="B132" s="27">
-        <v>41717</v>
+        <v>41716</v>
       </c>
       <c r="C132" s="69"/>
       <c r="D132" s="69"/>
@@ -5118,9 +5137,9 @@
       <c r="J132" s="67"/>
     </row>
     <row r="133" spans="1:10">
-      <c r="A133" s="132"/>
+      <c r="A133" s="81"/>
       <c r="B133" s="27">
-        <v>41718</v>
+        <v>41717</v>
       </c>
       <c r="C133" s="69"/>
       <c r="D133" s="69"/>
@@ -5135,9 +5154,9 @@
       <c r="J133" s="67"/>
     </row>
     <row r="134" spans="1:10">
-      <c r="A134" s="133"/>
+      <c r="A134" s="81"/>
       <c r="B134" s="27">
-        <v>41719</v>
+        <v>41718</v>
       </c>
       <c r="C134" s="69"/>
       <c r="D134" s="69"/>
@@ -5152,28 +5171,28 @@
       <c r="J134" s="67"/>
     </row>
     <row r="135" spans="1:10">
-      <c r="A135" s="141">
+      <c r="A135" s="82"/>
+      <c r="B135" s="27">
+        <v>41719</v>
+      </c>
+      <c r="C135" s="69"/>
+      <c r="D135" s="69"/>
+      <c r="E135" s="69"/>
+      <c r="F135" s="69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G135" s="67"/>
+      <c r="H135" s="67"/>
+      <c r="I135" s="67"/>
+      <c r="J135" s="67"/>
+    </row>
+    <row r="136" spans="1:10">
+      <c r="A136" s="83">
         <v>21</v>
       </c>
-      <c r="B135" s="26">
+      <c r="B136" s="26">
         <v>41722</v>
-      </c>
-      <c r="C135" s="55"/>
-      <c r="D135" s="55"/>
-      <c r="E135" s="55"/>
-      <c r="F135" s="55">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G135" s="29"/>
-      <c r="H135" s="29"/>
-      <c r="I135" s="29"/>
-      <c r="J135" s="29"/>
-    </row>
-    <row r="136" spans="1:10">
-      <c r="A136" s="142"/>
-      <c r="B136" s="26">
-        <v>41723</v>
       </c>
       <c r="C136" s="55"/>
       <c r="D136" s="55"/>
@@ -5188,9 +5207,9 @@
       <c r="J136" s="29"/>
     </row>
     <row r="137" spans="1:10">
-      <c r="A137" s="142"/>
+      <c r="A137" s="84"/>
       <c r="B137" s="26">
-        <v>41724</v>
+        <v>41723</v>
       </c>
       <c r="C137" s="55"/>
       <c r="D137" s="55"/>
@@ -5205,9 +5224,9 @@
       <c r="J137" s="29"/>
     </row>
     <row r="138" spans="1:10">
-      <c r="A138" s="142"/>
+      <c r="A138" s="84"/>
       <c r="B138" s="26">
-        <v>41725</v>
+        <v>41724</v>
       </c>
       <c r="C138" s="55"/>
       <c r="D138" s="55"/>
@@ -5222,9 +5241,9 @@
       <c r="J138" s="29"/>
     </row>
     <row r="139" spans="1:10">
-      <c r="A139" s="136"/>
+      <c r="A139" s="84"/>
       <c r="B139" s="26">
-        <v>41726</v>
+        <v>41725</v>
       </c>
       <c r="C139" s="55"/>
       <c r="D139" s="55"/>
@@ -5239,34 +5258,34 @@
       <c r="J139" s="29"/>
     </row>
     <row r="140" spans="1:10">
-      <c r="A140" s="131">
+      <c r="A140" s="85"/>
+      <c r="B140" s="26">
+        <v>41726</v>
+      </c>
+      <c r="C140" s="55"/>
+      <c r="D140" s="55"/>
+      <c r="E140" s="55"/>
+      <c r="F140" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G140" s="29"/>
+      <c r="H140" s="29"/>
+      <c r="I140" s="29"/>
+      <c r="J140" s="29"/>
+    </row>
+    <row r="141" spans="1:10">
+      <c r="A141" s="80">
         <v>22</v>
       </c>
-      <c r="B140" s="27">
+      <c r="B141" s="27">
         <v>41729</v>
-      </c>
-      <c r="C140" s="69"/>
-      <c r="D140" s="69"/>
-      <c r="E140" s="69"/>
-      <c r="F140" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G140" s="67"/>
-      <c r="H140" s="67"/>
-      <c r="I140" s="67"/>
-      <c r="J140" s="67"/>
-    </row>
-    <row r="141" spans="1:10">
-      <c r="A141" s="132"/>
-      <c r="B141" s="27">
-        <v>41730</v>
       </c>
       <c r="C141" s="69"/>
       <c r="D141" s="69"/>
       <c r="E141" s="69"/>
       <c r="F141" s="69">
-        <f t="shared" ref="F141:F172" si="3">E141</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G141" s="67"/>
@@ -5275,15 +5294,15 @@
       <c r="J141" s="67"/>
     </row>
     <row r="142" spans="1:10">
-      <c r="A142" s="132"/>
+      <c r="A142" s="81"/>
       <c r="B142" s="27">
-        <v>41731</v>
+        <v>41730</v>
       </c>
       <c r="C142" s="69"/>
       <c r="D142" s="69"/>
       <c r="E142" s="69"/>
       <c r="F142" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F142:F173" si="3">E142</f>
         <v>0</v>
       </c>
       <c r="G142" s="67"/>
@@ -5292,9 +5311,9 @@
       <c r="J142" s="67"/>
     </row>
     <row r="143" spans="1:10">
-      <c r="A143" s="132"/>
+      <c r="A143" s="81"/>
       <c r="B143" s="27">
-        <v>41732</v>
+        <v>41731</v>
       </c>
       <c r="C143" s="69"/>
       <c r="D143" s="69"/>
@@ -5309,9 +5328,9 @@
       <c r="J143" s="67"/>
     </row>
     <row r="144" spans="1:10">
-      <c r="A144" s="133"/>
+      <c r="A144" s="81"/>
       <c r="B144" s="27">
-        <v>41733</v>
+        <v>41732</v>
       </c>
       <c r="C144" s="69"/>
       <c r="D144" s="69"/>
@@ -5326,28 +5345,28 @@
       <c r="J144" s="67"/>
     </row>
     <row r="145" spans="1:10">
-      <c r="A145" s="141">
+      <c r="A145" s="82"/>
+      <c r="B145" s="27">
+        <v>41733</v>
+      </c>
+      <c r="C145" s="69"/>
+      <c r="D145" s="69"/>
+      <c r="E145" s="69"/>
+      <c r="F145" s="69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G145" s="67"/>
+      <c r="H145" s="67"/>
+      <c r="I145" s="67"/>
+      <c r="J145" s="67"/>
+    </row>
+    <row r="146" spans="1:10">
+      <c r="A146" s="83">
         <v>23</v>
       </c>
-      <c r="B145" s="26">
+      <c r="B146" s="26">
         <v>41736</v>
-      </c>
-      <c r="C145" s="55"/>
-      <c r="D145" s="55"/>
-      <c r="E145" s="55"/>
-      <c r="F145" s="55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G145" s="29"/>
-      <c r="H145" s="29"/>
-      <c r="I145" s="29"/>
-      <c r="J145" s="29"/>
-    </row>
-    <row r="146" spans="1:10">
-      <c r="A146" s="142"/>
-      <c r="B146" s="26">
-        <v>41737</v>
       </c>
       <c r="C146" s="55"/>
       <c r="D146" s="55"/>
@@ -5362,9 +5381,9 @@
       <c r="J146" s="29"/>
     </row>
     <row r="147" spans="1:10">
-      <c r="A147" s="142"/>
+      <c r="A147" s="84"/>
       <c r="B147" s="26">
-        <v>41738</v>
+        <v>41737</v>
       </c>
       <c r="C147" s="55"/>
       <c r="D147" s="55"/>
@@ -5379,9 +5398,9 @@
       <c r="J147" s="29"/>
     </row>
     <row r="148" spans="1:10">
-      <c r="A148" s="142"/>
+      <c r="A148" s="84"/>
       <c r="B148" s="26">
-        <v>41739</v>
+        <v>41738</v>
       </c>
       <c r="C148" s="55"/>
       <c r="D148" s="55"/>
@@ -5396,9 +5415,9 @@
       <c r="J148" s="29"/>
     </row>
     <row r="149" spans="1:10">
-      <c r="A149" s="136"/>
+      <c r="A149" s="84"/>
       <c r="B149" s="26">
-        <v>41740</v>
+        <v>41739</v>
       </c>
       <c r="C149" s="55"/>
       <c r="D149" s="55"/>
@@ -5413,28 +5432,28 @@
       <c r="J149" s="29"/>
     </row>
     <row r="150" spans="1:10">
-      <c r="A150" s="131">
+      <c r="A150" s="85"/>
+      <c r="B150" s="26">
+        <v>41740</v>
+      </c>
+      <c r="C150" s="55"/>
+      <c r="D150" s="55"/>
+      <c r="E150" s="55"/>
+      <c r="F150" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G150" s="29"/>
+      <c r="H150" s="29"/>
+      <c r="I150" s="29"/>
+      <c r="J150" s="29"/>
+    </row>
+    <row r="151" spans="1:10">
+      <c r="A151" s="80">
         <v>24</v>
       </c>
-      <c r="B150" s="27">
+      <c r="B151" s="27">
         <v>41743</v>
-      </c>
-      <c r="C150" s="69"/>
-      <c r="D150" s="69"/>
-      <c r="E150" s="69"/>
-      <c r="F150" s="69">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G150" s="67"/>
-      <c r="H150" s="67"/>
-      <c r="I150" s="67"/>
-      <c r="J150" s="67"/>
-    </row>
-    <row r="151" spans="1:10">
-      <c r="A151" s="132"/>
-      <c r="B151" s="27">
-        <v>41744</v>
       </c>
       <c r="C151" s="69"/>
       <c r="D151" s="69"/>
@@ -5449,9 +5468,9 @@
       <c r="J151" s="67"/>
     </row>
     <row r="152" spans="1:10">
-      <c r="A152" s="132"/>
+      <c r="A152" s="81"/>
       <c r="B152" s="27">
-        <v>41745</v>
+        <v>41744</v>
       </c>
       <c r="C152" s="69"/>
       <c r="D152" s="69"/>
@@ -5466,9 +5485,9 @@
       <c r="J152" s="67"/>
     </row>
     <row r="153" spans="1:10">
-      <c r="A153" s="132"/>
+      <c r="A153" s="81"/>
       <c r="B153" s="27">
-        <v>41746</v>
+        <v>41745</v>
       </c>
       <c r="C153" s="69"/>
       <c r="D153" s="69"/>
@@ -5483,9 +5502,9 @@
       <c r="J153" s="67"/>
     </row>
     <row r="154" spans="1:10">
-      <c r="A154" s="133"/>
+      <c r="A154" s="81"/>
       <c r="B154" s="27">
-        <v>41747</v>
+        <v>41746</v>
       </c>
       <c r="C154" s="69"/>
       <c r="D154" s="69"/>
@@ -5500,28 +5519,28 @@
       <c r="J154" s="67"/>
     </row>
     <row r="155" spans="1:10">
-      <c r="A155" s="141">
+      <c r="A155" s="82"/>
+      <c r="B155" s="27">
+        <v>41747</v>
+      </c>
+      <c r="C155" s="69"/>
+      <c r="D155" s="69"/>
+      <c r="E155" s="69"/>
+      <c r="F155" s="69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G155" s="67"/>
+      <c r="H155" s="67"/>
+      <c r="I155" s="67"/>
+      <c r="J155" s="67"/>
+    </row>
+    <row r="156" spans="1:10">
+      <c r="A156" s="83">
         <v>25</v>
       </c>
-      <c r="B155" s="26">
+      <c r="B156" s="26">
         <v>41750</v>
-      </c>
-      <c r="C155" s="55"/>
-      <c r="D155" s="55"/>
-      <c r="E155" s="55"/>
-      <c r="F155" s="55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G155" s="29"/>
-      <c r="H155" s="29"/>
-      <c r="I155" s="29"/>
-      <c r="J155" s="29"/>
-    </row>
-    <row r="156" spans="1:10">
-      <c r="A156" s="142"/>
-      <c r="B156" s="26">
-        <v>41751</v>
       </c>
       <c r="C156" s="55"/>
       <c r="D156" s="55"/>
@@ -5536,9 +5555,9 @@
       <c r="J156" s="29"/>
     </row>
     <row r="157" spans="1:10">
-      <c r="A157" s="142"/>
+      <c r="A157" s="84"/>
       <c r="B157" s="26">
-        <v>41752</v>
+        <v>41751</v>
       </c>
       <c r="C157" s="55"/>
       <c r="D157" s="55"/>
@@ -5553,9 +5572,9 @@
       <c r="J157" s="29"/>
     </row>
     <row r="158" spans="1:10">
-      <c r="A158" s="142"/>
+      <c r="A158" s="84"/>
       <c r="B158" s="26">
-        <v>41753</v>
+        <v>41752</v>
       </c>
       <c r="C158" s="55"/>
       <c r="D158" s="55"/>
@@ -5570,9 +5589,9 @@
       <c r="J158" s="29"/>
     </row>
     <row r="159" spans="1:10">
-      <c r="A159" s="136"/>
+      <c r="A159" s="84"/>
       <c r="B159" s="26">
-        <v>41754</v>
+        <v>41753</v>
       </c>
       <c r="C159" s="55"/>
       <c r="D159" s="55"/>
@@ -5587,28 +5606,28 @@
       <c r="J159" s="29"/>
     </row>
     <row r="160" spans="1:10">
-      <c r="A160" s="131">
+      <c r="A160" s="85"/>
+      <c r="B160" s="26">
+        <v>41754</v>
+      </c>
+      <c r="C160" s="55"/>
+      <c r="D160" s="55"/>
+      <c r="E160" s="55"/>
+      <c r="F160" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G160" s="29"/>
+      <c r="H160" s="29"/>
+      <c r="I160" s="29"/>
+      <c r="J160" s="29"/>
+    </row>
+    <row r="161" spans="1:10">
+      <c r="A161" s="80">
         <v>26</v>
       </c>
-      <c r="B160" s="27">
+      <c r="B161" s="27">
         <v>41757</v>
-      </c>
-      <c r="C160" s="69"/>
-      <c r="D160" s="69"/>
-      <c r="E160" s="69"/>
-      <c r="F160" s="69">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G160" s="67"/>
-      <c r="H160" s="67"/>
-      <c r="I160" s="67"/>
-      <c r="J160" s="67"/>
-    </row>
-    <row r="161" spans="1:10">
-      <c r="A161" s="132"/>
-      <c r="B161" s="27">
-        <v>41758</v>
       </c>
       <c r="C161" s="69"/>
       <c r="D161" s="69"/>
@@ -5623,9 +5642,9 @@
       <c r="J161" s="67"/>
     </row>
     <row r="162" spans="1:10">
-      <c r="A162" s="132"/>
+      <c r="A162" s="81"/>
       <c r="B162" s="27">
-        <v>41759</v>
+        <v>41758</v>
       </c>
       <c r="C162" s="69"/>
       <c r="D162" s="69"/>
@@ -5640,9 +5659,9 @@
       <c r="J162" s="67"/>
     </row>
     <row r="163" spans="1:10">
-      <c r="A163" s="132"/>
+      <c r="A163" s="81"/>
       <c r="B163" s="27">
-        <v>41760</v>
+        <v>41759</v>
       </c>
       <c r="C163" s="69"/>
       <c r="D163" s="69"/>
@@ -5657,9 +5676,9 @@
       <c r="J163" s="67"/>
     </row>
     <row r="164" spans="1:10">
-      <c r="A164" s="133"/>
+      <c r="A164" s="81"/>
       <c r="B164" s="27">
-        <v>41761</v>
+        <v>41760</v>
       </c>
       <c r="C164" s="69"/>
       <c r="D164" s="69"/>
@@ -5674,28 +5693,28 @@
       <c r="J164" s="67"/>
     </row>
     <row r="165" spans="1:10">
-      <c r="A165" s="141">
+      <c r="A165" s="82"/>
+      <c r="B165" s="27">
+        <v>41761</v>
+      </c>
+      <c r="C165" s="69"/>
+      <c r="D165" s="69"/>
+      <c r="E165" s="69"/>
+      <c r="F165" s="69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G165" s="67"/>
+      <c r="H165" s="67"/>
+      <c r="I165" s="67"/>
+      <c r="J165" s="67"/>
+    </row>
+    <row r="166" spans="1:10">
+      <c r="A166" s="83">
         <v>27</v>
       </c>
-      <c r="B165" s="26">
+      <c r="B166" s="26">
         <v>41764</v>
-      </c>
-      <c r="C165" s="55"/>
-      <c r="D165" s="55"/>
-      <c r="E165" s="55"/>
-      <c r="F165" s="55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G165" s="29"/>
-      <c r="H165" s="29"/>
-      <c r="I165" s="29"/>
-      <c r="J165" s="29"/>
-    </row>
-    <row r="166" spans="1:10">
-      <c r="A166" s="142"/>
-      <c r="B166" s="26">
-        <v>41765</v>
       </c>
       <c r="C166" s="55"/>
       <c r="D166" s="55"/>
@@ -5710,9 +5729,9 @@
       <c r="J166" s="29"/>
     </row>
     <row r="167" spans="1:10">
-      <c r="A167" s="142"/>
+      <c r="A167" s="84"/>
       <c r="B167" s="26">
-        <v>41766</v>
+        <v>41765</v>
       </c>
       <c r="C167" s="55"/>
       <c r="D167" s="55"/>
@@ -5727,9 +5746,9 @@
       <c r="J167" s="29"/>
     </row>
     <row r="168" spans="1:10">
-      <c r="A168" s="142"/>
+      <c r="A168" s="84"/>
       <c r="B168" s="26">
-        <v>41767</v>
+        <v>41766</v>
       </c>
       <c r="C168" s="55"/>
       <c r="D168" s="55"/>
@@ -5744,9 +5763,9 @@
       <c r="J168" s="29"/>
     </row>
     <row r="169" spans="1:10">
-      <c r="A169" s="136"/>
+      <c r="A169" s="84"/>
       <c r="B169" s="26">
-        <v>41768</v>
+        <v>41767</v>
       </c>
       <c r="C169" s="55"/>
       <c r="D169" s="55"/>
@@ -5761,28 +5780,28 @@
       <c r="J169" s="29"/>
     </row>
     <row r="170" spans="1:10">
-      <c r="A170" s="131">
+      <c r="A170" s="85"/>
+      <c r="B170" s="26">
+        <v>41768</v>
+      </c>
+      <c r="C170" s="55"/>
+      <c r="D170" s="55"/>
+      <c r="E170" s="55"/>
+      <c r="F170" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G170" s="29"/>
+      <c r="H170" s="29"/>
+      <c r="I170" s="29"/>
+      <c r="J170" s="29"/>
+    </row>
+    <row r="171" spans="1:10">
+      <c r="A171" s="80">
         <v>28</v>
       </c>
-      <c r="B170" s="27">
+      <c r="B171" s="27">
         <v>41771</v>
-      </c>
-      <c r="C170" s="69"/>
-      <c r="D170" s="69"/>
-      <c r="E170" s="69"/>
-      <c r="F170" s="69">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G170" s="67"/>
-      <c r="H170" s="67"/>
-      <c r="I170" s="67"/>
-      <c r="J170" s="67"/>
-    </row>
-    <row r="171" spans="1:10">
-      <c r="A171" s="132"/>
-      <c r="B171" s="27">
-        <v>41772</v>
       </c>
       <c r="C171" s="69"/>
       <c r="D171" s="69"/>
@@ -5797,9 +5816,9 @@
       <c r="J171" s="67"/>
     </row>
     <row r="172" spans="1:10">
-      <c r="A172" s="132"/>
+      <c r="A172" s="81"/>
       <c r="B172" s="27">
-        <v>41773</v>
+        <v>41772</v>
       </c>
       <c r="C172" s="69"/>
       <c r="D172" s="69"/>
@@ -5814,15 +5833,15 @@
       <c r="J172" s="67"/>
     </row>
     <row r="173" spans="1:10">
-      <c r="A173" s="132"/>
+      <c r="A173" s="81"/>
       <c r="B173" s="27">
-        <v>41774</v>
+        <v>41773</v>
       </c>
       <c r="C173" s="69"/>
       <c r="D173" s="69"/>
       <c r="E173" s="69"/>
       <c r="F173" s="69">
-        <f t="shared" ref="F173:F184" si="4">E173</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G173" s="67"/>
@@ -5831,15 +5850,15 @@
       <c r="J173" s="67"/>
     </row>
     <row r="174" spans="1:10">
-      <c r="A174" s="133"/>
+      <c r="A174" s="81"/>
       <c r="B174" s="27">
-        <v>41775</v>
+        <v>41774</v>
       </c>
       <c r="C174" s="69"/>
       <c r="D174" s="69"/>
       <c r="E174" s="69"/>
       <c r="F174" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F174:F185" si="4">E174</f>
         <v>0</v>
       </c>
       <c r="G174" s="67"/>
@@ -5848,28 +5867,28 @@
       <c r="J174" s="67"/>
     </row>
     <row r="175" spans="1:10">
-      <c r="A175" s="141">
+      <c r="A175" s="82"/>
+      <c r="B175" s="27">
+        <v>41775</v>
+      </c>
+      <c r="C175" s="69"/>
+      <c r="D175" s="69"/>
+      <c r="E175" s="69"/>
+      <c r="F175" s="69">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G175" s="67"/>
+      <c r="H175" s="67"/>
+      <c r="I175" s="67"/>
+      <c r="J175" s="67"/>
+    </row>
+    <row r="176" spans="1:10">
+      <c r="A176" s="83">
         <v>29</v>
       </c>
-      <c r="B175" s="26">
+      <c r="B176" s="26">
         <v>41778</v>
-      </c>
-      <c r="C175" s="55"/>
-      <c r="D175" s="55"/>
-      <c r="E175" s="55"/>
-      <c r="F175" s="55">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G175" s="29"/>
-      <c r="H175" s="29"/>
-      <c r="I175" s="29"/>
-      <c r="J175" s="29"/>
-    </row>
-    <row r="176" spans="1:10">
-      <c r="A176" s="142"/>
-      <c r="B176" s="26">
-        <v>41779</v>
       </c>
       <c r="C176" s="55"/>
       <c r="D176" s="55"/>
@@ -5884,9 +5903,9 @@
       <c r="J176" s="29"/>
     </row>
     <row r="177" spans="1:10">
-      <c r="A177" s="142"/>
+      <c r="A177" s="84"/>
       <c r="B177" s="26">
-        <v>41780</v>
+        <v>41779</v>
       </c>
       <c r="C177" s="55"/>
       <c r="D177" s="55"/>
@@ -5901,9 +5920,9 @@
       <c r="J177" s="29"/>
     </row>
     <row r="178" spans="1:10">
-      <c r="A178" s="142"/>
+      <c r="A178" s="84"/>
       <c r="B178" s="26">
-        <v>41781</v>
+        <v>41780</v>
       </c>
       <c r="C178" s="55"/>
       <c r="D178" s="55"/>
@@ -5918,9 +5937,9 @@
       <c r="J178" s="29"/>
     </row>
     <row r="179" spans="1:10">
-      <c r="A179" s="136"/>
+      <c r="A179" s="84"/>
       <c r="B179" s="26">
-        <v>41782</v>
+        <v>41781</v>
       </c>
       <c r="C179" s="55"/>
       <c r="D179" s="55"/>
@@ -5935,28 +5954,28 @@
       <c r="J179" s="29"/>
     </row>
     <row r="180" spans="1:10">
-      <c r="A180" s="143">
+      <c r="A180" s="85"/>
+      <c r="B180" s="26">
+        <v>41782</v>
+      </c>
+      <c r="C180" s="55"/>
+      <c r="D180" s="55"/>
+      <c r="E180" s="55"/>
+      <c r="F180" s="55">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G180" s="29"/>
+      <c r="H180" s="29"/>
+      <c r="I180" s="29"/>
+      <c r="J180" s="29"/>
+    </row>
+    <row r="181" spans="1:10">
+      <c r="A181" s="86">
         <v>30</v>
       </c>
-      <c r="B180" s="27">
+      <c r="B181" s="27">
         <v>41785</v>
-      </c>
-      <c r="C180" s="70"/>
-      <c r="D180" s="70"/>
-      <c r="E180" s="70"/>
-      <c r="F180" s="70">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G180" s="37"/>
-      <c r="H180" s="37"/>
-      <c r="I180" s="37"/>
-      <c r="J180" s="37"/>
-    </row>
-    <row r="181" spans="1:10">
-      <c r="A181" s="144"/>
-      <c r="B181" s="27">
-        <v>41786</v>
       </c>
       <c r="C181" s="70"/>
       <c r="D181" s="70"/>
@@ -5971,9 +5990,9 @@
       <c r="J181" s="37"/>
     </row>
     <row r="182" spans="1:10">
-      <c r="A182" s="144"/>
+      <c r="A182" s="87"/>
       <c r="B182" s="27">
-        <v>41787</v>
+        <v>41786</v>
       </c>
       <c r="C182" s="70"/>
       <c r="D182" s="70"/>
@@ -5988,9 +6007,9 @@
       <c r="J182" s="37"/>
     </row>
     <row r="183" spans="1:10">
-      <c r="A183" s="144"/>
+      <c r="A183" s="87"/>
       <c r="B183" s="27">
-        <v>41788</v>
+        <v>41787</v>
       </c>
       <c r="C183" s="70"/>
       <c r="D183" s="70"/>
@@ -6005,9 +6024,9 @@
       <c r="J183" s="37"/>
     </row>
     <row r="184" spans="1:10">
-      <c r="A184" s="145"/>
+      <c r="A184" s="87"/>
       <c r="B184" s="27">
-        <v>41789</v>
+        <v>41788</v>
       </c>
       <c r="C184" s="70"/>
       <c r="D184" s="70"/>
@@ -6022,16 +6041,21 @@
       <c r="J184" s="37"/>
     </row>
     <row r="185" spans="1:10">
-      <c r="A185" s="68"/>
-      <c r="B185" s="68"/>
-      <c r="C185" s="68"/>
-      <c r="D185" s="68"/>
-      <c r="E185" s="68"/>
-      <c r="F185" s="68"/>
-      <c r="G185" s="68"/>
-      <c r="H185" s="68"/>
-      <c r="I185" s="68"/>
-      <c r="J185" s="68"/>
+      <c r="A185" s="88"/>
+      <c r="B185" s="27">
+        <v>41789</v>
+      </c>
+      <c r="C185" s="70"/>
+      <c r="D185" s="70"/>
+      <c r="E185" s="70"/>
+      <c r="F185" s="70">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G185" s="37"/>
+      <c r="H185" s="37"/>
+      <c r="I185" s="37"/>
+      <c r="J185" s="37"/>
     </row>
     <row r="186" spans="1:10">
       <c r="A186" s="68"/>
@@ -6129,51 +6153,21 @@
       <c r="I193" s="68"/>
       <c r="J193" s="68"/>
     </row>
+    <row r="194" spans="1:10">
+      <c r="A194" s="68"/>
+      <c r="B194" s="68"/>
+      <c r="C194" s="68"/>
+      <c r="D194" s="68"/>
+      <c r="E194" s="68"/>
+      <c r="F194" s="68"/>
+      <c r="G194" s="68"/>
+      <c r="H194" s="68"/>
+      <c r="I194" s="68"/>
+      <c r="J194" s="68"/>
+    </row>
   </sheetData>
-  <mergeCells count="59">
-    <mergeCell ref="A170:A174"/>
-    <mergeCell ref="A175:A179"/>
-    <mergeCell ref="A180:A184"/>
-    <mergeCell ref="A140:A144"/>
-    <mergeCell ref="A145:A149"/>
-    <mergeCell ref="A150:A154"/>
-    <mergeCell ref="A155:A159"/>
-    <mergeCell ref="A160:A164"/>
-    <mergeCell ref="A60:A64"/>
-    <mergeCell ref="A65:A69"/>
-    <mergeCell ref="A47:A59"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="A165:A169"/>
-    <mergeCell ref="A120:A124"/>
-    <mergeCell ref="A125:A129"/>
-    <mergeCell ref="A130:A134"/>
-    <mergeCell ref="A135:A139"/>
-    <mergeCell ref="F48:F50"/>
-    <mergeCell ref="F51:F53"/>
-    <mergeCell ref="A105:A109"/>
-    <mergeCell ref="A110:A114"/>
-    <mergeCell ref="A115:A119"/>
-    <mergeCell ref="A90:A94"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="A75:A79"/>
-    <mergeCell ref="A85:A89"/>
-    <mergeCell ref="A80:A84"/>
-    <mergeCell ref="A95:A99"/>
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="A34:A46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="A19:A33"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="F31:F33"/>
+  <mergeCells count="60">
+    <mergeCell ref="F60:F61"/>
     <mergeCell ref="F54:F58"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="G2:N4"/>
@@ -6190,6 +6184,49 @@
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="A34:A46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="A86:A90"/>
+    <mergeCell ref="A81:A85"/>
+    <mergeCell ref="A96:A100"/>
+    <mergeCell ref="A101:A105"/>
+    <mergeCell ref="A60:A65"/>
+    <mergeCell ref="A66:A70"/>
+    <mergeCell ref="A47:A59"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A166:A170"/>
+    <mergeCell ref="A121:A125"/>
+    <mergeCell ref="A126:A130"/>
+    <mergeCell ref="A131:A135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="F48:F50"/>
+    <mergeCell ref="F51:F53"/>
+    <mergeCell ref="A106:A110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A120"/>
+    <mergeCell ref="A91:A95"/>
+    <mergeCell ref="A71:A75"/>
+    <mergeCell ref="A171:A175"/>
+    <mergeCell ref="A176:A180"/>
+    <mergeCell ref="A181:A185"/>
+    <mergeCell ref="A141:A145"/>
+    <mergeCell ref="A146:A150"/>
+    <mergeCell ref="A151:A155"/>
+    <mergeCell ref="A156:A160"/>
+    <mergeCell ref="A161:A165"/>
   </mergeCells>
   <conditionalFormatting sqref="M7">
     <cfRule type="cellIs" dxfId="3" priority="11" operator="greaterThan">
@@ -6573,29 +6610,10 @@
               <x14:cfIcon iconSet="3Symbols" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>M60</xm:sqref>
+          <xm:sqref>M60:M61</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="25" id="{E0DFC09D-C053-4D3D-A1C1-C5AF640FB5CD}">
-            <x14:iconSet custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>25</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num" gte="0">
-                <xm:f>168</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols" iconId="1"/>
-              <x14:cfIcon iconSet="3Symbols" iconId="2"/>
-              <x14:cfIcon iconSet="3Symbols" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>M61</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="24" id="{F1B6F2BC-B2AE-42D9-8427-52A717AE39CD}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6614,7 +6632,7 @@
           <xm:sqref>M62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="23" id="{EEF8AB81-584A-4839-AEE8-98BCAAB29DD2}">
+          <x14:cfRule type="iconSet" priority="24" id="{F1B6F2BC-B2AE-42D9-8427-52A717AE39CD}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6633,7 +6651,7 @@
           <xm:sqref>M63</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="22" id="{A1F90B4F-0784-43A3-A2A1-2A7C9438EE1A}">
+          <x14:cfRule type="iconSet" priority="23" id="{EEF8AB81-584A-4839-AEE8-98BCAAB29DD2}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6652,7 +6670,7 @@
           <xm:sqref>M64</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="21" id="{CDF48798-0C78-453D-9E98-93D1BB3C878A}">
+          <x14:cfRule type="iconSet" priority="22" id="{A1F90B4F-0784-43A3-A2A1-2A7C9438EE1A}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6671,7 +6689,7 @@
           <xm:sqref>M65</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="20" id="{524804E6-2BBA-4071-AB71-18BD193B4497}">
+          <x14:cfRule type="iconSet" priority="21" id="{CDF48798-0C78-453D-9E98-93D1BB3C878A}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6690,7 +6708,7 @@
           <xm:sqref>M66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="19" id="{F466D4E3-91DB-49AA-8E5A-7BD04BE8813F}">
+          <x14:cfRule type="iconSet" priority="20" id="{524804E6-2BBA-4071-AB71-18BD193B4497}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6707,6 +6725,25 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>M67</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="19" id="{F466D4E3-91DB-49AA-8E5A-7BD04BE8813F}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>25</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>168</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols" iconId="1"/>
+              <x14:cfIcon iconSet="3Symbols" iconId="2"/>
+              <x14:cfIcon iconSet="3Symbols" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>M68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="18" id="{C4227F9F-08CD-4A7C-B706-2C35F19616E7}">
@@ -6858,7 +6895,7 @@
               <x14:cfIcon iconSet="3Symbols" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>F14 F7:F8 F12 F18:F19 F21 F23:F24 F29 F34:F35 F39 F44:F45 F47 F51 F59:F184</xm:sqref>
+          <xm:sqref>F14 F7:F8 F12 F18:F19 F21 F23:F24 F29 F34:F35 F39 F44:F45 F47 F51 F59:F60 F62:F185</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="1" id="{D5E33E02-3F42-4321-B899-2604F055C762}">

</xml_diff>

<commit_message>
effort log 11/12/2013 - Khang
</commit_message>
<xml_diff>
--- a/1. Project management/9. Timelog/individual time log/AS_PM_TimeLog_DeadlineTeam_KhangHuynh.xlsx
+++ b/1. Project management/9. Timelog/individual time log/AS_PM_TimeLog_DeadlineTeam_KhangHuynh.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="191">
   <si>
     <t>Week</t>
   </si>
@@ -667,6 +667,18 @@
  + Use case "Hoi dap"
  + Quality Attribute
  + Business and Technical constraint</t>
+  </si>
+  <si>
+    <t>Training spring core
++ MySQL
++ Insert/Update/Delete</t>
+  </si>
+  <si>
+    <t>4:00PM</t>
+  </si>
+  <si>
+    <t>Create customer satisfaction survey report teamplate
+Create weekly report for week 7</t>
   </si>
 </sst>
 </file>
@@ -1208,10 +1220,184 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1220,9 +1406,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1231,177 +1414,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1713,7 +1725,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1724,7 +1736,7 @@
   <dimension ref="A3:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1839,10 +1851,10 @@
   <dimension ref="A1:O194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="6" topLeftCell="G60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="6" topLeftCell="G48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H61" sqref="H61"/>
+      <selection pane="bottomRight" activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1864,81 +1876,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="104"/>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="106"/>
+      <c r="A1" s="85"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="87"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="107" t="s">
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="108"/>
-      <c r="M2" s="108"/>
-      <c r="N2" s="109"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="90"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="124"/>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="125"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="111"/>
-      <c r="J3" s="111"/>
-      <c r="K3" s="111"/>
-      <c r="L3" s="111"/>
-      <c r="M3" s="111"/>
-      <c r="N3" s="112"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="93"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="126"/>
-      <c r="B4" s="127"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="127"/>
-      <c r="E4" s="127"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="113"/>
-      <c r="H4" s="114"/>
-      <c r="I4" s="114"/>
-      <c r="J4" s="114"/>
-      <c r="K4" s="114"/>
-      <c r="L4" s="114"/>
-      <c r="M4" s="114"/>
-      <c r="N4" s="115"/>
+      <c r="A4" s="107"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="95"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="96"/>
     </row>
     <row r="5" spans="1:15" ht="39" customHeight="1">
-      <c r="A5" s="133"/>
-      <c r="B5" s="134"/>
-      <c r="C5" s="134"/>
-      <c r="D5" s="134"/>
-      <c r="E5" s="135"/>
+      <c r="A5" s="114"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="116"/>
       <c r="F5" s="15"/>
       <c r="H5" s="41" t="s">
         <v>64</v>
@@ -1983,13 +1995,13 @@
       <c r="J6" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="100"/>
+      <c r="M6" s="100"/>
+      <c r="N6" s="100"/>
     </row>
     <row r="7" spans="1:15" ht="38.25">
-      <c r="A7" s="116">
+      <c r="A7" s="97">
         <v>1</v>
       </c>
       <c r="B7" s="16">
@@ -2015,10 +2027,10 @@
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="29"/>
-      <c r="K7" s="143" t="s">
+      <c r="K7" s="124" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="143"/>
+      <c r="L7" s="124"/>
       <c r="M7" s="32">
         <f>SUM(M8:M68)</f>
         <v>97.68</v>
@@ -2028,8 +2040,8 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="25.5">
-      <c r="A8" s="117"/>
-      <c r="B8" s="129">
+      <c r="A8" s="98"/>
+      <c r="B8" s="110">
         <v>41586</v>
       </c>
       <c r="C8" s="17">
@@ -2041,7 +2053,7 @@
       <c r="E8" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="131">
+      <c r="F8" s="112">
         <v>1.67</v>
       </c>
       <c r="G8" s="19" t="s">
@@ -2065,8 +2077,8 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="118"/>
-      <c r="B9" s="130"/>
+      <c r="A9" s="99"/>
+      <c r="B9" s="111"/>
       <c r="C9" s="17">
         <v>0.63194444444444442</v>
       </c>
@@ -2076,7 +2088,7 @@
       <c r="E9" s="18">
         <v>0.5</v>
       </c>
-      <c r="F9" s="132"/>
+      <c r="F9" s="113"/>
       <c r="G9" s="29" t="s">
         <v>23</v>
       </c>
@@ -2087,10 +2099,10 @@
       <c r="J9" s="29"/>
     </row>
     <row r="10" spans="1:15" s="63" customFormat="1">
-      <c r="A10" s="136">
+      <c r="A10" s="117">
         <v>2</v>
       </c>
-      <c r="B10" s="139">
+      <c r="B10" s="120">
         <v>41589</v>
       </c>
       <c r="C10" s="58" t="s">
@@ -2102,7 +2114,7 @@
       <c r="E10" s="59">
         <v>2.5</v>
       </c>
-      <c r="F10" s="141">
+      <c r="F10" s="122">
         <f>SUM(E10:E11)</f>
         <v>5</v>
       </c>
@@ -2116,8 +2128,8 @@
       <c r="J10" s="60"/>
     </row>
     <row r="11" spans="1:15" s="63" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A11" s="137"/>
-      <c r="B11" s="140"/>
+      <c r="A11" s="118"/>
+      <c r="B11" s="121"/>
       <c r="C11" s="58" t="s">
         <v>76</v>
       </c>
@@ -2127,7 +2139,7 @@
       <c r="E11" s="59">
         <v>2.5</v>
       </c>
-      <c r="F11" s="142"/>
+      <c r="F11" s="123"/>
       <c r="G11" s="60" t="s">
         <v>22</v>
       </c>
@@ -2140,8 +2152,8 @@
       <c r="J11" s="60"/>
     </row>
     <row r="12" spans="1:15" ht="51">
-      <c r="A12" s="137"/>
-      <c r="B12" s="90">
+      <c r="A12" s="118"/>
+      <c r="B12" s="125">
         <v>41590</v>
       </c>
       <c r="C12" s="22">
@@ -2153,7 +2165,7 @@
       <c r="E12" s="23">
         <v>2.25</v>
       </c>
-      <c r="F12" s="144">
+      <c r="F12" s="127">
         <v>3.75</v>
       </c>
       <c r="G12" s="30" t="s">
@@ -2180,8 +2192,8 @@
       <c r="O12" s="34"/>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A13" s="137"/>
-      <c r="B13" s="92"/>
+      <c r="A13" s="118"/>
+      <c r="B13" s="126"/>
       <c r="C13" s="22">
         <v>0.91666666666666663</v>
       </c>
@@ -2191,7 +2203,7 @@
       <c r="E13" s="23">
         <v>1.5</v>
       </c>
-      <c r="F13" s="145"/>
+      <c r="F13" s="128"/>
       <c r="G13" s="45" t="s">
         <v>28</v>
       </c>
@@ -2207,8 +2219,8 @@
       <c r="O13" s="34"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A14" s="137"/>
-      <c r="B14" s="90">
+      <c r="A14" s="118"/>
+      <c r="B14" s="125">
         <v>41591</v>
       </c>
       <c r="C14" s="22">
@@ -2220,7 +2232,7 @@
       <c r="E14" s="23">
         <v>2</v>
       </c>
-      <c r="F14" s="93">
+      <c r="F14" s="130">
         <v>4.5</v>
       </c>
       <c r="G14" s="45" t="s">
@@ -2238,8 +2250,8 @@
       <c r="O14" s="34"/>
     </row>
     <row r="15" spans="1:15" ht="25.5">
-      <c r="A15" s="137"/>
-      <c r="B15" s="91"/>
+      <c r="A15" s="118"/>
+      <c r="B15" s="129"/>
       <c r="C15" s="25">
         <v>0.5625</v>
       </c>
@@ -2249,7 +2261,7 @@
       <c r="E15" s="28">
         <v>2</v>
       </c>
-      <c r="F15" s="94"/>
+      <c r="F15" s="131"/>
       <c r="G15" s="30" t="s">
         <v>19</v>
       </c>
@@ -2266,8 +2278,8 @@
       <c r="N15" s="3"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A16" s="137"/>
-      <c r="B16" s="92"/>
+      <c r="A16" s="118"/>
+      <c r="B16" s="126"/>
       <c r="C16" s="25">
         <v>0.83333333333333337</v>
       </c>
@@ -2277,7 +2289,7 @@
       <c r="E16" s="28">
         <v>0.5</v>
       </c>
-      <c r="F16" s="95"/>
+      <c r="F16" s="132"/>
       <c r="G16" s="45" t="s">
         <v>28</v>
       </c>
@@ -2301,7 +2313,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A17" s="137"/>
+      <c r="A17" s="118"/>
       <c r="B17" s="47">
         <v>41592</v>
       </c>
@@ -2340,7 +2352,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="25.5">
-      <c r="A18" s="138"/>
+      <c r="A18" s="119"/>
       <c r="B18" s="42">
         <v>41593</v>
       </c>
@@ -2379,10 +2391,10 @@
       </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="98">
+      <c r="A19" s="137">
         <v>3</v>
       </c>
-      <c r="B19" s="96">
+      <c r="B19" s="134">
         <v>41596</v>
       </c>
       <c r="C19" s="53" t="s">
@@ -2394,7 +2406,7 @@
       <c r="E19" s="50">
         <v>0.5</v>
       </c>
-      <c r="F19" s="89">
+      <c r="F19" s="82">
         <f>SUM(E19:E20)</f>
         <v>3.5</v>
       </c>
@@ -2421,8 +2433,8 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="99"/>
-      <c r="B20" s="97"/>
+      <c r="A20" s="138"/>
+      <c r="B20" s="135"/>
       <c r="C20" s="53" t="s">
         <v>81</v>
       </c>
@@ -2432,7 +2444,7 @@
       <c r="E20" s="50">
         <v>3</v>
       </c>
-      <c r="F20" s="85"/>
+      <c r="F20" s="136"/>
       <c r="G20" s="49" t="s">
         <v>22</v>
       </c>
@@ -2449,8 +2461,8 @@
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="99"/>
-      <c r="B21" s="96">
+      <c r="A21" s="138"/>
+      <c r="B21" s="134">
         <v>41597</v>
       </c>
       <c r="C21" s="53" t="s">
@@ -2462,7 +2474,7 @@
       <c r="E21" s="50">
         <v>2</v>
       </c>
-      <c r="F21" s="89">
+      <c r="F21" s="82">
         <f>SUM(E21:E22)</f>
         <v>2.5</v>
       </c>
@@ -2482,8 +2494,8 @@
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="99"/>
-      <c r="B22" s="97"/>
+      <c r="A22" s="138"/>
+      <c r="B22" s="135"/>
       <c r="C22" s="53" t="s">
         <v>84</v>
       </c>
@@ -2493,7 +2505,7 @@
       <c r="E22" s="50">
         <v>0.5</v>
       </c>
-      <c r="F22" s="85"/>
+      <c r="F22" s="136"/>
       <c r="G22" s="49" t="s">
         <v>22</v>
       </c>
@@ -2517,7 +2529,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="26.25">
-      <c r="A23" s="99"/>
+      <c r="A23" s="138"/>
       <c r="B23" s="26">
         <v>41598</v>
       </c>
@@ -2557,7 +2569,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="26.25">
-      <c r="A24" s="99"/>
+      <c r="A24" s="138"/>
       <c r="B24" s="26">
         <v>41599</v>
       </c>
@@ -2570,7 +2582,7 @@
       <c r="E24" s="50">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F24" s="89">
+      <c r="F24" s="82">
         <f>SUM(E24:E28)</f>
         <v>7.0600000000000005</v>
       </c>
@@ -2588,7 +2600,7 @@
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="99"/>
+      <c r="A25" s="138"/>
       <c r="B25" s="26">
         <v>41599</v>
       </c>
@@ -2601,7 +2613,7 @@
       <c r="E25" s="50">
         <v>1.3</v>
       </c>
-      <c r="F25" s="101"/>
+      <c r="F25" s="83"/>
       <c r="G25" s="57" t="s">
         <v>19</v>
       </c>
@@ -2616,7 +2628,7 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="99"/>
+      <c r="A26" s="138"/>
       <c r="B26" s="26">
         <v>41599</v>
       </c>
@@ -2629,7 +2641,7 @@
       <c r="E26" s="50">
         <v>1.5</v>
       </c>
-      <c r="F26" s="101"/>
+      <c r="F26" s="83"/>
       <c r="G26" s="57" t="s">
         <v>24</v>
       </c>
@@ -2646,7 +2658,7 @@
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="99"/>
+      <c r="A27" s="138"/>
       <c r="B27" s="26">
         <v>41599</v>
       </c>
@@ -2659,7 +2671,7 @@
       <c r="E27" s="50">
         <v>2.1</v>
       </c>
-      <c r="F27" s="101"/>
+      <c r="F27" s="83"/>
       <c r="G27" s="29" t="s">
         <v>19</v>
       </c>
@@ -2681,7 +2693,7 @@
       </c>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="99"/>
+      <c r="A28" s="138"/>
       <c r="B28" s="26">
         <v>41599</v>
       </c>
@@ -2694,7 +2706,7 @@
       <c r="E28" s="50">
         <v>1</v>
       </c>
-      <c r="F28" s="102"/>
+      <c r="F28" s="84"/>
       <c r="G28" s="29" t="s">
         <v>22</v>
       </c>
@@ -2709,7 +2721,7 @@
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="99"/>
+      <c r="A29" s="138"/>
       <c r="B29" s="26">
         <v>41600</v>
       </c>
@@ -2722,7 +2734,7 @@
       <c r="E29" s="50">
         <v>1.25</v>
       </c>
-      <c r="F29" s="89">
+      <c r="F29" s="82">
         <f>SUM(E29:E30)</f>
         <v>3.25</v>
       </c>
@@ -2738,7 +2750,7 @@
       <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:14" ht="51">
-      <c r="A30" s="99"/>
+      <c r="A30" s="138"/>
       <c r="B30" s="26">
         <v>41600</v>
       </c>
@@ -2751,7 +2763,7 @@
       <c r="E30" s="50">
         <v>2</v>
       </c>
-      <c r="F30" s="85"/>
+      <c r="F30" s="136"/>
       <c r="G30" s="57" t="s">
         <v>22</v>
       </c>
@@ -2773,7 +2785,7 @@
       </c>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="99"/>
+      <c r="A31" s="138"/>
       <c r="B31" s="26">
         <v>41601</v>
       </c>
@@ -2786,7 +2798,7 @@
       <c r="E31" s="74">
         <v>0.25</v>
       </c>
-      <c r="F31" s="89">
+      <c r="F31" s="82">
         <f>SUM(E31:E33)</f>
         <v>4.6500000000000004</v>
       </c>
@@ -2800,7 +2812,7 @@
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="99"/>
+      <c r="A32" s="138"/>
       <c r="B32" s="26">
         <v>41601</v>
       </c>
@@ -2813,7 +2825,7 @@
       <c r="E32" s="50">
         <v>3.5</v>
       </c>
-      <c r="F32" s="101"/>
+      <c r="F32" s="83"/>
       <c r="G32" s="57" t="s">
         <v>22</v>
       </c>
@@ -2830,7 +2842,7 @@
       <c r="N32" s="3"/>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="100"/>
+      <c r="A33" s="139"/>
       <c r="B33" s="26">
         <v>41601</v>
       </c>
@@ -2843,7 +2855,7 @@
       <c r="E33" s="50">
         <v>0.9</v>
       </c>
-      <c r="F33" s="102"/>
+      <c r="F33" s="84"/>
       <c r="G33" s="57" t="s">
         <v>22</v>
       </c>
@@ -2902,7 +2914,7 @@
       </c>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="81"/>
+      <c r="A35" s="133"/>
       <c r="B35" s="27">
         <v>41604</v>
       </c>
@@ -2915,7 +2927,7 @@
       <c r="E35" s="28">
         <v>1</v>
       </c>
-      <c r="F35" s="103">
+      <c r="F35" s="140">
         <f>SUM(E35:E38)</f>
         <v>6.75</v>
       </c>
@@ -2933,7 +2945,7 @@
       <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="81"/>
+      <c r="A36" s="133"/>
       <c r="B36" s="27">
         <v>41604</v>
       </c>
@@ -2946,7 +2958,7 @@
       <c r="E36" s="76">
         <v>2.5</v>
       </c>
-      <c r="F36" s="81"/>
+      <c r="F36" s="133"/>
       <c r="G36" s="67" t="s">
         <v>23</v>
       </c>
@@ -2963,7 +2975,7 @@
       <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="81"/>
+      <c r="A37" s="133"/>
       <c r="B37" s="27">
         <v>41604</v>
       </c>
@@ -2976,7 +2988,7 @@
       <c r="E37" s="76">
         <v>1.25</v>
       </c>
-      <c r="F37" s="81"/>
+      <c r="F37" s="133"/>
       <c r="G37" s="67" t="s">
         <v>24</v>
       </c>
@@ -2993,7 +3005,7 @@
       <c r="N37" s="3"/>
     </row>
     <row r="38" spans="1:14" ht="51">
-      <c r="A38" s="81"/>
+      <c r="A38" s="133"/>
       <c r="B38" s="27">
         <v>41604</v>
       </c>
@@ -3006,7 +3018,7 @@
       <c r="E38" s="69">
         <v>2</v>
       </c>
-      <c r="F38" s="82"/>
+      <c r="F38" s="81"/>
       <c r="G38" s="67" t="s">
         <v>22</v>
       </c>
@@ -3032,7 +3044,7 @@
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="81"/>
+      <c r="A39" s="133"/>
       <c r="B39" s="27">
         <v>41605</v>
       </c>
@@ -3070,7 +3082,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" ht="25.5">
-      <c r="A40" s="81"/>
+      <c r="A40" s="133"/>
       <c r="B40" s="27">
         <v>41605</v>
       </c>
@@ -3083,7 +3095,7 @@
       <c r="E40" s="69">
         <v>0.5</v>
       </c>
-      <c r="F40" s="82"/>
+      <c r="F40" s="81"/>
       <c r="G40" s="67" t="s">
         <v>24</v>
       </c>
@@ -3100,7 +3112,7 @@
       <c r="N40" s="3"/>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="81"/>
+      <c r="A41" s="133"/>
       <c r="B41" s="27">
         <v>41606</v>
       </c>
@@ -3131,7 +3143,7 @@
       <c r="N41" s="3"/>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="81"/>
+      <c r="A42" s="133"/>
       <c r="B42" s="27">
         <v>41606</v>
       </c>
@@ -3144,7 +3156,7 @@
       <c r="E42" s="69">
         <v>1.75</v>
       </c>
-      <c r="F42" s="81"/>
+      <c r="F42" s="133"/>
       <c r="G42" s="67" t="s">
         <v>25</v>
       </c>
@@ -3159,7 +3171,7 @@
       <c r="N42" s="3"/>
     </row>
     <row r="43" spans="1:14" ht="25.5">
-      <c r="A43" s="81"/>
+      <c r="A43" s="133"/>
       <c r="B43" s="27">
         <v>41606</v>
       </c>
@@ -3172,7 +3184,7 @@
       <c r="E43" s="69">
         <v>2.75</v>
       </c>
-      <c r="F43" s="82"/>
+      <c r="F43" s="81"/>
       <c r="G43" s="67" t="s">
         <v>19</v>
       </c>
@@ -3196,7 +3208,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" ht="51">
-      <c r="A44" s="81"/>
+      <c r="A44" s="133"/>
       <c r="B44" s="27">
         <v>41607</v>
       </c>
@@ -3236,7 +3248,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" ht="38.25">
-      <c r="A45" s="81"/>
+      <c r="A45" s="133"/>
       <c r="B45" s="27">
         <v>41609</v>
       </c>
@@ -3269,7 +3281,7 @@
       <c r="N45" s="3"/>
     </row>
     <row r="46" spans="1:14" ht="25.5">
-      <c r="A46" s="82"/>
+      <c r="A46" s="81"/>
       <c r="B46" s="27">
         <v>41609</v>
       </c>
@@ -3282,7 +3294,7 @@
       <c r="E46" s="69">
         <v>2</v>
       </c>
-      <c r="F46" s="82"/>
+      <c r="F46" s="81"/>
       <c r="G46" s="67" t="s">
         <v>22</v>
       </c>
@@ -3301,7 +3313,7 @@
       <c r="N46" s="3"/>
     </row>
     <row r="47" spans="1:14" ht="63.75">
-      <c r="A47" s="83">
+      <c r="A47" s="141">
         <v>5</v>
       </c>
       <c r="B47" s="26">
@@ -3341,7 +3353,7 @@
       </c>
     </row>
     <row r="48" spans="1:14" ht="38.25">
-      <c r="A48" s="84"/>
+      <c r="A48" s="142"/>
       <c r="B48" s="26">
         <v>41611</v>
       </c>
@@ -3354,7 +3366,7 @@
       <c r="E48" s="55">
         <v>1.5</v>
       </c>
-      <c r="F48" s="83">
+      <c r="F48" s="141">
         <f>SUM(E48:E50)</f>
         <v>7</v>
       </c>
@@ -3372,7 +3384,7 @@
       <c r="N48" s="3"/>
     </row>
     <row r="49" spans="1:14" ht="51.75" customHeight="1">
-      <c r="A49" s="84"/>
+      <c r="A49" s="142"/>
       <c r="B49" s="26">
         <v>41611</v>
       </c>
@@ -3385,9 +3397,9 @@
       <c r="E49" s="55">
         <v>3.5</v>
       </c>
-      <c r="F49" s="84"/>
+      <c r="F49" s="142"/>
       <c r="G49" s="29" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="H49" s="65" t="s">
         <v>159</v>
@@ -3407,7 +3419,7 @@
       </c>
     </row>
     <row r="50" spans="1:14" ht="38.25">
-      <c r="A50" s="84"/>
+      <c r="A50" s="142"/>
       <c r="B50" s="26">
         <v>41611</v>
       </c>
@@ -3420,7 +3432,7 @@
       <c r="E50" s="55">
         <v>2</v>
       </c>
-      <c r="F50" s="85"/>
+      <c r="F50" s="136"/>
       <c r="G50" s="29" t="s">
         <v>22</v>
       </c>
@@ -3439,7 +3451,7 @@
       <c r="N50" s="3"/>
     </row>
     <row r="51" spans="1:14" ht="38.25">
-      <c r="A51" s="84"/>
+      <c r="A51" s="142"/>
       <c r="B51" s="26">
         <v>41612</v>
       </c>
@@ -3452,7 +3464,7 @@
       <c r="E51" s="55">
         <v>0.75</v>
       </c>
-      <c r="F51" s="83">
+      <c r="F51" s="141">
         <f>SUM(E52:E53)</f>
         <v>6.5</v>
       </c>
@@ -3481,7 +3493,7 @@
       </c>
     </row>
     <row r="52" spans="1:14" ht="76.5">
-      <c r="A52" s="84"/>
+      <c r="A52" s="142"/>
       <c r="B52" s="26">
         <v>41612</v>
       </c>
@@ -3494,7 +3506,7 @@
       <c r="E52" s="55">
         <v>4.5</v>
       </c>
-      <c r="F52" s="84"/>
+      <c r="F52" s="142"/>
       <c r="G52" s="29" t="s">
         <v>19</v>
       </c>
@@ -3509,7 +3521,7 @@
       <c r="N52" s="3"/>
     </row>
     <row r="53" spans="1:14" ht="38.25">
-      <c r="A53" s="84"/>
+      <c r="A53" s="142"/>
       <c r="B53" s="26">
         <v>41612</v>
       </c>
@@ -3522,7 +3534,7 @@
       <c r="E53" s="55">
         <v>2</v>
       </c>
-      <c r="F53" s="85"/>
+      <c r="F53" s="136"/>
       <c r="G53" s="29" t="s">
         <v>22</v>
       </c>
@@ -3539,7 +3551,7 @@
       <c r="N53" s="3"/>
     </row>
     <row r="54" spans="1:14" ht="38.25">
-      <c r="A54" s="84"/>
+      <c r="A54" s="142"/>
       <c r="B54" s="26">
         <v>41613</v>
       </c>
@@ -3552,7 +3564,7 @@
       <c r="E54" s="74">
         <v>3</v>
       </c>
-      <c r="F54" s="89">
+      <c r="F54" s="82">
         <f>SUM(E54:E58)</f>
         <v>7.82</v>
       </c>
@@ -3570,7 +3582,7 @@
       <c r="N54" s="3"/>
     </row>
     <row r="55" spans="1:14">
-      <c r="A55" s="84"/>
+      <c r="A55" s="142"/>
       <c r="B55" s="26">
         <v>41613</v>
       </c>
@@ -3583,7 +3595,7 @@
       <c r="E55" s="74">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F55" s="101"/>
+      <c r="F55" s="83"/>
       <c r="G55" s="29" t="s">
         <v>24</v>
       </c>
@@ -3598,7 +3610,7 @@
       <c r="N55" s="3"/>
     </row>
     <row r="56" spans="1:14" ht="51">
-      <c r="A56" s="84"/>
+      <c r="A56" s="142"/>
       <c r="B56" s="26">
         <v>41613</v>
       </c>
@@ -3611,7 +3623,7 @@
       <c r="E56" s="74">
         <v>1.5</v>
       </c>
-      <c r="F56" s="101"/>
+      <c r="F56" s="83"/>
       <c r="G56" s="29" t="s">
         <v>23</v>
       </c>
@@ -3626,7 +3638,7 @@
       <c r="N56" s="3"/>
     </row>
     <row r="57" spans="1:14" ht="25.5">
-      <c r="A57" s="84"/>
+      <c r="A57" s="142"/>
       <c r="B57" s="26">
         <v>41613</v>
       </c>
@@ -3639,7 +3651,7 @@
       <c r="E57" s="74">
         <v>0.66</v>
       </c>
-      <c r="F57" s="101"/>
+      <c r="F57" s="83"/>
       <c r="G57" s="29" t="s">
         <v>19</v>
       </c>
@@ -3654,7 +3666,7 @@
       <c r="N57" s="3"/>
     </row>
     <row r="58" spans="1:14" ht="25.5">
-      <c r="A58" s="84"/>
+      <c r="A58" s="142"/>
       <c r="B58" s="26">
         <v>41613</v>
       </c>
@@ -3667,7 +3679,7 @@
       <c r="E58" s="74">
         <v>1.5</v>
       </c>
-      <c r="F58" s="102"/>
+      <c r="F58" s="84"/>
       <c r="G58" s="29" t="s">
         <v>24</v>
       </c>
@@ -3689,7 +3701,7 @@
       </c>
     </row>
     <row r="59" spans="1:14" ht="76.5">
-      <c r="A59" s="85"/>
+      <c r="A59" s="136"/>
       <c r="B59" s="26">
         <v>41616</v>
       </c>
@@ -3775,7 +3787,7 @@
       </c>
     </row>
     <row r="61" spans="1:14" ht="51">
-      <c r="A61" s="81"/>
+      <c r="A61" s="133"/>
       <c r="B61" s="27">
         <v>41617</v>
       </c>
@@ -3788,7 +3800,7 @@
       <c r="E61" s="69">
         <v>2</v>
       </c>
-      <c r="F61" s="82"/>
+      <c r="F61" s="81"/>
       <c r="G61" s="67" t="s">
         <v>22</v>
       </c>
@@ -3804,20 +3816,30 @@
       <c r="M61" s="9"/>
       <c r="N61" s="3"/>
     </row>
-    <row r="62" spans="1:14">
-      <c r="A62" s="81"/>
+    <row r="62" spans="1:14" ht="38.25">
+      <c r="A62" s="133"/>
       <c r="B62" s="27">
         <v>41618</v>
       </c>
-      <c r="C62" s="69"/>
-      <c r="D62" s="69"/>
-      <c r="E62" s="69"/>
+      <c r="C62" s="72">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D62" s="72" t="s">
+        <v>189</v>
+      </c>
+      <c r="E62" s="69">
+        <v>2.5</v>
+      </c>
       <c r="F62" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G62" s="67"/>
-      <c r="H62" s="67"/>
+        <v>2.5</v>
+      </c>
+      <c r="G62" s="67" t="s">
+        <v>27</v>
+      </c>
+      <c r="H62" s="71" t="s">
+        <v>188</v>
+      </c>
       <c r="I62" s="67"/>
       <c r="J62" s="67"/>
       <c r="K62" s="7" t="s">
@@ -3832,20 +3854,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
-      <c r="A63" s="81"/>
+    <row r="63" spans="1:14" ht="25.5">
+      <c r="A63" s="133"/>
       <c r="B63" s="27">
         <v>41619</v>
       </c>
-      <c r="C63" s="69"/>
-      <c r="D63" s="69"/>
-      <c r="E63" s="69"/>
+      <c r="C63" s="69" t="s">
+        <v>157</v>
+      </c>
+      <c r="D63" s="69" t="s">
+        <v>179</v>
+      </c>
+      <c r="E63" s="69">
+        <v>1.5</v>
+      </c>
       <c r="F63" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G63" s="67"/>
-      <c r="H63" s="67"/>
+        <v>1.5</v>
+      </c>
+      <c r="G63" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="H63" s="71" t="s">
+        <v>190</v>
+      </c>
       <c r="I63" s="67"/>
       <c r="J63" s="67"/>
       <c r="K63" s="7" t="s">
@@ -3861,7 +3893,7 @@
       </c>
     </row>
     <row r="64" spans="1:14">
-      <c r="A64" s="81"/>
+      <c r="A64" s="133"/>
       <c r="B64" s="27">
         <v>41620</v>
       </c>
@@ -3889,7 +3921,7 @@
       </c>
     </row>
     <row r="65" spans="1:14">
-      <c r="A65" s="82"/>
+      <c r="A65" s="81"/>
       <c r="B65" s="27">
         <v>41621</v>
       </c>
@@ -3917,7 +3949,7 @@
       </c>
     </row>
     <row r="66" spans="1:14">
-      <c r="A66" s="83">
+      <c r="A66" s="141">
         <v>7</v>
       </c>
       <c r="B66" s="26">
@@ -3947,7 +3979,7 @@
       </c>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="84"/>
+      <c r="A67" s="142"/>
       <c r="B67" s="26">
         <v>41625</v>
       </c>
@@ -3975,7 +4007,7 @@
       </c>
     </row>
     <row r="68" spans="1:14">
-      <c r="A68" s="84"/>
+      <c r="A68" s="142"/>
       <c r="B68" s="26">
         <v>41626</v>
       </c>
@@ -4003,7 +4035,7 @@
       </c>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="84"/>
+      <c r="A69" s="142"/>
       <c r="B69" s="26">
         <v>41627</v>
       </c>
@@ -4020,7 +4052,7 @@
       <c r="J69" s="29"/>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="85"/>
+      <c r="A70" s="136"/>
       <c r="B70" s="26">
         <v>41628</v>
       </c>
@@ -4056,7 +4088,7 @@
       <c r="J71" s="67"/>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="81"/>
+      <c r="A72" s="133"/>
       <c r="B72" s="27">
         <v>41632</v>
       </c>
@@ -4073,7 +4105,7 @@
       <c r="J72" s="67"/>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="81"/>
+      <c r="A73" s="133"/>
       <c r="B73" s="27">
         <v>41633</v>
       </c>
@@ -4090,7 +4122,7 @@
       <c r="J73" s="67"/>
     </row>
     <row r="74" spans="1:14">
-      <c r="A74" s="81"/>
+      <c r="A74" s="133"/>
       <c r="B74" s="27">
         <v>41634</v>
       </c>
@@ -4107,7 +4139,7 @@
       <c r="J74" s="67"/>
     </row>
     <row r="75" spans="1:14">
-      <c r="A75" s="82"/>
+      <c r="A75" s="81"/>
       <c r="B75" s="27">
         <v>41635</v>
       </c>
@@ -4124,7 +4156,7 @@
       <c r="J75" s="67"/>
     </row>
     <row r="76" spans="1:14">
-      <c r="A76" s="83">
+      <c r="A76" s="141">
         <v>9</v>
       </c>
       <c r="B76" s="26">
@@ -4143,7 +4175,7 @@
       <c r="J76" s="29"/>
     </row>
     <row r="77" spans="1:14">
-      <c r="A77" s="84"/>
+      <c r="A77" s="142"/>
       <c r="B77" s="26">
         <v>41639</v>
       </c>
@@ -4160,7 +4192,7 @@
       <c r="J77" s="29"/>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="84"/>
+      <c r="A78" s="142"/>
       <c r="B78" s="26">
         <v>41640</v>
       </c>
@@ -4177,7 +4209,7 @@
       <c r="J78" s="29"/>
     </row>
     <row r="79" spans="1:14">
-      <c r="A79" s="84"/>
+      <c r="A79" s="142"/>
       <c r="B79" s="26">
         <v>41641</v>
       </c>
@@ -4194,7 +4226,7 @@
       <c r="J79" s="29"/>
     </row>
     <row r="80" spans="1:14">
-      <c r="A80" s="85"/>
+      <c r="A80" s="136"/>
       <c r="B80" s="26">
         <v>41642</v>
       </c>
@@ -4230,7 +4262,7 @@
       <c r="J81" s="67"/>
     </row>
     <row r="82" spans="1:10">
-      <c r="A82" s="81"/>
+      <c r="A82" s="133"/>
       <c r="B82" s="27">
         <v>41646</v>
       </c>
@@ -4247,7 +4279,7 @@
       <c r="J82" s="67"/>
     </row>
     <row r="83" spans="1:10">
-      <c r="A83" s="81"/>
+      <c r="A83" s="133"/>
       <c r="B83" s="27">
         <v>41647</v>
       </c>
@@ -4264,7 +4296,7 @@
       <c r="J83" s="67"/>
     </row>
     <row r="84" spans="1:10">
-      <c r="A84" s="81"/>
+      <c r="A84" s="133"/>
       <c r="B84" s="27">
         <v>41648</v>
       </c>
@@ -4281,7 +4313,7 @@
       <c r="J84" s="67"/>
     </row>
     <row r="85" spans="1:10">
-      <c r="A85" s="82"/>
+      <c r="A85" s="81"/>
       <c r="B85" s="27">
         <v>41649</v>
       </c>
@@ -4298,7 +4330,7 @@
       <c r="J85" s="67"/>
     </row>
     <row r="86" spans="1:10">
-      <c r="A86" s="83">
+      <c r="A86" s="141">
         <v>11</v>
       </c>
       <c r="B86" s="26">
@@ -4317,7 +4349,7 @@
       <c r="J86" s="29"/>
     </row>
     <row r="87" spans="1:10">
-      <c r="A87" s="84"/>
+      <c r="A87" s="142"/>
       <c r="B87" s="26">
         <v>41653</v>
       </c>
@@ -4333,8 +4365,8 @@
       <c r="I87" s="29"/>
       <c r="J87" s="29"/>
     </row>
-    <row r="88" spans="1:10" ht="409.6">
-      <c r="A88" s="84"/>
+    <row r="88" spans="1:10">
+      <c r="A88" s="142"/>
       <c r="B88" s="26">
         <v>41654</v>
       </c>
@@ -4351,7 +4383,7 @@
       <c r="J88" s="29"/>
     </row>
     <row r="89" spans="1:10">
-      <c r="A89" s="84"/>
+      <c r="A89" s="142"/>
       <c r="B89" s="26">
         <v>41655</v>
       </c>
@@ -4368,7 +4400,7 @@
       <c r="J89" s="29"/>
     </row>
     <row r="90" spans="1:10">
-      <c r="A90" s="85"/>
+      <c r="A90" s="136"/>
       <c r="B90" s="26">
         <v>41656</v>
       </c>
@@ -4404,7 +4436,7 @@
       <c r="J91" s="67"/>
     </row>
     <row r="92" spans="1:10">
-      <c r="A92" s="81"/>
+      <c r="A92" s="133"/>
       <c r="B92" s="27">
         <v>41660</v>
       </c>
@@ -4421,7 +4453,7 @@
       <c r="J92" s="67"/>
     </row>
     <row r="93" spans="1:10">
-      <c r="A93" s="81"/>
+      <c r="A93" s="133"/>
       <c r="B93" s="27">
         <v>41661</v>
       </c>
@@ -4438,7 +4470,7 @@
       <c r="J93" s="67"/>
     </row>
     <row r="94" spans="1:10">
-      <c r="A94" s="81"/>
+      <c r="A94" s="133"/>
       <c r="B94" s="27">
         <v>41662</v>
       </c>
@@ -4455,7 +4487,7 @@
       <c r="J94" s="67"/>
     </row>
     <row r="95" spans="1:10">
-      <c r="A95" s="82"/>
+      <c r="A95" s="81"/>
       <c r="B95" s="27">
         <v>41663</v>
       </c>
@@ -4472,7 +4504,7 @@
       <c r="J95" s="67"/>
     </row>
     <row r="96" spans="1:10">
-      <c r="A96" s="83">
+      <c r="A96" s="141">
         <v>13</v>
       </c>
       <c r="B96" s="26">
@@ -4493,7 +4525,7 @@
       <c r="J96" s="29"/>
     </row>
     <row r="97" spans="1:10">
-      <c r="A97" s="84"/>
+      <c r="A97" s="142"/>
       <c r="B97" s="26">
         <v>41667</v>
       </c>
@@ -4512,7 +4544,7 @@
       <c r="J97" s="29"/>
     </row>
     <row r="98" spans="1:10">
-      <c r="A98" s="84"/>
+      <c r="A98" s="142"/>
       <c r="B98" s="26">
         <v>41668</v>
       </c>
@@ -4531,7 +4563,7 @@
       <c r="J98" s="29"/>
     </row>
     <row r="99" spans="1:10">
-      <c r="A99" s="84"/>
+      <c r="A99" s="142"/>
       <c r="B99" s="26">
         <v>41669</v>
       </c>
@@ -4550,7 +4582,7 @@
       <c r="J99" s="29"/>
     </row>
     <row r="100" spans="1:10">
-      <c r="A100" s="85"/>
+      <c r="A100" s="136"/>
       <c r="B100" s="26">
         <v>41670</v>
       </c>
@@ -4590,7 +4622,7 @@
       <c r="J101" s="67"/>
     </row>
     <row r="102" spans="1:10">
-      <c r="A102" s="81"/>
+      <c r="A102" s="133"/>
       <c r="B102" s="27">
         <v>41674</v>
       </c>
@@ -4609,7 +4641,7 @@
       <c r="J102" s="67"/>
     </row>
     <row r="103" spans="1:10">
-      <c r="A103" s="81"/>
+      <c r="A103" s="133"/>
       <c r="B103" s="27">
         <v>41675</v>
       </c>
@@ -4628,7 +4660,7 @@
       <c r="J103" s="67"/>
     </row>
     <row r="104" spans="1:10">
-      <c r="A104" s="81"/>
+      <c r="A104" s="133"/>
       <c r="B104" s="27">
         <v>41676</v>
       </c>
@@ -4647,7 +4679,7 @@
       <c r="J104" s="67"/>
     </row>
     <row r="105" spans="1:10">
-      <c r="A105" s="82"/>
+      <c r="A105" s="81"/>
       <c r="B105" s="27">
         <v>41677</v>
       </c>
@@ -4666,7 +4698,7 @@
       <c r="J105" s="67"/>
     </row>
     <row r="106" spans="1:10">
-      <c r="A106" s="83">
+      <c r="A106" s="141">
         <v>15</v>
       </c>
       <c r="B106" s="26">
@@ -4685,7 +4717,7 @@
       <c r="J106" s="29"/>
     </row>
     <row r="107" spans="1:10">
-      <c r="A107" s="84"/>
+      <c r="A107" s="142"/>
       <c r="B107" s="26">
         <v>41681</v>
       </c>
@@ -4702,7 +4734,7 @@
       <c r="J107" s="29"/>
     </row>
     <row r="108" spans="1:10">
-      <c r="A108" s="84"/>
+      <c r="A108" s="142"/>
       <c r="B108" s="26">
         <v>41682</v>
       </c>
@@ -4719,7 +4751,7 @@
       <c r="J108" s="29"/>
     </row>
     <row r="109" spans="1:10">
-      <c r="A109" s="84"/>
+      <c r="A109" s="142"/>
       <c r="B109" s="26">
         <v>41683</v>
       </c>
@@ -4736,7 +4768,7 @@
       <c r="J109" s="29"/>
     </row>
     <row r="110" spans="1:10">
-      <c r="A110" s="85"/>
+      <c r="A110" s="136"/>
       <c r="B110" s="26">
         <v>41684</v>
       </c>
@@ -4772,7 +4804,7 @@
       <c r="J111" s="67"/>
     </row>
     <row r="112" spans="1:10">
-      <c r="A112" s="81"/>
+      <c r="A112" s="133"/>
       <c r="B112" s="27">
         <v>41688</v>
       </c>
@@ -4789,7 +4821,7 @@
       <c r="J112" s="67"/>
     </row>
     <row r="113" spans="1:10">
-      <c r="A113" s="81"/>
+      <c r="A113" s="133"/>
       <c r="B113" s="27">
         <v>41689</v>
       </c>
@@ -4806,7 +4838,7 @@
       <c r="J113" s="67"/>
     </row>
     <row r="114" spans="1:10">
-      <c r="A114" s="81"/>
+      <c r="A114" s="133"/>
       <c r="B114" s="27">
         <v>41690</v>
       </c>
@@ -4823,7 +4855,7 @@
       <c r="J114" s="67"/>
     </row>
     <row r="115" spans="1:10">
-      <c r="A115" s="82"/>
+      <c r="A115" s="81"/>
       <c r="B115" s="27">
         <v>41691</v>
       </c>
@@ -4840,7 +4872,7 @@
       <c r="J115" s="67"/>
     </row>
     <row r="116" spans="1:10">
-      <c r="A116" s="83">
+      <c r="A116" s="141">
         <v>17</v>
       </c>
       <c r="B116" s="26">
@@ -4859,7 +4891,7 @@
       <c r="J116" s="29"/>
     </row>
     <row r="117" spans="1:10">
-      <c r="A117" s="84"/>
+      <c r="A117" s="142"/>
       <c r="B117" s="26">
         <v>41695</v>
       </c>
@@ -4876,7 +4908,7 @@
       <c r="J117" s="29"/>
     </row>
     <row r="118" spans="1:10">
-      <c r="A118" s="84"/>
+      <c r="A118" s="142"/>
       <c r="B118" s="26">
         <v>41696</v>
       </c>
@@ -4893,7 +4925,7 @@
       <c r="J118" s="29"/>
     </row>
     <row r="119" spans="1:10">
-      <c r="A119" s="84"/>
+      <c r="A119" s="142"/>
       <c r="B119" s="26">
         <v>41697</v>
       </c>
@@ -4910,7 +4942,7 @@
       <c r="J119" s="29"/>
     </row>
     <row r="120" spans="1:10">
-      <c r="A120" s="85"/>
+      <c r="A120" s="136"/>
       <c r="B120" s="26">
         <v>41698</v>
       </c>
@@ -4946,7 +4978,7 @@
       <c r="J121" s="67"/>
     </row>
     <row r="122" spans="1:10">
-      <c r="A122" s="81"/>
+      <c r="A122" s="133"/>
       <c r="B122" s="27">
         <v>41702</v>
       </c>
@@ -4963,7 +4995,7 @@
       <c r="J122" s="67"/>
     </row>
     <row r="123" spans="1:10">
-      <c r="A123" s="81"/>
+      <c r="A123" s="133"/>
       <c r="B123" s="27">
         <v>41703</v>
       </c>
@@ -4980,7 +5012,7 @@
       <c r="J123" s="67"/>
     </row>
     <row r="124" spans="1:10">
-      <c r="A124" s="81"/>
+      <c r="A124" s="133"/>
       <c r="B124" s="27">
         <v>41704</v>
       </c>
@@ -4997,7 +5029,7 @@
       <c r="J124" s="67"/>
     </row>
     <row r="125" spans="1:10">
-      <c r="A125" s="82"/>
+      <c r="A125" s="81"/>
       <c r="B125" s="27">
         <v>41705</v>
       </c>
@@ -5014,7 +5046,7 @@
       <c r="J125" s="67"/>
     </row>
     <row r="126" spans="1:10">
-      <c r="A126" s="83">
+      <c r="A126" s="141">
         <v>19</v>
       </c>
       <c r="B126" s="26">
@@ -5033,7 +5065,7 @@
       <c r="J126" s="29"/>
     </row>
     <row r="127" spans="1:10">
-      <c r="A127" s="84"/>
+      <c r="A127" s="142"/>
       <c r="B127" s="26">
         <v>41709</v>
       </c>
@@ -5050,7 +5082,7 @@
       <c r="J127" s="29"/>
     </row>
     <row r="128" spans="1:10">
-      <c r="A128" s="84"/>
+      <c r="A128" s="142"/>
       <c r="B128" s="26">
         <v>41710</v>
       </c>
@@ -5067,7 +5099,7 @@
       <c r="J128" s="29"/>
     </row>
     <row r="129" spans="1:10">
-      <c r="A129" s="84"/>
+      <c r="A129" s="142"/>
       <c r="B129" s="26">
         <v>41711</v>
       </c>
@@ -5084,7 +5116,7 @@
       <c r="J129" s="29"/>
     </row>
     <row r="130" spans="1:10">
-      <c r="A130" s="85"/>
+      <c r="A130" s="136"/>
       <c r="B130" s="26">
         <v>41712</v>
       </c>
@@ -5120,7 +5152,7 @@
       <c r="J131" s="67"/>
     </row>
     <row r="132" spans="1:10">
-      <c r="A132" s="81"/>
+      <c r="A132" s="133"/>
       <c r="B132" s="27">
         <v>41716</v>
       </c>
@@ -5137,7 +5169,7 @@
       <c r="J132" s="67"/>
     </row>
     <row r="133" spans="1:10">
-      <c r="A133" s="81"/>
+      <c r="A133" s="133"/>
       <c r="B133" s="27">
         <v>41717</v>
       </c>
@@ -5154,7 +5186,7 @@
       <c r="J133" s="67"/>
     </row>
     <row r="134" spans="1:10">
-      <c r="A134" s="81"/>
+      <c r="A134" s="133"/>
       <c r="B134" s="27">
         <v>41718</v>
       </c>
@@ -5171,7 +5203,7 @@
       <c r="J134" s="67"/>
     </row>
     <row r="135" spans="1:10">
-      <c r="A135" s="82"/>
+      <c r="A135" s="81"/>
       <c r="B135" s="27">
         <v>41719</v>
       </c>
@@ -5188,7 +5220,7 @@
       <c r="J135" s="67"/>
     </row>
     <row r="136" spans="1:10">
-      <c r="A136" s="83">
+      <c r="A136" s="141">
         <v>21</v>
       </c>
       <c r="B136" s="26">
@@ -5207,7 +5239,7 @@
       <c r="J136" s="29"/>
     </row>
     <row r="137" spans="1:10">
-      <c r="A137" s="84"/>
+      <c r="A137" s="142"/>
       <c r="B137" s="26">
         <v>41723</v>
       </c>
@@ -5224,7 +5256,7 @@
       <c r="J137" s="29"/>
     </row>
     <row r="138" spans="1:10">
-      <c r="A138" s="84"/>
+      <c r="A138" s="142"/>
       <c r="B138" s="26">
         <v>41724</v>
       </c>
@@ -5241,7 +5273,7 @@
       <c r="J138" s="29"/>
     </row>
     <row r="139" spans="1:10">
-      <c r="A139" s="84"/>
+      <c r="A139" s="142"/>
       <c r="B139" s="26">
         <v>41725</v>
       </c>
@@ -5258,7 +5290,7 @@
       <c r="J139" s="29"/>
     </row>
     <row r="140" spans="1:10">
-      <c r="A140" s="85"/>
+      <c r="A140" s="136"/>
       <c r="B140" s="26">
         <v>41726</v>
       </c>
@@ -5294,7 +5326,7 @@
       <c r="J141" s="67"/>
     </row>
     <row r="142" spans="1:10">
-      <c r="A142" s="81"/>
+      <c r="A142" s="133"/>
       <c r="B142" s="27">
         <v>41730</v>
       </c>
@@ -5311,7 +5343,7 @@
       <c r="J142" s="67"/>
     </row>
     <row r="143" spans="1:10">
-      <c r="A143" s="81"/>
+      <c r="A143" s="133"/>
       <c r="B143" s="27">
         <v>41731</v>
       </c>
@@ -5328,7 +5360,7 @@
       <c r="J143" s="67"/>
     </row>
     <row r="144" spans="1:10">
-      <c r="A144" s="81"/>
+      <c r="A144" s="133"/>
       <c r="B144" s="27">
         <v>41732</v>
       </c>
@@ -5345,7 +5377,7 @@
       <c r="J144" s="67"/>
     </row>
     <row r="145" spans="1:10">
-      <c r="A145" s="82"/>
+      <c r="A145" s="81"/>
       <c r="B145" s="27">
         <v>41733</v>
       </c>
@@ -5362,7 +5394,7 @@
       <c r="J145" s="67"/>
     </row>
     <row r="146" spans="1:10">
-      <c r="A146" s="83">
+      <c r="A146" s="141">
         <v>23</v>
       </c>
       <c r="B146" s="26">
@@ -5381,7 +5413,7 @@
       <c r="J146" s="29"/>
     </row>
     <row r="147" spans="1:10">
-      <c r="A147" s="84"/>
+      <c r="A147" s="142"/>
       <c r="B147" s="26">
         <v>41737</v>
       </c>
@@ -5398,7 +5430,7 @@
       <c r="J147" s="29"/>
     </row>
     <row r="148" spans="1:10">
-      <c r="A148" s="84"/>
+      <c r="A148" s="142"/>
       <c r="B148" s="26">
         <v>41738</v>
       </c>
@@ -5415,7 +5447,7 @@
       <c r="J148" s="29"/>
     </row>
     <row r="149" spans="1:10">
-      <c r="A149" s="84"/>
+      <c r="A149" s="142"/>
       <c r="B149" s="26">
         <v>41739</v>
       </c>
@@ -5432,7 +5464,7 @@
       <c r="J149" s="29"/>
     </row>
     <row r="150" spans="1:10">
-      <c r="A150" s="85"/>
+      <c r="A150" s="136"/>
       <c r="B150" s="26">
         <v>41740</v>
       </c>
@@ -5468,7 +5500,7 @@
       <c r="J151" s="67"/>
     </row>
     <row r="152" spans="1:10">
-      <c r="A152" s="81"/>
+      <c r="A152" s="133"/>
       <c r="B152" s="27">
         <v>41744</v>
       </c>
@@ -5485,7 +5517,7 @@
       <c r="J152" s="67"/>
     </row>
     <row r="153" spans="1:10">
-      <c r="A153" s="81"/>
+      <c r="A153" s="133"/>
       <c r="B153" s="27">
         <v>41745</v>
       </c>
@@ -5502,7 +5534,7 @@
       <c r="J153" s="67"/>
     </row>
     <row r="154" spans="1:10">
-      <c r="A154" s="81"/>
+      <c r="A154" s="133"/>
       <c r="B154" s="27">
         <v>41746</v>
       </c>
@@ -5519,7 +5551,7 @@
       <c r="J154" s="67"/>
     </row>
     <row r="155" spans="1:10">
-      <c r="A155" s="82"/>
+      <c r="A155" s="81"/>
       <c r="B155" s="27">
         <v>41747</v>
       </c>
@@ -5536,7 +5568,7 @@
       <c r="J155" s="67"/>
     </row>
     <row r="156" spans="1:10">
-      <c r="A156" s="83">
+      <c r="A156" s="141">
         <v>25</v>
       </c>
       <c r="B156" s="26">
@@ -5555,7 +5587,7 @@
       <c r="J156" s="29"/>
     </row>
     <row r="157" spans="1:10">
-      <c r="A157" s="84"/>
+      <c r="A157" s="142"/>
       <c r="B157" s="26">
         <v>41751</v>
       </c>
@@ -5572,7 +5604,7 @@
       <c r="J157" s="29"/>
     </row>
     <row r="158" spans="1:10">
-      <c r="A158" s="84"/>
+      <c r="A158" s="142"/>
       <c r="B158" s="26">
         <v>41752</v>
       </c>
@@ -5589,7 +5621,7 @@
       <c r="J158" s="29"/>
     </row>
     <row r="159" spans="1:10">
-      <c r="A159" s="84"/>
+      <c r="A159" s="142"/>
       <c r="B159" s="26">
         <v>41753</v>
       </c>
@@ -5606,7 +5638,7 @@
       <c r="J159" s="29"/>
     </row>
     <row r="160" spans="1:10">
-      <c r="A160" s="85"/>
+      <c r="A160" s="136"/>
       <c r="B160" s="26">
         <v>41754</v>
       </c>
@@ -5642,7 +5674,7 @@
       <c r="J161" s="67"/>
     </row>
     <row r="162" spans="1:10">
-      <c r="A162" s="81"/>
+      <c r="A162" s="133"/>
       <c r="B162" s="27">
         <v>41758</v>
       </c>
@@ -5659,7 +5691,7 @@
       <c r="J162" s="67"/>
     </row>
     <row r="163" spans="1:10">
-      <c r="A163" s="81"/>
+      <c r="A163" s="133"/>
       <c r="B163" s="27">
         <v>41759</v>
       </c>
@@ -5676,7 +5708,7 @@
       <c r="J163" s="67"/>
     </row>
     <row r="164" spans="1:10">
-      <c r="A164" s="81"/>
+      <c r="A164" s="133"/>
       <c r="B164" s="27">
         <v>41760</v>
       </c>
@@ -5693,7 +5725,7 @@
       <c r="J164" s="67"/>
     </row>
     <row r="165" spans="1:10">
-      <c r="A165" s="82"/>
+      <c r="A165" s="81"/>
       <c r="B165" s="27">
         <v>41761</v>
       </c>
@@ -5710,7 +5742,7 @@
       <c r="J165" s="67"/>
     </row>
     <row r="166" spans="1:10">
-      <c r="A166" s="83">
+      <c r="A166" s="141">
         <v>27</v>
       </c>
       <c r="B166" s="26">
@@ -5729,7 +5761,7 @@
       <c r="J166" s="29"/>
     </row>
     <row r="167" spans="1:10">
-      <c r="A167" s="84"/>
+      <c r="A167" s="142"/>
       <c r="B167" s="26">
         <v>41765</v>
       </c>
@@ -5746,7 +5778,7 @@
       <c r="J167" s="29"/>
     </row>
     <row r="168" spans="1:10">
-      <c r="A168" s="84"/>
+      <c r="A168" s="142"/>
       <c r="B168" s="26">
         <v>41766</v>
       </c>
@@ -5763,7 +5795,7 @@
       <c r="J168" s="29"/>
     </row>
     <row r="169" spans="1:10">
-      <c r="A169" s="84"/>
+      <c r="A169" s="142"/>
       <c r="B169" s="26">
         <v>41767</v>
       </c>
@@ -5780,7 +5812,7 @@
       <c r="J169" s="29"/>
     </row>
     <row r="170" spans="1:10">
-      <c r="A170" s="85"/>
+      <c r="A170" s="136"/>
       <c r="B170" s="26">
         <v>41768</v>
       </c>
@@ -5816,7 +5848,7 @@
       <c r="J171" s="67"/>
     </row>
     <row r="172" spans="1:10">
-      <c r="A172" s="81"/>
+      <c r="A172" s="133"/>
       <c r="B172" s="27">
         <v>41772</v>
       </c>
@@ -5833,7 +5865,7 @@
       <c r="J172" s="67"/>
     </row>
     <row r="173" spans="1:10">
-      <c r="A173" s="81"/>
+      <c r="A173" s="133"/>
       <c r="B173" s="27">
         <v>41773</v>
       </c>
@@ -5850,7 +5882,7 @@
       <c r="J173" s="67"/>
     </row>
     <row r="174" spans="1:10">
-      <c r="A174" s="81"/>
+      <c r="A174" s="133"/>
       <c r="B174" s="27">
         <v>41774</v>
       </c>
@@ -5867,7 +5899,7 @@
       <c r="J174" s="67"/>
     </row>
     <row r="175" spans="1:10">
-      <c r="A175" s="82"/>
+      <c r="A175" s="81"/>
       <c r="B175" s="27">
         <v>41775</v>
       </c>
@@ -5884,7 +5916,7 @@
       <c r="J175" s="67"/>
     </row>
     <row r="176" spans="1:10">
-      <c r="A176" s="83">
+      <c r="A176" s="141">
         <v>29</v>
       </c>
       <c r="B176" s="26">
@@ -5903,7 +5935,7 @@
       <c r="J176" s="29"/>
     </row>
     <row r="177" spans="1:10">
-      <c r="A177" s="84"/>
+      <c r="A177" s="142"/>
       <c r="B177" s="26">
         <v>41779</v>
       </c>
@@ -5920,7 +5952,7 @@
       <c r="J177" s="29"/>
     </row>
     <row r="178" spans="1:10">
-      <c r="A178" s="84"/>
+      <c r="A178" s="142"/>
       <c r="B178" s="26">
         <v>41780</v>
       </c>
@@ -5937,7 +5969,7 @@
       <c r="J178" s="29"/>
     </row>
     <row r="179" spans="1:10">
-      <c r="A179" s="84"/>
+      <c r="A179" s="142"/>
       <c r="B179" s="26">
         <v>41781</v>
       </c>
@@ -5954,7 +5986,7 @@
       <c r="J179" s="29"/>
     </row>
     <row r="180" spans="1:10">
-      <c r="A180" s="85"/>
+      <c r="A180" s="136"/>
       <c r="B180" s="26">
         <v>41782</v>
       </c>
@@ -5971,7 +6003,7 @@
       <c r="J180" s="29"/>
     </row>
     <row r="181" spans="1:10">
-      <c r="A181" s="86">
+      <c r="A181" s="143">
         <v>30</v>
       </c>
       <c r="B181" s="27">
@@ -5990,7 +6022,7 @@
       <c r="J181" s="37"/>
     </row>
     <row r="182" spans="1:10">
-      <c r="A182" s="87"/>
+      <c r="A182" s="144"/>
       <c r="B182" s="27">
         <v>41786</v>
       </c>
@@ -6007,7 +6039,7 @@
       <c r="J182" s="37"/>
     </row>
     <row r="183" spans="1:10">
-      <c r="A183" s="87"/>
+      <c r="A183" s="144"/>
       <c r="B183" s="27">
         <v>41787</v>
       </c>
@@ -6024,7 +6056,7 @@
       <c r="J183" s="37"/>
     </row>
     <row r="184" spans="1:10">
-      <c r="A184" s="87"/>
+      <c r="A184" s="144"/>
       <c r="B184" s="27">
         <v>41788</v>
       </c>
@@ -6041,7 +6073,7 @@
       <c r="J184" s="37"/>
     </row>
     <row r="185" spans="1:10">
-      <c r="A185" s="88"/>
+      <c r="A185" s="145"/>
       <c r="B185" s="27">
         <v>41789</v>
       </c>
@@ -6167,6 +6199,50 @@
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="A171:A175"/>
+    <mergeCell ref="A176:A180"/>
+    <mergeCell ref="A181:A185"/>
+    <mergeCell ref="A141:A145"/>
+    <mergeCell ref="A146:A150"/>
+    <mergeCell ref="A151:A155"/>
+    <mergeCell ref="A156:A160"/>
+    <mergeCell ref="A161:A165"/>
+    <mergeCell ref="A60:A65"/>
+    <mergeCell ref="A66:A70"/>
+    <mergeCell ref="A47:A59"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A166:A170"/>
+    <mergeCell ref="A121:A125"/>
+    <mergeCell ref="A126:A130"/>
+    <mergeCell ref="A131:A135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="F48:F50"/>
+    <mergeCell ref="F51:F53"/>
+    <mergeCell ref="A106:A110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A120"/>
+    <mergeCell ref="A91:A95"/>
+    <mergeCell ref="A71:A75"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="A86:A90"/>
+    <mergeCell ref="A81:A85"/>
+    <mergeCell ref="A96:A100"/>
+    <mergeCell ref="A101:A105"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="A34:A46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="F31:F33"/>
     <mergeCell ref="F60:F61"/>
     <mergeCell ref="F54:F58"/>
     <mergeCell ref="A1:N1"/>
@@ -6183,50 +6259,6 @@
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="A34:A46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="A19:A33"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="A86:A90"/>
-    <mergeCell ref="A81:A85"/>
-    <mergeCell ref="A96:A100"/>
-    <mergeCell ref="A101:A105"/>
-    <mergeCell ref="A60:A65"/>
-    <mergeCell ref="A66:A70"/>
-    <mergeCell ref="A47:A59"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="A166:A170"/>
-    <mergeCell ref="A121:A125"/>
-    <mergeCell ref="A126:A130"/>
-    <mergeCell ref="A131:A135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="F48:F50"/>
-    <mergeCell ref="F51:F53"/>
-    <mergeCell ref="A106:A110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A120"/>
-    <mergeCell ref="A91:A95"/>
-    <mergeCell ref="A71:A75"/>
-    <mergeCell ref="A171:A175"/>
-    <mergeCell ref="A176:A180"/>
-    <mergeCell ref="A181:A185"/>
-    <mergeCell ref="A141:A145"/>
-    <mergeCell ref="A146:A150"/>
-    <mergeCell ref="A151:A155"/>
-    <mergeCell ref="A156:A160"/>
-    <mergeCell ref="A161:A165"/>
   </mergeCells>
   <conditionalFormatting sqref="M7">
     <cfRule type="cellIs" dxfId="3" priority="11" operator="greaterThan">

</xml_diff>

<commit_message>
effort 18/12 khang huynh
</commit_message>
<xml_diff>
--- a/1. Project management/9. Timelog/individual time log/AS_PM_TimeLog_DeadlineTeam_KhangHuynh.xlsx
+++ b/1. Project management/9. Timelog/individual time log/AS_PM_TimeLog_DeadlineTeam_KhangHuynh.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="204">
   <si>
     <t>Week</t>
   </si>
@@ -719,6 +719,14 @@
   </si>
   <si>
     <t>Training validation with spring in Java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update requirement plan
+Create weekly report 5
+</t>
+  </si>
+  <si>
+    <t>Update Architecture Drivers Specification</t>
   </si>
 </sst>
 </file>
@@ -1275,21 +1283,84 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="8" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1406,69 +1477,6 @@
     </xf>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1780,7 +1788,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1903,10 +1911,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O199"/>
+  <dimension ref="A1:O200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="6" topLeftCell="G70" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="6" ySplit="6" topLeftCell="G67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="H73" sqref="H73"/>
@@ -1931,81 +1939,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="89"/>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="91"/>
+      <c r="A1" s="110"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="112"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A2" s="105" t="s">
+      <c r="A2" s="126" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="92" t="s">
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="113" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="93"/>
-      <c r="N2" s="94"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="114"/>
+      <c r="M2" s="114"/>
+      <c r="N2" s="115"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="129" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="109"/>
-      <c r="C3" s="109"/>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="97"/>
+      <c r="B3" s="130"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="117"/>
+      <c r="I3" s="117"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="117"/>
+      <c r="L3" s="117"/>
+      <c r="M3" s="117"/>
+      <c r="N3" s="118"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="111"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="113"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="99"/>
-      <c r="N4" s="100"/>
+      <c r="A4" s="132"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="133"/>
+      <c r="D4" s="133"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="134"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="120"/>
+      <c r="I4" s="120"/>
+      <c r="J4" s="120"/>
+      <c r="K4" s="120"/>
+      <c r="L4" s="120"/>
+      <c r="M4" s="120"/>
+      <c r="N4" s="121"/>
     </row>
     <row r="5" spans="1:15" ht="39" customHeight="1">
-      <c r="A5" s="118"/>
-      <c r="B5" s="119"/>
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="120"/>
+      <c r="A5" s="139"/>
+      <c r="B5" s="140"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="141"/>
       <c r="F5" s="15"/>
       <c r="H5" s="41" t="s">
         <v>64</v>
@@ -2050,13 +2058,13 @@
       <c r="J6" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="104"/>
-      <c r="L6" s="104"/>
-      <c r="M6" s="104"/>
-      <c r="N6" s="104"/>
+      <c r="K6" s="125"/>
+      <c r="L6" s="125"/>
+      <c r="M6" s="125"/>
+      <c r="N6" s="125"/>
     </row>
     <row r="7" spans="1:15" ht="38.25">
-      <c r="A7" s="101">
+      <c r="A7" s="122">
         <v>1</v>
       </c>
       <c r="B7" s="16">
@@ -2082,12 +2090,12 @@
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="29"/>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="128"/>
+      <c r="L7" s="101"/>
       <c r="M7" s="32">
-        <f>SUM(M8:M73)</f>
+        <f>SUM(M8:M74)</f>
         <v>97.68</v>
       </c>
       <c r="N7" s="3" t="s">
@@ -2095,8 +2103,8 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="25.5">
-      <c r="A8" s="102"/>
-      <c r="B8" s="114">
+      <c r="A8" s="123"/>
+      <c r="B8" s="135">
         <v>41586</v>
       </c>
       <c r="C8" s="17">
@@ -2108,7 +2116,7 @@
       <c r="E8" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="116">
+      <c r="F8" s="137">
         <v>1.67</v>
       </c>
       <c r="G8" s="19" t="s">
@@ -2132,8 +2140,8 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="103"/>
-      <c r="B9" s="115"/>
+      <c r="A9" s="124"/>
+      <c r="B9" s="136"/>
       <c r="C9" s="17">
         <v>0.63194444444444442</v>
       </c>
@@ -2143,7 +2151,7 @@
       <c r="E9" s="18">
         <v>0.5</v>
       </c>
-      <c r="F9" s="117"/>
+      <c r="F9" s="138"/>
       <c r="G9" s="29" t="s">
         <v>23</v>
       </c>
@@ -2154,10 +2162,10 @@
       <c r="J9" s="29"/>
     </row>
     <row r="10" spans="1:15" s="63" customFormat="1">
-      <c r="A10" s="121">
+      <c r="A10" s="142">
         <v>2</v>
       </c>
-      <c r="B10" s="124">
+      <c r="B10" s="145">
         <v>41589</v>
       </c>
       <c r="C10" s="58" t="s">
@@ -2169,7 +2177,7 @@
       <c r="E10" s="59">
         <v>2.5</v>
       </c>
-      <c r="F10" s="126">
+      <c r="F10" s="147">
         <f>SUM(E10:E11)</f>
         <v>5</v>
       </c>
@@ -2183,8 +2191,8 @@
       <c r="J10" s="60"/>
     </row>
     <row r="11" spans="1:15" s="63" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A11" s="122"/>
-      <c r="B11" s="125"/>
+      <c r="A11" s="143"/>
+      <c r="B11" s="146"/>
       <c r="C11" s="58" t="s">
         <v>76</v>
       </c>
@@ -2194,7 +2202,7 @@
       <c r="E11" s="59">
         <v>2.5</v>
       </c>
-      <c r="F11" s="127"/>
+      <c r="F11" s="148"/>
       <c r="G11" s="60" t="s">
         <v>22</v>
       </c>
@@ -2207,8 +2215,8 @@
       <c r="J11" s="60"/>
     </row>
     <row r="12" spans="1:15" ht="51">
-      <c r="A12" s="122"/>
-      <c r="B12" s="129">
+      <c r="A12" s="143"/>
+      <c r="B12" s="102">
         <v>41590</v>
       </c>
       <c r="C12" s="22">
@@ -2220,7 +2228,7 @@
       <c r="E12" s="23">
         <v>2.25</v>
       </c>
-      <c r="F12" s="131">
+      <c r="F12" s="104">
         <v>3.75</v>
       </c>
       <c r="G12" s="30" t="s">
@@ -2247,8 +2255,8 @@
       <c r="O12" s="34"/>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A13" s="122"/>
-      <c r="B13" s="130"/>
+      <c r="A13" s="143"/>
+      <c r="B13" s="103"/>
       <c r="C13" s="22">
         <v>0.91666666666666663</v>
       </c>
@@ -2258,7 +2266,7 @@
       <c r="E13" s="23">
         <v>1.5</v>
       </c>
-      <c r="F13" s="132"/>
+      <c r="F13" s="105"/>
       <c r="G13" s="45" t="s">
         <v>28</v>
       </c>
@@ -2274,8 +2282,8 @@
       <c r="O13" s="34"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A14" s="122"/>
-      <c r="B14" s="129">
+      <c r="A14" s="143"/>
+      <c r="B14" s="102">
         <v>41591</v>
       </c>
       <c r="C14" s="22">
@@ -2287,7 +2295,7 @@
       <c r="E14" s="23">
         <v>2</v>
       </c>
-      <c r="F14" s="134">
+      <c r="F14" s="107">
         <v>4.5</v>
       </c>
       <c r="G14" s="45" t="s">
@@ -2305,8 +2313,8 @@
       <c r="O14" s="34"/>
     </row>
     <row r="15" spans="1:15" ht="25.5">
-      <c r="A15" s="122"/>
-      <c r="B15" s="133"/>
+      <c r="A15" s="143"/>
+      <c r="B15" s="106"/>
       <c r="C15" s="25">
         <v>0.5625</v>
       </c>
@@ -2316,7 +2324,7 @@
       <c r="E15" s="28">
         <v>2</v>
       </c>
-      <c r="F15" s="135"/>
+      <c r="F15" s="108"/>
       <c r="G15" s="30" t="s">
         <v>19</v>
       </c>
@@ -2333,8 +2341,8 @@
       <c r="N15" s="3"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A16" s="122"/>
-      <c r="B16" s="130"/>
+      <c r="A16" s="143"/>
+      <c r="B16" s="103"/>
       <c r="C16" s="25">
         <v>0.83333333333333337</v>
       </c>
@@ -2344,7 +2352,7 @@
       <c r="E16" s="28">
         <v>0.5</v>
       </c>
-      <c r="F16" s="136"/>
+      <c r="F16" s="109"/>
       <c r="G16" s="45" t="s">
         <v>28</v>
       </c>
@@ -2368,7 +2376,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A17" s="122"/>
+      <c r="A17" s="143"/>
       <c r="B17" s="47">
         <v>41592</v>
       </c>
@@ -2407,7 +2415,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="25.5">
-      <c r="A18" s="123"/>
+      <c r="A18" s="144"/>
       <c r="B18" s="42">
         <v>41593</v>
       </c>
@@ -2446,10 +2454,10 @@
       </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="140">
+      <c r="A19" s="95">
         <v>3</v>
       </c>
-      <c r="B19" s="137">
+      <c r="B19" s="93">
         <v>41596</v>
       </c>
       <c r="C19" s="53" t="s">
@@ -2461,7 +2469,7 @@
       <c r="E19" s="50">
         <v>0.5</v>
       </c>
-      <c r="F19" s="86">
+      <c r="F19" s="92">
         <f>SUM(E19:E20)</f>
         <v>3.5</v>
       </c>
@@ -2480,7 +2488,7 @@
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="9">
-        <f>SUM(E76:E80)</f>
+        <f>SUM(E77:E81)</f>
         <v>0</v>
       </c>
       <c r="N19" s="3" t="s">
@@ -2488,8 +2496,8 @@
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="141"/>
-      <c r="B20" s="138"/>
+      <c r="A20" s="96"/>
+      <c r="B20" s="94"/>
       <c r="C20" s="53" t="s">
         <v>81</v>
       </c>
@@ -2499,7 +2507,7 @@
       <c r="E20" s="50">
         <v>3</v>
       </c>
-      <c r="F20" s="139"/>
+      <c r="F20" s="88"/>
       <c r="G20" s="49" t="s">
         <v>22</v>
       </c>
@@ -2516,8 +2524,8 @@
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="141"/>
-      <c r="B21" s="137">
+      <c r="A21" s="96"/>
+      <c r="B21" s="93">
         <v>41597</v>
       </c>
       <c r="C21" s="53" t="s">
@@ -2529,7 +2537,7 @@
       <c r="E21" s="50">
         <v>2</v>
       </c>
-      <c r="F21" s="86">
+      <c r="F21" s="92">
         <f>SUM(E21:E22)</f>
         <v>2.5</v>
       </c>
@@ -2549,8 +2557,8 @@
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="141"/>
-      <c r="B22" s="138"/>
+      <c r="A22" s="96"/>
+      <c r="B22" s="94"/>
       <c r="C22" s="53" t="s">
         <v>84</v>
       </c>
@@ -2560,7 +2568,7 @@
       <c r="E22" s="50">
         <v>0.5</v>
       </c>
-      <c r="F22" s="139"/>
+      <c r="F22" s="88"/>
       <c r="G22" s="49" t="s">
         <v>22</v>
       </c>
@@ -2576,7 +2584,7 @@
       </c>
       <c r="L22" s="5"/>
       <c r="M22" s="9">
-        <f>SUM(E81:E85)</f>
+        <f>SUM(E82:E86)</f>
         <v>0</v>
       </c>
       <c r="N22" s="3" t="s">
@@ -2584,7 +2592,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="26.25">
-      <c r="A23" s="141"/>
+      <c r="A23" s="96"/>
       <c r="B23" s="26">
         <v>41598</v>
       </c>
@@ -2598,7 +2606,7 @@
         <v>4</v>
       </c>
       <c r="F23" s="55">
-        <f t="shared" ref="F23:F82" si="0">E23</f>
+        <f t="shared" ref="F23:F83" si="0">E23</f>
         <v>4</v>
       </c>
       <c r="G23" s="57" t="s">
@@ -2616,7 +2624,7 @@
       </c>
       <c r="L23" s="5"/>
       <c r="M23" s="9">
-        <f>SUM(E86:E90)</f>
+        <f>SUM(E87:E91)</f>
         <v>0</v>
       </c>
       <c r="N23" s="3" t="s">
@@ -2624,7 +2632,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="26.25">
-      <c r="A24" s="141"/>
+      <c r="A24" s="96"/>
       <c r="B24" s="26">
         <v>41599</v>
       </c>
@@ -2637,7 +2645,7 @@
       <c r="E24" s="50">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F24" s="86">
+      <c r="F24" s="92">
         <f>SUM(E24:E28)</f>
         <v>7.0600000000000005</v>
       </c>
@@ -2655,7 +2663,7 @@
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="141"/>
+      <c r="A25" s="96"/>
       <c r="B25" s="26">
         <v>41599</v>
       </c>
@@ -2668,7 +2676,7 @@
       <c r="E25" s="50">
         <v>1.3</v>
       </c>
-      <c r="F25" s="87"/>
+      <c r="F25" s="98"/>
       <c r="G25" s="57" t="s">
         <v>19</v>
       </c>
@@ -2683,7 +2691,7 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="141"/>
+      <c r="A26" s="96"/>
       <c r="B26" s="26">
         <v>41599</v>
       </c>
@@ -2696,7 +2704,7 @@
       <c r="E26" s="50">
         <v>1.5</v>
       </c>
-      <c r="F26" s="87"/>
+      <c r="F26" s="98"/>
       <c r="G26" s="57" t="s">
         <v>24</v>
       </c>
@@ -2713,7 +2721,7 @@
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="141"/>
+      <c r="A27" s="96"/>
       <c r="B27" s="26">
         <v>41599</v>
       </c>
@@ -2726,7 +2734,7 @@
       <c r="E27" s="50">
         <v>2.1</v>
       </c>
-      <c r="F27" s="87"/>
+      <c r="F27" s="98"/>
       <c r="G27" s="29" t="s">
         <v>19</v>
       </c>
@@ -2740,7 +2748,7 @@
       </c>
       <c r="L27" s="5"/>
       <c r="M27" s="9">
-        <f>SUM(E91:E95)</f>
+        <f>SUM(E92:E96)</f>
         <v>0</v>
       </c>
       <c r="N27" s="3" t="s">
@@ -2748,7 +2756,7 @@
       </c>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="141"/>
+      <c r="A28" s="96"/>
       <c r="B28" s="26">
         <v>41599</v>
       </c>
@@ -2761,7 +2769,7 @@
       <c r="E28" s="50">
         <v>1</v>
       </c>
-      <c r="F28" s="88"/>
+      <c r="F28" s="99"/>
       <c r="G28" s="29" t="s">
         <v>22</v>
       </c>
@@ -2776,7 +2784,7 @@
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="141"/>
+      <c r="A29" s="96"/>
       <c r="B29" s="26">
         <v>41600</v>
       </c>
@@ -2789,7 +2797,7 @@
       <c r="E29" s="50">
         <v>1.25</v>
       </c>
-      <c r="F29" s="86">
+      <c r="F29" s="92">
         <f>SUM(E29:E30)</f>
         <v>3.25</v>
       </c>
@@ -2805,7 +2813,7 @@
       <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:14" ht="51">
-      <c r="A30" s="141"/>
+      <c r="A30" s="96"/>
       <c r="B30" s="26">
         <v>41600</v>
       </c>
@@ -2818,7 +2826,7 @@
       <c r="E30" s="50">
         <v>2</v>
       </c>
-      <c r="F30" s="139"/>
+      <c r="F30" s="88"/>
       <c r="G30" s="57" t="s">
         <v>22</v>
       </c>
@@ -2832,7 +2840,7 @@
       </c>
       <c r="L30" s="5"/>
       <c r="M30" s="9">
-        <f>SUM(E96:E100)</f>
+        <f>SUM(E97:E101)</f>
         <v>0</v>
       </c>
       <c r="N30" s="3" t="s">
@@ -2840,7 +2848,7 @@
       </c>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="141"/>
+      <c r="A31" s="96"/>
       <c r="B31" s="26">
         <v>41601</v>
       </c>
@@ -2853,7 +2861,7 @@
       <c r="E31" s="74">
         <v>0.25</v>
       </c>
-      <c r="F31" s="86">
+      <c r="F31" s="92">
         <f>SUM(E31:E33)</f>
         <v>4.6500000000000004</v>
       </c>
@@ -2867,7 +2875,7 @@
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="141"/>
+      <c r="A32" s="96"/>
       <c r="B32" s="26">
         <v>41601</v>
       </c>
@@ -2880,7 +2888,7 @@
       <c r="E32" s="50">
         <v>3.5</v>
       </c>
-      <c r="F32" s="87"/>
+      <c r="F32" s="98"/>
       <c r="G32" s="57" t="s">
         <v>22</v>
       </c>
@@ -2897,7 +2905,7 @@
       <c r="N32" s="3"/>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33" s="142"/>
+      <c r="A33" s="97"/>
       <c r="B33" s="26">
         <v>41601</v>
       </c>
@@ -2910,7 +2918,7 @@
       <c r="E33" s="50">
         <v>0.9</v>
       </c>
-      <c r="F33" s="88"/>
+      <c r="F33" s="99"/>
       <c r="G33" s="57" t="s">
         <v>22</v>
       </c>
@@ -2961,7 +2969,7 @@
       </c>
       <c r="L34" s="5"/>
       <c r="M34" s="9">
-        <f>SUM(E101:E105)</f>
+        <f>SUM(E102:E106)</f>
         <v>0</v>
       </c>
       <c r="N34" s="3" t="s">
@@ -2969,7 +2977,7 @@
       </c>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="85"/>
+      <c r="A35" s="84"/>
       <c r="B35" s="27">
         <v>41604</v>
       </c>
@@ -2982,7 +2990,7 @@
       <c r="E35" s="28">
         <v>1</v>
       </c>
-      <c r="F35" s="143">
+      <c r="F35" s="100">
         <f>SUM(E35:E38)</f>
         <v>6.75</v>
       </c>
@@ -3000,7 +3008,7 @@
       <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="85"/>
+      <c r="A36" s="84"/>
       <c r="B36" s="27">
         <v>41604</v>
       </c>
@@ -3013,7 +3021,7 @@
       <c r="E36" s="76">
         <v>2.5</v>
       </c>
-      <c r="F36" s="85"/>
+      <c r="F36" s="84"/>
       <c r="G36" s="67" t="s">
         <v>23</v>
       </c>
@@ -3030,7 +3038,7 @@
       <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="85"/>
+      <c r="A37" s="84"/>
       <c r="B37" s="27">
         <v>41604</v>
       </c>
@@ -3043,7 +3051,7 @@
       <c r="E37" s="76">
         <v>1.25</v>
       </c>
-      <c r="F37" s="85"/>
+      <c r="F37" s="84"/>
       <c r="G37" s="67" t="s">
         <v>24</v>
       </c>
@@ -3060,7 +3068,7 @@
       <c r="N37" s="3"/>
     </row>
     <row r="38" spans="1:14" ht="38.25">
-      <c r="A38" s="85"/>
+      <c r="A38" s="84"/>
       <c r="B38" s="27">
         <v>41604</v>
       </c>
@@ -3073,7 +3081,7 @@
       <c r="E38" s="69">
         <v>2</v>
       </c>
-      <c r="F38" s="84"/>
+      <c r="F38" s="85"/>
       <c r="G38" s="67" t="s">
         <v>22</v>
       </c>
@@ -3091,7 +3099,7 @@
       </c>
       <c r="L38" s="5"/>
       <c r="M38" s="9">
-        <f>SUM(E106:E110)</f>
+        <f>SUM(E107:E111)</f>
         <v>0</v>
       </c>
       <c r="N38" s="3" t="s">
@@ -3099,7 +3107,7 @@
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="85"/>
+      <c r="A39" s="84"/>
       <c r="B39" s="27">
         <v>41605</v>
       </c>
@@ -3129,7 +3137,7 @@
       </c>
       <c r="L39" s="5"/>
       <c r="M39" s="9">
-        <f>SUM(E111:E115)</f>
+        <f>SUM(E112:E116)</f>
         <v>0</v>
       </c>
       <c r="N39" s="3" t="s">
@@ -3137,7 +3145,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" ht="25.5">
-      <c r="A40" s="85"/>
+      <c r="A40" s="84"/>
       <c r="B40" s="27">
         <v>41605</v>
       </c>
@@ -3150,7 +3158,7 @@
       <c r="E40" s="69">
         <v>0.5</v>
       </c>
-      <c r="F40" s="84"/>
+      <c r="F40" s="85"/>
       <c r="G40" s="67" t="s">
         <v>24</v>
       </c>
@@ -3167,7 +3175,7 @@
       <c r="N40" s="3"/>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="85"/>
+      <c r="A41" s="84"/>
       <c r="B41" s="27">
         <v>41606</v>
       </c>
@@ -3198,7 +3206,7 @@
       <c r="N41" s="3"/>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="85"/>
+      <c r="A42" s="84"/>
       <c r="B42" s="27">
         <v>41606</v>
       </c>
@@ -3211,7 +3219,7 @@
       <c r="E42" s="69">
         <v>1.75</v>
       </c>
-      <c r="F42" s="85"/>
+      <c r="F42" s="84"/>
       <c r="G42" s="67" t="s">
         <v>25</v>
       </c>
@@ -3226,7 +3234,7 @@
       <c r="N42" s="3"/>
     </row>
     <row r="43" spans="1:14" ht="25.5">
-      <c r="A43" s="85"/>
+      <c r="A43" s="84"/>
       <c r="B43" s="27">
         <v>41606</v>
       </c>
@@ -3239,7 +3247,7 @@
       <c r="E43" s="69">
         <v>2.75</v>
       </c>
-      <c r="F43" s="84"/>
+      <c r="F43" s="85"/>
       <c r="G43" s="67" t="s">
         <v>19</v>
       </c>
@@ -3255,7 +3263,7 @@
       </c>
       <c r="L43" s="5"/>
       <c r="M43" s="9">
-        <f>SUM(E116:E120)</f>
+        <f>SUM(E117:E121)</f>
         <v>0</v>
       </c>
       <c r="N43" s="3" t="s">
@@ -3263,7 +3271,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" ht="51">
-      <c r="A44" s="85"/>
+      <c r="A44" s="84"/>
       <c r="B44" s="27">
         <v>41607</v>
       </c>
@@ -3295,7 +3303,7 @@
       </c>
       <c r="L44" s="5"/>
       <c r="M44" s="9">
-        <f>SUM(E121:E125)</f>
+        <f>SUM(E122:E126)</f>
         <v>0</v>
       </c>
       <c r="N44" s="3" t="s">
@@ -3303,7 +3311,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" ht="38.25">
-      <c r="A45" s="85"/>
+      <c r="A45" s="84"/>
       <c r="B45" s="27">
         <v>41609</v>
       </c>
@@ -3336,7 +3344,7 @@
       <c r="N45" s="3"/>
     </row>
     <row r="46" spans="1:14" ht="25.5">
-      <c r="A46" s="84"/>
+      <c r="A46" s="85"/>
       <c r="B46" s="27">
         <v>41609</v>
       </c>
@@ -3349,7 +3357,7 @@
       <c r="E46" s="69">
         <v>2</v>
       </c>
-      <c r="F46" s="84"/>
+      <c r="F46" s="85"/>
       <c r="G46" s="67" t="s">
         <v>22</v>
       </c>
@@ -3368,7 +3376,7 @@
       <c r="N46" s="3"/>
     </row>
     <row r="47" spans="1:14" ht="63.75">
-      <c r="A47" s="144">
+      <c r="A47" s="86">
         <v>5</v>
       </c>
       <c r="B47" s="26">
@@ -3400,7 +3408,7 @@
       </c>
       <c r="L47" s="5"/>
       <c r="M47" s="9">
-        <f>SUM(E126:E130)</f>
+        <f>SUM(E127:E131)</f>
         <v>0</v>
       </c>
       <c r="N47" s="3" t="s">
@@ -3408,7 +3416,7 @@
       </c>
     </row>
     <row r="48" spans="1:14" ht="38.25">
-      <c r="A48" s="145"/>
+      <c r="A48" s="87"/>
       <c r="B48" s="26">
         <v>41611</v>
       </c>
@@ -3421,7 +3429,7 @@
       <c r="E48" s="55">
         <v>1.5</v>
       </c>
-      <c r="F48" s="144">
+      <c r="F48" s="86">
         <f>SUM(E48:E50)</f>
         <v>7</v>
       </c>
@@ -3439,7 +3447,7 @@
       <c r="N48" s="3"/>
     </row>
     <row r="49" spans="1:14" ht="51.75" customHeight="1">
-      <c r="A49" s="145"/>
+      <c r="A49" s="87"/>
       <c r="B49" s="26">
         <v>41611</v>
       </c>
@@ -3452,7 +3460,7 @@
       <c r="E49" s="55">
         <v>3.5</v>
       </c>
-      <c r="F49" s="145"/>
+      <c r="F49" s="87"/>
       <c r="G49" s="29" t="s">
         <v>27</v>
       </c>
@@ -3466,7 +3474,7 @@
       </c>
       <c r="L49" s="5"/>
       <c r="M49" s="9">
-        <f>SUM(E131:E135)</f>
+        <f>SUM(E132:E136)</f>
         <v>0</v>
       </c>
       <c r="N49" s="3" t="s">
@@ -3474,7 +3482,7 @@
       </c>
     </row>
     <row r="50" spans="1:14" ht="38.25">
-      <c r="A50" s="145"/>
+      <c r="A50" s="87"/>
       <c r="B50" s="26">
         <v>41611</v>
       </c>
@@ -3487,7 +3495,7 @@
       <c r="E50" s="55">
         <v>2</v>
       </c>
-      <c r="F50" s="139"/>
+      <c r="F50" s="88"/>
       <c r="G50" s="29" t="s">
         <v>22</v>
       </c>
@@ -3506,7 +3514,7 @@
       <c r="N50" s="3"/>
     </row>
     <row r="51" spans="1:14" ht="38.25">
-      <c r="A51" s="145"/>
+      <c r="A51" s="87"/>
       <c r="B51" s="26">
         <v>41612</v>
       </c>
@@ -3519,7 +3527,7 @@
       <c r="E51" s="55">
         <v>0.75</v>
       </c>
-      <c r="F51" s="144">
+      <c r="F51" s="86">
         <f>SUM(E52:E53)</f>
         <v>6.5</v>
       </c>
@@ -3540,7 +3548,7 @@
       </c>
       <c r="L51" s="5"/>
       <c r="M51" s="9">
-        <f>SUM(E136:E140)</f>
+        <f>SUM(E137:E141)</f>
         <v>0</v>
       </c>
       <c r="N51" s="3" t="s">
@@ -3548,7 +3556,7 @@
       </c>
     </row>
     <row r="52" spans="1:14" ht="76.5">
-      <c r="A52" s="145"/>
+      <c r="A52" s="87"/>
       <c r="B52" s="26">
         <v>41612</v>
       </c>
@@ -3561,7 +3569,7 @@
       <c r="E52" s="55">
         <v>4.5</v>
       </c>
-      <c r="F52" s="145"/>
+      <c r="F52" s="87"/>
       <c r="G52" s="29" t="s">
         <v>19</v>
       </c>
@@ -3576,7 +3584,7 @@
       <c r="N52" s="3"/>
     </row>
     <row r="53" spans="1:14" ht="38.25">
-      <c r="A53" s="145"/>
+      <c r="A53" s="87"/>
       <c r="B53" s="26">
         <v>41612</v>
       </c>
@@ -3589,7 +3597,7 @@
       <c r="E53" s="55">
         <v>2</v>
       </c>
-      <c r="F53" s="139"/>
+      <c r="F53" s="88"/>
       <c r="G53" s="29" t="s">
         <v>22</v>
       </c>
@@ -3606,7 +3614,7 @@
       <c r="N53" s="3"/>
     </row>
     <row r="54" spans="1:14" ht="38.25">
-      <c r="A54" s="145"/>
+      <c r="A54" s="87"/>
       <c r="B54" s="26">
         <v>41613</v>
       </c>
@@ -3619,7 +3627,7 @@
       <c r="E54" s="74">
         <v>3</v>
       </c>
-      <c r="F54" s="86">
+      <c r="F54" s="92">
         <f>SUM(E54:E58)</f>
         <v>7.82</v>
       </c>
@@ -3637,7 +3645,7 @@
       <c r="N54" s="3"/>
     </row>
     <row r="55" spans="1:14">
-      <c r="A55" s="145"/>
+      <c r="A55" s="87"/>
       <c r="B55" s="26">
         <v>41613</v>
       </c>
@@ -3650,7 +3658,7 @@
       <c r="E55" s="74">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F55" s="87"/>
+      <c r="F55" s="98"/>
       <c r="G55" s="29" t="s">
         <v>24</v>
       </c>
@@ -3665,7 +3673,7 @@
       <c r="N55" s="3"/>
     </row>
     <row r="56" spans="1:14" ht="51">
-      <c r="A56" s="145"/>
+      <c r="A56" s="87"/>
       <c r="B56" s="26">
         <v>41613</v>
       </c>
@@ -3678,7 +3686,7 @@
       <c r="E56" s="74">
         <v>1.5</v>
       </c>
-      <c r="F56" s="87"/>
+      <c r="F56" s="98"/>
       <c r="G56" s="29" t="s">
         <v>23</v>
       </c>
@@ -3693,7 +3701,7 @@
       <c r="N56" s="3"/>
     </row>
     <row r="57" spans="1:14" ht="25.5">
-      <c r="A57" s="145"/>
+      <c r="A57" s="87"/>
       <c r="B57" s="26">
         <v>41613</v>
       </c>
@@ -3706,7 +3714,7 @@
       <c r="E57" s="74">
         <v>0.66</v>
       </c>
-      <c r="F57" s="87"/>
+      <c r="F57" s="98"/>
       <c r="G57" s="29" t="s">
         <v>19</v>
       </c>
@@ -3721,7 +3729,7 @@
       <c r="N57" s="3"/>
     </row>
     <row r="58" spans="1:14" ht="25.5">
-      <c r="A58" s="145"/>
+      <c r="A58" s="87"/>
       <c r="B58" s="26">
         <v>41613</v>
       </c>
@@ -3734,7 +3742,7 @@
       <c r="E58" s="74">
         <v>1.5</v>
       </c>
-      <c r="F58" s="88"/>
+      <c r="F58" s="99"/>
       <c r="G58" s="29" t="s">
         <v>24</v>
       </c>
@@ -3748,7 +3756,7 @@
       </c>
       <c r="L58" s="5"/>
       <c r="M58" s="9">
-        <f>SUM(E141:E145)</f>
+        <f>SUM(E142:E146)</f>
         <v>0</v>
       </c>
       <c r="N58" s="3" t="s">
@@ -3756,7 +3764,7 @@
       </c>
     </row>
     <row r="59" spans="1:14" ht="76.5">
-      <c r="A59" s="139"/>
+      <c r="A59" s="88"/>
       <c r="B59" s="26">
         <v>41616</v>
       </c>
@@ -3790,7 +3798,7 @@
       </c>
       <c r="L59" s="5"/>
       <c r="M59" s="9">
-        <f>SUM(E146:E150)</f>
+        <f>SUM(E147:E151)</f>
         <v>0</v>
       </c>
       <c r="N59" s="3" t="s">
@@ -3834,7 +3842,7 @@
       </c>
       <c r="L60" s="5"/>
       <c r="M60" s="9">
-        <f>SUM(E151:E155)</f>
+        <f>SUM(E152:E156)</f>
         <v>0</v>
       </c>
       <c r="N60" s="3" t="s">
@@ -3842,7 +3850,7 @@
       </c>
     </row>
     <row r="61" spans="1:14" ht="51">
-      <c r="A61" s="85"/>
+      <c r="A61" s="84"/>
       <c r="B61" s="27">
         <v>41617</v>
       </c>
@@ -3855,7 +3863,7 @@
       <c r="E61" s="69">
         <v>2</v>
       </c>
-      <c r="F61" s="84"/>
+      <c r="F61" s="85"/>
       <c r="G61" s="67" t="s">
         <v>22</v>
       </c>
@@ -3872,7 +3880,7 @@
       <c r="N61" s="3"/>
     </row>
     <row r="62" spans="1:14" ht="38.25">
-      <c r="A62" s="85"/>
+      <c r="A62" s="84"/>
       <c r="B62" s="27">
         <v>41618</v>
       </c>
@@ -3902,7 +3910,7 @@
       </c>
       <c r="L62" s="5"/>
       <c r="M62" s="9">
-        <f>SUM(E156:E160)</f>
+        <f>SUM(E157:E161)</f>
         <v>0</v>
       </c>
       <c r="N62" s="3" t="s">
@@ -3910,7 +3918,7 @@
       </c>
     </row>
     <row r="63" spans="1:14" ht="25.5">
-      <c r="A63" s="85"/>
+      <c r="A63" s="84"/>
       <c r="B63" s="27">
         <v>41619</v>
       </c>
@@ -3940,7 +3948,7 @@
       </c>
       <c r="L63" s="5"/>
       <c r="M63" s="9">
-        <f>SUM(E161:E165)</f>
+        <f>SUM(E162:E166)</f>
         <v>0</v>
       </c>
       <c r="N63" s="3" t="s">
@@ -3948,7 +3956,7 @@
       </c>
     </row>
     <row r="64" spans="1:14" ht="25.5">
-      <c r="A64" s="85"/>
+      <c r="A64" s="84"/>
       <c r="B64" s="27">
         <v>41620</v>
       </c>
@@ -3979,7 +3987,7 @@
       <c r="N64" s="3"/>
     </row>
     <row r="65" spans="1:14">
-      <c r="A65" s="85"/>
+      <c r="A65" s="84"/>
       <c r="B65" s="27">
         <v>41620</v>
       </c>
@@ -3992,7 +4000,7 @@
       <c r="E65" s="69">
         <v>1</v>
       </c>
-      <c r="F65" s="85"/>
+      <c r="F65" s="84"/>
       <c r="G65" s="67" t="s">
         <v>19</v>
       </c>
@@ -4007,7 +4015,7 @@
       <c r="N65" s="3"/>
     </row>
     <row r="66" spans="1:14">
-      <c r="A66" s="85"/>
+      <c r="A66" s="84"/>
       <c r="B66" s="27">
         <v>41620</v>
       </c>
@@ -4020,7 +4028,7 @@
       <c r="E66" s="69">
         <v>3</v>
       </c>
-      <c r="F66" s="84"/>
+      <c r="F66" s="85"/>
       <c r="G66" s="67" t="s">
         <v>25</v>
       </c>
@@ -4034,7 +4042,7 @@
       </c>
       <c r="L66" s="5"/>
       <c r="M66" s="9">
-        <f>SUM(E166:E170)</f>
+        <f>SUM(E167:E171)</f>
         <v>0</v>
       </c>
       <c r="N66" s="3" t="s">
@@ -4042,7 +4050,7 @@
       </c>
     </row>
     <row r="67" spans="1:14" ht="25.5">
-      <c r="A67" s="85"/>
+      <c r="A67" s="84"/>
       <c r="B67" s="27">
         <v>41621</v>
       </c>
@@ -4073,7 +4081,7 @@
       <c r="N67" s="3"/>
     </row>
     <row r="68" spans="1:14" ht="26.25">
-      <c r="A68" s="85"/>
+      <c r="A68" s="84"/>
       <c r="B68" s="27">
         <v>41621</v>
       </c>
@@ -4086,7 +4094,7 @@
       <c r="E68" s="69">
         <v>1</v>
       </c>
-      <c r="F68" s="84"/>
+      <c r="F68" s="85"/>
       <c r="G68" s="67" t="s">
         <v>22</v>
       </c>
@@ -4100,7 +4108,7 @@
       </c>
       <c r="L68" s="5"/>
       <c r="M68" s="9">
-        <f>SUM(E171:E175)</f>
+        <f>SUM(E172:E176)</f>
         <v>0</v>
       </c>
       <c r="N68" s="3" t="s">
@@ -4108,7 +4116,7 @@
       </c>
     </row>
     <row r="69" spans="1:14" ht="64.5">
-      <c r="A69" s="84"/>
+      <c r="A69" s="85"/>
       <c r="B69" s="27">
         <v>41623</v>
       </c>
@@ -4139,7 +4147,7 @@
       <c r="N69" s="3"/>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="144">
+      <c r="A70" s="86">
         <v>7</v>
       </c>
       <c r="B70" s="26">
@@ -4171,7 +4179,7 @@
       </c>
       <c r="L70" s="5"/>
       <c r="M70" s="9">
-        <f>SUM(E176:E180)</f>
+        <f>SUM(E177:E181)</f>
         <v>0</v>
       </c>
       <c r="N70" s="3" t="s">
@@ -4179,7 +4187,7 @@
       </c>
     </row>
     <row r="71" spans="1:14">
-      <c r="A71" s="145"/>
+      <c r="A71" s="87"/>
       <c r="B71" s="26">
         <v>41625</v>
       </c>
@@ -4192,23 +4200,29 @@
       <c r="E71" s="55">
         <v>2</v>
       </c>
-      <c r="F71" s="55">
-        <f t="shared" ref="F71" si="1">E71</f>
-        <v>2</v>
+      <c r="F71" s="86">
+        <f>SUM(E71:E73)</f>
+        <v>5</v>
       </c>
       <c r="G71" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="H71" s="29"/>
-      <c r="I71" s="29"/>
-      <c r="J71" s="29"/>
+      <c r="H71" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="I71" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="J71" s="29" t="s">
+        <v>200</v>
+      </c>
       <c r="K71" s="7"/>
       <c r="L71" s="5"/>
       <c r="M71" s="9"/>
       <c r="N71" s="3"/>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="145"/>
+      <c r="A72" s="87"/>
       <c r="B72" s="26">
         <v>41625</v>
       </c>
@@ -4221,56 +4235,49 @@
       <c r="E72" s="55">
         <v>2</v>
       </c>
-      <c r="F72" s="55">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
+      <c r="F72" s="87"/>
       <c r="G72" s="29" t="s">
         <v>27</v>
       </c>
       <c r="H72" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="I72" s="29" t="s">
-        <v>199</v>
-      </c>
-      <c r="J72" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="K72" s="7" t="s">
-        <v>52</v>
-      </c>
+      <c r="I72" s="29"/>
+      <c r="J72" s="29"/>
+      <c r="K72" s="7"/>
       <c r="L72" s="5"/>
-      <c r="M72" s="9">
-        <f>SUM(E181:E185)</f>
-        <v>0</v>
-      </c>
-      <c r="N72" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14">
-      <c r="A73" s="145"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="3"/>
+    </row>
+    <row r="73" spans="1:14" ht="38.25">
+      <c r="A73" s="87"/>
       <c r="B73" s="26">
-        <v>41626</v>
-      </c>
-      <c r="C73" s="55"/>
-      <c r="D73" s="55"/>
-      <c r="E73" s="55"/>
-      <c r="F73" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G73" s="29"/>
-      <c r="H73" s="29"/>
+        <v>41625</v>
+      </c>
+      <c r="C73" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="D73" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="E73" s="55">
+        <v>1</v>
+      </c>
+      <c r="F73" s="88"/>
+      <c r="G73" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H73" s="65" t="s">
+        <v>202</v>
+      </c>
       <c r="I73" s="29"/>
       <c r="J73" s="29"/>
       <c r="K73" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L73" s="5"/>
       <c r="M73" s="9">
-        <f>SUM(E186:E190)</f>
+        <f>SUM(E182:E186)</f>
         <v>0</v>
       </c>
       <c r="N73" s="3" t="s">
@@ -4278,9 +4285,9 @@
       </c>
     </row>
     <row r="74" spans="1:14">
-      <c r="A74" s="145"/>
+      <c r="A74" s="87"/>
       <c r="B74" s="26">
-        <v>41627</v>
+        <v>41626</v>
       </c>
       <c r="C74" s="55"/>
       <c r="D74" s="55"/>
@@ -4293,11 +4300,22 @@
       <c r="H74" s="29"/>
       <c r="I74" s="29"/>
       <c r="J74" s="29"/>
+      <c r="K74" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L74" s="5"/>
+      <c r="M74" s="9">
+        <f>SUM(E187:E191)</f>
+        <v>0</v>
+      </c>
+      <c r="N74" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="75" spans="1:14">
-      <c r="A75" s="139"/>
+      <c r="A75" s="87"/>
       <c r="B75" s="26">
-        <v>41628</v>
+        <v>41627</v>
       </c>
       <c r="C75" s="55"/>
       <c r="D75" s="55"/>
@@ -4312,28 +4330,28 @@
       <c r="J75" s="29"/>
     </row>
     <row r="76" spans="1:14">
-      <c r="A76" s="83">
+      <c r="A76" s="88"/>
+      <c r="B76" s="26">
+        <v>41628</v>
+      </c>
+      <c r="C76" s="55"/>
+      <c r="D76" s="55"/>
+      <c r="E76" s="55"/>
+      <c r="F76" s="55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G76" s="29"/>
+      <c r="H76" s="29"/>
+      <c r="I76" s="29"/>
+      <c r="J76" s="29"/>
+    </row>
+    <row r="77" spans="1:14">
+      <c r="A77" s="83">
         <v>8</v>
       </c>
-      <c r="B76" s="27">
+      <c r="B77" s="27">
         <v>41631</v>
-      </c>
-      <c r="C76" s="69"/>
-      <c r="D76" s="69"/>
-      <c r="E76" s="69"/>
-      <c r="F76" s="69">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G76" s="67"/>
-      <c r="H76" s="67"/>
-      <c r="I76" s="67"/>
-      <c r="J76" s="67"/>
-    </row>
-    <row r="77" spans="1:14">
-      <c r="A77" s="85"/>
-      <c r="B77" s="27">
-        <v>41632</v>
       </c>
       <c r="C77" s="69"/>
       <c r="D77" s="69"/>
@@ -4348,9 +4366,9 @@
       <c r="J77" s="67"/>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="85"/>
+      <c r="A78" s="84"/>
       <c r="B78" s="27">
-        <v>41633</v>
+        <v>41632</v>
       </c>
       <c r="C78" s="69"/>
       <c r="D78" s="69"/>
@@ -4365,9 +4383,9 @@
       <c r="J78" s="67"/>
     </row>
     <row r="79" spans="1:14">
-      <c r="A79" s="85"/>
+      <c r="A79" s="84"/>
       <c r="B79" s="27">
-        <v>41634</v>
+        <v>41633</v>
       </c>
       <c r="C79" s="69"/>
       <c r="D79" s="69"/>
@@ -4384,7 +4402,7 @@
     <row r="80" spans="1:14">
       <c r="A80" s="84"/>
       <c r="B80" s="27">
-        <v>41635</v>
+        <v>41634</v>
       </c>
       <c r="C80" s="69"/>
       <c r="D80" s="69"/>
@@ -4399,28 +4417,28 @@
       <c r="J80" s="67"/>
     </row>
     <row r="81" spans="1:10">
-      <c r="A81" s="144">
+      <c r="A81" s="85"/>
+      <c r="B81" s="27">
+        <v>41635</v>
+      </c>
+      <c r="C81" s="69"/>
+      <c r="D81" s="69"/>
+      <c r="E81" s="69"/>
+      <c r="F81" s="69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G81" s="67"/>
+      <c r="H81" s="67"/>
+      <c r="I81" s="67"/>
+      <c r="J81" s="67"/>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="86">
         <v>9</v>
       </c>
-      <c r="B81" s="26">
+      <c r="B82" s="26">
         <v>41638</v>
-      </c>
-      <c r="C81" s="55"/>
-      <c r="D81" s="55"/>
-      <c r="E81" s="55"/>
-      <c r="F81" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G81" s="29"/>
-      <c r="H81" s="29"/>
-      <c r="I81" s="29"/>
-      <c r="J81" s="29"/>
-    </row>
-    <row r="82" spans="1:10">
-      <c r="A82" s="145"/>
-      <c r="B82" s="26">
-        <v>41639</v>
       </c>
       <c r="C82" s="55"/>
       <c r="D82" s="55"/>
@@ -4435,15 +4453,15 @@
       <c r="J82" s="29"/>
     </row>
     <row r="83" spans="1:10">
-      <c r="A83" s="145"/>
+      <c r="A83" s="87"/>
       <c r="B83" s="26">
-        <v>41640</v>
+        <v>41639</v>
       </c>
       <c r="C83" s="55"/>
       <c r="D83" s="55"/>
       <c r="E83" s="55"/>
       <c r="F83" s="55">
-        <f t="shared" ref="F83:F114" si="2">E83</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G83" s="29"/>
@@ -4452,15 +4470,15 @@
       <c r="J83" s="29"/>
     </row>
     <row r="84" spans="1:10">
-      <c r="A84" s="145"/>
+      <c r="A84" s="87"/>
       <c r="B84" s="26">
-        <v>41641</v>
+        <v>41640</v>
       </c>
       <c r="C84" s="55"/>
       <c r="D84" s="55"/>
       <c r="E84" s="55"/>
       <c r="F84" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F84:F115" si="1">E84</f>
         <v>0</v>
       </c>
       <c r="G84" s="29"/>
@@ -4469,15 +4487,15 @@
       <c r="J84" s="29"/>
     </row>
     <row r="85" spans="1:10">
-      <c r="A85" s="139"/>
+      <c r="A85" s="87"/>
       <c r="B85" s="26">
-        <v>41642</v>
+        <v>41641</v>
       </c>
       <c r="C85" s="55"/>
       <c r="D85" s="55"/>
       <c r="E85" s="55"/>
       <c r="F85" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G85" s="29"/>
@@ -4486,34 +4504,34 @@
       <c r="J85" s="29"/>
     </row>
     <row r="86" spans="1:10">
-      <c r="A86" s="83">
+      <c r="A86" s="88"/>
+      <c r="B86" s="26">
+        <v>41642</v>
+      </c>
+      <c r="C86" s="55"/>
+      <c r="D86" s="55"/>
+      <c r="E86" s="55"/>
+      <c r="F86" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G86" s="29"/>
+      <c r="H86" s="29"/>
+      <c r="I86" s="29"/>
+      <c r="J86" s="29"/>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="83">
         <v>10</v>
       </c>
-      <c r="B86" s="27">
+      <c r="B87" s="27">
         <v>41645</v>
-      </c>
-      <c r="C86" s="69"/>
-      <c r="D86" s="69"/>
-      <c r="E86" s="69"/>
-      <c r="F86" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G86" s="67"/>
-      <c r="H86" s="67"/>
-      <c r="I86" s="67"/>
-      <c r="J86" s="67"/>
-    </row>
-    <row r="87" spans="1:10">
-      <c r="A87" s="85"/>
-      <c r="B87" s="27">
-        <v>41646</v>
       </c>
       <c r="C87" s="69"/>
       <c r="D87" s="69"/>
       <c r="E87" s="69"/>
       <c r="F87" s="69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G87" s="67"/>
@@ -4522,15 +4540,15 @@
       <c r="J87" s="67"/>
     </row>
     <row r="88" spans="1:10">
-      <c r="A88" s="85"/>
+      <c r="A88" s="84"/>
       <c r="B88" s="27">
-        <v>41647</v>
+        <v>41646</v>
       </c>
       <c r="C88" s="69"/>
       <c r="D88" s="69"/>
       <c r="E88" s="69"/>
       <c r="F88" s="69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G88" s="67"/>
@@ -4539,15 +4557,15 @@
       <c r="J88" s="67"/>
     </row>
     <row r="89" spans="1:10">
-      <c r="A89" s="85"/>
+      <c r="A89" s="84"/>
       <c r="B89" s="27">
-        <v>41648</v>
+        <v>41647</v>
       </c>
       <c r="C89" s="69"/>
       <c r="D89" s="69"/>
       <c r="E89" s="69"/>
       <c r="F89" s="69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G89" s="67"/>
@@ -4558,13 +4576,13 @@
     <row r="90" spans="1:10">
       <c r="A90" s="84"/>
       <c r="B90" s="27">
-        <v>41649</v>
+        <v>41648</v>
       </c>
       <c r="C90" s="69"/>
       <c r="D90" s="69"/>
       <c r="E90" s="69"/>
       <c r="F90" s="69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G90" s="67"/>
@@ -4573,34 +4591,34 @@
       <c r="J90" s="67"/>
     </row>
     <row r="91" spans="1:10">
-      <c r="A91" s="144">
+      <c r="A91" s="85"/>
+      <c r="B91" s="27">
+        <v>41649</v>
+      </c>
+      <c r="C91" s="69"/>
+      <c r="D91" s="69"/>
+      <c r="E91" s="69"/>
+      <c r="F91" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G91" s="67"/>
+      <c r="H91" s="67"/>
+      <c r="I91" s="67"/>
+      <c r="J91" s="67"/>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" s="86">
         <v>11</v>
       </c>
-      <c r="B91" s="26">
+      <c r="B92" s="26">
         <v>41652</v>
-      </c>
-      <c r="C91" s="55"/>
-      <c r="D91" s="55"/>
-      <c r="E91" s="55"/>
-      <c r="F91" s="55">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G91" s="29"/>
-      <c r="H91" s="29"/>
-      <c r="I91" s="29"/>
-      <c r="J91" s="29"/>
-    </row>
-    <row r="92" spans="1:10">
-      <c r="A92" s="145"/>
-      <c r="B92" s="26">
-        <v>41653</v>
       </c>
       <c r="C92" s="55"/>
       <c r="D92" s="55"/>
       <c r="E92" s="55"/>
       <c r="F92" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G92" s="29"/>
@@ -4609,15 +4627,15 @@
       <c r="J92" s="29"/>
     </row>
     <row r="93" spans="1:10">
-      <c r="A93" s="145"/>
+      <c r="A93" s="87"/>
       <c r="B93" s="26">
-        <v>41654</v>
+        <v>41653</v>
       </c>
       <c r="C93" s="55"/>
       <c r="D93" s="55"/>
       <c r="E93" s="55"/>
       <c r="F93" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G93" s="29"/>
@@ -4626,15 +4644,15 @@
       <c r="J93" s="29"/>
     </row>
     <row r="94" spans="1:10">
-      <c r="A94" s="145"/>
+      <c r="A94" s="87"/>
       <c r="B94" s="26">
-        <v>41655</v>
+        <v>41654</v>
       </c>
       <c r="C94" s="55"/>
       <c r="D94" s="55"/>
       <c r="E94" s="55"/>
       <c r="F94" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G94" s="29"/>
@@ -4643,15 +4661,15 @@
       <c r="J94" s="29"/>
     </row>
     <row r="95" spans="1:10">
-      <c r="A95" s="139"/>
+      <c r="A95" s="87"/>
       <c r="B95" s="26">
-        <v>41656</v>
+        <v>41655</v>
       </c>
       <c r="C95" s="55"/>
       <c r="D95" s="55"/>
       <c r="E95" s="55"/>
       <c r="F95" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G95" s="29"/>
@@ -4660,34 +4678,34 @@
       <c r="J95" s="29"/>
     </row>
     <row r="96" spans="1:10">
-      <c r="A96" s="83">
+      <c r="A96" s="88"/>
+      <c r="B96" s="26">
+        <v>41656</v>
+      </c>
+      <c r="C96" s="55"/>
+      <c r="D96" s="55"/>
+      <c r="E96" s="55"/>
+      <c r="F96" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G96" s="29"/>
+      <c r="H96" s="29"/>
+      <c r="I96" s="29"/>
+      <c r="J96" s="29"/>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="83">
         <v>12</v>
       </c>
-      <c r="B96" s="27">
+      <c r="B97" s="27">
         <v>41659</v>
-      </c>
-      <c r="C96" s="69"/>
-      <c r="D96" s="69"/>
-      <c r="E96" s="69"/>
-      <c r="F96" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G96" s="67"/>
-      <c r="H96" s="67"/>
-      <c r="I96" s="67"/>
-      <c r="J96" s="67"/>
-    </row>
-    <row r="97" spans="1:10">
-      <c r="A97" s="85"/>
-      <c r="B97" s="27">
-        <v>41660</v>
       </c>
       <c r="C97" s="69"/>
       <c r="D97" s="69"/>
       <c r="E97" s="69"/>
       <c r="F97" s="69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G97" s="67"/>
@@ -4696,15 +4714,15 @@
       <c r="J97" s="67"/>
     </row>
     <row r="98" spans="1:10">
-      <c r="A98" s="85"/>
+      <c r="A98" s="84"/>
       <c r="B98" s="27">
-        <v>41661</v>
+        <v>41660</v>
       </c>
       <c r="C98" s="69"/>
       <c r="D98" s="69"/>
       <c r="E98" s="69"/>
       <c r="F98" s="69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G98" s="67"/>
@@ -4713,15 +4731,15 @@
       <c r="J98" s="67"/>
     </row>
     <row r="99" spans="1:10">
-      <c r="A99" s="85"/>
+      <c r="A99" s="84"/>
       <c r="B99" s="27">
-        <v>41662</v>
+        <v>41661</v>
       </c>
       <c r="C99" s="69"/>
       <c r="D99" s="69"/>
       <c r="E99" s="69"/>
       <c r="F99" s="69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G99" s="67"/>
@@ -4732,13 +4750,13 @@
     <row r="100" spans="1:10">
       <c r="A100" s="84"/>
       <c r="B100" s="27">
-        <v>41663</v>
+        <v>41662</v>
       </c>
       <c r="C100" s="69"/>
       <c r="D100" s="69"/>
       <c r="E100" s="69"/>
       <c r="F100" s="69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G100" s="67"/>
@@ -4747,36 +4765,34 @@
       <c r="J100" s="67"/>
     </row>
     <row r="101" spans="1:10">
-      <c r="A101" s="144">
+      <c r="A101" s="85"/>
+      <c r="B101" s="27">
+        <v>41663</v>
+      </c>
+      <c r="C101" s="69"/>
+      <c r="D101" s="69"/>
+      <c r="E101" s="69"/>
+      <c r="F101" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G101" s="67"/>
+      <c r="H101" s="67"/>
+      <c r="I101" s="67"/>
+      <c r="J101" s="67"/>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="86">
         <v>13</v>
       </c>
-      <c r="B101" s="26">
+      <c r="B102" s="26">
         <v>41666</v>
-      </c>
-      <c r="C101" s="55"/>
-      <c r="D101" s="55"/>
-      <c r="E101" s="55"/>
-      <c r="F101" s="55">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G101" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="H101" s="29"/>
-      <c r="I101" s="29"/>
-      <c r="J101" s="29"/>
-    </row>
-    <row r="102" spans="1:10">
-      <c r="A102" s="145"/>
-      <c r="B102" s="26">
-        <v>41667</v>
       </c>
       <c r="C102" s="55"/>
       <c r="D102" s="55"/>
       <c r="E102" s="55"/>
       <c r="F102" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G102" s="29" t="s">
@@ -4787,15 +4803,15 @@
       <c r="J102" s="29"/>
     </row>
     <row r="103" spans="1:10">
-      <c r="A103" s="145"/>
+      <c r="A103" s="87"/>
       <c r="B103" s="26">
-        <v>41668</v>
+        <v>41667</v>
       </c>
       <c r="C103" s="55"/>
       <c r="D103" s="55"/>
       <c r="E103" s="55"/>
       <c r="F103" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G103" s="29" t="s">
@@ -4806,15 +4822,15 @@
       <c r="J103" s="29"/>
     </row>
     <row r="104" spans="1:10">
-      <c r="A104" s="145"/>
+      <c r="A104" s="87"/>
       <c r="B104" s="26">
-        <v>41669</v>
+        <v>41668</v>
       </c>
       <c r="C104" s="55"/>
       <c r="D104" s="55"/>
       <c r="E104" s="55"/>
       <c r="F104" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G104" s="29" t="s">
@@ -4825,15 +4841,15 @@
       <c r="J104" s="29"/>
     </row>
     <row r="105" spans="1:10">
-      <c r="A105" s="139"/>
+      <c r="A105" s="87"/>
       <c r="B105" s="26">
-        <v>41670</v>
+        <v>41669</v>
       </c>
       <c r="C105" s="55"/>
       <c r="D105" s="55"/>
       <c r="E105" s="55"/>
       <c r="F105" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G105" s="29" t="s">
@@ -4844,36 +4860,36 @@
       <c r="J105" s="29"/>
     </row>
     <row r="106" spans="1:10">
-      <c r="A106" s="83">
+      <c r="A106" s="88"/>
+      <c r="B106" s="26">
+        <v>41670</v>
+      </c>
+      <c r="C106" s="55"/>
+      <c r="D106" s="55"/>
+      <c r="E106" s="55"/>
+      <c r="F106" s="55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G106" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="H106" s="29"/>
+      <c r="I106" s="29"/>
+      <c r="J106" s="29"/>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107" s="83">
         <v>14</v>
       </c>
-      <c r="B106" s="27">
+      <c r="B107" s="27">
         <v>41673</v>
-      </c>
-      <c r="C106" s="69"/>
-      <c r="D106" s="69"/>
-      <c r="E106" s="69"/>
-      <c r="F106" s="69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G106" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="H106" s="67"/>
-      <c r="I106" s="67"/>
-      <c r="J106" s="67"/>
-    </row>
-    <row r="107" spans="1:10">
-      <c r="A107" s="85"/>
-      <c r="B107" s="27">
-        <v>41674</v>
       </c>
       <c r="C107" s="69"/>
       <c r="D107" s="69"/>
       <c r="E107" s="69"/>
       <c r="F107" s="69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G107" s="37" t="s">
@@ -4884,15 +4900,15 @@
       <c r="J107" s="67"/>
     </row>
     <row r="108" spans="1:10">
-      <c r="A108" s="85"/>
+      <c r="A108" s="84"/>
       <c r="B108" s="27">
-        <v>41675</v>
+        <v>41674</v>
       </c>
       <c r="C108" s="69"/>
       <c r="D108" s="69"/>
       <c r="E108" s="69"/>
       <c r="F108" s="69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G108" s="37" t="s">
@@ -4903,15 +4919,15 @@
       <c r="J108" s="67"/>
     </row>
     <row r="109" spans="1:10">
-      <c r="A109" s="85"/>
+      <c r="A109" s="84"/>
       <c r="B109" s="27">
-        <v>41676</v>
+        <v>41675</v>
       </c>
       <c r="C109" s="69"/>
       <c r="D109" s="69"/>
       <c r="E109" s="69"/>
       <c r="F109" s="69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G109" s="37" t="s">
@@ -4924,13 +4940,13 @@
     <row r="110" spans="1:10">
       <c r="A110" s="84"/>
       <c r="B110" s="27">
-        <v>41677</v>
+        <v>41676</v>
       </c>
       <c r="C110" s="69"/>
       <c r="D110" s="69"/>
       <c r="E110" s="69"/>
       <c r="F110" s="69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G110" s="37" t="s">
@@ -4941,34 +4957,36 @@
       <c r="J110" s="67"/>
     </row>
     <row r="111" spans="1:10">
-      <c r="A111" s="144">
+      <c r="A111" s="85"/>
+      <c r="B111" s="27">
+        <v>41677</v>
+      </c>
+      <c r="C111" s="69"/>
+      <c r="D111" s="69"/>
+      <c r="E111" s="69"/>
+      <c r="F111" s="69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G111" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="H111" s="67"/>
+      <c r="I111" s="67"/>
+      <c r="J111" s="67"/>
+    </row>
+    <row r="112" spans="1:10">
+      <c r="A112" s="86">
         <v>15</v>
       </c>
-      <c r="B111" s="26">
+      <c r="B112" s="26">
         <v>41680</v>
-      </c>
-      <c r="C111" s="55"/>
-      <c r="D111" s="55"/>
-      <c r="E111" s="55"/>
-      <c r="F111" s="55">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G111" s="29"/>
-      <c r="H111" s="29"/>
-      <c r="I111" s="29"/>
-      <c r="J111" s="29"/>
-    </row>
-    <row r="112" spans="1:10">
-      <c r="A112" s="145"/>
-      <c r="B112" s="26">
-        <v>41681</v>
       </c>
       <c r="C112" s="55"/>
       <c r="D112" s="55"/>
       <c r="E112" s="55"/>
       <c r="F112" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G112" s="29"/>
@@ -4977,15 +4995,15 @@
       <c r="J112" s="29"/>
     </row>
     <row r="113" spans="1:10">
-      <c r="A113" s="145"/>
+      <c r="A113" s="87"/>
       <c r="B113" s="26">
-        <v>41682</v>
+        <v>41681</v>
       </c>
       <c r="C113" s="55"/>
       <c r="D113" s="55"/>
       <c r="E113" s="55"/>
       <c r="F113" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G113" s="29"/>
@@ -4994,15 +5012,15 @@
       <c r="J113" s="29"/>
     </row>
     <row r="114" spans="1:10">
-      <c r="A114" s="145"/>
+      <c r="A114" s="87"/>
       <c r="B114" s="26">
-        <v>41683</v>
+        <v>41682</v>
       </c>
       <c r="C114" s="55"/>
       <c r="D114" s="55"/>
       <c r="E114" s="55"/>
       <c r="F114" s="55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G114" s="29"/>
@@ -5011,15 +5029,15 @@
       <c r="J114" s="29"/>
     </row>
     <row r="115" spans="1:10">
-      <c r="A115" s="139"/>
+      <c r="A115" s="87"/>
       <c r="B115" s="26">
-        <v>41684</v>
+        <v>41683</v>
       </c>
       <c r="C115" s="55"/>
       <c r="D115" s="55"/>
       <c r="E115" s="55"/>
       <c r="F115" s="55">
-        <f t="shared" ref="F115:F146" si="3">E115</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G115" s="29"/>
@@ -5028,34 +5046,34 @@
       <c r="J115" s="29"/>
     </row>
     <row r="116" spans="1:10">
-      <c r="A116" s="83">
+      <c r="A116" s="88"/>
+      <c r="B116" s="26">
+        <v>41684</v>
+      </c>
+      <c r="C116" s="55"/>
+      <c r="D116" s="55"/>
+      <c r="E116" s="55"/>
+      <c r="F116" s="55">
+        <f t="shared" ref="F116:F147" si="2">E116</f>
+        <v>0</v>
+      </c>
+      <c r="G116" s="29"/>
+      <c r="H116" s="29"/>
+      <c r="I116" s="29"/>
+      <c r="J116" s="29"/>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" s="83">
         <v>16</v>
       </c>
-      <c r="B116" s="27">
+      <c r="B117" s="27">
         <v>41687</v>
-      </c>
-      <c r="C116" s="69"/>
-      <c r="D116" s="69"/>
-      <c r="E116" s="69"/>
-      <c r="F116" s="69">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G116" s="67"/>
-      <c r="H116" s="67"/>
-      <c r="I116" s="67"/>
-      <c r="J116" s="67"/>
-    </row>
-    <row r="117" spans="1:10">
-      <c r="A117" s="85"/>
-      <c r="B117" s="27">
-        <v>41688</v>
       </c>
       <c r="C117" s="69"/>
       <c r="D117" s="69"/>
       <c r="E117" s="69"/>
       <c r="F117" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G117" s="67"/>
@@ -5064,15 +5082,15 @@
       <c r="J117" s="67"/>
     </row>
     <row r="118" spans="1:10">
-      <c r="A118" s="85"/>
+      <c r="A118" s="84"/>
       <c r="B118" s="27">
-        <v>41689</v>
+        <v>41688</v>
       </c>
       <c r="C118" s="69"/>
       <c r="D118" s="69"/>
       <c r="E118" s="69"/>
       <c r="F118" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G118" s="67"/>
@@ -5081,15 +5099,15 @@
       <c r="J118" s="67"/>
     </row>
     <row r="119" spans="1:10">
-      <c r="A119" s="85"/>
+      <c r="A119" s="84"/>
       <c r="B119" s="27">
-        <v>41690</v>
+        <v>41689</v>
       </c>
       <c r="C119" s="69"/>
       <c r="D119" s="69"/>
       <c r="E119" s="69"/>
       <c r="F119" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G119" s="67"/>
@@ -5100,13 +5118,13 @@
     <row r="120" spans="1:10">
       <c r="A120" s="84"/>
       <c r="B120" s="27">
-        <v>41691</v>
+        <v>41690</v>
       </c>
       <c r="C120" s="69"/>
       <c r="D120" s="69"/>
       <c r="E120" s="69"/>
       <c r="F120" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G120" s="67"/>
@@ -5115,34 +5133,34 @@
       <c r="J120" s="67"/>
     </row>
     <row r="121" spans="1:10">
-      <c r="A121" s="144">
+      <c r="A121" s="85"/>
+      <c r="B121" s="27">
+        <v>41691</v>
+      </c>
+      <c r="C121" s="69"/>
+      <c r="D121" s="69"/>
+      <c r="E121" s="69"/>
+      <c r="F121" s="69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G121" s="67"/>
+      <c r="H121" s="67"/>
+      <c r="I121" s="67"/>
+      <c r="J121" s="67"/>
+    </row>
+    <row r="122" spans="1:10">
+      <c r="A122" s="86">
         <v>17</v>
       </c>
-      <c r="B121" s="26">
+      <c r="B122" s="26">
         <v>41694</v>
-      </c>
-      <c r="C121" s="55"/>
-      <c r="D121" s="55"/>
-      <c r="E121" s="55"/>
-      <c r="F121" s="55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G121" s="29"/>
-      <c r="H121" s="29"/>
-      <c r="I121" s="29"/>
-      <c r="J121" s="29"/>
-    </row>
-    <row r="122" spans="1:10">
-      <c r="A122" s="145"/>
-      <c r="B122" s="26">
-        <v>41695</v>
       </c>
       <c r="C122" s="55"/>
       <c r="D122" s="55"/>
       <c r="E122" s="55"/>
       <c r="F122" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G122" s="29"/>
@@ -5151,15 +5169,15 @@
       <c r="J122" s="29"/>
     </row>
     <row r="123" spans="1:10">
-      <c r="A123" s="145"/>
+      <c r="A123" s="87"/>
       <c r="B123" s="26">
-        <v>41696</v>
+        <v>41695</v>
       </c>
       <c r="C123" s="55"/>
       <c r="D123" s="55"/>
       <c r="E123" s="55"/>
       <c r="F123" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G123" s="29"/>
@@ -5168,15 +5186,15 @@
       <c r="J123" s="29"/>
     </row>
     <row r="124" spans="1:10">
-      <c r="A124" s="145"/>
+      <c r="A124" s="87"/>
       <c r="B124" s="26">
-        <v>41697</v>
+        <v>41696</v>
       </c>
       <c r="C124" s="55"/>
       <c r="D124" s="55"/>
       <c r="E124" s="55"/>
       <c r="F124" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G124" s="29"/>
@@ -5185,15 +5203,15 @@
       <c r="J124" s="29"/>
     </row>
     <row r="125" spans="1:10">
-      <c r="A125" s="139"/>
+      <c r="A125" s="87"/>
       <c r="B125" s="26">
-        <v>41698</v>
+        <v>41697</v>
       </c>
       <c r="C125" s="55"/>
       <c r="D125" s="55"/>
       <c r="E125" s="55"/>
       <c r="F125" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G125" s="29"/>
@@ -5202,34 +5220,34 @@
       <c r="J125" s="29"/>
     </row>
     <row r="126" spans="1:10">
-      <c r="A126" s="83">
+      <c r="A126" s="88"/>
+      <c r="B126" s="26">
+        <v>41698</v>
+      </c>
+      <c r="C126" s="55"/>
+      <c r="D126" s="55"/>
+      <c r="E126" s="55"/>
+      <c r="F126" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G126" s="29"/>
+      <c r="H126" s="29"/>
+      <c r="I126" s="29"/>
+      <c r="J126" s="29"/>
+    </row>
+    <row r="127" spans="1:10">
+      <c r="A127" s="83">
         <v>18</v>
       </c>
-      <c r="B126" s="27">
+      <c r="B127" s="27">
         <v>41701</v>
-      </c>
-      <c r="C126" s="69"/>
-      <c r="D126" s="69"/>
-      <c r="E126" s="69"/>
-      <c r="F126" s="69">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G126" s="67"/>
-      <c r="H126" s="67"/>
-      <c r="I126" s="67"/>
-      <c r="J126" s="67"/>
-    </row>
-    <row r="127" spans="1:10">
-      <c r="A127" s="85"/>
-      <c r="B127" s="27">
-        <v>41702</v>
       </c>
       <c r="C127" s="69"/>
       <c r="D127" s="69"/>
       <c r="E127" s="69"/>
       <c r="F127" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G127" s="67"/>
@@ -5238,15 +5256,15 @@
       <c r="J127" s="67"/>
     </row>
     <row r="128" spans="1:10">
-      <c r="A128" s="85"/>
+      <c r="A128" s="84"/>
       <c r="B128" s="27">
-        <v>41703</v>
+        <v>41702</v>
       </c>
       <c r="C128" s="69"/>
       <c r="D128" s="69"/>
       <c r="E128" s="69"/>
       <c r="F128" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G128" s="67"/>
@@ -5255,15 +5273,15 @@
       <c r="J128" s="67"/>
     </row>
     <row r="129" spans="1:10">
-      <c r="A129" s="85"/>
+      <c r="A129" s="84"/>
       <c r="B129" s="27">
-        <v>41704</v>
+        <v>41703</v>
       </c>
       <c r="C129" s="69"/>
       <c r="D129" s="69"/>
       <c r="E129" s="69"/>
       <c r="F129" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G129" s="67"/>
@@ -5274,13 +5292,13 @@
     <row r="130" spans="1:10">
       <c r="A130" s="84"/>
       <c r="B130" s="27">
-        <v>41705</v>
+        <v>41704</v>
       </c>
       <c r="C130" s="69"/>
       <c r="D130" s="69"/>
       <c r="E130" s="69"/>
       <c r="F130" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G130" s="67"/>
@@ -5289,34 +5307,34 @@
       <c r="J130" s="67"/>
     </row>
     <row r="131" spans="1:10">
-      <c r="A131" s="144">
+      <c r="A131" s="85"/>
+      <c r="B131" s="27">
+        <v>41705</v>
+      </c>
+      <c r="C131" s="69"/>
+      <c r="D131" s="69"/>
+      <c r="E131" s="69"/>
+      <c r="F131" s="69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G131" s="67"/>
+      <c r="H131" s="67"/>
+      <c r="I131" s="67"/>
+      <c r="J131" s="67"/>
+    </row>
+    <row r="132" spans="1:10">
+      <c r="A132" s="86">
         <v>19</v>
       </c>
-      <c r="B131" s="26">
+      <c r="B132" s="26">
         <v>41708</v>
-      </c>
-      <c r="C131" s="55"/>
-      <c r="D131" s="55"/>
-      <c r="E131" s="55"/>
-      <c r="F131" s="55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G131" s="29"/>
-      <c r="H131" s="29"/>
-      <c r="I131" s="29"/>
-      <c r="J131" s="29"/>
-    </row>
-    <row r="132" spans="1:10">
-      <c r="A132" s="145"/>
-      <c r="B132" s="26">
-        <v>41709</v>
       </c>
       <c r="C132" s="55"/>
       <c r="D132" s="55"/>
       <c r="E132" s="55"/>
       <c r="F132" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G132" s="29"/>
@@ -5325,15 +5343,15 @@
       <c r="J132" s="29"/>
     </row>
     <row r="133" spans="1:10">
-      <c r="A133" s="145"/>
+      <c r="A133" s="87"/>
       <c r="B133" s="26">
-        <v>41710</v>
+        <v>41709</v>
       </c>
       <c r="C133" s="55"/>
       <c r="D133" s="55"/>
       <c r="E133" s="55"/>
       <c r="F133" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G133" s="29"/>
@@ -5342,15 +5360,15 @@
       <c r="J133" s="29"/>
     </row>
     <row r="134" spans="1:10">
-      <c r="A134" s="145"/>
+      <c r="A134" s="87"/>
       <c r="B134" s="26">
-        <v>41711</v>
+        <v>41710</v>
       </c>
       <c r="C134" s="55"/>
       <c r="D134" s="55"/>
       <c r="E134" s="55"/>
       <c r="F134" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G134" s="29"/>
@@ -5359,15 +5377,15 @@
       <c r="J134" s="29"/>
     </row>
     <row r="135" spans="1:10">
-      <c r="A135" s="139"/>
+      <c r="A135" s="87"/>
       <c r="B135" s="26">
-        <v>41712</v>
+        <v>41711</v>
       </c>
       <c r="C135" s="55"/>
       <c r="D135" s="55"/>
       <c r="E135" s="55"/>
       <c r="F135" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G135" s="29"/>
@@ -5376,34 +5394,34 @@
       <c r="J135" s="29"/>
     </row>
     <row r="136" spans="1:10">
-      <c r="A136" s="83">
+      <c r="A136" s="88"/>
+      <c r="B136" s="26">
+        <v>41712</v>
+      </c>
+      <c r="C136" s="55"/>
+      <c r="D136" s="55"/>
+      <c r="E136" s="55"/>
+      <c r="F136" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G136" s="29"/>
+      <c r="H136" s="29"/>
+      <c r="I136" s="29"/>
+      <c r="J136" s="29"/>
+    </row>
+    <row r="137" spans="1:10">
+      <c r="A137" s="83">
         <v>20</v>
       </c>
-      <c r="B136" s="27">
+      <c r="B137" s="27">
         <v>41715</v>
-      </c>
-      <c r="C136" s="69"/>
-      <c r="D136" s="69"/>
-      <c r="E136" s="69"/>
-      <c r="F136" s="69">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G136" s="67"/>
-      <c r="H136" s="67"/>
-      <c r="I136" s="67"/>
-      <c r="J136" s="67"/>
-    </row>
-    <row r="137" spans="1:10">
-      <c r="A137" s="85"/>
-      <c r="B137" s="27">
-        <v>41716</v>
       </c>
       <c r="C137" s="69"/>
       <c r="D137" s="69"/>
       <c r="E137" s="69"/>
       <c r="F137" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G137" s="67"/>
@@ -5412,15 +5430,15 @@
       <c r="J137" s="67"/>
     </row>
     <row r="138" spans="1:10">
-      <c r="A138" s="85"/>
+      <c r="A138" s="84"/>
       <c r="B138" s="27">
-        <v>41717</v>
+        <v>41716</v>
       </c>
       <c r="C138" s="69"/>
       <c r="D138" s="69"/>
       <c r="E138" s="69"/>
       <c r="F138" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G138" s="67"/>
@@ -5429,15 +5447,15 @@
       <c r="J138" s="67"/>
     </row>
     <row r="139" spans="1:10">
-      <c r="A139" s="85"/>
+      <c r="A139" s="84"/>
       <c r="B139" s="27">
-        <v>41718</v>
+        <v>41717</v>
       </c>
       <c r="C139" s="69"/>
       <c r="D139" s="69"/>
       <c r="E139" s="69"/>
       <c r="F139" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G139" s="67"/>
@@ -5448,13 +5466,13 @@
     <row r="140" spans="1:10">
       <c r="A140" s="84"/>
       <c r="B140" s="27">
-        <v>41719</v>
+        <v>41718</v>
       </c>
       <c r="C140" s="69"/>
       <c r="D140" s="69"/>
       <c r="E140" s="69"/>
       <c r="F140" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G140" s="67"/>
@@ -5463,34 +5481,34 @@
       <c r="J140" s="67"/>
     </row>
     <row r="141" spans="1:10">
-      <c r="A141" s="144">
+      <c r="A141" s="85"/>
+      <c r="B141" s="27">
+        <v>41719</v>
+      </c>
+      <c r="C141" s="69"/>
+      <c r="D141" s="69"/>
+      <c r="E141" s="69"/>
+      <c r="F141" s="69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G141" s="67"/>
+      <c r="H141" s="67"/>
+      <c r="I141" s="67"/>
+      <c r="J141" s="67"/>
+    </row>
+    <row r="142" spans="1:10">
+      <c r="A142" s="86">
         <v>21</v>
       </c>
-      <c r="B141" s="26">
+      <c r="B142" s="26">
         <v>41722</v>
-      </c>
-      <c r="C141" s="55"/>
-      <c r="D141" s="55"/>
-      <c r="E141" s="55"/>
-      <c r="F141" s="55">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G141" s="29"/>
-      <c r="H141" s="29"/>
-      <c r="I141" s="29"/>
-      <c r="J141" s="29"/>
-    </row>
-    <row r="142" spans="1:10">
-      <c r="A142" s="145"/>
-      <c r="B142" s="26">
-        <v>41723</v>
       </c>
       <c r="C142" s="55"/>
       <c r="D142" s="55"/>
       <c r="E142" s="55"/>
       <c r="F142" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G142" s="29"/>
@@ -5499,15 +5517,15 @@
       <c r="J142" s="29"/>
     </row>
     <row r="143" spans="1:10">
-      <c r="A143" s="145"/>
+      <c r="A143" s="87"/>
       <c r="B143" s="26">
-        <v>41724</v>
+        <v>41723</v>
       </c>
       <c r="C143" s="55"/>
       <c r="D143" s="55"/>
       <c r="E143" s="55"/>
       <c r="F143" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G143" s="29"/>
@@ -5516,15 +5534,15 @@
       <c r="J143" s="29"/>
     </row>
     <row r="144" spans="1:10">
-      <c r="A144" s="145"/>
+      <c r="A144" s="87"/>
       <c r="B144" s="26">
-        <v>41725</v>
+        <v>41724</v>
       </c>
       <c r="C144" s="55"/>
       <c r="D144" s="55"/>
       <c r="E144" s="55"/>
       <c r="F144" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G144" s="29"/>
@@ -5533,15 +5551,15 @@
       <c r="J144" s="29"/>
     </row>
     <row r="145" spans="1:10">
-      <c r="A145" s="139"/>
+      <c r="A145" s="87"/>
       <c r="B145" s="26">
-        <v>41726</v>
+        <v>41725</v>
       </c>
       <c r="C145" s="55"/>
       <c r="D145" s="55"/>
       <c r="E145" s="55"/>
       <c r="F145" s="55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G145" s="29"/>
@@ -5550,34 +5568,34 @@
       <c r="J145" s="29"/>
     </row>
     <row r="146" spans="1:10">
-      <c r="A146" s="83">
+      <c r="A146" s="88"/>
+      <c r="B146" s="26">
+        <v>41726</v>
+      </c>
+      <c r="C146" s="55"/>
+      <c r="D146" s="55"/>
+      <c r="E146" s="55"/>
+      <c r="F146" s="55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G146" s="29"/>
+      <c r="H146" s="29"/>
+      <c r="I146" s="29"/>
+      <c r="J146" s="29"/>
+    </row>
+    <row r="147" spans="1:10">
+      <c r="A147" s="83">
         <v>22</v>
       </c>
-      <c r="B146" s="27">
+      <c r="B147" s="27">
         <v>41729</v>
-      </c>
-      <c r="C146" s="69"/>
-      <c r="D146" s="69"/>
-      <c r="E146" s="69"/>
-      <c r="F146" s="69">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G146" s="67"/>
-      <c r="H146" s="67"/>
-      <c r="I146" s="67"/>
-      <c r="J146" s="67"/>
-    </row>
-    <row r="147" spans="1:10">
-      <c r="A147" s="85"/>
-      <c r="B147" s="27">
-        <v>41730</v>
       </c>
       <c r="C147" s="69"/>
       <c r="D147" s="69"/>
       <c r="E147" s="69"/>
       <c r="F147" s="69">
-        <f t="shared" ref="F147:F178" si="4">E147</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G147" s="67"/>
@@ -5586,15 +5604,15 @@
       <c r="J147" s="67"/>
     </row>
     <row r="148" spans="1:10">
-      <c r="A148" s="85"/>
+      <c r="A148" s="84"/>
       <c r="B148" s="27">
-        <v>41731</v>
+        <v>41730</v>
       </c>
       <c r="C148" s="69"/>
       <c r="D148" s="69"/>
       <c r="E148" s="69"/>
       <c r="F148" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F148:F179" si="3">E148</f>
         <v>0</v>
       </c>
       <c r="G148" s="67"/>
@@ -5603,15 +5621,15 @@
       <c r="J148" s="67"/>
     </row>
     <row r="149" spans="1:10">
-      <c r="A149" s="85"/>
+      <c r="A149" s="84"/>
       <c r="B149" s="27">
-        <v>41732</v>
+        <v>41731</v>
       </c>
       <c r="C149" s="69"/>
       <c r="D149" s="69"/>
       <c r="E149" s="69"/>
       <c r="F149" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G149" s="67"/>
@@ -5622,13 +5640,13 @@
     <row r="150" spans="1:10">
       <c r="A150" s="84"/>
       <c r="B150" s="27">
-        <v>41733</v>
+        <v>41732</v>
       </c>
       <c r="C150" s="69"/>
       <c r="D150" s="69"/>
       <c r="E150" s="69"/>
       <c r="F150" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G150" s="67"/>
@@ -5637,34 +5655,34 @@
       <c r="J150" s="67"/>
     </row>
     <row r="151" spans="1:10">
-      <c r="A151" s="144">
+      <c r="A151" s="85"/>
+      <c r="B151" s="27">
+        <v>41733</v>
+      </c>
+      <c r="C151" s="69"/>
+      <c r="D151" s="69"/>
+      <c r="E151" s="69"/>
+      <c r="F151" s="69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G151" s="67"/>
+      <c r="H151" s="67"/>
+      <c r="I151" s="67"/>
+      <c r="J151" s="67"/>
+    </row>
+    <row r="152" spans="1:10">
+      <c r="A152" s="86">
         <v>23</v>
       </c>
-      <c r="B151" s="26">
+      <c r="B152" s="26">
         <v>41736</v>
-      </c>
-      <c r="C151" s="55"/>
-      <c r="D151" s="55"/>
-      <c r="E151" s="55"/>
-      <c r="F151" s="55">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G151" s="29"/>
-      <c r="H151" s="29"/>
-      <c r="I151" s="29"/>
-      <c r="J151" s="29"/>
-    </row>
-    <row r="152" spans="1:10">
-      <c r="A152" s="145"/>
-      <c r="B152" s="26">
-        <v>41737</v>
       </c>
       <c r="C152" s="55"/>
       <c r="D152" s="55"/>
       <c r="E152" s="55"/>
       <c r="F152" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G152" s="29"/>
@@ -5673,15 +5691,15 @@
       <c r="J152" s="29"/>
     </row>
     <row r="153" spans="1:10">
-      <c r="A153" s="145"/>
+      <c r="A153" s="87"/>
       <c r="B153" s="26">
-        <v>41738</v>
+        <v>41737</v>
       </c>
       <c r="C153" s="55"/>
       <c r="D153" s="55"/>
       <c r="E153" s="55"/>
       <c r="F153" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G153" s="29"/>
@@ -5690,15 +5708,15 @@
       <c r="J153" s="29"/>
     </row>
     <row r="154" spans="1:10">
-      <c r="A154" s="145"/>
+      <c r="A154" s="87"/>
       <c r="B154" s="26">
-        <v>41739</v>
+        <v>41738</v>
       </c>
       <c r="C154" s="55"/>
       <c r="D154" s="55"/>
       <c r="E154" s="55"/>
       <c r="F154" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G154" s="29"/>
@@ -5707,15 +5725,15 @@
       <c r="J154" s="29"/>
     </row>
     <row r="155" spans="1:10">
-      <c r="A155" s="139"/>
+      <c r="A155" s="87"/>
       <c r="B155" s="26">
-        <v>41740</v>
+        <v>41739</v>
       </c>
       <c r="C155" s="55"/>
       <c r="D155" s="55"/>
       <c r="E155" s="55"/>
       <c r="F155" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G155" s="29"/>
@@ -5724,34 +5742,34 @@
       <c r="J155" s="29"/>
     </row>
     <row r="156" spans="1:10">
-      <c r="A156" s="83">
+      <c r="A156" s="88"/>
+      <c r="B156" s="26">
+        <v>41740</v>
+      </c>
+      <c r="C156" s="55"/>
+      <c r="D156" s="55"/>
+      <c r="E156" s="55"/>
+      <c r="F156" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G156" s="29"/>
+      <c r="H156" s="29"/>
+      <c r="I156" s="29"/>
+      <c r="J156" s="29"/>
+    </row>
+    <row r="157" spans="1:10">
+      <c r="A157" s="83">
         <v>24</v>
       </c>
-      <c r="B156" s="27">
+      <c r="B157" s="27">
         <v>41743</v>
-      </c>
-      <c r="C156" s="69"/>
-      <c r="D156" s="69"/>
-      <c r="E156" s="69"/>
-      <c r="F156" s="69">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G156" s="67"/>
-      <c r="H156" s="67"/>
-      <c r="I156" s="67"/>
-      <c r="J156" s="67"/>
-    </row>
-    <row r="157" spans="1:10">
-      <c r="A157" s="85"/>
-      <c r="B157" s="27">
-        <v>41744</v>
       </c>
       <c r="C157" s="69"/>
       <c r="D157" s="69"/>
       <c r="E157" s="69"/>
       <c r="F157" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G157" s="67"/>
@@ -5760,15 +5778,15 @@
       <c r="J157" s="67"/>
     </row>
     <row r="158" spans="1:10">
-      <c r="A158" s="85"/>
+      <c r="A158" s="84"/>
       <c r="B158" s="27">
-        <v>41745</v>
+        <v>41744</v>
       </c>
       <c r="C158" s="69"/>
       <c r="D158" s="69"/>
       <c r="E158" s="69"/>
       <c r="F158" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G158" s="67"/>
@@ -5777,15 +5795,15 @@
       <c r="J158" s="67"/>
     </row>
     <row r="159" spans="1:10">
-      <c r="A159" s="85"/>
+      <c r="A159" s="84"/>
       <c r="B159" s="27">
-        <v>41746</v>
+        <v>41745</v>
       </c>
       <c r="C159" s="69"/>
       <c r="D159" s="69"/>
       <c r="E159" s="69"/>
       <c r="F159" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G159" s="67"/>
@@ -5796,13 +5814,13 @@
     <row r="160" spans="1:10">
       <c r="A160" s="84"/>
       <c r="B160" s="27">
-        <v>41747</v>
+        <v>41746</v>
       </c>
       <c r="C160" s="69"/>
       <c r="D160" s="69"/>
       <c r="E160" s="69"/>
       <c r="F160" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G160" s="67"/>
@@ -5811,34 +5829,34 @@
       <c r="J160" s="67"/>
     </row>
     <row r="161" spans="1:10">
-      <c r="A161" s="144">
+      <c r="A161" s="85"/>
+      <c r="B161" s="27">
+        <v>41747</v>
+      </c>
+      <c r="C161" s="69"/>
+      <c r="D161" s="69"/>
+      <c r="E161" s="69"/>
+      <c r="F161" s="69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G161" s="67"/>
+      <c r="H161" s="67"/>
+      <c r="I161" s="67"/>
+      <c r="J161" s="67"/>
+    </row>
+    <row r="162" spans="1:10">
+      <c r="A162" s="86">
         <v>25</v>
       </c>
-      <c r="B161" s="26">
+      <c r="B162" s="26">
         <v>41750</v>
-      </c>
-      <c r="C161" s="55"/>
-      <c r="D161" s="55"/>
-      <c r="E161" s="55"/>
-      <c r="F161" s="55">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G161" s="29"/>
-      <c r="H161" s="29"/>
-      <c r="I161" s="29"/>
-      <c r="J161" s="29"/>
-    </row>
-    <row r="162" spans="1:10">
-      <c r="A162" s="145"/>
-      <c r="B162" s="26">
-        <v>41751</v>
       </c>
       <c r="C162" s="55"/>
       <c r="D162" s="55"/>
       <c r="E162" s="55"/>
       <c r="F162" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G162" s="29"/>
@@ -5847,15 +5865,15 @@
       <c r="J162" s="29"/>
     </row>
     <row r="163" spans="1:10">
-      <c r="A163" s="145"/>
+      <c r="A163" s="87"/>
       <c r="B163" s="26">
-        <v>41752</v>
+        <v>41751</v>
       </c>
       <c r="C163" s="55"/>
       <c r="D163" s="55"/>
       <c r="E163" s="55"/>
       <c r="F163" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G163" s="29"/>
@@ -5864,15 +5882,15 @@
       <c r="J163" s="29"/>
     </row>
     <row r="164" spans="1:10">
-      <c r="A164" s="145"/>
+      <c r="A164" s="87"/>
       <c r="B164" s="26">
-        <v>41753</v>
+        <v>41752</v>
       </c>
       <c r="C164" s="55"/>
       <c r="D164" s="55"/>
       <c r="E164" s="55"/>
       <c r="F164" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G164" s="29"/>
@@ -5881,15 +5899,15 @@
       <c r="J164" s="29"/>
     </row>
     <row r="165" spans="1:10">
-      <c r="A165" s="139"/>
+      <c r="A165" s="87"/>
       <c r="B165" s="26">
-        <v>41754</v>
+        <v>41753</v>
       </c>
       <c r="C165" s="55"/>
       <c r="D165" s="55"/>
       <c r="E165" s="55"/>
       <c r="F165" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G165" s="29"/>
@@ -5898,34 +5916,34 @@
       <c r="J165" s="29"/>
     </row>
     <row r="166" spans="1:10">
-      <c r="A166" s="83">
+      <c r="A166" s="88"/>
+      <c r="B166" s="26">
+        <v>41754</v>
+      </c>
+      <c r="C166" s="55"/>
+      <c r="D166" s="55"/>
+      <c r="E166" s="55"/>
+      <c r="F166" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G166" s="29"/>
+      <c r="H166" s="29"/>
+      <c r="I166" s="29"/>
+      <c r="J166" s="29"/>
+    </row>
+    <row r="167" spans="1:10">
+      <c r="A167" s="83">
         <v>26</v>
       </c>
-      <c r="B166" s="27">
+      <c r="B167" s="27">
         <v>41757</v>
-      </c>
-      <c r="C166" s="69"/>
-      <c r="D166" s="69"/>
-      <c r="E166" s="69"/>
-      <c r="F166" s="69">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G166" s="67"/>
-      <c r="H166" s="67"/>
-      <c r="I166" s="67"/>
-      <c r="J166" s="67"/>
-    </row>
-    <row r="167" spans="1:10">
-      <c r="A167" s="85"/>
-      <c r="B167" s="27">
-        <v>41758</v>
       </c>
       <c r="C167" s="69"/>
       <c r="D167" s="69"/>
       <c r="E167" s="69"/>
       <c r="F167" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G167" s="67"/>
@@ -5934,15 +5952,15 @@
       <c r="J167" s="67"/>
     </row>
     <row r="168" spans="1:10">
-      <c r="A168" s="85"/>
+      <c r="A168" s="84"/>
       <c r="B168" s="27">
-        <v>41759</v>
+        <v>41758</v>
       </c>
       <c r="C168" s="69"/>
       <c r="D168" s="69"/>
       <c r="E168" s="69"/>
       <c r="F168" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G168" s="67"/>
@@ -5951,15 +5969,15 @@
       <c r="J168" s="67"/>
     </row>
     <row r="169" spans="1:10">
-      <c r="A169" s="85"/>
+      <c r="A169" s="84"/>
       <c r="B169" s="27">
-        <v>41760</v>
+        <v>41759</v>
       </c>
       <c r="C169" s="69"/>
       <c r="D169" s="69"/>
       <c r="E169" s="69"/>
       <c r="F169" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G169" s="67"/>
@@ -5970,13 +5988,13 @@
     <row r="170" spans="1:10">
       <c r="A170" s="84"/>
       <c r="B170" s="27">
-        <v>41761</v>
+        <v>41760</v>
       </c>
       <c r="C170" s="69"/>
       <c r="D170" s="69"/>
       <c r="E170" s="69"/>
       <c r="F170" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G170" s="67"/>
@@ -5985,34 +6003,34 @@
       <c r="J170" s="67"/>
     </row>
     <row r="171" spans="1:10">
-      <c r="A171" s="144">
+      <c r="A171" s="85"/>
+      <c r="B171" s="27">
+        <v>41761</v>
+      </c>
+      <c r="C171" s="69"/>
+      <c r="D171" s="69"/>
+      <c r="E171" s="69"/>
+      <c r="F171" s="69">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G171" s="67"/>
+      <c r="H171" s="67"/>
+      <c r="I171" s="67"/>
+      <c r="J171" s="67"/>
+    </row>
+    <row r="172" spans="1:10">
+      <c r="A172" s="86">
         <v>27</v>
       </c>
-      <c r="B171" s="26">
+      <c r="B172" s="26">
         <v>41764</v>
-      </c>
-      <c r="C171" s="55"/>
-      <c r="D171" s="55"/>
-      <c r="E171" s="55"/>
-      <c r="F171" s="55">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G171" s="29"/>
-      <c r="H171" s="29"/>
-      <c r="I171" s="29"/>
-      <c r="J171" s="29"/>
-    </row>
-    <row r="172" spans="1:10">
-      <c r="A172" s="145"/>
-      <c r="B172" s="26">
-        <v>41765</v>
       </c>
       <c r="C172" s="55"/>
       <c r="D172" s="55"/>
       <c r="E172" s="55"/>
       <c r="F172" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G172" s="29"/>
@@ -6021,15 +6039,15 @@
       <c r="J172" s="29"/>
     </row>
     <row r="173" spans="1:10">
-      <c r="A173" s="145"/>
+      <c r="A173" s="87"/>
       <c r="B173" s="26">
-        <v>41766</v>
+        <v>41765</v>
       </c>
       <c r="C173" s="55"/>
       <c r="D173" s="55"/>
       <c r="E173" s="55"/>
       <c r="F173" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G173" s="29"/>
@@ -6038,15 +6056,15 @@
       <c r="J173" s="29"/>
     </row>
     <row r="174" spans="1:10">
-      <c r="A174" s="145"/>
+      <c r="A174" s="87"/>
       <c r="B174" s="26">
-        <v>41767</v>
+        <v>41766</v>
       </c>
       <c r="C174" s="55"/>
       <c r="D174" s="55"/>
       <c r="E174" s="55"/>
       <c r="F174" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G174" s="29"/>
@@ -6055,15 +6073,15 @@
       <c r="J174" s="29"/>
     </row>
     <row r="175" spans="1:10">
-      <c r="A175" s="139"/>
+      <c r="A175" s="87"/>
       <c r="B175" s="26">
-        <v>41768</v>
+        <v>41767</v>
       </c>
       <c r="C175" s="55"/>
       <c r="D175" s="55"/>
       <c r="E175" s="55"/>
       <c r="F175" s="55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G175" s="29"/>
@@ -6072,34 +6090,34 @@
       <c r="J175" s="29"/>
     </row>
     <row r="176" spans="1:10">
-      <c r="A176" s="83">
+      <c r="A176" s="88"/>
+      <c r="B176" s="26">
+        <v>41768</v>
+      </c>
+      <c r="C176" s="55"/>
+      <c r="D176" s="55"/>
+      <c r="E176" s="55"/>
+      <c r="F176" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G176" s="29"/>
+      <c r="H176" s="29"/>
+      <c r="I176" s="29"/>
+      <c r="J176" s="29"/>
+    </row>
+    <row r="177" spans="1:10">
+      <c r="A177" s="83">
         <v>28</v>
       </c>
-      <c r="B176" s="27">
+      <c r="B177" s="27">
         <v>41771</v>
-      </c>
-      <c r="C176" s="69"/>
-      <c r="D176" s="69"/>
-      <c r="E176" s="69"/>
-      <c r="F176" s="69">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G176" s="67"/>
-      <c r="H176" s="67"/>
-      <c r="I176" s="67"/>
-      <c r="J176" s="67"/>
-    </row>
-    <row r="177" spans="1:10">
-      <c r="A177" s="85"/>
-      <c r="B177" s="27">
-        <v>41772</v>
       </c>
       <c r="C177" s="69"/>
       <c r="D177" s="69"/>
       <c r="E177" s="69"/>
       <c r="F177" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G177" s="67"/>
@@ -6108,15 +6126,15 @@
       <c r="J177" s="67"/>
     </row>
     <row r="178" spans="1:10">
-      <c r="A178" s="85"/>
+      <c r="A178" s="84"/>
       <c r="B178" s="27">
-        <v>41773</v>
+        <v>41772</v>
       </c>
       <c r="C178" s="69"/>
       <c r="D178" s="69"/>
       <c r="E178" s="69"/>
       <c r="F178" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G178" s="67"/>
@@ -6125,15 +6143,15 @@
       <c r="J178" s="67"/>
     </row>
     <row r="179" spans="1:10">
-      <c r="A179" s="85"/>
+      <c r="A179" s="84"/>
       <c r="B179" s="27">
-        <v>41774</v>
+        <v>41773</v>
       </c>
       <c r="C179" s="69"/>
       <c r="D179" s="69"/>
       <c r="E179" s="69"/>
       <c r="F179" s="69">
-        <f t="shared" ref="F179:F190" si="5">E179</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G179" s="67"/>
@@ -6144,13 +6162,13 @@
     <row r="180" spans="1:10">
       <c r="A180" s="84"/>
       <c r="B180" s="27">
-        <v>41775</v>
+        <v>41774</v>
       </c>
       <c r="C180" s="69"/>
       <c r="D180" s="69"/>
       <c r="E180" s="69"/>
       <c r="F180" s="69">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="F180:F191" si="4">E180</f>
         <v>0</v>
       </c>
       <c r="G180" s="67"/>
@@ -6159,34 +6177,34 @@
       <c r="J180" s="67"/>
     </row>
     <row r="181" spans="1:10">
-      <c r="A181" s="144">
+      <c r="A181" s="85"/>
+      <c r="B181" s="27">
+        <v>41775</v>
+      </c>
+      <c r="C181" s="69"/>
+      <c r="D181" s="69"/>
+      <c r="E181" s="69"/>
+      <c r="F181" s="69">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G181" s="67"/>
+      <c r="H181" s="67"/>
+      <c r="I181" s="67"/>
+      <c r="J181" s="67"/>
+    </row>
+    <row r="182" spans="1:10">
+      <c r="A182" s="86">
         <v>29</v>
       </c>
-      <c r="B181" s="26">
+      <c r="B182" s="26">
         <v>41778</v>
-      </c>
-      <c r="C181" s="55"/>
-      <c r="D181" s="55"/>
-      <c r="E181" s="55"/>
-      <c r="F181" s="55">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G181" s="29"/>
-      <c r="H181" s="29"/>
-      <c r="I181" s="29"/>
-      <c r="J181" s="29"/>
-    </row>
-    <row r="182" spans="1:10">
-      <c r="A182" s="145"/>
-      <c r="B182" s="26">
-        <v>41779</v>
       </c>
       <c r="C182" s="55"/>
       <c r="D182" s="55"/>
       <c r="E182" s="55"/>
       <c r="F182" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G182" s="29"/>
@@ -6195,15 +6213,15 @@
       <c r="J182" s="29"/>
     </row>
     <row r="183" spans="1:10">
-      <c r="A183" s="145"/>
+      <c r="A183" s="87"/>
       <c r="B183" s="26">
-        <v>41780</v>
+        <v>41779</v>
       </c>
       <c r="C183" s="55"/>
       <c r="D183" s="55"/>
       <c r="E183" s="55"/>
       <c r="F183" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G183" s="29"/>
@@ -6212,15 +6230,15 @@
       <c r="J183" s="29"/>
     </row>
     <row r="184" spans="1:10">
-      <c r="A184" s="145"/>
+      <c r="A184" s="87"/>
       <c r="B184" s="26">
-        <v>41781</v>
+        <v>41780</v>
       </c>
       <c r="C184" s="55"/>
       <c r="D184" s="55"/>
       <c r="E184" s="55"/>
       <c r="F184" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G184" s="29"/>
@@ -6229,15 +6247,15 @@
       <c r="J184" s="29"/>
     </row>
     <row r="185" spans="1:10">
-      <c r="A185" s="139"/>
+      <c r="A185" s="87"/>
       <c r="B185" s="26">
-        <v>41782</v>
+        <v>41781</v>
       </c>
       <c r="C185" s="55"/>
       <c r="D185" s="55"/>
       <c r="E185" s="55"/>
       <c r="F185" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G185" s="29"/>
@@ -6246,34 +6264,34 @@
       <c r="J185" s="29"/>
     </row>
     <row r="186" spans="1:10">
-      <c r="A186" s="146">
+      <c r="A186" s="88"/>
+      <c r="B186" s="26">
+        <v>41782</v>
+      </c>
+      <c r="C186" s="55"/>
+      <c r="D186" s="55"/>
+      <c r="E186" s="55"/>
+      <c r="F186" s="55">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G186" s="29"/>
+      <c r="H186" s="29"/>
+      <c r="I186" s="29"/>
+      <c r="J186" s="29"/>
+    </row>
+    <row r="187" spans="1:10">
+      <c r="A187" s="89">
         <v>30</v>
       </c>
-      <c r="B186" s="27">
+      <c r="B187" s="27">
         <v>41785</v>
-      </c>
-      <c r="C186" s="70"/>
-      <c r="D186" s="70"/>
-      <c r="E186" s="70"/>
-      <c r="F186" s="70">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G186" s="37"/>
-      <c r="H186" s="37"/>
-      <c r="I186" s="37"/>
-      <c r="J186" s="37"/>
-    </row>
-    <row r="187" spans="1:10">
-      <c r="A187" s="147"/>
-      <c r="B187" s="27">
-        <v>41786</v>
       </c>
       <c r="C187" s="70"/>
       <c r="D187" s="70"/>
       <c r="E187" s="70"/>
       <c r="F187" s="70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G187" s="37"/>
@@ -6282,15 +6300,15 @@
       <c r="J187" s="37"/>
     </row>
     <row r="188" spans="1:10">
-      <c r="A188" s="147"/>
+      <c r="A188" s="90"/>
       <c r="B188" s="27">
-        <v>41787</v>
+        <v>41786</v>
       </c>
       <c r="C188" s="70"/>
       <c r="D188" s="70"/>
       <c r="E188" s="70"/>
       <c r="F188" s="70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G188" s="37"/>
@@ -6299,15 +6317,15 @@
       <c r="J188" s="37"/>
     </row>
     <row r="189" spans="1:10">
-      <c r="A189" s="147"/>
+      <c r="A189" s="90"/>
       <c r="B189" s="27">
-        <v>41788</v>
+        <v>41787</v>
       </c>
       <c r="C189" s="70"/>
       <c r="D189" s="70"/>
       <c r="E189" s="70"/>
       <c r="F189" s="70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G189" s="37"/>
@@ -6316,15 +6334,15 @@
       <c r="J189" s="37"/>
     </row>
     <row r="190" spans="1:10">
-      <c r="A190" s="148"/>
+      <c r="A190" s="90"/>
       <c r="B190" s="27">
-        <v>41789</v>
+        <v>41788</v>
       </c>
       <c r="C190" s="70"/>
       <c r="D190" s="70"/>
       <c r="E190" s="70"/>
       <c r="F190" s="70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G190" s="37"/>
@@ -6333,16 +6351,21 @@
       <c r="J190" s="37"/>
     </row>
     <row r="191" spans="1:10">
-      <c r="A191" s="68"/>
-      <c r="B191" s="68"/>
-      <c r="C191" s="68"/>
-      <c r="D191" s="68"/>
-      <c r="E191" s="68"/>
-      <c r="F191" s="68"/>
-      <c r="G191" s="68"/>
-      <c r="H191" s="68"/>
-      <c r="I191" s="68"/>
-      <c r="J191" s="68"/>
+      <c r="A191" s="91"/>
+      <c r="B191" s="27">
+        <v>41789</v>
+      </c>
+      <c r="C191" s="70"/>
+      <c r="D191" s="70"/>
+      <c r="E191" s="70"/>
+      <c r="F191" s="70">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G191" s="37"/>
+      <c r="H191" s="37"/>
+      <c r="I191" s="37"/>
+      <c r="J191" s="37"/>
     </row>
     <row r="192" spans="1:10">
       <c r="A192" s="68"/>
@@ -6440,54 +6463,21 @@
       <c r="I199" s="68"/>
       <c r="J199" s="68"/>
     </row>
+    <row r="200" spans="1:10">
+      <c r="A200" s="68"/>
+      <c r="B200" s="68"/>
+      <c r="C200" s="68"/>
+      <c r="D200" s="68"/>
+      <c r="E200" s="68"/>
+      <c r="F200" s="68"/>
+      <c r="G200" s="68"/>
+      <c r="H200" s="68"/>
+      <c r="I200" s="68"/>
+      <c r="J200" s="68"/>
+    </row>
   </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="A60:A69"/>
-    <mergeCell ref="A176:A180"/>
-    <mergeCell ref="A181:A185"/>
-    <mergeCell ref="A186:A190"/>
-    <mergeCell ref="A146:A150"/>
-    <mergeCell ref="A151:A155"/>
-    <mergeCell ref="A156:A160"/>
-    <mergeCell ref="A161:A165"/>
-    <mergeCell ref="A166:A170"/>
-    <mergeCell ref="A70:A75"/>
-    <mergeCell ref="A86:A90"/>
-    <mergeCell ref="A101:A105"/>
-    <mergeCell ref="A106:A110"/>
-    <mergeCell ref="A47:A59"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="A171:A175"/>
-    <mergeCell ref="A126:A130"/>
-    <mergeCell ref="A131:A135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A145"/>
-    <mergeCell ref="F48:F50"/>
-    <mergeCell ref="F51:F53"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A120"/>
-    <mergeCell ref="A121:A125"/>
-    <mergeCell ref="A96:A100"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="A81:A85"/>
-    <mergeCell ref="A91:A95"/>
-    <mergeCell ref="A34:A46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="A19:A33"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="F14:F16"/>
+  <mergeCells count="63">
+    <mergeCell ref="F71:F73"/>
     <mergeCell ref="F67:F68"/>
     <mergeCell ref="F64:F66"/>
     <mergeCell ref="F60:F61"/>
@@ -6504,18 +6494,64 @@
     <mergeCell ref="A10:A18"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="F10:F11"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="A34:A46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A19:A33"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="A47:A59"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A172:A176"/>
+    <mergeCell ref="A127:A131"/>
+    <mergeCell ref="A132:A136"/>
+    <mergeCell ref="A137:A141"/>
+    <mergeCell ref="A142:A146"/>
+    <mergeCell ref="F48:F50"/>
+    <mergeCell ref="F51:F53"/>
+    <mergeCell ref="A112:A116"/>
+    <mergeCell ref="A117:A121"/>
+    <mergeCell ref="A122:A126"/>
+    <mergeCell ref="A97:A101"/>
+    <mergeCell ref="A77:A81"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="A92:A96"/>
+    <mergeCell ref="A60:A69"/>
+    <mergeCell ref="A177:A181"/>
+    <mergeCell ref="A182:A186"/>
+    <mergeCell ref="A187:A191"/>
+    <mergeCell ref="A147:A151"/>
+    <mergeCell ref="A152:A156"/>
+    <mergeCell ref="A157:A161"/>
+    <mergeCell ref="A162:A166"/>
+    <mergeCell ref="A167:A171"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A87:A91"/>
+    <mergeCell ref="A102:A106"/>
+    <mergeCell ref="A107:A111"/>
   </mergeCells>
   <conditionalFormatting sqref="M7">
-    <cfRule type="cellIs" dxfId="3" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="16" operator="greaterThan">
       <formula>5000</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="17" operator="lessThan">
       <formula>700</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="18" operator="greaterThan">
       <formula>4704</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="19" operator="between">
       <formula>700</formula>
       <formula>4704</formula>
     </cfRule>
@@ -6529,7 +6565,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="51" id="{0DBDD361-8DEA-4440-A822-84D52DAF7126}">
+          <x14:cfRule type="iconSet" priority="52" id="{0DBDD361-8DEA-4440-A822-84D52DAF7126}">
             <x14:iconSet iconSet="3Symbols" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6548,7 +6584,7 @@
           <xm:sqref>M12:M14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="50" id="{B559C907-CDCA-4CF9-AE11-AB3B902CAD1C}">
+          <x14:cfRule type="iconSet" priority="51" id="{B559C907-CDCA-4CF9-AE11-AB3B902CAD1C}">
             <x14:iconSet iconSet="3Symbols" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6567,7 +6603,7 @@
           <xm:sqref>M16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="48" id="{71646626-2950-4450-989F-AF3A1BD8FAC2}">
+          <x14:cfRule type="iconSet" priority="49" id="{71646626-2950-4450-989F-AF3A1BD8FAC2}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6586,7 +6622,7 @@
           <xm:sqref>M18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="45" id="{F3D4927F-C508-4AEC-AE77-5B47D8246C97}">
+          <x14:cfRule type="iconSet" priority="46" id="{F3D4927F-C508-4AEC-AE77-5B47D8246C97}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6605,7 +6641,7 @@
           <xm:sqref>M19:M21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="44" id="{6C6B1EFA-99FD-4C7D-9FDE-A1C62DFDC4A6}">
+          <x14:cfRule type="iconSet" priority="45" id="{6C6B1EFA-99FD-4C7D-9FDE-A1C62DFDC4A6}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6624,7 +6660,7 @@
           <xm:sqref>M22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="43" id="{728DDD0C-59C2-4EAA-A943-37D530A87696}">
+          <x14:cfRule type="iconSet" priority="44" id="{728DDD0C-59C2-4EAA-A943-37D530A87696}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6643,7 +6679,7 @@
           <xm:sqref>M23:M26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="42" id="{9AF6B611-56EC-46E2-A851-4E09E28F0C39}">
+          <x14:cfRule type="iconSet" priority="43" id="{9AF6B611-56EC-46E2-A851-4E09E28F0C39}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6662,7 +6698,7 @@
           <xm:sqref>M27:M29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="41" id="{7A1C8DB1-F7B5-44DF-B6AD-BD94518E2F59}">
+          <x14:cfRule type="iconSet" priority="42" id="{7A1C8DB1-F7B5-44DF-B6AD-BD94518E2F59}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6681,7 +6717,7 @@
           <xm:sqref>M30:M33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="40" id="{798FB9D7-6FEF-4CEA-8CC2-45EE73486721}">
+          <x14:cfRule type="iconSet" priority="41" id="{798FB9D7-6FEF-4CEA-8CC2-45EE73486721}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6700,7 +6736,7 @@
           <xm:sqref>M34:M37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="39" id="{9D5A3639-C9C5-40BD-82EE-496926295966}">
+          <x14:cfRule type="iconSet" priority="40" id="{9D5A3639-C9C5-40BD-82EE-496926295966}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6719,7 +6755,7 @@
           <xm:sqref>M38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="38" id="{042E6B91-B838-419B-9746-9D04172CBCE2}">
+          <x14:cfRule type="iconSet" priority="39" id="{042E6B91-B838-419B-9746-9D04172CBCE2}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6738,7 +6774,7 @@
           <xm:sqref>M39:M42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="37" id="{87212A6D-7255-4CD9-B0F3-3C906F80977E}">
+          <x14:cfRule type="iconSet" priority="38" id="{87212A6D-7255-4CD9-B0F3-3C906F80977E}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6757,7 +6793,7 @@
           <xm:sqref>M43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="36" id="{BEBCA1A1-AA3F-4294-8922-9827332C0668}">
+          <x14:cfRule type="iconSet" priority="37" id="{BEBCA1A1-AA3F-4294-8922-9827332C0668}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6776,7 +6812,7 @@
           <xm:sqref>M44:M46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="35" id="{3793385C-190C-4A90-AF72-EEE9712F504F}">
+          <x14:cfRule type="iconSet" priority="36" id="{3793385C-190C-4A90-AF72-EEE9712F504F}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6795,7 +6831,7 @@
           <xm:sqref>M47:M48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="34" id="{21C6FD3D-522C-4661-AE5D-284F6FC787D0}">
+          <x14:cfRule type="iconSet" priority="35" id="{21C6FD3D-522C-4661-AE5D-284F6FC787D0}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6814,7 +6850,7 @@
           <xm:sqref>M49:M50</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="33" id="{09871DA7-81C7-4675-89F3-BE2EDB05B9C9}">
+          <x14:cfRule type="iconSet" priority="34" id="{09871DA7-81C7-4675-89F3-BE2EDB05B9C9}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6833,7 +6869,7 @@
           <xm:sqref>M51:M57</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="32" id="{50D35A91-6584-4A00-B008-2B93AA187052}">
+          <x14:cfRule type="iconSet" priority="33" id="{50D35A91-6584-4A00-B008-2B93AA187052}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6852,7 +6888,7 @@
           <xm:sqref>M58</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="31" id="{10AA0BAB-E7C1-450C-B7A5-276ADB69B0B2}">
+          <x14:cfRule type="iconSet" priority="32" id="{10AA0BAB-E7C1-450C-B7A5-276ADB69B0B2}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6871,7 +6907,7 @@
           <xm:sqref>M59</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="30" id="{0A1ADE65-D185-454C-92B2-B6FA367CBA04}">
+          <x14:cfRule type="iconSet" priority="31" id="{0A1ADE65-D185-454C-92B2-B6FA367CBA04}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6890,7 +6926,7 @@
           <xm:sqref>M60:M61</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="29" id="{E0DFC09D-C053-4D3D-A1C1-C5AF640FB5CD}">
+          <x14:cfRule type="iconSet" priority="30" id="{E0DFC09D-C053-4D3D-A1C1-C5AF640FB5CD}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6909,7 +6945,7 @@
           <xm:sqref>M62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="28" id="{F1B6F2BC-B2AE-42D9-8427-52A717AE39CD}">
+          <x14:cfRule type="iconSet" priority="29" id="{F1B6F2BC-B2AE-42D9-8427-52A717AE39CD}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6928,7 +6964,7 @@
           <xm:sqref>M63:M65</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="27" id="{EEF8AB81-584A-4839-AEE8-98BCAAB29DD2}">
+          <x14:cfRule type="iconSet" priority="28" id="{EEF8AB81-584A-4839-AEE8-98BCAAB29DD2}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6947,7 +6983,7 @@
           <xm:sqref>M66:M67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="26" id="{A1F90B4F-0784-43A3-A2A1-2A7C9438EE1A}">
+          <x14:cfRule type="iconSet" priority="27" id="{A1F90B4F-0784-43A3-A2A1-2A7C9438EE1A}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6966,7 +7002,7 @@
           <xm:sqref>M68:M69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="25" id="{CDF48798-0C78-453D-9E98-93D1BB3C878A}">
+          <x14:cfRule type="iconSet" priority="26" id="{CDF48798-0C78-453D-9E98-93D1BB3C878A}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -6982,29 +7018,10 @@
               <x14:cfIcon iconSet="3Symbols" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>M70:M71</xm:sqref>
+          <xm:sqref>M70:M72</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="24" id="{524804E6-2BBA-4071-AB71-18BD193B4497}">
-            <x14:iconSet custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>25</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num" gte="0">
-                <xm:f>168</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols" iconId="1"/>
-              <x14:cfIcon iconSet="3Symbols" iconId="2"/>
-              <x14:cfIcon iconSet="3Symbols" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>M72</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="23" id="{F466D4E3-91DB-49AA-8E5A-7BD04BE8813F}">
+          <x14:cfRule type="iconSet" priority="25" id="{524804E6-2BBA-4071-AB71-18BD193B4497}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7023,7 +7040,26 @@
           <xm:sqref>M73</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="22" id="{C4227F9F-08CD-4A7C-B706-2C35F19616E7}">
+          <x14:cfRule type="iconSet" priority="24" id="{F466D4E3-91DB-49AA-8E5A-7BD04BE8813F}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>25</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>168</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols" iconId="1"/>
+              <x14:cfIcon iconSet="3Symbols" iconId="2"/>
+              <x14:cfIcon iconSet="3Symbols" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>M74</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="23" id="{C4227F9F-08CD-4A7C-B706-2C35F19616E7}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7042,7 +7078,7 @@
           <xm:sqref>M8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="14" id="{6C49D5EC-FFC3-40B5-BEF3-C08FEAABBFA7}">
+          <x14:cfRule type="iconSet" priority="15" id="{6C49D5EC-FFC3-40B5-BEF3-C08FEAABBFA7}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7061,7 +7097,7 @@
           <xm:sqref>F17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="12" id="{13950B4A-31F8-40DD-922D-DC2CA60F3002}">
+          <x14:cfRule type="iconSet" priority="13" id="{13950B4A-31F8-40DD-922D-DC2CA60F3002}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7080,7 +7116,7 @@
           <xm:sqref>F10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="10" id="{35213755-788E-43C8-B75E-72DA17285D4A}">
+          <x14:cfRule type="iconSet" priority="11" id="{35213755-788E-43C8-B75E-72DA17285D4A}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7099,7 +7135,7 @@
           <xm:sqref>F31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="9" id="{D436B0D1-9C41-4290-A1C3-9BA213613E2C}">
+          <x14:cfRule type="iconSet" priority="10" id="{D436B0D1-9C41-4290-A1C3-9BA213613E2C}">
             <x14:iconSet iconSet="3Symbols" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7118,7 +7154,7 @@
           <xm:sqref>M17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="8" id="{814260D3-C9B5-4AD4-A23C-2BEE7D803396}">
+          <x14:cfRule type="iconSet" priority="9" id="{814260D3-C9B5-4AD4-A23C-2BEE7D803396}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7137,7 +7173,7 @@
           <xm:sqref>F41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="6" id="{DDA1B89F-47D5-4064-9758-21B8F5AF18F7}">
+          <x14:cfRule type="iconSet" priority="7" id="{DDA1B89F-47D5-4064-9758-21B8F5AF18F7}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7156,7 +7192,7 @@
           <xm:sqref>F48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="5" id="{D5E33E02-3F42-4321-B899-2604F055C762}">
+          <x14:cfRule type="iconSet" priority="6" id="{D5E33E02-3F42-4321-B899-2604F055C762}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7175,7 +7211,7 @@
           <xm:sqref>F54</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="55" id="{F4E0A23A-4149-4A2A-B8B1-3E1EE910632F}">
+          <x14:cfRule type="iconSet" priority="56" id="{F4E0A23A-4149-4A2A-B8B1-3E1EE910632F}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7191,10 +7227,10 @@
               <x14:cfIcon iconSet="3Symbols" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>F14 F7:F8 F12 F18:F19 F21 F23:F24 F29 F34:F35 F39 F44:F45 F47 F51 F59:F60 F72:F190 F67 F62:F64</xm:sqref>
+          <xm:sqref>F14 F7:F8 F12 F18:F19 F21 F23:F24 F29 F34:F35 F39 F44:F45 F47 F51 F59:F60 F74:F191 F67 F62:F64</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="3" id="{C53BB270-1B91-44C9-A614-EB8FD19B8FAB}">
+          <x14:cfRule type="iconSet" priority="4" id="{C53BB270-1B91-44C9-A614-EB8FD19B8FAB}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7213,7 +7249,7 @@
           <xm:sqref>F69</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{D5C65E63-B452-4133-B3D5-04E19AE90D5C}">
+          <x14:cfRule type="iconSet" priority="3" id="{D5C65E63-B452-4133-B3D5-04E19AE90D5C}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7232,7 +7268,7 @@
           <xm:sqref>F70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{08FB1A00-EF89-48D5-AB1A-304AB7CDE158}">
+          <x14:cfRule type="iconSet" priority="2" id="{08FB1A00-EF89-48D5-AB1A-304AB7CDE158}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>

</xml_diff>